<commit_message>
Fixing the date for Fundamentals
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,366 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>09.05.202414</t>
-  </si>
-  <si>
-    <t>09.05.202415</t>
-  </si>
-  <si>
-    <t>09.05.202416</t>
-  </si>
-  <si>
-    <t>09.05.202417</t>
-  </si>
-  <si>
-    <t>09.05.202418</t>
-  </si>
-  <si>
-    <t>09.05.202419</t>
-  </si>
-  <si>
-    <t>09.05.202420</t>
-  </si>
-  <si>
-    <t>09.05.202421</t>
-  </si>
-  <si>
-    <t>09.05.202422</t>
-  </si>
-  <si>
-    <t>09.05.202423</t>
-  </si>
-  <si>
-    <t>10.05.20240</t>
-  </si>
-  <si>
-    <t>10.05.20241</t>
-  </si>
-  <si>
-    <t>10.05.20242</t>
-  </si>
-  <si>
-    <t>10.05.20243</t>
-  </si>
-  <si>
-    <t>10.05.20244</t>
-  </si>
-  <si>
-    <t>10.05.20245</t>
-  </si>
-  <si>
-    <t>10.05.20246</t>
-  </si>
-  <si>
-    <t>10.05.20247</t>
-  </si>
-  <si>
-    <t>10.05.20248</t>
-  </si>
-  <si>
-    <t>10.05.20249</t>
-  </si>
-  <si>
-    <t>10.05.202410</t>
-  </si>
-  <si>
-    <t>10.05.202411</t>
-  </si>
-  <si>
-    <t>10.05.202412</t>
-  </si>
-  <si>
-    <t>10.05.202413</t>
-  </si>
-  <si>
-    <t>10.05.202414</t>
-  </si>
-  <si>
-    <t>10.05.202415</t>
-  </si>
-  <si>
-    <t>10.05.202416</t>
-  </si>
-  <si>
-    <t>10.05.202417</t>
-  </si>
-  <si>
-    <t>10.05.202418</t>
-  </si>
-  <si>
-    <t>10.05.202419</t>
-  </si>
-  <si>
-    <t>10.05.202420</t>
-  </si>
-  <si>
-    <t>10.05.202421</t>
-  </si>
-  <si>
-    <t>10.05.202422</t>
-  </si>
-  <si>
-    <t>10.05.202423</t>
-  </si>
-  <si>
-    <t>11.05.20240</t>
-  </si>
-  <si>
-    <t>11.05.20241</t>
-  </si>
-  <si>
-    <t>11.05.20242</t>
-  </si>
-  <si>
-    <t>11.05.20243</t>
-  </si>
-  <si>
-    <t>11.05.20244</t>
-  </si>
-  <si>
-    <t>11.05.20245</t>
-  </si>
-  <si>
-    <t>11.05.20246</t>
-  </si>
-  <si>
-    <t>11.05.20247</t>
-  </si>
-  <si>
-    <t>11.05.20248</t>
-  </si>
-  <si>
-    <t>11.05.20249</t>
-  </si>
-  <si>
-    <t>11.05.202410</t>
-  </si>
-  <si>
-    <t>11.05.202411</t>
-  </si>
-  <si>
-    <t>11.05.202412</t>
-  </si>
-  <si>
-    <t>11.05.202413</t>
-  </si>
-  <si>
-    <t>11.05.202414</t>
-  </si>
-  <si>
-    <t>11.05.202415</t>
-  </si>
-  <si>
-    <t>11.05.202416</t>
-  </si>
-  <si>
-    <t>11.05.202417</t>
-  </si>
-  <si>
-    <t>11.05.202418</t>
-  </si>
-  <si>
-    <t>11.05.202419</t>
-  </si>
-  <si>
-    <t>11.05.202420</t>
-  </si>
-  <si>
-    <t>11.05.202421</t>
-  </si>
-  <si>
-    <t>11.05.202422</t>
-  </si>
-  <si>
-    <t>11.05.202423</t>
-  </si>
-  <si>
-    <t>12.05.20240</t>
-  </si>
-  <si>
-    <t>12.05.20241</t>
-  </si>
-  <si>
-    <t>12.05.20242</t>
-  </si>
-  <si>
-    <t>12.05.20243</t>
-  </si>
-  <si>
-    <t>12.05.20244</t>
-  </si>
-  <si>
-    <t>12.05.20245</t>
-  </si>
-  <si>
-    <t>12.05.20246</t>
-  </si>
-  <si>
-    <t>12.05.20247</t>
-  </si>
-  <si>
-    <t>12.05.20248</t>
-  </si>
-  <si>
-    <t>12.05.20249</t>
-  </si>
-  <si>
-    <t>12.05.202410</t>
-  </si>
-  <si>
-    <t>12.05.202411</t>
-  </si>
-  <si>
-    <t>12.05.202412</t>
-  </si>
-  <si>
-    <t>12.05.202413</t>
-  </si>
-  <si>
-    <t>12.05.202414</t>
-  </si>
-  <si>
-    <t>12.05.202415</t>
-  </si>
-  <si>
-    <t>12.05.202416</t>
-  </si>
-  <si>
-    <t>12.05.202417</t>
-  </si>
-  <si>
-    <t>12.05.202418</t>
-  </si>
-  <si>
-    <t>12.05.202419</t>
-  </si>
-  <si>
-    <t>12.05.202420</t>
-  </si>
-  <si>
-    <t>12.05.202421</t>
-  </si>
-  <si>
-    <t>12.05.202422</t>
-  </si>
-  <si>
-    <t>12.05.202423</t>
-  </si>
-  <si>
-    <t>13.05.20240</t>
-  </si>
-  <si>
-    <t>13.05.20241</t>
-  </si>
-  <si>
-    <t>13.05.20242</t>
-  </si>
-  <si>
-    <t>13.05.20243</t>
-  </si>
-  <si>
-    <t>13.05.20244</t>
-  </si>
-  <si>
-    <t>13.05.20245</t>
-  </si>
-  <si>
-    <t>13.05.20246</t>
-  </si>
-  <si>
-    <t>13.05.20247</t>
-  </si>
-  <si>
-    <t>13.05.20248</t>
-  </si>
-  <si>
-    <t>13.05.20249</t>
-  </si>
-  <si>
-    <t>13.05.202410</t>
-  </si>
-  <si>
-    <t>13.05.202411</t>
-  </si>
-  <si>
-    <t>13.05.202412</t>
-  </si>
-  <si>
-    <t>13.05.202413</t>
-  </si>
-  <si>
-    <t>13.05.202414</t>
-  </si>
-  <si>
-    <t>13.05.202415</t>
-  </si>
-  <si>
-    <t>13.05.202416</t>
-  </si>
-  <si>
-    <t>13.05.202417</t>
-  </si>
-  <si>
-    <t>13.05.202418</t>
-  </si>
-  <si>
-    <t>13.05.202419</t>
-  </si>
-  <si>
-    <t>13.05.202420</t>
-  </si>
-  <si>
-    <t>13.05.202421</t>
-  </si>
-  <si>
-    <t>13.05.202422</t>
-  </si>
-  <si>
-    <t>13.05.202423</t>
-  </si>
-  <si>
-    <t>14.05.20240</t>
-  </si>
-  <si>
-    <t>14.05.20241</t>
-  </si>
-  <si>
-    <t>14.05.20242</t>
-  </si>
-  <si>
-    <t>14.05.20243</t>
-  </si>
-  <si>
-    <t>14.05.20244</t>
-  </si>
-  <si>
-    <t>14.05.20245</t>
-  </si>
-  <si>
-    <t>14.05.20246</t>
-  </si>
-  <si>
-    <t>14.05.20247</t>
-  </si>
-  <si>
-    <t>14.05.20248</t>
-  </si>
-  <si>
-    <t>14.05.20249</t>
-  </si>
-  <si>
-    <t>14.05.202410</t>
-  </si>
-  <si>
-    <t>14.05.202411</t>
-  </si>
-  <si>
-    <t>14.05.202412</t>
-  </si>
-  <si>
-    <t>14.05.202413</t>
-  </si>
-  <si>
     <t>14.05.202414</t>
   </si>
   <si>
@@ -533,6 +173,366 @@
   </si>
   <si>
     <t>16.05.202414</t>
+  </si>
+  <si>
+    <t>16.05.202415</t>
+  </si>
+  <si>
+    <t>16.05.202416</t>
+  </si>
+  <si>
+    <t>16.05.202417</t>
+  </si>
+  <si>
+    <t>16.05.202418</t>
+  </si>
+  <si>
+    <t>16.05.202419</t>
+  </si>
+  <si>
+    <t>16.05.202420</t>
+  </si>
+  <si>
+    <t>16.05.202421</t>
+  </si>
+  <si>
+    <t>16.05.202422</t>
+  </si>
+  <si>
+    <t>16.05.202423</t>
+  </si>
+  <si>
+    <t>17.05.20240</t>
+  </si>
+  <si>
+    <t>17.05.20241</t>
+  </si>
+  <si>
+    <t>17.05.20242</t>
+  </si>
+  <si>
+    <t>17.05.20243</t>
+  </si>
+  <si>
+    <t>17.05.20244</t>
+  </si>
+  <si>
+    <t>17.05.20245</t>
+  </si>
+  <si>
+    <t>17.05.20246</t>
+  </si>
+  <si>
+    <t>17.05.20247</t>
+  </si>
+  <si>
+    <t>17.05.20248</t>
+  </si>
+  <si>
+    <t>17.05.20249</t>
+  </si>
+  <si>
+    <t>17.05.202410</t>
+  </si>
+  <si>
+    <t>17.05.202411</t>
+  </si>
+  <si>
+    <t>17.05.202412</t>
+  </si>
+  <si>
+    <t>17.05.202413</t>
+  </si>
+  <si>
+    <t>17.05.202414</t>
+  </si>
+  <si>
+    <t>17.05.202415</t>
+  </si>
+  <si>
+    <t>17.05.202416</t>
+  </si>
+  <si>
+    <t>17.05.202417</t>
+  </si>
+  <si>
+    <t>17.05.202418</t>
+  </si>
+  <si>
+    <t>17.05.202419</t>
+  </si>
+  <si>
+    <t>17.05.202420</t>
+  </si>
+  <si>
+    <t>17.05.202421</t>
+  </si>
+  <si>
+    <t>17.05.202422</t>
+  </si>
+  <si>
+    <t>17.05.202423</t>
+  </si>
+  <si>
+    <t>18.05.20240</t>
+  </si>
+  <si>
+    <t>18.05.20241</t>
+  </si>
+  <si>
+    <t>18.05.20242</t>
+  </si>
+  <si>
+    <t>18.05.20243</t>
+  </si>
+  <si>
+    <t>18.05.20244</t>
+  </si>
+  <si>
+    <t>18.05.20245</t>
+  </si>
+  <si>
+    <t>18.05.20246</t>
+  </si>
+  <si>
+    <t>18.05.20247</t>
+  </si>
+  <si>
+    <t>18.05.20248</t>
+  </si>
+  <si>
+    <t>18.05.20249</t>
+  </si>
+  <si>
+    <t>18.05.202410</t>
+  </si>
+  <si>
+    <t>18.05.202411</t>
+  </si>
+  <si>
+    <t>18.05.202412</t>
+  </si>
+  <si>
+    <t>18.05.202413</t>
+  </si>
+  <si>
+    <t>18.05.202414</t>
+  </si>
+  <si>
+    <t>18.05.202415</t>
+  </si>
+  <si>
+    <t>18.05.202416</t>
+  </si>
+  <si>
+    <t>18.05.202417</t>
+  </si>
+  <si>
+    <t>18.05.202418</t>
+  </si>
+  <si>
+    <t>18.05.202419</t>
+  </si>
+  <si>
+    <t>18.05.202420</t>
+  </si>
+  <si>
+    <t>18.05.202421</t>
+  </si>
+  <si>
+    <t>18.05.202422</t>
+  </si>
+  <si>
+    <t>18.05.202423</t>
+  </si>
+  <si>
+    <t>19.05.20240</t>
+  </si>
+  <si>
+    <t>19.05.20241</t>
+  </si>
+  <si>
+    <t>19.05.20242</t>
+  </si>
+  <si>
+    <t>19.05.20243</t>
+  </si>
+  <si>
+    <t>19.05.20244</t>
+  </si>
+  <si>
+    <t>19.05.20245</t>
+  </si>
+  <si>
+    <t>19.05.20246</t>
+  </si>
+  <si>
+    <t>19.05.20247</t>
+  </si>
+  <si>
+    <t>19.05.20248</t>
+  </si>
+  <si>
+    <t>19.05.20249</t>
+  </si>
+  <si>
+    <t>19.05.202410</t>
+  </si>
+  <si>
+    <t>19.05.202411</t>
+  </si>
+  <si>
+    <t>19.05.202412</t>
+  </si>
+  <si>
+    <t>19.05.202413</t>
+  </si>
+  <si>
+    <t>19.05.202414</t>
+  </si>
+  <si>
+    <t>19.05.202415</t>
+  </si>
+  <si>
+    <t>19.05.202416</t>
+  </si>
+  <si>
+    <t>19.05.202417</t>
+  </si>
+  <si>
+    <t>19.05.202418</t>
+  </si>
+  <si>
+    <t>19.05.202419</t>
+  </si>
+  <si>
+    <t>19.05.202420</t>
+  </si>
+  <si>
+    <t>19.05.202421</t>
+  </si>
+  <si>
+    <t>19.05.202422</t>
+  </si>
+  <si>
+    <t>19.05.202423</t>
+  </si>
+  <si>
+    <t>20.05.20240</t>
+  </si>
+  <si>
+    <t>20.05.20241</t>
+  </si>
+  <si>
+    <t>20.05.20242</t>
+  </si>
+  <si>
+    <t>20.05.20243</t>
+  </si>
+  <si>
+    <t>20.05.20244</t>
+  </si>
+  <si>
+    <t>20.05.20245</t>
+  </si>
+  <si>
+    <t>20.05.20246</t>
+  </si>
+  <si>
+    <t>20.05.20247</t>
+  </si>
+  <si>
+    <t>20.05.20248</t>
+  </si>
+  <si>
+    <t>20.05.20249</t>
+  </si>
+  <si>
+    <t>20.05.202410</t>
+  </si>
+  <si>
+    <t>20.05.202411</t>
+  </si>
+  <si>
+    <t>20.05.202412</t>
+  </si>
+  <si>
+    <t>20.05.202413</t>
+  </si>
+  <si>
+    <t>20.05.202414</t>
+  </si>
+  <si>
+    <t>20.05.202415</t>
+  </si>
+  <si>
+    <t>20.05.202416</t>
+  </si>
+  <si>
+    <t>20.05.202417</t>
+  </si>
+  <si>
+    <t>20.05.202418</t>
+  </si>
+  <si>
+    <t>20.05.202419</t>
+  </si>
+  <si>
+    <t>20.05.202420</t>
+  </si>
+  <si>
+    <t>20.05.202421</t>
+  </si>
+  <si>
+    <t>20.05.202422</t>
+  </si>
+  <si>
+    <t>20.05.202423</t>
+  </si>
+  <si>
+    <t>21.05.20240</t>
+  </si>
+  <si>
+    <t>21.05.20241</t>
+  </si>
+  <si>
+    <t>21.05.20242</t>
+  </si>
+  <si>
+    <t>21.05.20243</t>
+  </si>
+  <si>
+    <t>21.05.20244</t>
+  </si>
+  <si>
+    <t>21.05.20245</t>
+  </si>
+  <si>
+    <t>21.05.20246</t>
+  </si>
+  <si>
+    <t>21.05.20247</t>
+  </si>
+  <si>
+    <t>21.05.20248</t>
+  </si>
+  <si>
+    <t>21.05.20249</t>
+  </si>
+  <si>
+    <t>21.05.202410</t>
+  </si>
+  <si>
+    <t>21.05.202411</t>
+  </si>
+  <si>
+    <t>21.05.202412</t>
+  </si>
+  <si>
+    <t>21.05.202413</t>
+  </si>
+  <si>
+    <t>21.05.202414</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B4">
         <v>16</v>
       </c>
       <c r="C4">
-        <v>0.248</v>
+        <v>2.631</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
       <c r="C5">
-        <v>0.441</v>
+        <v>2.029</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B6">
         <v>18</v>
       </c>
       <c r="C6">
-        <v>0.385</v>
+        <v>1.161</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B7">
         <v>19</v>
       </c>
       <c r="C7">
-        <v>0.228</v>
+        <v>0.4</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
       <c r="C8">
-        <v>0.033</v>
+        <v>0.037</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B10">
         <v>22</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45421</v>
+        <v>45426</v>
       </c>
       <c r="B11">
         <v>23</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
       <c r="C18">
-        <v>0.077</v>
+        <v>0.083</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
       <c r="C19">
-        <v>0.409</v>
+        <v>0.414</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20">
-        <v>1.001</v>
+        <v>0.99</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B21">
         <v>9</v>
       </c>
       <c r="C21">
-        <v>1.71</v>
+        <v>1.598</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22">
-        <v>2.421</v>
+        <v>2.015</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B23">
         <v>11</v>
       </c>
       <c r="C23">
-        <v>3.102</v>
+        <v>2.805</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B24">
         <v>12</v>
       </c>
       <c r="C24">
-        <v>3.235</v>
+        <v>3.001</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B25">
         <v>13</v>
       </c>
       <c r="C25">
-        <v>3.243</v>
+        <v>3.143</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B26">
         <v>14</v>
       </c>
       <c r="C26">
-        <v>3.114</v>
+        <v>3.108</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B27">
         <v>15</v>
       </c>
       <c r="C27">
-        <v>2.581</v>
+        <v>2.903</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B28">
         <v>16</v>
       </c>
       <c r="C28">
-        <v>2.127</v>
+        <v>2.217</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B29">
         <v>17</v>
       </c>
       <c r="C29">
-        <v>1.69</v>
+        <v>1.919</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B30">
         <v>18</v>
       </c>
       <c r="C30">
-        <v>1.041</v>
+        <v>1.215</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B31">
         <v>19</v>
       </c>
       <c r="C31">
-        <v>0.332</v>
+        <v>0.398</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B32">
         <v>20</v>
       </c>
       <c r="C32">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B33">
         <v>21</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B34">
         <v>22</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45422</v>
+        <v>45427</v>
       </c>
       <c r="B35">
         <v>23</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B42">
         <v>6</v>
       </c>
       <c r="C42">
-        <v>0.076</v>
+        <v>0.102</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B43">
         <v>7</v>
       </c>
       <c r="C43">
-        <v>0.391</v>
+        <v>0.393</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B44">
         <v>8</v>
       </c>
       <c r="C44">
-        <v>1.261</v>
+        <v>1.026</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B45">
         <v>9</v>
       </c>
       <c r="C45">
-        <v>1.893</v>
+        <v>1.628</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B46">
         <v>10</v>
       </c>
       <c r="C46">
-        <v>2.352</v>
+        <v>2.147</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B47">
         <v>11</v>
       </c>
       <c r="C47">
-        <v>2.863</v>
+        <v>2.833</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B48">
         <v>12</v>
       </c>
       <c r="C48">
-        <v>2.857</v>
+        <v>2.931</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B49">
         <v>13</v>
       </c>
       <c r="C49">
-        <v>2.931</v>
+        <v>2.769</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B50">
         <v>14</v>
       </c>
       <c r="C50">
-        <v>2.654</v>
+        <v>2.733</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B51">
         <v>15</v>
       </c>
       <c r="C51">
-        <v>2.169</v>
+        <v>2.201</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B52">
         <v>16</v>
       </c>
       <c r="C52">
-        <v>1.878</v>
+        <v>1.773</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B53">
         <v>17</v>
       </c>
       <c r="C53">
-        <v>1.249</v>
+        <v>1.309</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B54">
         <v>18</v>
       </c>
       <c r="C54">
-        <v>0.706</v>
+        <v>0.803</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B55">
         <v>19</v>
       </c>
       <c r="C55">
-        <v>0.262</v>
+        <v>0.329</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B56">
         <v>20</v>
       </c>
       <c r="C56">
-        <v>0.033</v>
+        <v>0.037</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B57">
         <v>21</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B58">
         <v>22</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45423</v>
+        <v>45428</v>
       </c>
       <c r="B59">
         <v>23</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B66">
         <v>6</v>
       </c>
       <c r="C66">
-        <v>0.049</v>
+        <v>0.08</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B67">
         <v>7</v>
       </c>
       <c r="C67">
-        <v>0.229</v>
+        <v>0.41</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B68">
         <v>8</v>
       </c>
       <c r="C68">
-        <v>0.445</v>
+        <v>0.667</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B69">
         <v>9</v>
       </c>
       <c r="C69">
-        <v>0.923</v>
+        <v>1.021</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B70">
         <v>10</v>
       </c>
       <c r="C70">
-        <v>1.232</v>
+        <v>1.595</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B71">
         <v>11</v>
       </c>
       <c r="C71">
-        <v>1.292</v>
+        <v>1.846</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B72">
         <v>12</v>
       </c>
       <c r="C72">
-        <v>1.745</v>
+        <v>2.11</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B73">
         <v>13</v>
       </c>
       <c r="C73">
-        <v>1.964</v>
+        <v>2.034</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B74">
         <v>14</v>
       </c>
       <c r="C74">
-        <v>1.961</v>
+        <v>1.797</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B75">
         <v>15</v>
       </c>
       <c r="C75">
-        <v>1.765</v>
+        <v>1.421</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B76">
         <v>16</v>
       </c>
       <c r="C76">
-        <v>1.492</v>
+        <v>1.191</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B77">
         <v>17</v>
       </c>
       <c r="C77">
-        <v>0.925</v>
+        <v>0.844</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B78">
         <v>18</v>
       </c>
       <c r="C78">
-        <v>0.5570000000000001</v>
+        <v>0.433</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B79">
         <v>19</v>
       </c>
       <c r="C79">
-        <v>0.226</v>
+        <v>0.182</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B80">
         <v>20</v>
       </c>
       <c r="C80">
-        <v>0.031</v>
+        <v>0.038</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B81">
         <v>21</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B82">
         <v>22</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45424</v>
+        <v>45429</v>
       </c>
       <c r="B83">
         <v>23</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B87">
         <v>3</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B88">
         <v>4</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B89">
         <v>5</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B90">
         <v>6</v>
       </c>
       <c r="C90">
-        <v>0.076</v>
+        <v>0.079</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B91">
         <v>7</v>
       </c>
       <c r="C91">
-        <v>0.41</v>
+        <v>0.387</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B92">
         <v>8</v>
       </c>
       <c r="C92">
-        <v>0.965</v>
+        <v>0.667</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B93">
         <v>9</v>
       </c>
       <c r="C93">
-        <v>1.319</v>
+        <v>1.08</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B94">
         <v>10</v>
       </c>
       <c r="C94">
-        <v>1.819</v>
+        <v>1.753</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B95">
         <v>11</v>
       </c>
       <c r="C95">
-        <v>2.625</v>
+        <v>2.045</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B96">
         <v>12</v>
       </c>
       <c r="C96">
-        <v>2.824</v>
+        <v>2.307</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B97">
         <v>13</v>
       </c>
       <c r="C97">
-        <v>2.913</v>
+        <v>2.376</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B98">
         <v>14</v>
       </c>
       <c r="C98">
-        <v>2.976</v>
+        <v>2.143</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B99">
         <v>15</v>
       </c>
       <c r="C99">
-        <v>2.659</v>
+        <v>2.012</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B100">
         <v>16</v>
       </c>
       <c r="C100">
-        <v>2.103</v>
+        <v>1.782</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B101">
         <v>17</v>
       </c>
       <c r="C101">
-        <v>1.496</v>
+        <v>1.296</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B102">
         <v>18</v>
       </c>
       <c r="C102">
-        <v>0.899</v>
+        <v>0.802</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B103">
         <v>19</v>
       </c>
       <c r="C103">
-        <v>0.269</v>
+        <v>0.277</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B104">
         <v>20</v>
       </c>
       <c r="C104">
-        <v>0.033</v>
+        <v>0.037</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B105">
         <v>21</v>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B106">
         <v>22</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45425</v>
+        <v>45430</v>
       </c>
       <c r="B107">
         <v>23</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B112">
         <v>4</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B113">
         <v>5</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B114">
         <v>6</v>
       </c>
       <c r="C114">
-        <v>0.054</v>
+        <v>0.081</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B115">
         <v>7</v>
       </c>
       <c r="C115">
-        <v>0.349</v>
+        <v>0.401</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B116">
         <v>8</v>
       </c>
       <c r="C116">
-        <v>0.9409999999999999</v>
+        <v>0.984</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B117">
         <v>9</v>
       </c>
       <c r="C117">
-        <v>1.249</v>
+        <v>1.573</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B118">
         <v>10</v>
       </c>
       <c r="C118">
-        <v>1.866</v>
+        <v>1.961</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B119">
         <v>11</v>
       </c>
       <c r="C119">
-        <v>2.475</v>
+        <v>2.969</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B120">
         <v>12</v>
       </c>
       <c r="C120">
-        <v>2.671</v>
+        <v>3.016</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B121">
         <v>13</v>
       </c>
       <c r="C121">
-        <v>2.83</v>
+        <v>3.039</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B122">
         <v>14</v>
       </c>
       <c r="C122">
-        <v>2.947</v>
+        <v>2.851</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B123">
         <v>15</v>
       </c>
       <c r="C123">
-        <v>2.497</v>
+        <v>2.503</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B124">
         <v>16</v>
       </c>
       <c r="C124">
-        <v>1.923</v>
+        <v>1.963</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B125">
         <v>17</v>
       </c>
       <c r="C125">
-        <v>1.505</v>
+        <v>1.437</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B126">
         <v>18</v>
       </c>
       <c r="C126">
-        <v>0.895</v>
+        <v>0.906</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B127">
         <v>19</v>
       </c>
       <c r="C127">
-        <v>0.243</v>
+        <v>0.258</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B128">
         <v>20</v>
       </c>
       <c r="C128">
-        <v>0.033</v>
+        <v>0.036</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B129">
         <v>21</v>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B130">
         <v>22</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B131">
         <v>23</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B134">
         <v>2</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B136">
         <v>4</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B137">
         <v>5</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B138">
         <v>6</v>
       </c>
       <c r="C138">
-        <v>0.076</v>
+        <v>0.048</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B139">
         <v>7</v>
       </c>
       <c r="C139">
-        <v>0.353</v>
+        <v>0.127</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B140">
         <v>8</v>
       </c>
       <c r="C140">
-        <v>1.084</v>
+        <v>0.307</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B141">
         <v>9</v>
       </c>
       <c r="C141">
-        <v>1.719</v>
+        <v>0.65</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B142">
         <v>10</v>
       </c>
       <c r="C142">
-        <v>2.4</v>
+        <v>0.93</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B143">
         <v>11</v>
       </c>
       <c r="C143">
-        <v>2.91</v>
+        <v>1.042</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B144">
         <v>12</v>
       </c>
       <c r="C144">
-        <v>3.118</v>
+        <v>1.29</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B145">
         <v>13</v>
       </c>
       <c r="C145">
-        <v>3.093</v>
+        <v>1.402</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B146">
         <v>14</v>
       </c>
       <c r="C146">
-        <v>3.131</v>
+        <v>1.353</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B147">
         <v>15</v>
       </c>
       <c r="C147">
-        <v>2.997</v>
+        <v>1.309</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B148">
         <v>16</v>
       </c>
       <c r="C148">
-        <v>2.067</v>
+        <v>1.102</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B149">
         <v>17</v>
       </c>
       <c r="C149">
-        <v>1.662</v>
+        <v>0.764</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B150">
         <v>18</v>
       </c>
       <c r="C150">
-        <v>0.979</v>
+        <v>0.433</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B151">
         <v>19</v>
       </c>
       <c r="C151">
-        <v>0.311</v>
+        <v>0.186</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B152">
         <v>20</v>
       </c>
       <c r="C152">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B153">
         <v>21</v>
@@ -3044,7 +3044,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B154">
         <v>22</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B155">
         <v>23</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B158">
         <v>2</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B159">
         <v>3</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B160">
         <v>4</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B161">
         <v>5</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B162">
         <v>6</v>
       </c>
       <c r="C162">
-        <v>0.054</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B163">
         <v>7</v>
       </c>
       <c r="C163">
-        <v>0.356</v>
+        <v>0.412</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B164">
         <v>8</v>
       </c>
       <c r="C164">
-        <v>0.532</v>
+        <v>0.96</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B165">
         <v>9</v>
       </c>
       <c r="C165">
-        <v>0.995</v>
+        <v>1.236</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B166">
         <v>10</v>
       </c>
       <c r="C166">
-        <v>1.559</v>
+        <v>1.932</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B167">
         <v>11</v>
       </c>
       <c r="C167">
-        <v>1.925</v>
+        <v>2.308</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B168">
         <v>12</v>
       </c>
       <c r="C168">
-        <v>1.968</v>
+        <v>2.437</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B169">
         <v>13</v>
       </c>
       <c r="C169">
-        <v>2.261</v>
+        <v>2.585</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B170">
         <v>14</v>
       </c>
       <c r="C170">
-        <v>2.063</v>
+        <v>2.678</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the 15 min Forecast for Imperial and Astro
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,339 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>14.05.202414</t>
-  </si>
-  <si>
-    <t>14.05.202415</t>
-  </si>
-  <si>
-    <t>14.05.202416</t>
-  </si>
-  <si>
-    <t>14.05.202417</t>
-  </si>
-  <si>
-    <t>14.05.202418</t>
-  </si>
-  <si>
-    <t>14.05.202419</t>
-  </si>
-  <si>
-    <t>14.05.202420</t>
-  </si>
-  <si>
-    <t>14.05.202421</t>
-  </si>
-  <si>
-    <t>14.05.202422</t>
-  </si>
-  <si>
-    <t>14.05.202423</t>
-  </si>
-  <si>
-    <t>15.05.20240</t>
-  </si>
-  <si>
-    <t>15.05.20241</t>
-  </si>
-  <si>
-    <t>15.05.20242</t>
-  </si>
-  <si>
-    <t>15.05.20243</t>
-  </si>
-  <si>
-    <t>15.05.20244</t>
-  </si>
-  <si>
-    <t>15.05.20245</t>
-  </si>
-  <si>
-    <t>15.05.20246</t>
-  </si>
-  <si>
-    <t>15.05.20247</t>
-  </si>
-  <si>
-    <t>15.05.20248</t>
-  </si>
-  <si>
-    <t>15.05.20249</t>
-  </si>
-  <si>
-    <t>15.05.202410</t>
-  </si>
-  <si>
-    <t>15.05.202411</t>
-  </si>
-  <si>
-    <t>15.05.202412</t>
-  </si>
-  <si>
-    <t>15.05.202413</t>
-  </si>
-  <si>
-    <t>15.05.202414</t>
-  </si>
-  <si>
-    <t>15.05.202415</t>
-  </si>
-  <si>
-    <t>15.05.202416</t>
-  </si>
-  <si>
-    <t>15.05.202417</t>
-  </si>
-  <si>
-    <t>15.05.202418</t>
-  </si>
-  <si>
-    <t>15.05.202419</t>
-  </si>
-  <si>
-    <t>15.05.202420</t>
-  </si>
-  <si>
-    <t>15.05.202421</t>
-  </si>
-  <si>
-    <t>15.05.202422</t>
-  </si>
-  <si>
-    <t>15.05.202423</t>
-  </si>
-  <si>
-    <t>16.05.20240</t>
-  </si>
-  <si>
-    <t>16.05.20241</t>
-  </si>
-  <si>
-    <t>16.05.20242</t>
-  </si>
-  <si>
-    <t>16.05.20243</t>
-  </si>
-  <si>
-    <t>16.05.20244</t>
-  </si>
-  <si>
-    <t>16.05.20245</t>
-  </si>
-  <si>
-    <t>16.05.20246</t>
-  </si>
-  <si>
-    <t>16.05.20247</t>
-  </si>
-  <si>
-    <t>16.05.20248</t>
-  </si>
-  <si>
-    <t>16.05.20249</t>
-  </si>
-  <si>
-    <t>16.05.202410</t>
-  </si>
-  <si>
-    <t>16.05.202411</t>
-  </si>
-  <si>
-    <t>16.05.202412</t>
-  </si>
-  <si>
-    <t>16.05.202413</t>
-  </si>
-  <si>
-    <t>16.05.202414</t>
-  </si>
-  <si>
-    <t>16.05.202415</t>
-  </si>
-  <si>
-    <t>16.05.202416</t>
-  </si>
-  <si>
-    <t>16.05.202417</t>
-  </si>
-  <si>
-    <t>16.05.202418</t>
-  </si>
-  <si>
-    <t>16.05.202419</t>
-  </si>
-  <si>
-    <t>16.05.202420</t>
-  </si>
-  <si>
-    <t>16.05.202421</t>
-  </si>
-  <si>
-    <t>16.05.202422</t>
-  </si>
-  <si>
-    <t>16.05.202423</t>
-  </si>
-  <si>
-    <t>17.05.20240</t>
-  </si>
-  <si>
-    <t>17.05.20241</t>
-  </si>
-  <si>
-    <t>17.05.20242</t>
-  </si>
-  <si>
-    <t>17.05.20243</t>
-  </si>
-  <si>
-    <t>17.05.20244</t>
-  </si>
-  <si>
-    <t>17.05.20245</t>
-  </si>
-  <si>
-    <t>17.05.20246</t>
-  </si>
-  <si>
-    <t>17.05.20247</t>
-  </si>
-  <si>
-    <t>17.05.20248</t>
-  </si>
-  <si>
-    <t>17.05.20249</t>
-  </si>
-  <si>
-    <t>17.05.202410</t>
-  </si>
-  <si>
-    <t>17.05.202411</t>
-  </si>
-  <si>
-    <t>17.05.202412</t>
-  </si>
-  <si>
-    <t>17.05.202413</t>
-  </si>
-  <si>
-    <t>17.05.202414</t>
-  </si>
-  <si>
-    <t>17.05.202415</t>
-  </si>
-  <si>
-    <t>17.05.202416</t>
-  </si>
-  <si>
-    <t>17.05.202417</t>
-  </si>
-  <si>
-    <t>17.05.202418</t>
-  </si>
-  <si>
-    <t>17.05.202419</t>
-  </si>
-  <si>
-    <t>17.05.202420</t>
-  </si>
-  <si>
-    <t>17.05.202421</t>
-  </si>
-  <si>
-    <t>17.05.202422</t>
-  </si>
-  <si>
-    <t>17.05.202423</t>
-  </si>
-  <si>
-    <t>18.05.20240</t>
-  </si>
-  <si>
-    <t>18.05.20241</t>
-  </si>
-  <si>
-    <t>18.05.20242</t>
-  </si>
-  <si>
-    <t>18.05.20243</t>
-  </si>
-  <si>
-    <t>18.05.20244</t>
-  </si>
-  <si>
-    <t>18.05.20245</t>
-  </si>
-  <si>
-    <t>18.05.20246</t>
-  </si>
-  <si>
-    <t>18.05.20247</t>
-  </si>
-  <si>
-    <t>18.05.20248</t>
-  </si>
-  <si>
-    <t>18.05.20249</t>
-  </si>
-  <si>
-    <t>18.05.202410</t>
-  </si>
-  <si>
-    <t>18.05.202411</t>
-  </si>
-  <si>
-    <t>18.05.202412</t>
-  </si>
-  <si>
-    <t>18.05.202413</t>
-  </si>
-  <si>
-    <t>18.05.202414</t>
-  </si>
-  <si>
-    <t>18.05.202415</t>
-  </si>
-  <si>
-    <t>18.05.202416</t>
-  </si>
-  <si>
-    <t>18.05.202417</t>
-  </si>
-  <si>
-    <t>18.05.202418</t>
-  </si>
-  <si>
-    <t>18.05.202419</t>
-  </si>
-  <si>
-    <t>18.05.202420</t>
-  </si>
-  <si>
-    <t>18.05.202421</t>
-  </si>
-  <si>
-    <t>18.05.202422</t>
-  </si>
-  <si>
-    <t>18.05.202423</t>
-  </si>
-  <si>
-    <t>19.05.20240</t>
-  </si>
-  <si>
-    <t>19.05.20241</t>
-  </si>
-  <si>
-    <t>19.05.20242</t>
-  </si>
-  <si>
-    <t>19.05.20243</t>
-  </si>
-  <si>
-    <t>19.05.20244</t>
-  </si>
-  <si>
     <t>19.05.20245</t>
   </si>
   <si>
@@ -533,6 +200,339 @@
   </si>
   <si>
     <t>21.05.202414</t>
+  </si>
+  <si>
+    <t>21.05.202415</t>
+  </si>
+  <si>
+    <t>21.05.202416</t>
+  </si>
+  <si>
+    <t>21.05.202417</t>
+  </si>
+  <si>
+    <t>21.05.202418</t>
+  </si>
+  <si>
+    <t>21.05.202419</t>
+  </si>
+  <si>
+    <t>21.05.202420</t>
+  </si>
+  <si>
+    <t>21.05.202421</t>
+  </si>
+  <si>
+    <t>21.05.202422</t>
+  </si>
+  <si>
+    <t>21.05.202423</t>
+  </si>
+  <si>
+    <t>22.05.20240</t>
+  </si>
+  <si>
+    <t>22.05.20241</t>
+  </si>
+  <si>
+    <t>22.05.20242</t>
+  </si>
+  <si>
+    <t>22.05.20243</t>
+  </si>
+  <si>
+    <t>22.05.20244</t>
+  </si>
+  <si>
+    <t>22.05.20245</t>
+  </si>
+  <si>
+    <t>22.05.20246</t>
+  </si>
+  <si>
+    <t>22.05.20247</t>
+  </si>
+  <si>
+    <t>22.05.20248</t>
+  </si>
+  <si>
+    <t>22.05.20249</t>
+  </si>
+  <si>
+    <t>22.05.202410</t>
+  </si>
+  <si>
+    <t>22.05.202411</t>
+  </si>
+  <si>
+    <t>22.05.202412</t>
+  </si>
+  <si>
+    <t>22.05.202413</t>
+  </si>
+  <si>
+    <t>22.05.202414</t>
+  </si>
+  <si>
+    <t>22.05.202415</t>
+  </si>
+  <si>
+    <t>22.05.202416</t>
+  </si>
+  <si>
+    <t>22.05.202417</t>
+  </si>
+  <si>
+    <t>22.05.202418</t>
+  </si>
+  <si>
+    <t>22.05.202419</t>
+  </si>
+  <si>
+    <t>22.05.202420</t>
+  </si>
+  <si>
+    <t>22.05.202421</t>
+  </si>
+  <si>
+    <t>22.05.202422</t>
+  </si>
+  <si>
+    <t>22.05.202423</t>
+  </si>
+  <si>
+    <t>23.05.20240</t>
+  </si>
+  <si>
+    <t>23.05.20241</t>
+  </si>
+  <si>
+    <t>23.05.20242</t>
+  </si>
+  <si>
+    <t>23.05.20243</t>
+  </si>
+  <si>
+    <t>23.05.20244</t>
+  </si>
+  <si>
+    <t>23.05.20245</t>
+  </si>
+  <si>
+    <t>23.05.20246</t>
+  </si>
+  <si>
+    <t>23.05.20247</t>
+  </si>
+  <si>
+    <t>23.05.20248</t>
+  </si>
+  <si>
+    <t>23.05.20249</t>
+  </si>
+  <si>
+    <t>23.05.202410</t>
+  </si>
+  <si>
+    <t>23.05.202411</t>
+  </si>
+  <si>
+    <t>23.05.202412</t>
+  </si>
+  <si>
+    <t>23.05.202413</t>
+  </si>
+  <si>
+    <t>23.05.202414</t>
+  </si>
+  <si>
+    <t>23.05.202415</t>
+  </si>
+  <si>
+    <t>23.05.202416</t>
+  </si>
+  <si>
+    <t>23.05.202417</t>
+  </si>
+  <si>
+    <t>23.05.202418</t>
+  </si>
+  <si>
+    <t>23.05.202419</t>
+  </si>
+  <si>
+    <t>23.05.202420</t>
+  </si>
+  <si>
+    <t>23.05.202421</t>
+  </si>
+  <si>
+    <t>23.05.202422</t>
+  </si>
+  <si>
+    <t>23.05.202423</t>
+  </si>
+  <si>
+    <t>24.05.20240</t>
+  </si>
+  <si>
+    <t>24.05.20241</t>
+  </si>
+  <si>
+    <t>24.05.20242</t>
+  </si>
+  <si>
+    <t>24.05.20243</t>
+  </si>
+  <si>
+    <t>24.05.20244</t>
+  </si>
+  <si>
+    <t>24.05.20245</t>
+  </si>
+  <si>
+    <t>24.05.20246</t>
+  </si>
+  <si>
+    <t>24.05.20247</t>
+  </si>
+  <si>
+    <t>24.05.20248</t>
+  </si>
+  <si>
+    <t>24.05.20249</t>
+  </si>
+  <si>
+    <t>24.05.202410</t>
+  </si>
+  <si>
+    <t>24.05.202411</t>
+  </si>
+  <si>
+    <t>24.05.202412</t>
+  </si>
+  <si>
+    <t>24.05.202413</t>
+  </si>
+  <si>
+    <t>24.05.202414</t>
+  </si>
+  <si>
+    <t>24.05.202415</t>
+  </si>
+  <si>
+    <t>24.05.202416</t>
+  </si>
+  <si>
+    <t>24.05.202417</t>
+  </si>
+  <si>
+    <t>24.05.202418</t>
+  </si>
+  <si>
+    <t>24.05.202419</t>
+  </si>
+  <si>
+    <t>24.05.202420</t>
+  </si>
+  <si>
+    <t>24.05.202421</t>
+  </si>
+  <si>
+    <t>24.05.202422</t>
+  </si>
+  <si>
+    <t>24.05.202423</t>
+  </si>
+  <si>
+    <t>25.05.20240</t>
+  </si>
+  <si>
+    <t>25.05.20241</t>
+  </si>
+  <si>
+    <t>25.05.20242</t>
+  </si>
+  <si>
+    <t>25.05.20243</t>
+  </si>
+  <si>
+    <t>25.05.20244</t>
+  </si>
+  <si>
+    <t>25.05.20245</t>
+  </si>
+  <si>
+    <t>25.05.20246</t>
+  </si>
+  <si>
+    <t>25.05.20247</t>
+  </si>
+  <si>
+    <t>25.05.20248</t>
+  </si>
+  <si>
+    <t>25.05.20249</t>
+  </si>
+  <si>
+    <t>25.05.202410</t>
+  </si>
+  <si>
+    <t>25.05.202411</t>
+  </si>
+  <si>
+    <t>25.05.202412</t>
+  </si>
+  <si>
+    <t>25.05.202413</t>
+  </si>
+  <si>
+    <t>25.05.202414</t>
+  </si>
+  <si>
+    <t>25.05.202415</t>
+  </si>
+  <si>
+    <t>25.05.202416</t>
+  </si>
+  <si>
+    <t>25.05.202417</t>
+  </si>
+  <si>
+    <t>25.05.202418</t>
+  </si>
+  <si>
+    <t>25.05.202419</t>
+  </si>
+  <si>
+    <t>25.05.202420</t>
+  </si>
+  <si>
+    <t>25.05.202421</t>
+  </si>
+  <si>
+    <t>25.05.202422</t>
+  </si>
+  <si>
+    <t>25.05.202423</t>
+  </si>
+  <si>
+    <t>26.05.20240</t>
+  </si>
+  <si>
+    <t>26.05.20241</t>
+  </si>
+  <si>
+    <t>26.05.20242</t>
+  </si>
+  <si>
+    <t>26.05.20243</t>
+  </si>
+  <si>
+    <t>26.05.20244</t>
+  </si>
+  <si>
+    <t>26.05.20245</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>2.631</v>
+        <v>0.416</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>2.029</v>
+        <v>1.021</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>1.161</v>
+        <v>1.649</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>0.4</v>
+        <v>2.161</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>0.037</v>
+        <v>2.994</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>3.123</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2.901</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45426</v>
+        <v>45431</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2.779</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2.27</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1.788</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1.431</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.944</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.379</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.036</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C18">
-        <v>0.083</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>0.414</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45427</v>
+        <v>45431</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C20">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>1.598</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>2.015</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>2.805</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>3.001</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>3.143</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>3.108</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C27">
-        <v>2.903</v>
+        <v>0.076</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>2.217</v>
+        <v>0.392</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>1.919</v>
+        <v>0.77</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C30">
-        <v>1.215</v>
+        <v>1.186</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C31">
-        <v>0.398</v>
+        <v>1.834</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>0.037</v>
+        <v>2.122</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>2.537</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>2.622</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45427</v>
+        <v>45432</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>2.604</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2.307</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1.83</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1.298</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>0.701</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>0.237</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>0.036</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C42">
-        <v>0.102</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C43">
-        <v>0.393</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45428</v>
+        <v>45432</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C44">
-        <v>1.026</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>1.628</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>2.147</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B47">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>2.833</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C48">
-        <v>2.931</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C49">
-        <v>2.769</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C50">
-        <v>2.733</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C51">
-        <v>2.201</v>
+        <v>0.076</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C52">
-        <v>1.773</v>
+        <v>0.379</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B53">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C53">
-        <v>1.309</v>
+        <v>0.718</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C54">
-        <v>0.803</v>
+        <v>1.259</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B55">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C55">
-        <v>0.329</v>
+        <v>1.88</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C56">
-        <v>0.037</v>
+        <v>2.789</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B57">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>2.878</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>2.806</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45428</v>
+        <v>45433</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>2.798</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>2.49</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1.787</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1.312</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>0.256</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>0.036</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C66">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C67">
-        <v>0.41</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45429</v>
+        <v>45433</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C68">
-        <v>0.667</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>1.021</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>1.595</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C71">
-        <v>1.846</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C72">
-        <v>2.11</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B73">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C73">
-        <v>2.034</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B74">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C74">
-        <v>1.797</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B75">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C75">
-        <v>1.421</v>
+        <v>0.076</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B76">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C76">
-        <v>1.191</v>
+        <v>0.38</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C77">
-        <v>0.844</v>
+        <v>0.973</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C78">
-        <v>0.433</v>
+        <v>1.563</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B79">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C79">
-        <v>0.182</v>
+        <v>2.025</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B80">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C80">
-        <v>0.038</v>
+        <v>2.155</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B81">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>2.069</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B82">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>2.033</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45429</v>
+        <v>45434</v>
       </c>
       <c r="B83">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>2.081</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1.611</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1.358</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.842</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>0.472</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B88">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>0.236</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B90">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C90">
-        <v>0.079</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B91">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C91">
-        <v>0.387</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45430</v>
+        <v>45434</v>
       </c>
       <c r="B92">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C92">
-        <v>0.667</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B93">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C93">
-        <v>1.08</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B94">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C94">
-        <v>1.753</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B95">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C95">
-        <v>2.045</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B96">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C96">
-        <v>2.307</v>
+        <v>0</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B97">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C97">
-        <v>2.376</v>
+        <v>0</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B98">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C98">
-        <v>2.143</v>
+        <v>0</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B99">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C99">
-        <v>2.012</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B100">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C100">
-        <v>1.782</v>
+        <v>0.413</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B101">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C101">
-        <v>1.296</v>
+        <v>0.624</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B102">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C102">
-        <v>0.802</v>
+        <v>1.044</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B103">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C103">
-        <v>0.277</v>
+        <v>1.742</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B104">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C104">
-        <v>0.037</v>
+        <v>2.234</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B105">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>2.665</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B106">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>2.598</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45430</v>
+        <v>45435</v>
       </c>
       <c r="B107">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>2.472</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>2.04</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>1.459</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>0.468</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B112">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>0.204</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B113">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B114">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C114">
-        <v>0.081</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B115">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C115">
-        <v>0.401</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45431</v>
+        <v>45435</v>
       </c>
       <c r="B116">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C116">
-        <v>0.984</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B117">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C117">
-        <v>1.573</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B118">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C118">
-        <v>1.961</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B119">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C119">
-        <v>2.969</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B120">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C120">
-        <v>3.016</v>
+        <v>0</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B121">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C121">
-        <v>3.039</v>
+        <v>0</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B122">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C122">
-        <v>2.851</v>
+        <v>0</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B123">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C123">
-        <v>2.503</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B124">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C124">
-        <v>1.963</v>
+        <v>0.309</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B125">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C125">
-        <v>1.437</v>
+        <v>0.58</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B126">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C126">
-        <v>0.906</v>
+        <v>1.06</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B127">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C127">
-        <v>0.258</v>
+        <v>1.341</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B128">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C128">
-        <v>0.036</v>
+        <v>1.797</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B129">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1.957</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B130">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>2.255</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45431</v>
+        <v>45436</v>
       </c>
       <c r="B131">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>2.155</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>2.026</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>1.725</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>1.264</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B135">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>0.794</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B136">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>0.302</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>0.036</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B138">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C138">
-        <v>0.048</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B139">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C139">
-        <v>0.127</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45432</v>
+        <v>45436</v>
       </c>
       <c r="B140">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C140">
-        <v>0.307</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B141">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C141">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B142">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C142">
-        <v>0.93</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B143">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C143">
-        <v>1.042</v>
+        <v>0</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B144">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C144">
-        <v>1.29</v>
+        <v>0</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B145">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C145">
-        <v>1.402</v>
+        <v>0</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B146">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C146">
-        <v>1.353</v>
+        <v>0</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B147">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C147">
-        <v>1.309</v>
+        <v>0.098</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B148">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C148">
-        <v>1.102</v>
+        <v>0.395</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B149">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C149">
-        <v>0.764</v>
+        <v>1.131</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B150">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C150">
-        <v>0.433</v>
+        <v>1.827</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B151">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C151">
-        <v>0.186</v>
+        <v>2.399</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B152">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C152">
-        <v>0.037</v>
+        <v>2.87</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B153">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>2.809</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B154">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>2.873</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45432</v>
+        <v>45437</v>
       </c>
       <c r="B155">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>2.792</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B156">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>2.717</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>2.033</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B158">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>1.664</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B159">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>0.992</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B160">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>0.379</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B161">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B162">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C162">
-        <v>0.08400000000000001</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B163">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C163">
-        <v>0.412</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45433</v>
+        <v>45437</v>
       </c>
       <c r="B164">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C164">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45433</v>
+        <v>45438</v>
       </c>
       <c r="B165">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C165">
-        <v>1.236</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45433</v>
+        <v>45438</v>
       </c>
       <c r="B166">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C166">
-        <v>1.932</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45433</v>
+        <v>45438</v>
       </c>
       <c r="B167">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C167">
-        <v>2.308</v>
+        <v>0</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45433</v>
+        <v>45438</v>
       </c>
       <c r="B168">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C168">
-        <v>2.437</v>
+        <v>0</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45433</v>
+        <v>45438</v>
       </c>
       <c r="B169">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C169">
-        <v>2.585</v>
+        <v>0</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45433</v>
+        <v>45438</v>
       </c>
       <c r="B170">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C170">
-        <v>2.678</v>
+        <v>0</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the first version of the 15 min forecast algorithms got Imperial and Astro
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>19.05.20245</t>
-  </si>
-  <si>
-    <t>19.05.20246</t>
-  </si>
-  <si>
-    <t>19.05.20247</t>
-  </si>
-  <si>
-    <t>19.05.20248</t>
-  </si>
-  <si>
-    <t>19.05.20249</t>
-  </si>
-  <si>
-    <t>19.05.202410</t>
-  </si>
-  <si>
-    <t>19.05.202411</t>
-  </si>
-  <si>
-    <t>19.05.202412</t>
-  </si>
-  <si>
-    <t>19.05.202413</t>
-  </si>
-  <si>
-    <t>19.05.202414</t>
-  </si>
-  <si>
-    <t>19.05.202415</t>
-  </si>
-  <si>
-    <t>19.05.202416</t>
-  </si>
-  <si>
-    <t>19.05.202417</t>
-  </si>
-  <si>
-    <t>19.05.202418</t>
-  </si>
-  <si>
-    <t>19.05.202419</t>
-  </si>
-  <si>
-    <t>19.05.202420</t>
-  </si>
-  <si>
-    <t>19.05.202421</t>
-  </si>
-  <si>
-    <t>19.05.202422</t>
-  </si>
-  <si>
-    <t>19.05.202423</t>
-  </si>
-  <si>
-    <t>20.05.20240</t>
-  </si>
-  <si>
-    <t>20.05.20241</t>
-  </si>
-  <si>
-    <t>20.05.20242</t>
-  </si>
-  <si>
-    <t>20.05.20243</t>
-  </si>
-  <si>
-    <t>20.05.20244</t>
-  </si>
-  <si>
-    <t>20.05.20245</t>
-  </si>
-  <si>
-    <t>20.05.20246</t>
-  </si>
-  <si>
-    <t>20.05.20247</t>
-  </si>
-  <si>
-    <t>20.05.20248</t>
-  </si>
-  <si>
-    <t>20.05.20249</t>
-  </si>
-  <si>
-    <t>20.05.202410</t>
-  </si>
-  <si>
-    <t>20.05.202411</t>
-  </si>
-  <si>
-    <t>20.05.202412</t>
-  </si>
-  <si>
-    <t>20.05.202413</t>
-  </si>
-  <si>
-    <t>20.05.202414</t>
-  </si>
-  <si>
-    <t>20.05.202415</t>
-  </si>
-  <si>
-    <t>20.05.202416</t>
-  </si>
-  <si>
-    <t>20.05.202417</t>
-  </si>
-  <si>
-    <t>20.05.202418</t>
-  </si>
-  <si>
-    <t>20.05.202419</t>
-  </si>
-  <si>
-    <t>20.05.202420</t>
-  </si>
-  <si>
-    <t>20.05.202421</t>
-  </si>
-  <si>
-    <t>20.05.202422</t>
-  </si>
-  <si>
-    <t>20.05.202423</t>
-  </si>
-  <si>
-    <t>21.05.20240</t>
-  </si>
-  <si>
-    <t>21.05.20241</t>
-  </si>
-  <si>
-    <t>21.05.20242</t>
-  </si>
-  <si>
-    <t>21.05.20243</t>
-  </si>
-  <si>
-    <t>21.05.20244</t>
-  </si>
-  <si>
-    <t>21.05.20245</t>
-  </si>
-  <si>
-    <t>21.05.20246</t>
-  </si>
-  <si>
-    <t>21.05.20247</t>
-  </si>
-  <si>
-    <t>21.05.20248</t>
-  </si>
-  <si>
-    <t>21.05.20249</t>
-  </si>
-  <si>
-    <t>21.05.202410</t>
-  </si>
-  <si>
-    <t>21.05.202411</t>
-  </si>
-  <si>
-    <t>21.05.202412</t>
-  </si>
-  <si>
-    <t>21.05.202413</t>
-  </si>
-  <si>
-    <t>21.05.202414</t>
-  </si>
-  <si>
-    <t>21.05.202415</t>
-  </si>
-  <si>
-    <t>21.05.202416</t>
-  </si>
-  <si>
-    <t>21.05.202417</t>
-  </si>
-  <si>
-    <t>21.05.202418</t>
-  </si>
-  <si>
-    <t>21.05.202419</t>
-  </si>
-  <si>
-    <t>21.05.202420</t>
-  </si>
-  <si>
-    <t>21.05.202421</t>
-  </si>
-  <si>
-    <t>21.05.202422</t>
-  </si>
-  <si>
-    <t>21.05.202423</t>
-  </si>
-  <si>
-    <t>22.05.20240</t>
-  </si>
-  <si>
-    <t>22.05.20241</t>
-  </si>
-  <si>
-    <t>22.05.20242</t>
-  </si>
-  <si>
-    <t>22.05.20243</t>
-  </si>
-  <si>
-    <t>22.05.20244</t>
-  </si>
-  <si>
-    <t>22.05.20245</t>
-  </si>
-  <si>
-    <t>22.05.20246</t>
-  </si>
-  <si>
-    <t>22.05.20247</t>
-  </si>
-  <si>
-    <t>22.05.20248</t>
-  </si>
-  <si>
-    <t>22.05.20249</t>
-  </si>
-  <si>
-    <t>22.05.202410</t>
-  </si>
-  <si>
-    <t>22.05.202411</t>
-  </si>
-  <si>
-    <t>22.05.202412</t>
-  </si>
-  <si>
-    <t>22.05.202413</t>
-  </si>
-  <si>
-    <t>22.05.202414</t>
-  </si>
-  <si>
-    <t>22.05.202415</t>
-  </si>
-  <si>
-    <t>22.05.202416</t>
-  </si>
-  <si>
-    <t>22.05.202417</t>
-  </si>
-  <si>
-    <t>22.05.202418</t>
-  </si>
-  <si>
-    <t>22.05.202419</t>
-  </si>
-  <si>
-    <t>22.05.202420</t>
-  </si>
-  <si>
-    <t>22.05.202421</t>
-  </si>
-  <si>
-    <t>22.05.202422</t>
-  </si>
-  <si>
-    <t>22.05.202423</t>
-  </si>
-  <si>
-    <t>23.05.20240</t>
-  </si>
-  <si>
-    <t>23.05.20241</t>
-  </si>
-  <si>
-    <t>23.05.20242</t>
-  </si>
-  <si>
-    <t>23.05.20243</t>
-  </si>
-  <si>
-    <t>23.05.20244</t>
-  </si>
-  <si>
-    <t>23.05.20245</t>
-  </si>
-  <si>
-    <t>23.05.20246</t>
-  </si>
-  <si>
-    <t>23.05.20247</t>
-  </si>
-  <si>
-    <t>23.05.20248</t>
-  </si>
-  <si>
-    <t>23.05.20249</t>
-  </si>
-  <si>
-    <t>23.05.202410</t>
-  </si>
-  <si>
-    <t>23.05.202411</t>
-  </si>
-  <si>
-    <t>23.05.202412</t>
-  </si>
-  <si>
-    <t>23.05.202413</t>
-  </si>
-  <si>
-    <t>23.05.202414</t>
-  </si>
-  <si>
-    <t>23.05.202415</t>
-  </si>
-  <si>
-    <t>23.05.202416</t>
-  </si>
-  <si>
-    <t>23.05.202417</t>
-  </si>
-  <si>
-    <t>23.05.202418</t>
-  </si>
-  <si>
-    <t>23.05.202419</t>
-  </si>
-  <si>
-    <t>23.05.202420</t>
-  </si>
-  <si>
-    <t>23.05.202421</t>
-  </si>
-  <si>
-    <t>23.05.202422</t>
-  </si>
-  <si>
-    <t>23.05.202423</t>
-  </si>
-  <si>
-    <t>24.05.20240</t>
-  </si>
-  <si>
-    <t>24.05.20241</t>
-  </si>
-  <si>
-    <t>24.05.20242</t>
-  </si>
-  <si>
-    <t>24.05.20243</t>
-  </si>
-  <si>
-    <t>24.05.20244</t>
-  </si>
-  <si>
-    <t>24.05.20245</t>
-  </si>
-  <si>
-    <t>24.05.20246</t>
-  </si>
-  <si>
-    <t>24.05.20247</t>
-  </si>
-  <si>
-    <t>24.05.20248</t>
-  </si>
-  <si>
-    <t>24.05.20249</t>
-  </si>
-  <si>
-    <t>24.05.202410</t>
-  </si>
-  <si>
-    <t>24.05.202411</t>
-  </si>
-  <si>
-    <t>24.05.202412</t>
-  </si>
-  <si>
-    <t>24.05.202413</t>
-  </si>
-  <si>
-    <t>24.05.202414</t>
-  </si>
-  <si>
-    <t>24.05.202415</t>
-  </si>
-  <si>
-    <t>24.05.202416</t>
-  </si>
-  <si>
-    <t>24.05.202417</t>
-  </si>
-  <si>
-    <t>24.05.202418</t>
-  </si>
-  <si>
-    <t>24.05.202419</t>
-  </si>
-  <si>
-    <t>24.05.202420</t>
-  </si>
-  <si>
-    <t>24.05.202421</t>
-  </si>
-  <si>
-    <t>24.05.202422</t>
-  </si>
-  <si>
-    <t>24.05.202423</t>
-  </si>
-  <si>
-    <t>25.05.20240</t>
-  </si>
-  <si>
-    <t>25.05.20241</t>
-  </si>
-  <si>
-    <t>25.05.20242</t>
-  </si>
-  <si>
-    <t>25.05.20243</t>
-  </si>
-  <si>
-    <t>25.05.20244</t>
-  </si>
-  <si>
-    <t>25.05.20245</t>
-  </si>
-  <si>
-    <t>25.05.20246</t>
-  </si>
-  <si>
-    <t>25.05.20247</t>
-  </si>
-  <si>
-    <t>25.05.20248</t>
-  </si>
-  <si>
-    <t>25.05.20249</t>
-  </si>
-  <si>
-    <t>25.05.202410</t>
-  </si>
-  <si>
-    <t>25.05.202411</t>
-  </si>
-  <si>
-    <t>25.05.202412</t>
-  </si>
-  <si>
-    <t>25.05.202413</t>
-  </si>
-  <si>
-    <t>25.05.202414</t>
-  </si>
-  <si>
-    <t>25.05.202415</t>
-  </si>
-  <si>
-    <t>25.05.202416</t>
-  </si>
-  <si>
-    <t>25.05.202417</t>
-  </si>
-  <si>
-    <t>25.05.202418</t>
-  </si>
-  <si>
-    <t>25.05.202419</t>
-  </si>
-  <si>
-    <t>25.05.202420</t>
-  </si>
-  <si>
-    <t>25.05.202421</t>
-  </si>
-  <si>
-    <t>25.05.202422</t>
-  </si>
-  <si>
-    <t>25.05.202423</t>
-  </si>
-  <si>
-    <t>26.05.20240</t>
-  </si>
-  <si>
-    <t>26.05.20241</t>
-  </si>
-  <si>
-    <t>26.05.20242</t>
-  </si>
-  <si>
-    <t>26.05.20243</t>
-  </si>
-  <si>
-    <t>26.05.20244</t>
-  </si>
-  <si>
-    <t>26.05.20245</t>
+    <t>30.05.202414</t>
+  </si>
+  <si>
+    <t>30.05.202415</t>
+  </si>
+  <si>
+    <t>30.05.202416</t>
+  </si>
+  <si>
+    <t>30.05.202417</t>
+  </si>
+  <si>
+    <t>30.05.202418</t>
+  </si>
+  <si>
+    <t>30.05.202419</t>
+  </si>
+  <si>
+    <t>30.05.202420</t>
+  </si>
+  <si>
+    <t>30.05.202421</t>
+  </si>
+  <si>
+    <t>30.05.202422</t>
+  </si>
+  <si>
+    <t>30.05.202423</t>
+  </si>
+  <si>
+    <t>31.05.20240</t>
+  </si>
+  <si>
+    <t>31.05.20241</t>
+  </si>
+  <si>
+    <t>31.05.20242</t>
+  </si>
+  <si>
+    <t>31.05.20243</t>
+  </si>
+  <si>
+    <t>31.05.20244</t>
+  </si>
+  <si>
+    <t>31.05.20245</t>
+  </si>
+  <si>
+    <t>31.05.20246</t>
+  </si>
+  <si>
+    <t>31.05.20247</t>
+  </si>
+  <si>
+    <t>31.05.20248</t>
+  </si>
+  <si>
+    <t>31.05.20249</t>
+  </si>
+  <si>
+    <t>31.05.202410</t>
+  </si>
+  <si>
+    <t>31.05.202411</t>
+  </si>
+  <si>
+    <t>31.05.202412</t>
+  </si>
+  <si>
+    <t>31.05.202413</t>
+  </si>
+  <si>
+    <t>31.05.202414</t>
+  </si>
+  <si>
+    <t>31.05.202415</t>
+  </si>
+  <si>
+    <t>31.05.202416</t>
+  </si>
+  <si>
+    <t>31.05.202417</t>
+  </si>
+  <si>
+    <t>31.05.202418</t>
+  </si>
+  <si>
+    <t>31.05.202419</t>
+  </si>
+  <si>
+    <t>31.05.202420</t>
+  </si>
+  <si>
+    <t>31.05.202421</t>
+  </si>
+  <si>
+    <t>31.05.202422</t>
+  </si>
+  <si>
+    <t>31.05.202423</t>
+  </si>
+  <si>
+    <t>01.06.20240</t>
+  </si>
+  <si>
+    <t>01.06.20241</t>
+  </si>
+  <si>
+    <t>01.06.20242</t>
+  </si>
+  <si>
+    <t>01.06.20243</t>
+  </si>
+  <si>
+    <t>01.06.20244</t>
+  </si>
+  <si>
+    <t>01.06.20245</t>
+  </si>
+  <si>
+    <t>01.06.20246</t>
+  </si>
+  <si>
+    <t>01.06.20247</t>
+  </si>
+  <si>
+    <t>01.06.20248</t>
+  </si>
+  <si>
+    <t>01.06.20249</t>
+  </si>
+  <si>
+    <t>01.06.202410</t>
+  </si>
+  <si>
+    <t>01.06.202411</t>
+  </si>
+  <si>
+    <t>01.06.202412</t>
+  </si>
+  <si>
+    <t>01.06.202413</t>
+  </si>
+  <si>
+    <t>01.06.202414</t>
+  </si>
+  <si>
+    <t>01.06.202415</t>
+  </si>
+  <si>
+    <t>01.06.202416</t>
+  </si>
+  <si>
+    <t>01.06.202417</t>
+  </si>
+  <si>
+    <t>01.06.202418</t>
+  </si>
+  <si>
+    <t>01.06.202419</t>
+  </si>
+  <si>
+    <t>01.06.202420</t>
+  </si>
+  <si>
+    <t>01.06.202421</t>
+  </si>
+  <si>
+    <t>01.06.202422</t>
+  </si>
+  <si>
+    <t>01.06.202423</t>
+  </si>
+  <si>
+    <t>02.06.20240</t>
+  </si>
+  <si>
+    <t>02.06.20241</t>
+  </si>
+  <si>
+    <t>02.06.20242</t>
+  </si>
+  <si>
+    <t>02.06.20243</t>
+  </si>
+  <si>
+    <t>02.06.20244</t>
+  </si>
+  <si>
+    <t>02.06.20245</t>
+  </si>
+  <si>
+    <t>02.06.20246</t>
+  </si>
+  <si>
+    <t>02.06.20247</t>
+  </si>
+  <si>
+    <t>02.06.20248</t>
+  </si>
+  <si>
+    <t>02.06.20249</t>
+  </si>
+  <si>
+    <t>02.06.202410</t>
+  </si>
+  <si>
+    <t>02.06.202411</t>
+  </si>
+  <si>
+    <t>02.06.202412</t>
+  </si>
+  <si>
+    <t>02.06.202413</t>
+  </si>
+  <si>
+    <t>02.06.202414</t>
+  </si>
+  <si>
+    <t>02.06.202415</t>
+  </si>
+  <si>
+    <t>02.06.202416</t>
+  </si>
+  <si>
+    <t>02.06.202417</t>
+  </si>
+  <si>
+    <t>02.06.202418</t>
+  </si>
+  <si>
+    <t>02.06.202419</t>
+  </si>
+  <si>
+    <t>02.06.202420</t>
+  </si>
+  <si>
+    <t>02.06.202421</t>
+  </si>
+  <si>
+    <t>02.06.202422</t>
+  </si>
+  <si>
+    <t>02.06.202423</t>
+  </si>
+  <si>
+    <t>03.06.20240</t>
+  </si>
+  <si>
+    <t>03.06.20241</t>
+  </si>
+  <si>
+    <t>03.06.20242</t>
+  </si>
+  <si>
+    <t>03.06.20243</t>
+  </si>
+  <si>
+    <t>03.06.20244</t>
+  </si>
+  <si>
+    <t>03.06.20245</t>
+  </si>
+  <si>
+    <t>03.06.20246</t>
+  </si>
+  <si>
+    <t>03.06.20247</t>
+  </si>
+  <si>
+    <t>03.06.20248</t>
+  </si>
+  <si>
+    <t>03.06.20249</t>
+  </si>
+  <si>
+    <t>03.06.202410</t>
+  </si>
+  <si>
+    <t>03.06.202411</t>
+  </si>
+  <si>
+    <t>03.06.202412</t>
+  </si>
+  <si>
+    <t>03.06.202413</t>
+  </si>
+  <si>
+    <t>03.06.202414</t>
+  </si>
+  <si>
+    <t>03.06.202415</t>
+  </si>
+  <si>
+    <t>03.06.202416</t>
+  </si>
+  <si>
+    <t>03.06.202417</t>
+  </si>
+  <si>
+    <t>03.06.202418</t>
+  </si>
+  <si>
+    <t>03.06.202419</t>
+  </si>
+  <si>
+    <t>03.06.202420</t>
+  </si>
+  <si>
+    <t>03.06.202421</t>
+  </si>
+  <si>
+    <t>03.06.202422</t>
+  </si>
+  <si>
+    <t>03.06.202423</t>
+  </si>
+  <si>
+    <t>04.06.20240</t>
+  </si>
+  <si>
+    <t>04.06.20241</t>
+  </si>
+  <si>
+    <t>04.06.20242</t>
+  </si>
+  <si>
+    <t>04.06.20243</t>
+  </si>
+  <si>
+    <t>04.06.20244</t>
+  </si>
+  <si>
+    <t>04.06.20245</t>
+  </si>
+  <si>
+    <t>04.06.20246</t>
+  </si>
+  <si>
+    <t>04.06.20247</t>
+  </si>
+  <si>
+    <t>04.06.20248</t>
+  </si>
+  <si>
+    <t>04.06.20249</t>
+  </si>
+  <si>
+    <t>04.06.202410</t>
+  </si>
+  <si>
+    <t>04.06.202411</t>
+  </si>
+  <si>
+    <t>04.06.202412</t>
+  </si>
+  <si>
+    <t>04.06.202413</t>
+  </si>
+  <si>
+    <t>04.06.202414</t>
+  </si>
+  <si>
+    <t>04.06.202415</t>
+  </si>
+  <si>
+    <t>04.06.202416</t>
+  </si>
+  <si>
+    <t>04.06.202417</t>
+  </si>
+  <si>
+    <t>04.06.202418</t>
+  </si>
+  <si>
+    <t>04.06.202419</t>
+  </si>
+  <si>
+    <t>04.06.202420</t>
+  </si>
+  <si>
+    <t>04.06.202421</t>
+  </si>
+  <si>
+    <t>04.06.202422</t>
+  </si>
+  <si>
+    <t>04.06.202423</t>
+  </si>
+  <si>
+    <t>05.06.20240</t>
+  </si>
+  <si>
+    <t>05.06.20241</t>
+  </si>
+  <si>
+    <t>05.06.20242</t>
+  </si>
+  <si>
+    <t>05.06.20243</t>
+  </si>
+  <si>
+    <t>05.06.20244</t>
+  </si>
+  <si>
+    <t>05.06.20245</t>
+  </si>
+  <si>
+    <t>05.06.20246</t>
+  </si>
+  <si>
+    <t>05.06.20247</t>
+  </si>
+  <si>
+    <t>05.06.20248</t>
+  </si>
+  <si>
+    <t>05.06.20249</t>
+  </si>
+  <si>
+    <t>05.06.202410</t>
+  </si>
+  <si>
+    <t>05.06.202411</t>
+  </si>
+  <si>
+    <t>05.06.202412</t>
+  </si>
+  <si>
+    <t>05.06.202413</t>
+  </si>
+  <si>
+    <t>05.06.202414</t>
+  </si>
+  <si>
+    <t>05.06.202415</t>
+  </si>
+  <si>
+    <t>05.06.202416</t>
+  </si>
+  <si>
+    <t>05.06.202417</t>
+  </si>
+  <si>
+    <t>05.06.202418</t>
+  </si>
+  <si>
+    <t>05.06.202419</t>
+  </si>
+  <si>
+    <t>05.06.202420</t>
+  </si>
+  <si>
+    <t>05.06.202421</t>
+  </si>
+  <si>
+    <t>05.06.202422</t>
+  </si>
+  <si>
+    <t>05.06.202423</t>
+  </si>
+  <si>
+    <t>06.06.20240</t>
+  </si>
+  <si>
+    <t>06.06.20241</t>
+  </si>
+  <si>
+    <t>06.06.20242</t>
+  </si>
+  <si>
+    <t>06.06.20243</t>
+  </si>
+  <si>
+    <t>06.06.20244</t>
+  </si>
+  <si>
+    <t>06.06.20245</t>
+  </si>
+  <si>
+    <t>06.06.20246</t>
+  </si>
+  <si>
+    <t>06.06.20247</t>
+  </si>
+  <si>
+    <t>06.06.20248</t>
+  </si>
+  <si>
+    <t>06.06.20249</t>
+  </si>
+  <si>
+    <t>06.06.202410</t>
+  </si>
+  <si>
+    <t>06.06.202411</t>
+  </si>
+  <si>
+    <t>06.06.202412</t>
+  </si>
+  <si>
+    <t>06.06.202413</t>
+  </si>
+  <si>
+    <t>06.06.202414</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>0.416</v>
+        <v>0.639</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>1.021</v>
+        <v>0.461</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>1.649</v>
+        <v>0.137</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>2.161</v>
+        <v>0.133</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>2.994</v>
+        <v>0.046</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>3.123</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B10">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C10">
-        <v>2.901</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45431</v>
+        <v>45442</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>2.779</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1.788</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B14">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>1.431</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B15">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>0.944</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B16">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>0.379</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.101</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B19">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.376</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45431</v>
+        <v>45443</v>
       </c>
       <c r="B20">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1.859</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2.447</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2.848</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2.927</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>2.881</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2.773</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>0.076</v>
+        <v>2.317</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>0.392</v>
+        <v>1.791</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B29">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>0.77</v>
+        <v>1.369</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B30">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C30">
-        <v>1.186</v>
+        <v>0.804</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B31">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C31">
-        <v>1.834</v>
+        <v>0.299</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C32">
-        <v>2.122</v>
+        <v>0.046</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B33">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C33">
-        <v>2.537</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B34">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C34">
-        <v>2.622</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45432</v>
+        <v>45443</v>
       </c>
       <c r="B35">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C35">
-        <v>2.604</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B36">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>2.307</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B37">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>1.83</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B38">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>1.298</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B39">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C39">
-        <v>0.701</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B40">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C40">
-        <v>0.237</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B41">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C41">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B42">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.093</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B43">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.443</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45432</v>
+        <v>45444</v>
       </c>
       <c r="B44">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1.218</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1.887</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>2.184</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>2.616</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>2.631</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>2.707</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C51">
-        <v>0.076</v>
+        <v>2.342</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>0.379</v>
+        <v>2.043</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C53">
-        <v>0.718</v>
+        <v>1.613</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C54">
-        <v>1.259</v>
+        <v>1.117</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B55">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C55">
-        <v>1.88</v>
+        <v>0.475</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B56">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C56">
-        <v>2.789</v>
+        <v>0.074</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B57">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C57">
-        <v>2.878</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B58">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C58">
-        <v>2.806</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45433</v>
+        <v>45444</v>
       </c>
       <c r="B59">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C59">
-        <v>2.798</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B60">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>2.49</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B61">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C61">
-        <v>1.787</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B62">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C62">
-        <v>1.312</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B63">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C63">
-        <v>0.79</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B64">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C64">
-        <v>0.256</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B65">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C65">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B66">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B67">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>0.489</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45433</v>
+        <v>45445</v>
       </c>
       <c r="B68">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1.237</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>2.027</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>2.872</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B72">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>2.849</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>2.844</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>2.822</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B75">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C75">
-        <v>0.076</v>
+        <v>2.62</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B76">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C76">
-        <v>0.38</v>
+        <v>2.082</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B77">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C77">
-        <v>0.973</v>
+        <v>1.649</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B78">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C78">
-        <v>1.563</v>
+        <v>1.158</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B79">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C79">
-        <v>2.025</v>
+        <v>0.46</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B80">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C80">
-        <v>2.155</v>
+        <v>0.076</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B81">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C81">
-        <v>2.069</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B82">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C82">
-        <v>2.033</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="B83">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C83">
-        <v>2.081</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B84">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C84">
-        <v>1.611</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B85">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C85">
-        <v>1.358</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B86">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C86">
-        <v>0.842</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B87">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C87">
-        <v>0.472</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B88">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C88">
-        <v>0.236</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B89">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C89">
-        <v>0.038</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B90">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B91">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.441</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45434</v>
+        <v>45446</v>
       </c>
       <c r="B92">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.795</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1.572</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1.924</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B95">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>2.619</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B96">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>2.675</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>2.715</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B98">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>2.318</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B99">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C99">
-        <v>0.08400000000000001</v>
+        <v>1.872</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B100">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C100">
-        <v>0.413</v>
+        <v>1.514</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B101">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C101">
-        <v>0.624</v>
+        <v>1.025</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B102">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C102">
-        <v>1.044</v>
+        <v>0.727</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B103">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C103">
-        <v>1.742</v>
+        <v>0.299</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B104">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C104">
-        <v>2.234</v>
+        <v>0.055</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B105">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C105">
-        <v>2.665</v>
+        <v>0</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B106">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C106">
-        <v>2.598</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45435</v>
+        <v>45446</v>
       </c>
       <c r="B107">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C107">
-        <v>2.472</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B108">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>2.04</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B109">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C109">
-        <v>1.459</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B110">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C110">
-        <v>0.925</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B111">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C111">
-        <v>0.468</v>
+        <v>0</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B112">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C112">
-        <v>0.204</v>
+        <v>0</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B113">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C113">
-        <v>0.042</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B114">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>0.115</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B115">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.445</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="B116">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1.175</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B117">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1.938</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>2.407</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B119">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>2.613</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B120">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>2.519</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B121">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>2.577</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B122">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>2.471</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B123">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C123">
-        <v>0.08400000000000001</v>
+        <v>2.124</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B124">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C124">
-        <v>0.309</v>
+        <v>1.72</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B125">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C125">
-        <v>0.58</v>
+        <v>1.11</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B126">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C126">
-        <v>1.06</v>
+        <v>0.727</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B127">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C127">
-        <v>1.341</v>
+        <v>0.307</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B128">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C128">
-        <v>1.797</v>
+        <v>0.055</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B129">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C129">
-        <v>1.957</v>
+        <v>0</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B130">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C130">
-        <v>2.255</v>
+        <v>0</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="B131">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C131">
-        <v>2.155</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B132">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C132">
-        <v>2.026</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B133">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C133">
-        <v>1.725</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B134">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C134">
-        <v>1.264</v>
+        <v>0</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B135">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C135">
-        <v>0.794</v>
+        <v>0</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B136">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C136">
-        <v>0.302</v>
+        <v>0</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B137">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C137">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B138">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>0.097</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B139">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45436</v>
+        <v>45448</v>
       </c>
       <c r="B140">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>0.572</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B141">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>0.952</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>1.354</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B143">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>2.041</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B144">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>1.868</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B145">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>2.552</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B146">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>2.485</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B147">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C147">
-        <v>0.098</v>
+        <v>2.387</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B148">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C148">
-        <v>0.395</v>
+        <v>1.991</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B149">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C149">
-        <v>1.131</v>
+        <v>1.457</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B150">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C150">
-        <v>1.827</v>
+        <v>0.916</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B151">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C151">
-        <v>2.399</v>
+        <v>0.406</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B152">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C152">
-        <v>2.87</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B153">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C153">
-        <v>2.809</v>
+        <v>0</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B154">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C154">
-        <v>2.873</v>
+        <v>0</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="B155">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C155">
-        <v>2.792</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B156">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C156">
-        <v>2.717</v>
+        <v>0</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B157">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C157">
-        <v>2.033</v>
+        <v>0</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B158">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C158">
-        <v>1.664</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B159">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C159">
-        <v>0.992</v>
+        <v>0</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B160">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C160">
-        <v>0.379</v>
+        <v>0</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B161">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C161">
-        <v>0.037</v>
+        <v>0</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B162">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>0.082</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B163">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>0.361</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45437</v>
+        <v>45449</v>
       </c>
       <c r="B164">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>0.986</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="B165">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>1.652</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="B166">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>2.32</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="B167">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>2.676</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="B168">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>2.675</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="B169">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>2.778</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="B170">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C170">
-        <v>0</v>
+        <v>2.737</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the Uplaoder for Transelectrica weekly consumption and production files used in Decision Making
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>30.05.202414</t>
-  </si>
-  <si>
-    <t>30.05.202415</t>
-  </si>
-  <si>
-    <t>30.05.202416</t>
-  </si>
-  <si>
-    <t>30.05.202417</t>
-  </si>
-  <si>
-    <t>30.05.202418</t>
-  </si>
-  <si>
-    <t>30.05.202419</t>
-  </si>
-  <si>
-    <t>30.05.202420</t>
-  </si>
-  <si>
-    <t>30.05.202421</t>
-  </si>
-  <si>
-    <t>30.05.202422</t>
-  </si>
-  <si>
-    <t>30.05.202423</t>
-  </si>
-  <si>
-    <t>31.05.20240</t>
-  </si>
-  <si>
-    <t>31.05.20241</t>
-  </si>
-  <si>
-    <t>31.05.20242</t>
-  </si>
-  <si>
-    <t>31.05.20243</t>
-  </si>
-  <si>
-    <t>31.05.20244</t>
-  </si>
-  <si>
-    <t>31.05.20245</t>
-  </si>
-  <si>
-    <t>31.05.20246</t>
-  </si>
-  <si>
-    <t>31.05.20247</t>
-  </si>
-  <si>
-    <t>31.05.20248</t>
-  </si>
-  <si>
-    <t>31.05.20249</t>
-  </si>
-  <si>
-    <t>31.05.202410</t>
-  </si>
-  <si>
-    <t>31.05.202411</t>
-  </si>
-  <si>
-    <t>31.05.202412</t>
-  </si>
-  <si>
-    <t>31.05.202413</t>
-  </si>
-  <si>
-    <t>31.05.202414</t>
-  </si>
-  <si>
-    <t>31.05.202415</t>
-  </si>
-  <si>
-    <t>31.05.202416</t>
-  </si>
-  <si>
-    <t>31.05.202417</t>
-  </si>
-  <si>
-    <t>31.05.202418</t>
-  </si>
-  <si>
-    <t>31.05.202419</t>
-  </si>
-  <si>
-    <t>31.05.202420</t>
-  </si>
-  <si>
-    <t>31.05.202421</t>
-  </si>
-  <si>
-    <t>31.05.202422</t>
-  </si>
-  <si>
-    <t>31.05.202423</t>
-  </si>
-  <si>
-    <t>01.06.20240</t>
-  </si>
-  <si>
-    <t>01.06.20241</t>
-  </si>
-  <si>
-    <t>01.06.20242</t>
-  </si>
-  <si>
-    <t>01.06.20243</t>
-  </si>
-  <si>
-    <t>01.06.20244</t>
-  </si>
-  <si>
-    <t>01.06.20245</t>
-  </si>
-  <si>
-    <t>01.06.20246</t>
-  </si>
-  <si>
-    <t>01.06.20247</t>
-  </si>
-  <si>
-    <t>01.06.20248</t>
-  </si>
-  <si>
-    <t>01.06.20249</t>
-  </si>
-  <si>
-    <t>01.06.202410</t>
-  </si>
-  <si>
-    <t>01.06.202411</t>
-  </si>
-  <si>
-    <t>01.06.202412</t>
-  </si>
-  <si>
-    <t>01.06.202413</t>
-  </si>
-  <si>
-    <t>01.06.202414</t>
-  </si>
-  <si>
-    <t>01.06.202415</t>
-  </si>
-  <si>
-    <t>01.06.202416</t>
-  </si>
-  <si>
-    <t>01.06.202417</t>
-  </si>
-  <si>
-    <t>01.06.202418</t>
-  </si>
-  <si>
-    <t>01.06.202419</t>
-  </si>
-  <si>
-    <t>01.06.202420</t>
-  </si>
-  <si>
-    <t>01.06.202421</t>
-  </si>
-  <si>
-    <t>01.06.202422</t>
-  </si>
-  <si>
-    <t>01.06.202423</t>
-  </si>
-  <si>
-    <t>02.06.20240</t>
-  </si>
-  <si>
-    <t>02.06.20241</t>
-  </si>
-  <si>
-    <t>02.06.20242</t>
-  </si>
-  <si>
-    <t>02.06.20243</t>
-  </si>
-  <si>
-    <t>02.06.20244</t>
-  </si>
-  <si>
-    <t>02.06.20245</t>
-  </si>
-  <si>
-    <t>02.06.20246</t>
-  </si>
-  <si>
-    <t>02.06.20247</t>
-  </si>
-  <si>
-    <t>02.06.20248</t>
-  </si>
-  <si>
-    <t>02.06.20249</t>
-  </si>
-  <si>
-    <t>02.06.202410</t>
-  </si>
-  <si>
-    <t>02.06.202411</t>
-  </si>
-  <si>
-    <t>02.06.202412</t>
-  </si>
-  <si>
-    <t>02.06.202413</t>
-  </si>
-  <si>
-    <t>02.06.202414</t>
-  </si>
-  <si>
-    <t>02.06.202415</t>
-  </si>
-  <si>
-    <t>02.06.202416</t>
-  </si>
-  <si>
-    <t>02.06.202417</t>
-  </si>
-  <si>
-    <t>02.06.202418</t>
-  </si>
-  <si>
-    <t>02.06.202419</t>
-  </si>
-  <si>
-    <t>02.06.202420</t>
-  </si>
-  <si>
-    <t>02.06.202421</t>
-  </si>
-  <si>
-    <t>02.06.202422</t>
-  </si>
-  <si>
-    <t>02.06.202423</t>
-  </si>
-  <si>
-    <t>03.06.20240</t>
-  </si>
-  <si>
-    <t>03.06.20241</t>
-  </si>
-  <si>
-    <t>03.06.20242</t>
-  </si>
-  <si>
-    <t>03.06.20243</t>
-  </si>
-  <si>
-    <t>03.06.20244</t>
-  </si>
-  <si>
-    <t>03.06.20245</t>
-  </si>
-  <si>
-    <t>03.06.20246</t>
-  </si>
-  <si>
-    <t>03.06.20247</t>
-  </si>
-  <si>
-    <t>03.06.20248</t>
-  </si>
-  <si>
-    <t>03.06.20249</t>
-  </si>
-  <si>
-    <t>03.06.202410</t>
-  </si>
-  <si>
-    <t>03.06.202411</t>
-  </si>
-  <si>
-    <t>03.06.202412</t>
-  </si>
-  <si>
-    <t>03.06.202413</t>
-  </si>
-  <si>
-    <t>03.06.202414</t>
-  </si>
-  <si>
-    <t>03.06.202415</t>
-  </si>
-  <si>
-    <t>03.06.202416</t>
-  </si>
-  <si>
-    <t>03.06.202417</t>
-  </si>
-  <si>
-    <t>03.06.202418</t>
-  </si>
-  <si>
-    <t>03.06.202419</t>
-  </si>
-  <si>
-    <t>03.06.202420</t>
-  </si>
-  <si>
-    <t>03.06.202421</t>
-  </si>
-  <si>
-    <t>03.06.202422</t>
-  </si>
-  <si>
-    <t>03.06.202423</t>
-  </si>
-  <si>
-    <t>04.06.20240</t>
-  </si>
-  <si>
-    <t>04.06.20241</t>
-  </si>
-  <si>
-    <t>04.06.20242</t>
-  </si>
-  <si>
-    <t>04.06.20243</t>
-  </si>
-  <si>
-    <t>04.06.20244</t>
-  </si>
-  <si>
-    <t>04.06.20245</t>
-  </si>
-  <si>
-    <t>04.06.20246</t>
-  </si>
-  <si>
-    <t>04.06.20247</t>
-  </si>
-  <si>
-    <t>04.06.20248</t>
-  </si>
-  <si>
-    <t>04.06.20249</t>
-  </si>
-  <si>
-    <t>04.06.202410</t>
-  </si>
-  <si>
-    <t>04.06.202411</t>
-  </si>
-  <si>
-    <t>04.06.202412</t>
-  </si>
-  <si>
-    <t>04.06.202413</t>
-  </si>
-  <si>
-    <t>04.06.202414</t>
-  </si>
-  <si>
-    <t>04.06.202415</t>
-  </si>
-  <si>
-    <t>04.06.202416</t>
-  </si>
-  <si>
-    <t>04.06.202417</t>
-  </si>
-  <si>
-    <t>04.06.202418</t>
-  </si>
-  <si>
-    <t>04.06.202419</t>
-  </si>
-  <si>
-    <t>04.06.202420</t>
-  </si>
-  <si>
-    <t>04.06.202421</t>
-  </si>
-  <si>
-    <t>04.06.202422</t>
-  </si>
-  <si>
-    <t>04.06.202423</t>
-  </si>
-  <si>
-    <t>05.06.20240</t>
-  </si>
-  <si>
-    <t>05.06.20241</t>
-  </si>
-  <si>
-    <t>05.06.20242</t>
-  </si>
-  <si>
-    <t>05.06.20243</t>
-  </si>
-  <si>
-    <t>05.06.20244</t>
-  </si>
-  <si>
-    <t>05.06.20245</t>
-  </si>
-  <si>
-    <t>05.06.20246</t>
-  </si>
-  <si>
-    <t>05.06.20247</t>
-  </si>
-  <si>
-    <t>05.06.20248</t>
-  </si>
-  <si>
-    <t>05.06.20249</t>
-  </si>
-  <si>
-    <t>05.06.202410</t>
-  </si>
-  <si>
-    <t>05.06.202411</t>
-  </si>
-  <si>
-    <t>05.06.202412</t>
-  </si>
-  <si>
-    <t>05.06.202413</t>
-  </si>
-  <si>
-    <t>05.06.202414</t>
-  </si>
-  <si>
-    <t>05.06.202415</t>
-  </si>
-  <si>
-    <t>05.06.202416</t>
-  </si>
-  <si>
-    <t>05.06.202417</t>
-  </si>
-  <si>
-    <t>05.06.202418</t>
-  </si>
-  <si>
-    <t>05.06.202419</t>
-  </si>
-  <si>
-    <t>05.06.202420</t>
-  </si>
-  <si>
-    <t>05.06.202421</t>
-  </si>
-  <si>
-    <t>05.06.202422</t>
-  </si>
-  <si>
-    <t>05.06.202423</t>
-  </si>
-  <si>
-    <t>06.06.20240</t>
-  </si>
-  <si>
-    <t>06.06.20241</t>
-  </si>
-  <si>
-    <t>06.06.20242</t>
-  </si>
-  <si>
-    <t>06.06.20243</t>
-  </si>
-  <si>
-    <t>06.06.20244</t>
-  </si>
-  <si>
-    <t>06.06.20245</t>
-  </si>
-  <si>
-    <t>06.06.20246</t>
-  </si>
-  <si>
-    <t>06.06.20247</t>
-  </si>
-  <si>
-    <t>06.06.20248</t>
-  </si>
-  <si>
-    <t>06.06.20249</t>
-  </si>
-  <si>
-    <t>06.06.202410</t>
-  </si>
-  <si>
-    <t>06.06.202411</t>
-  </si>
-  <si>
-    <t>06.06.202412</t>
-  </si>
-  <si>
-    <t>06.06.202413</t>
-  </si>
-  <si>
-    <t>06.06.202414</t>
+    <t>10.06.202410</t>
+  </si>
+  <si>
+    <t>10.06.202411</t>
+  </si>
+  <si>
+    <t>10.06.202412</t>
+  </si>
+  <si>
+    <t>10.06.202413</t>
+  </si>
+  <si>
+    <t>10.06.202414</t>
+  </si>
+  <si>
+    <t>10.06.202415</t>
+  </si>
+  <si>
+    <t>10.06.202416</t>
+  </si>
+  <si>
+    <t>10.06.202417</t>
+  </si>
+  <si>
+    <t>10.06.202418</t>
+  </si>
+  <si>
+    <t>10.06.202419</t>
+  </si>
+  <si>
+    <t>10.06.202420</t>
+  </si>
+  <si>
+    <t>10.06.202421</t>
+  </si>
+  <si>
+    <t>10.06.202422</t>
+  </si>
+  <si>
+    <t>10.06.202423</t>
+  </si>
+  <si>
+    <t>11.06.20240</t>
+  </si>
+  <si>
+    <t>11.06.20241</t>
+  </si>
+  <si>
+    <t>11.06.20242</t>
+  </si>
+  <si>
+    <t>11.06.20243</t>
+  </si>
+  <si>
+    <t>11.06.20244</t>
+  </si>
+  <si>
+    <t>11.06.20245</t>
+  </si>
+  <si>
+    <t>11.06.20246</t>
+  </si>
+  <si>
+    <t>11.06.20247</t>
+  </si>
+  <si>
+    <t>11.06.20248</t>
+  </si>
+  <si>
+    <t>11.06.20249</t>
+  </si>
+  <si>
+    <t>11.06.202410</t>
+  </si>
+  <si>
+    <t>11.06.202411</t>
+  </si>
+  <si>
+    <t>11.06.202412</t>
+  </si>
+  <si>
+    <t>11.06.202413</t>
+  </si>
+  <si>
+    <t>11.06.202414</t>
+  </si>
+  <si>
+    <t>11.06.202415</t>
+  </si>
+  <si>
+    <t>11.06.202416</t>
+  </si>
+  <si>
+    <t>11.06.202417</t>
+  </si>
+  <si>
+    <t>11.06.202418</t>
+  </si>
+  <si>
+    <t>11.06.202419</t>
+  </si>
+  <si>
+    <t>11.06.202420</t>
+  </si>
+  <si>
+    <t>11.06.202421</t>
+  </si>
+  <si>
+    <t>11.06.202422</t>
+  </si>
+  <si>
+    <t>11.06.202423</t>
+  </si>
+  <si>
+    <t>12.06.20240</t>
+  </si>
+  <si>
+    <t>12.06.20241</t>
+  </si>
+  <si>
+    <t>12.06.20242</t>
+  </si>
+  <si>
+    <t>12.06.20243</t>
+  </si>
+  <si>
+    <t>12.06.20244</t>
+  </si>
+  <si>
+    <t>12.06.20245</t>
+  </si>
+  <si>
+    <t>12.06.20246</t>
+  </si>
+  <si>
+    <t>12.06.20247</t>
+  </si>
+  <si>
+    <t>12.06.20248</t>
+  </si>
+  <si>
+    <t>12.06.20249</t>
+  </si>
+  <si>
+    <t>12.06.202410</t>
+  </si>
+  <si>
+    <t>12.06.202411</t>
+  </si>
+  <si>
+    <t>12.06.202412</t>
+  </si>
+  <si>
+    <t>12.06.202413</t>
+  </si>
+  <si>
+    <t>12.06.202414</t>
+  </si>
+  <si>
+    <t>12.06.202415</t>
+  </si>
+  <si>
+    <t>12.06.202416</t>
+  </si>
+  <si>
+    <t>12.06.202417</t>
+  </si>
+  <si>
+    <t>12.06.202418</t>
+  </si>
+  <si>
+    <t>12.06.202419</t>
+  </si>
+  <si>
+    <t>12.06.202420</t>
+  </si>
+  <si>
+    <t>12.06.202421</t>
+  </si>
+  <si>
+    <t>12.06.202422</t>
+  </si>
+  <si>
+    <t>12.06.202423</t>
+  </si>
+  <si>
+    <t>13.06.20240</t>
+  </si>
+  <si>
+    <t>13.06.20241</t>
+  </si>
+  <si>
+    <t>13.06.20242</t>
+  </si>
+  <si>
+    <t>13.06.20243</t>
+  </si>
+  <si>
+    <t>13.06.20244</t>
+  </si>
+  <si>
+    <t>13.06.20245</t>
+  </si>
+  <si>
+    <t>13.06.20246</t>
+  </si>
+  <si>
+    <t>13.06.20247</t>
+  </si>
+  <si>
+    <t>13.06.20248</t>
+  </si>
+  <si>
+    <t>13.06.20249</t>
+  </si>
+  <si>
+    <t>13.06.202410</t>
+  </si>
+  <si>
+    <t>13.06.202411</t>
+  </si>
+  <si>
+    <t>13.06.202412</t>
+  </si>
+  <si>
+    <t>13.06.202413</t>
+  </si>
+  <si>
+    <t>13.06.202414</t>
+  </si>
+  <si>
+    <t>13.06.202415</t>
+  </si>
+  <si>
+    <t>13.06.202416</t>
+  </si>
+  <si>
+    <t>13.06.202417</t>
+  </si>
+  <si>
+    <t>13.06.202418</t>
+  </si>
+  <si>
+    <t>13.06.202419</t>
+  </si>
+  <si>
+    <t>13.06.202420</t>
+  </si>
+  <si>
+    <t>13.06.202421</t>
+  </si>
+  <si>
+    <t>13.06.202422</t>
+  </si>
+  <si>
+    <t>13.06.202423</t>
+  </si>
+  <si>
+    <t>14.06.20240</t>
+  </si>
+  <si>
+    <t>14.06.20241</t>
+  </si>
+  <si>
+    <t>14.06.20242</t>
+  </si>
+  <si>
+    <t>14.06.20243</t>
+  </si>
+  <si>
+    <t>14.06.20244</t>
+  </si>
+  <si>
+    <t>14.06.20245</t>
+  </si>
+  <si>
+    <t>14.06.20246</t>
+  </si>
+  <si>
+    <t>14.06.20247</t>
+  </si>
+  <si>
+    <t>14.06.20248</t>
+  </si>
+  <si>
+    <t>14.06.20249</t>
+  </si>
+  <si>
+    <t>14.06.202410</t>
+  </si>
+  <si>
+    <t>14.06.202411</t>
+  </si>
+  <si>
+    <t>14.06.202412</t>
+  </si>
+  <si>
+    <t>14.06.202413</t>
+  </si>
+  <si>
+    <t>14.06.202414</t>
+  </si>
+  <si>
+    <t>14.06.202415</t>
+  </si>
+  <si>
+    <t>14.06.202416</t>
+  </si>
+  <si>
+    <t>14.06.202417</t>
+  </si>
+  <si>
+    <t>14.06.202418</t>
+  </si>
+  <si>
+    <t>14.06.202419</t>
+  </si>
+  <si>
+    <t>14.06.202420</t>
+  </si>
+  <si>
+    <t>14.06.202421</t>
+  </si>
+  <si>
+    <t>14.06.202422</t>
+  </si>
+  <si>
+    <t>14.06.202423</t>
+  </si>
+  <si>
+    <t>15.06.20240</t>
+  </si>
+  <si>
+    <t>15.06.20241</t>
+  </si>
+  <si>
+    <t>15.06.20242</t>
+  </si>
+  <si>
+    <t>15.06.20243</t>
+  </si>
+  <si>
+    <t>15.06.20244</t>
+  </si>
+  <si>
+    <t>15.06.20245</t>
+  </si>
+  <si>
+    <t>15.06.20246</t>
+  </si>
+  <si>
+    <t>15.06.20247</t>
+  </si>
+  <si>
+    <t>15.06.20248</t>
+  </si>
+  <si>
+    <t>15.06.20249</t>
+  </si>
+  <si>
+    <t>15.06.202410</t>
+  </si>
+  <si>
+    <t>15.06.202411</t>
+  </si>
+  <si>
+    <t>15.06.202412</t>
+  </si>
+  <si>
+    <t>15.06.202413</t>
+  </si>
+  <si>
+    <t>15.06.202414</t>
+  </si>
+  <si>
+    <t>15.06.202415</t>
+  </si>
+  <si>
+    <t>15.06.202416</t>
+  </si>
+  <si>
+    <t>15.06.202417</t>
+  </si>
+  <si>
+    <t>15.06.202418</t>
+  </si>
+  <si>
+    <t>15.06.202419</t>
+  </si>
+  <si>
+    <t>15.06.202420</t>
+  </si>
+  <si>
+    <t>15.06.202421</t>
+  </si>
+  <si>
+    <t>15.06.202422</t>
+  </si>
+  <si>
+    <t>15.06.202423</t>
+  </si>
+  <si>
+    <t>16.06.20240</t>
+  </si>
+  <si>
+    <t>16.06.20241</t>
+  </si>
+  <si>
+    <t>16.06.20242</t>
+  </si>
+  <si>
+    <t>16.06.20243</t>
+  </si>
+  <si>
+    <t>16.06.20244</t>
+  </si>
+  <si>
+    <t>16.06.20245</t>
+  </si>
+  <si>
+    <t>16.06.20246</t>
+  </si>
+  <si>
+    <t>16.06.20247</t>
+  </si>
+  <si>
+    <t>16.06.20248</t>
+  </si>
+  <si>
+    <t>16.06.20249</t>
+  </si>
+  <si>
+    <t>16.06.202410</t>
+  </si>
+  <si>
+    <t>16.06.202411</t>
+  </si>
+  <si>
+    <t>16.06.202412</t>
+  </si>
+  <si>
+    <t>16.06.202413</t>
+  </si>
+  <si>
+    <t>16.06.202414</t>
+  </si>
+  <si>
+    <t>16.06.202415</t>
+  </si>
+  <si>
+    <t>16.06.202416</t>
+  </si>
+  <si>
+    <t>16.06.202417</t>
+  </si>
+  <si>
+    <t>16.06.202418</t>
+  </si>
+  <si>
+    <t>16.06.202419</t>
+  </si>
+  <si>
+    <t>16.06.202420</t>
+  </si>
+  <si>
+    <t>16.06.202421</t>
+  </si>
+  <si>
+    <t>16.06.202422</t>
+  </si>
+  <si>
+    <t>16.06.202423</t>
+  </si>
+  <si>
+    <t>17.06.20240</t>
+  </si>
+  <si>
+    <t>17.06.20241</t>
+  </si>
+  <si>
+    <t>17.06.20242</t>
+  </si>
+  <si>
+    <t>17.06.20243</t>
+  </si>
+  <si>
+    <t>17.06.20244</t>
+  </si>
+  <si>
+    <t>17.06.20245</t>
+  </si>
+  <si>
+    <t>17.06.20246</t>
+  </si>
+  <si>
+    <t>17.06.20247</t>
+  </si>
+  <si>
+    <t>17.06.20248</t>
+  </si>
+  <si>
+    <t>17.06.20249</t>
+  </si>
+  <si>
+    <t>17.06.202410</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0.639</v>
+        <v>1.075</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>0.461</v>
+        <v>2.711</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>0.137</v>
+        <v>2.163</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0.133</v>
+        <v>1.856</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0.046</v>
+        <v>1.399</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.999</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.784</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45442</v>
+        <v>45453</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.282</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45443</v>
+        <v>45453</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45443</v>
+        <v>45453</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45443</v>
+        <v>45453</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45443</v>
+        <v>45453</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>0.101</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>0.376</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>1.08</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>1.859</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>2.447</v>
+        <v>0.094</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>2.848</v>
+        <v>0.443</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>2.927</v>
+        <v>1.108</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>2.881</v>
+        <v>1.819</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>2.773</v>
+        <v>2.417</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>2.317</v>
+        <v>2.614</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>1.791</v>
+        <v>2.261</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>1.369</v>
+        <v>2.011</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>0.804</v>
+        <v>1.838</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0.299</v>
+        <v>1.729</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>0.046</v>
+        <v>1.478</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1.157</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.889</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45443</v>
+        <v>45454</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.444</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45444</v>
+        <v>45454</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45444</v>
+        <v>45454</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45444</v>
+        <v>45454</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45444</v>
+        <v>45454</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>0.093</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>0.443</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>0.68</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>1.218</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>1.887</v>
+        <v>0.079</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B47">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>2.184</v>
+        <v>0.33</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>2.616</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>2.631</v>
+        <v>0.896</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>2.707</v>
+        <v>1.127</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>2.342</v>
+        <v>1.392</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>2.043</v>
+        <v>1.702</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B53">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>1.613</v>
+        <v>1.914</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>1.117</v>
+        <v>1.581</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B55">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>0.475</v>
+        <v>1.426</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>0.074</v>
+        <v>1.185</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B57">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45444</v>
+        <v>45455</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.368</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45445</v>
+        <v>45455</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.074</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45445</v>
+        <v>45455</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45445</v>
+        <v>45455</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45445</v>
+        <v>45455</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>0.489</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>1.237</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>2.027</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>2.7</v>
+        <v>0.097</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>2.872</v>
+        <v>0.414</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>2.849</v>
+        <v>0.616</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B73">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>2.844</v>
+        <v>0.99</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B74">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>2.822</v>
+        <v>1.707</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B75">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>2.62</v>
+        <v>1.751</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B76">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>2.082</v>
+        <v>1.908</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>1.649</v>
+        <v>2.082</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>1.158</v>
+        <v>1.918</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B79">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C79">
-        <v>0.46</v>
+        <v>1.769</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B80">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>0.076</v>
+        <v>1.359</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B81">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B82">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45445</v>
+        <v>45456</v>
       </c>
       <c r="B83">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.276</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45446</v>
+        <v>45456</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.055</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45446</v>
+        <v>45456</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45446</v>
+        <v>45456</v>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45446</v>
+        <v>45456</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B88">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B90">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>0.08699999999999999</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B91">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>0.441</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B92">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>0.795</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B93">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C93">
-        <v>1.572</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B94">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>1.924</v>
+        <v>0.097</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B95">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C95">
-        <v>2.619</v>
+        <v>0.381</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B96">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>2.675</v>
+        <v>0.579</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B97">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>2.715</v>
+        <v>0.962</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B98">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C98">
-        <v>2.318</v>
+        <v>1.345</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B99">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C99">
-        <v>1.872</v>
+        <v>1.742</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B100">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C100">
-        <v>1.514</v>
+        <v>1.878</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B101">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C101">
-        <v>1.025</v>
+        <v>1.796</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B102">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C102">
-        <v>0.727</v>
+        <v>1.78</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B103">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C103">
-        <v>0.299</v>
+        <v>1.724</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B104">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C104">
-        <v>0.055</v>
+        <v>1.471</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B105">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>1.073</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B106">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>0.765</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45446</v>
+        <v>45457</v>
       </c>
       <c r="B107">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45447</v>
+        <v>45457</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45447</v>
+        <v>45457</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45447</v>
+        <v>45457</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45447</v>
+        <v>45457</v>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B112">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B113">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B114">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C114">
-        <v>0.115</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B115">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>0.445</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B116">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>1.175</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B117">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>1.938</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B118">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>2.407</v>
+        <v>0.111</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B119">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>2.613</v>
+        <v>0.446</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B120">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <v>2.519</v>
+        <v>1.108</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B121">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C121">
-        <v>2.577</v>
+        <v>1.821</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B122">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C122">
-        <v>2.471</v>
+        <v>2.438</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B123">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C123">
-        <v>2.124</v>
+        <v>2.822</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B124">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C124">
-        <v>1.72</v>
+        <v>2.856</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B125">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C125">
-        <v>1.11</v>
+        <v>2.786</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B126">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C126">
-        <v>0.727</v>
+        <v>2.383</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B127">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C127">
-        <v>0.307</v>
+        <v>2.046</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B128">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C128">
-        <v>0.055</v>
+        <v>1.79</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B129">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1.376</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B130">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>0.874</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45447</v>
+        <v>45458</v>
       </c>
       <c r="B131">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.449</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45448</v>
+        <v>45458</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.077</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45448</v>
+        <v>45458</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45448</v>
+        <v>45458</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45448</v>
+        <v>45458</v>
       </c>
       <c r="B135">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B136">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B138">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C138">
-        <v>0.097</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B139">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>0.369</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B140">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C140">
-        <v>0.572</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B141">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C141">
-        <v>0.952</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B142">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C142">
-        <v>1.354</v>
+        <v>0.118</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B143">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>2.041</v>
+        <v>0.375</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B144">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C144">
-        <v>1.868</v>
+        <v>0.97</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B145">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>2.552</v>
+        <v>1.635</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B146">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C146">
-        <v>2.485</v>
+        <v>2.209</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B147">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C147">
-        <v>2.387</v>
+        <v>2.546</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B148">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C148">
-        <v>1.991</v>
+        <v>2.764</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B149">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C149">
-        <v>1.457</v>
+        <v>2.863</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B150">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C150">
-        <v>0.916</v>
+        <v>2.961</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B151">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C151">
-        <v>0.406</v>
+        <v>2.868</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B152">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C152">
-        <v>0.07199999999999999</v>
+        <v>2.45</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B153">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>1.815</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B154">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>1.141</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45448</v>
+        <v>45459</v>
       </c>
       <c r="B155">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45449</v>
+        <v>45459</v>
       </c>
       <c r="B156">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45449</v>
+        <v>45459</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45449</v>
+        <v>45459</v>
       </c>
       <c r="B158">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45449</v>
+        <v>45459</v>
       </c>
       <c r="B159">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B160">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B161">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B162">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C162">
-        <v>0.082</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B163">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C163">
-        <v>0.361</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B164">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>0.986</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B165">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C165">
-        <v>1.652</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B166">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C166">
-        <v>2.32</v>
+        <v>0.117</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B167">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>2.676</v>
+        <v>0.462</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B168">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C168">
-        <v>2.675</v>
+        <v>1.133</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B169">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C169">
-        <v>2.778</v>
+        <v>1.806</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45449</v>
+        <v>45460</v>
       </c>
       <c r="B170">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C170">
-        <v>2.737</v>
+        <v>2.417</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Installing the xrdl for reading .xls file for processing the files from Transelectrica
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,144 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>10.06.202410</t>
-  </si>
-  <si>
-    <t>10.06.202411</t>
-  </si>
-  <si>
-    <t>10.06.202412</t>
-  </si>
-  <si>
-    <t>10.06.202413</t>
-  </si>
-  <si>
-    <t>10.06.202414</t>
-  </si>
-  <si>
-    <t>10.06.202415</t>
-  </si>
-  <si>
-    <t>10.06.202416</t>
-  </si>
-  <si>
-    <t>10.06.202417</t>
-  </si>
-  <si>
-    <t>10.06.202418</t>
-  </si>
-  <si>
-    <t>10.06.202419</t>
-  </si>
-  <si>
-    <t>10.06.202420</t>
-  </si>
-  <si>
-    <t>10.06.202421</t>
-  </si>
-  <si>
-    <t>10.06.202422</t>
-  </si>
-  <si>
-    <t>10.06.202423</t>
-  </si>
-  <si>
-    <t>11.06.20240</t>
-  </si>
-  <si>
-    <t>11.06.20241</t>
-  </si>
-  <si>
-    <t>11.06.20242</t>
-  </si>
-  <si>
-    <t>11.06.20243</t>
-  </si>
-  <si>
-    <t>11.06.20244</t>
-  </si>
-  <si>
-    <t>11.06.20245</t>
-  </si>
-  <si>
-    <t>11.06.20246</t>
-  </si>
-  <si>
-    <t>11.06.20247</t>
-  </si>
-  <si>
-    <t>11.06.20248</t>
-  </si>
-  <si>
-    <t>11.06.20249</t>
-  </si>
-  <si>
-    <t>11.06.202410</t>
-  </si>
-  <si>
-    <t>11.06.202411</t>
-  </si>
-  <si>
-    <t>11.06.202412</t>
-  </si>
-  <si>
-    <t>11.06.202413</t>
-  </si>
-  <si>
-    <t>11.06.202414</t>
-  </si>
-  <si>
-    <t>11.06.202415</t>
-  </si>
-  <si>
-    <t>11.06.202416</t>
-  </si>
-  <si>
-    <t>11.06.202417</t>
-  </si>
-  <si>
-    <t>11.06.202418</t>
-  </si>
-  <si>
-    <t>11.06.202419</t>
-  </si>
-  <si>
-    <t>11.06.202420</t>
-  </si>
-  <si>
-    <t>11.06.202421</t>
-  </si>
-  <si>
-    <t>11.06.202422</t>
-  </si>
-  <si>
-    <t>11.06.202423</t>
-  </si>
-  <si>
-    <t>12.06.20240</t>
-  </si>
-  <si>
-    <t>12.06.20241</t>
-  </si>
-  <si>
-    <t>12.06.20242</t>
-  </si>
-  <si>
-    <t>12.06.20243</t>
-  </si>
-  <si>
-    <t>12.06.20244</t>
-  </si>
-  <si>
-    <t>12.06.20245</t>
-  </si>
-  <si>
-    <t>12.06.20246</t>
-  </si>
-  <si>
-    <t>12.06.20247</t>
-  </si>
-  <si>
     <t>12.06.20248</t>
   </si>
   <si>
@@ -533,6 +395,144 @@
   </si>
   <si>
     <t>17.06.202410</t>
+  </si>
+  <si>
+    <t>17.06.202411</t>
+  </si>
+  <si>
+    <t>17.06.202412</t>
+  </si>
+  <si>
+    <t>17.06.202413</t>
+  </si>
+  <si>
+    <t>17.06.202414</t>
+  </si>
+  <si>
+    <t>17.06.202415</t>
+  </si>
+  <si>
+    <t>17.06.202416</t>
+  </si>
+  <si>
+    <t>17.06.202417</t>
+  </si>
+  <si>
+    <t>17.06.202418</t>
+  </si>
+  <si>
+    <t>17.06.202419</t>
+  </si>
+  <si>
+    <t>17.06.202420</t>
+  </si>
+  <si>
+    <t>17.06.202421</t>
+  </si>
+  <si>
+    <t>17.06.202422</t>
+  </si>
+  <si>
+    <t>17.06.202423</t>
+  </si>
+  <si>
+    <t>18.06.20240</t>
+  </si>
+  <si>
+    <t>18.06.20241</t>
+  </si>
+  <si>
+    <t>18.06.20242</t>
+  </si>
+  <si>
+    <t>18.06.20243</t>
+  </si>
+  <si>
+    <t>18.06.20244</t>
+  </si>
+  <si>
+    <t>18.06.20245</t>
+  </si>
+  <si>
+    <t>18.06.20246</t>
+  </si>
+  <si>
+    <t>18.06.20247</t>
+  </si>
+  <si>
+    <t>18.06.20248</t>
+  </si>
+  <si>
+    <t>18.06.20249</t>
+  </si>
+  <si>
+    <t>18.06.202410</t>
+  </si>
+  <si>
+    <t>18.06.202411</t>
+  </si>
+  <si>
+    <t>18.06.202412</t>
+  </si>
+  <si>
+    <t>18.06.202413</t>
+  </si>
+  <si>
+    <t>18.06.202414</t>
+  </si>
+  <si>
+    <t>18.06.202415</t>
+  </si>
+  <si>
+    <t>18.06.202416</t>
+  </si>
+  <si>
+    <t>18.06.202417</t>
+  </si>
+  <si>
+    <t>18.06.202418</t>
+  </si>
+  <si>
+    <t>18.06.202419</t>
+  </si>
+  <si>
+    <t>18.06.202420</t>
+  </si>
+  <si>
+    <t>18.06.202421</t>
+  </si>
+  <si>
+    <t>18.06.202422</t>
+  </si>
+  <si>
+    <t>18.06.202423</t>
+  </si>
+  <si>
+    <t>19.06.20240</t>
+  </si>
+  <si>
+    <t>19.06.20241</t>
+  </si>
+  <si>
+    <t>19.06.20242</t>
+  </si>
+  <si>
+    <t>19.06.20243</t>
+  </si>
+  <si>
+    <t>19.06.20244</t>
+  </si>
+  <si>
+    <t>19.06.20245</t>
+  </si>
+  <si>
+    <t>19.06.20246</t>
+  </si>
+  <si>
+    <t>19.06.20247</t>
+  </si>
+  <si>
+    <t>19.06.20248</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>1.075</v>
+        <v>2.392</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>2.711</v>
+        <v>2.949</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>2.163</v>
+        <v>3.003</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>1.856</v>
+        <v>2.717</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>1.399</v>
+        <v>2.44</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>0.999</v>
+        <v>1.772</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>0.784</v>
+        <v>1.208</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B11">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>0.282</v>
+        <v>0.776</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12">
-        <v>0.046</v>
+        <v>0.386</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B13">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.168</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B14">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="B15">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45454</v>
+        <v>45455</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45454</v>
+        <v>45455</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1182,10 +1182,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>0.094</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C23">
-        <v>0.443</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>1.108</v>
+        <v>0.081</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25">
-        <v>1.819</v>
+        <v>0.335</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>2.417</v>
+        <v>0.57</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>2.614</v>
+        <v>0.912</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B28">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>2.261</v>
+        <v>1.257</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B29">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>2.011</v>
+        <v>1.771</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B30">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C30">
-        <v>1.838</v>
+        <v>1.816</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B31">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>1.729</v>
+        <v>1.835</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B32">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C32">
-        <v>1.478</v>
+        <v>1.984</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B33">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C33">
-        <v>1.157</v>
+        <v>1.892</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B34">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C34">
-        <v>0.889</v>
+        <v>1.863</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B35">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C35">
-        <v>0.444</v>
+        <v>1.312</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C36">
-        <v>0.075</v>
+        <v>0.759</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B37">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.426</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B38">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>0.077</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="B39">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45455</v>
+        <v>45456</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45455</v>
+        <v>45456</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1518,10 +1518,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B45">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C46">
-        <v>0.079</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C48">
-        <v>0.5659999999999999</v>
+        <v>0.097</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C49">
-        <v>0.896</v>
+        <v>0.454</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B50">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>1.127</v>
+        <v>0.729</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B51">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51">
-        <v>1.392</v>
+        <v>1.291</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B52">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C52">
-        <v>1.702</v>
+        <v>1.786</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B53">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C53">
-        <v>1.914</v>
+        <v>2.329</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B54">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C54">
-        <v>1.581</v>
+        <v>2.683</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B55">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C55">
-        <v>1.426</v>
+        <v>2.793</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B56">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C56">
-        <v>1.185</v>
+        <v>2.825</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B57">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C57">
-        <v>0.95</v>
+        <v>2.65</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B58">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C58">
-        <v>0.73</v>
+        <v>2.288</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B59">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C59">
-        <v>0.368</v>
+        <v>1.683</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B60">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C60">
-        <v>0.074</v>
+        <v>1.143</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B61">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.507</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B62">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>0.097</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="B63">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45456</v>
+        <v>45457</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45456</v>
+        <v>45457</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,10 +1840,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B68">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1854,10 +1854,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B69">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B70">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C70">
-        <v>0.097</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B71">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C71">
-        <v>0.414</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B72">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C72">
-        <v>0.616</v>
+        <v>0.145</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B73">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C73">
-        <v>0.99</v>
+        <v>0.488</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B74">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C74">
-        <v>1.707</v>
+        <v>1.058</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B75">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C75">
-        <v>1.751</v>
+        <v>2.075</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B76">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C76">
-        <v>1.908</v>
+        <v>2.706</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B77">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C77">
-        <v>2.082</v>
+        <v>2.957</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B78">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C78">
-        <v>1.918</v>
+        <v>3.257</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B79">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C79">
-        <v>1.769</v>
+        <v>3.314</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B80">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C80">
-        <v>1.359</v>
+        <v>3.295</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B81">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C81">
-        <v>0.925</v>
+        <v>2.996</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B82">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C82">
-        <v>0.67</v>
+        <v>2.467</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B83">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C83">
-        <v>0.276</v>
+        <v>1.797</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B84">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C84">
-        <v>0.055</v>
+        <v>1.154</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B85">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.535</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B86">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.107</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="B87">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45457</v>
+        <v>45458</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45457</v>
+        <v>45458</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B91">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B92">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2190,10 +2190,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B93">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B94">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C94">
-        <v>0.097</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B95">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C95">
-        <v>0.381</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B96">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C96">
-        <v>0.579</v>
+        <v>0.125</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B97">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C97">
-        <v>0.962</v>
+        <v>0.37</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B98">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C98">
-        <v>1.345</v>
+        <v>0.968</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B99">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C99">
-        <v>1.742</v>
+        <v>1.783</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B100">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C100">
-        <v>1.878</v>
+        <v>2.407</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B101">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C101">
-        <v>1.796</v>
+        <v>2.932</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B102">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C102">
-        <v>1.78</v>
+        <v>3.071</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B103">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C103">
-        <v>1.724</v>
+        <v>3.008</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B104">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C104">
-        <v>1.471</v>
+        <v>2.819</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B105">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C105">
-        <v>1.073</v>
+        <v>2.681</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B106">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C106">
-        <v>0.765</v>
+        <v>2.033</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B107">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C107">
-        <v>0.416</v>
+        <v>1.65</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B108">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C108">
-        <v>0.075</v>
+        <v>1.123</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B109">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B110">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.077</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="B111">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45458</v>
+        <v>45459</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45458</v>
+        <v>45459</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B114">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B115">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2512,10 +2512,10 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B116">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -2526,10 +2526,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B117">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B118">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C118">
-        <v>0.111</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B119">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C119">
-        <v>0.446</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B120">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C120">
-        <v>1.108</v>
+        <v>0.111</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B121">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C121">
-        <v>1.821</v>
+        <v>0.446</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B122">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C122">
-        <v>2.438</v>
+        <v>1.169</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B123">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C123">
-        <v>2.822</v>
+        <v>1.839</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B124">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C124">
-        <v>2.856</v>
+        <v>2.425</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B125">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C125">
-        <v>2.786</v>
+        <v>2.871</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B126">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C126">
-        <v>2.383</v>
+        <v>3.071</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B127">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C127">
-        <v>2.046</v>
+        <v>3.259</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B128">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C128">
-        <v>1.79</v>
+        <v>3.151</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B129">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C129">
-        <v>1.376</v>
+        <v>2.868</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B130">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C130">
-        <v>0.874</v>
+        <v>2.462</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B131">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C131">
-        <v>0.449</v>
+        <v>1.813</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B132">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C132">
-        <v>0.077</v>
+        <v>1.154</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B133">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>0.512</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B134">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>0.107</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="B135">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45459</v>
+        <v>45460</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45459</v>
+        <v>45460</v>
       </c>
       <c r="B137">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B138">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B139">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2848,10 +2848,10 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B140">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -2862,10 +2862,10 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B141">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B142">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C142">
-        <v>0.118</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B143">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C143">
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B144">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C144">
-        <v>0.97</v>
+        <v>0.14</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B145">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C145">
-        <v>1.635</v>
+        <v>0.487</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B146">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C146">
-        <v>2.209</v>
+        <v>1.225</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B147">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C147">
-        <v>2.546</v>
+        <v>1.954</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B148">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C148">
-        <v>2.764</v>
+        <v>2.496</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B149">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C149">
-        <v>2.863</v>
+        <v>2.914</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B150">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C150">
-        <v>2.961</v>
+        <v>3.111</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B151">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C151">
-        <v>2.868</v>
+        <v>3.15</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B152">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C152">
-        <v>2.45</v>
+        <v>3.064</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B153">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C153">
-        <v>1.815</v>
+        <v>2.868</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B154">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C154">
-        <v>1.141</v>
+        <v>2.459</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B155">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C155">
-        <v>0.48</v>
+        <v>1.815</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B156">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C156">
-        <v>0.08699999999999999</v>
+        <v>1.154</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B157">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B158">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45459</v>
+        <v>45461</v>
       </c>
       <c r="B159">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45460</v>
+        <v>45461</v>
       </c>
       <c r="B160">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45460</v>
+        <v>45461</v>
       </c>
       <c r="B161">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B162">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B163">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3184,10 +3184,10 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B164">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -3198,10 +3198,10 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B165">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B166">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C166">
-        <v>0.117</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B167">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C167">
-        <v>0.462</v>
+        <v>0</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B168">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C168">
-        <v>1.133</v>
+        <v>0.151</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B169">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C169">
-        <v>1.806</v>
+        <v>0.489</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="B170">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C170">
-        <v>2.417</v>
+        <v>1.229</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the models for Imperial enhanced with the real-time production
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>12.06.20248</t>
-  </si>
-  <si>
-    <t>12.06.20249</t>
-  </si>
-  <si>
-    <t>12.06.202410</t>
-  </si>
-  <si>
-    <t>12.06.202411</t>
-  </si>
-  <si>
-    <t>12.06.202412</t>
-  </si>
-  <si>
-    <t>12.06.202413</t>
-  </si>
-  <si>
-    <t>12.06.202414</t>
-  </si>
-  <si>
-    <t>12.06.202415</t>
-  </si>
-  <si>
-    <t>12.06.202416</t>
-  </si>
-  <si>
-    <t>12.06.202417</t>
-  </si>
-  <si>
-    <t>12.06.202418</t>
-  </si>
-  <si>
-    <t>12.06.202419</t>
-  </si>
-  <si>
-    <t>12.06.202420</t>
-  </si>
-  <si>
-    <t>12.06.202421</t>
-  </si>
-  <si>
-    <t>12.06.202422</t>
-  </si>
-  <si>
-    <t>12.06.202423</t>
-  </si>
-  <si>
-    <t>13.06.20240</t>
-  </si>
-  <si>
-    <t>13.06.20241</t>
-  </si>
-  <si>
-    <t>13.06.20242</t>
-  </si>
-  <si>
-    <t>13.06.20243</t>
-  </si>
-  <si>
-    <t>13.06.20244</t>
-  </si>
-  <si>
-    <t>13.06.20245</t>
-  </si>
-  <si>
-    <t>13.06.20246</t>
-  </si>
-  <si>
-    <t>13.06.20247</t>
-  </si>
-  <si>
-    <t>13.06.20248</t>
-  </si>
-  <si>
-    <t>13.06.20249</t>
-  </si>
-  <si>
-    <t>13.06.202410</t>
-  </si>
-  <si>
-    <t>13.06.202411</t>
-  </si>
-  <si>
-    <t>13.06.202412</t>
-  </si>
-  <si>
-    <t>13.06.202413</t>
-  </si>
-  <si>
-    <t>13.06.202414</t>
-  </si>
-  <si>
-    <t>13.06.202415</t>
-  </si>
-  <si>
-    <t>13.06.202416</t>
-  </si>
-  <si>
-    <t>13.06.202417</t>
-  </si>
-  <si>
-    <t>13.06.202418</t>
-  </si>
-  <si>
-    <t>13.06.202419</t>
-  </si>
-  <si>
-    <t>13.06.202420</t>
-  </si>
-  <si>
-    <t>13.06.202421</t>
-  </si>
-  <si>
-    <t>13.06.202422</t>
-  </si>
-  <si>
-    <t>13.06.202423</t>
-  </si>
-  <si>
-    <t>14.06.20240</t>
-  </si>
-  <si>
-    <t>14.06.20241</t>
-  </si>
-  <si>
-    <t>14.06.20242</t>
-  </si>
-  <si>
-    <t>14.06.20243</t>
-  </si>
-  <si>
-    <t>14.06.20244</t>
-  </si>
-  <si>
-    <t>14.06.20245</t>
-  </si>
-  <si>
-    <t>14.06.20246</t>
-  </si>
-  <si>
-    <t>14.06.20247</t>
-  </si>
-  <si>
-    <t>14.06.20248</t>
-  </si>
-  <si>
-    <t>14.06.20249</t>
-  </si>
-  <si>
-    <t>14.06.202410</t>
-  </si>
-  <si>
-    <t>14.06.202411</t>
-  </si>
-  <si>
-    <t>14.06.202412</t>
-  </si>
-  <si>
-    <t>14.06.202413</t>
-  </si>
-  <si>
-    <t>14.06.202414</t>
-  </si>
-  <si>
-    <t>14.06.202415</t>
-  </si>
-  <si>
-    <t>14.06.202416</t>
-  </si>
-  <si>
-    <t>14.06.202417</t>
-  </si>
-  <si>
-    <t>14.06.202418</t>
-  </si>
-  <si>
-    <t>14.06.202419</t>
-  </si>
-  <si>
-    <t>14.06.202420</t>
-  </si>
-  <si>
-    <t>14.06.202421</t>
-  </si>
-  <si>
-    <t>14.06.202422</t>
-  </si>
-  <si>
-    <t>14.06.202423</t>
-  </si>
-  <si>
-    <t>15.06.20240</t>
-  </si>
-  <si>
-    <t>15.06.20241</t>
-  </si>
-  <si>
-    <t>15.06.20242</t>
-  </si>
-  <si>
-    <t>15.06.20243</t>
-  </si>
-  <si>
-    <t>15.06.20244</t>
-  </si>
-  <si>
-    <t>15.06.20245</t>
-  </si>
-  <si>
-    <t>15.06.20246</t>
-  </si>
-  <si>
-    <t>15.06.20247</t>
-  </si>
-  <si>
-    <t>15.06.20248</t>
-  </si>
-  <si>
-    <t>15.06.20249</t>
-  </si>
-  <si>
-    <t>15.06.202410</t>
-  </si>
-  <si>
-    <t>15.06.202411</t>
-  </si>
-  <si>
-    <t>15.06.202412</t>
-  </si>
-  <si>
-    <t>15.06.202413</t>
-  </si>
-  <si>
-    <t>15.06.202414</t>
-  </si>
-  <si>
-    <t>15.06.202415</t>
-  </si>
-  <si>
-    <t>15.06.202416</t>
-  </si>
-  <si>
-    <t>15.06.202417</t>
-  </si>
-  <si>
-    <t>15.06.202418</t>
-  </si>
-  <si>
-    <t>15.06.202419</t>
-  </si>
-  <si>
-    <t>15.06.202420</t>
-  </si>
-  <si>
-    <t>15.06.202421</t>
-  </si>
-  <si>
-    <t>15.06.202422</t>
-  </si>
-  <si>
-    <t>15.06.202423</t>
-  </si>
-  <si>
-    <t>16.06.20240</t>
-  </si>
-  <si>
-    <t>16.06.20241</t>
-  </si>
-  <si>
-    <t>16.06.20242</t>
-  </si>
-  <si>
-    <t>16.06.20243</t>
-  </si>
-  <si>
-    <t>16.06.20244</t>
-  </si>
-  <si>
-    <t>16.06.20245</t>
-  </si>
-  <si>
-    <t>16.06.20246</t>
-  </si>
-  <si>
-    <t>16.06.20247</t>
-  </si>
-  <si>
-    <t>16.06.20248</t>
-  </si>
-  <si>
-    <t>16.06.20249</t>
-  </si>
-  <si>
-    <t>16.06.202410</t>
-  </si>
-  <si>
-    <t>16.06.202411</t>
-  </si>
-  <si>
-    <t>16.06.202412</t>
-  </si>
-  <si>
-    <t>16.06.202413</t>
-  </si>
-  <si>
-    <t>16.06.202414</t>
-  </si>
-  <si>
-    <t>16.06.202415</t>
-  </si>
-  <si>
-    <t>16.06.202416</t>
-  </si>
-  <si>
-    <t>16.06.202417</t>
-  </si>
-  <si>
-    <t>16.06.202418</t>
-  </si>
-  <si>
-    <t>16.06.202419</t>
-  </si>
-  <si>
-    <t>16.06.202420</t>
-  </si>
-  <si>
-    <t>16.06.202421</t>
-  </si>
-  <si>
-    <t>16.06.202422</t>
-  </si>
-  <si>
-    <t>16.06.202423</t>
-  </si>
-  <si>
-    <t>17.06.20240</t>
-  </si>
-  <si>
-    <t>17.06.20241</t>
-  </si>
-  <si>
-    <t>17.06.20242</t>
-  </si>
-  <si>
-    <t>17.06.20243</t>
-  </si>
-  <si>
-    <t>17.06.20244</t>
-  </si>
-  <si>
-    <t>17.06.20245</t>
-  </si>
-  <si>
-    <t>17.06.20246</t>
-  </si>
-  <si>
-    <t>17.06.20247</t>
-  </si>
-  <si>
-    <t>17.06.20248</t>
-  </si>
-  <si>
-    <t>17.06.20249</t>
-  </si>
-  <si>
-    <t>17.06.202410</t>
-  </si>
-  <si>
-    <t>17.06.202411</t>
-  </si>
-  <si>
-    <t>17.06.202412</t>
-  </si>
-  <si>
-    <t>17.06.202413</t>
-  </si>
-  <si>
-    <t>17.06.202414</t>
-  </si>
-  <si>
-    <t>17.06.202415</t>
-  </si>
-  <si>
-    <t>17.06.202416</t>
-  </si>
-  <si>
-    <t>17.06.202417</t>
-  </si>
-  <si>
-    <t>17.06.202418</t>
-  </si>
-  <si>
-    <t>17.06.202419</t>
-  </si>
-  <si>
-    <t>17.06.202420</t>
-  </si>
-  <si>
-    <t>17.06.202421</t>
-  </si>
-  <si>
-    <t>17.06.202422</t>
-  </si>
-  <si>
-    <t>17.06.202423</t>
-  </si>
-  <si>
-    <t>18.06.20240</t>
-  </si>
-  <si>
-    <t>18.06.20241</t>
-  </si>
-  <si>
-    <t>18.06.20242</t>
-  </si>
-  <si>
-    <t>18.06.20243</t>
-  </si>
-  <si>
-    <t>18.06.20244</t>
-  </si>
-  <si>
-    <t>18.06.20245</t>
-  </si>
-  <si>
-    <t>18.06.20246</t>
-  </si>
-  <si>
-    <t>18.06.20247</t>
-  </si>
-  <si>
-    <t>18.06.20248</t>
-  </si>
-  <si>
-    <t>18.06.20249</t>
-  </si>
-  <si>
-    <t>18.06.202410</t>
-  </si>
-  <si>
-    <t>18.06.202411</t>
-  </si>
-  <si>
-    <t>18.06.202412</t>
-  </si>
-  <si>
-    <t>18.06.202413</t>
-  </si>
-  <si>
-    <t>18.06.202414</t>
-  </si>
-  <si>
-    <t>18.06.202415</t>
-  </si>
-  <si>
-    <t>18.06.202416</t>
-  </si>
-  <si>
-    <t>18.06.202417</t>
-  </si>
-  <si>
-    <t>18.06.202418</t>
-  </si>
-  <si>
-    <t>18.06.202419</t>
-  </si>
-  <si>
-    <t>18.06.202420</t>
-  </si>
-  <si>
-    <t>18.06.202421</t>
-  </si>
-  <si>
-    <t>18.06.202422</t>
-  </si>
-  <si>
-    <t>18.06.202423</t>
-  </si>
-  <si>
-    <t>19.06.20240</t>
-  </si>
-  <si>
-    <t>19.06.20241</t>
-  </si>
-  <si>
-    <t>19.06.20242</t>
-  </si>
-  <si>
-    <t>19.06.20243</t>
-  </si>
-  <si>
-    <t>19.06.20244</t>
-  </si>
-  <si>
-    <t>19.06.20245</t>
-  </si>
-  <si>
-    <t>19.06.20246</t>
-  </si>
-  <si>
-    <t>19.06.20247</t>
-  </si>
-  <si>
-    <t>19.06.20248</t>
+    <t>19.06.202412</t>
+  </si>
+  <si>
+    <t>19.06.202413</t>
+  </si>
+  <si>
+    <t>19.06.202414</t>
+  </si>
+  <si>
+    <t>19.06.202415</t>
+  </si>
+  <si>
+    <t>19.06.202416</t>
+  </si>
+  <si>
+    <t>19.06.202417</t>
+  </si>
+  <si>
+    <t>19.06.202418</t>
+  </si>
+  <si>
+    <t>19.06.202419</t>
+  </si>
+  <si>
+    <t>19.06.202420</t>
+  </si>
+  <si>
+    <t>19.06.202421</t>
+  </si>
+  <si>
+    <t>19.06.202422</t>
+  </si>
+  <si>
+    <t>19.06.202423</t>
+  </si>
+  <si>
+    <t>20.06.20240</t>
+  </si>
+  <si>
+    <t>20.06.20241</t>
+  </si>
+  <si>
+    <t>20.06.20242</t>
+  </si>
+  <si>
+    <t>20.06.20243</t>
+  </si>
+  <si>
+    <t>20.06.20244</t>
+  </si>
+  <si>
+    <t>20.06.20245</t>
+  </si>
+  <si>
+    <t>20.06.20246</t>
+  </si>
+  <si>
+    <t>20.06.20247</t>
+  </si>
+  <si>
+    <t>20.06.20248</t>
+  </si>
+  <si>
+    <t>20.06.20249</t>
+  </si>
+  <si>
+    <t>20.06.202410</t>
+  </si>
+  <si>
+    <t>20.06.202411</t>
+  </si>
+  <si>
+    <t>20.06.202412</t>
+  </si>
+  <si>
+    <t>20.06.202413</t>
+  </si>
+  <si>
+    <t>20.06.202414</t>
+  </si>
+  <si>
+    <t>20.06.202415</t>
+  </si>
+  <si>
+    <t>20.06.202416</t>
+  </si>
+  <si>
+    <t>20.06.202417</t>
+  </si>
+  <si>
+    <t>20.06.202418</t>
+  </si>
+  <si>
+    <t>20.06.202419</t>
+  </si>
+  <si>
+    <t>20.06.202420</t>
+  </si>
+  <si>
+    <t>20.06.202421</t>
+  </si>
+  <si>
+    <t>20.06.202422</t>
+  </si>
+  <si>
+    <t>20.06.202423</t>
+  </si>
+  <si>
+    <t>21.06.20240</t>
+  </si>
+  <si>
+    <t>21.06.20241</t>
+  </si>
+  <si>
+    <t>21.06.20242</t>
+  </si>
+  <si>
+    <t>21.06.20243</t>
+  </si>
+  <si>
+    <t>21.06.20244</t>
+  </si>
+  <si>
+    <t>21.06.20245</t>
+  </si>
+  <si>
+    <t>21.06.20246</t>
+  </si>
+  <si>
+    <t>21.06.20247</t>
+  </si>
+  <si>
+    <t>21.06.20248</t>
+  </si>
+  <si>
+    <t>21.06.20249</t>
+  </si>
+  <si>
+    <t>21.06.202410</t>
+  </si>
+  <si>
+    <t>21.06.202411</t>
+  </si>
+  <si>
+    <t>21.06.202412</t>
+  </si>
+  <si>
+    <t>21.06.202413</t>
+  </si>
+  <si>
+    <t>21.06.202414</t>
+  </si>
+  <si>
+    <t>21.06.202415</t>
+  </si>
+  <si>
+    <t>21.06.202416</t>
+  </si>
+  <si>
+    <t>21.06.202417</t>
+  </si>
+  <si>
+    <t>21.06.202418</t>
+  </si>
+  <si>
+    <t>21.06.202419</t>
+  </si>
+  <si>
+    <t>21.06.202420</t>
+  </si>
+  <si>
+    <t>21.06.202421</t>
+  </si>
+  <si>
+    <t>21.06.202422</t>
+  </si>
+  <si>
+    <t>21.06.202423</t>
+  </si>
+  <si>
+    <t>22.06.20240</t>
+  </si>
+  <si>
+    <t>22.06.20241</t>
+  </si>
+  <si>
+    <t>22.06.20242</t>
+  </si>
+  <si>
+    <t>22.06.20243</t>
+  </si>
+  <si>
+    <t>22.06.20244</t>
+  </si>
+  <si>
+    <t>22.06.20245</t>
+  </si>
+  <si>
+    <t>22.06.20246</t>
+  </si>
+  <si>
+    <t>22.06.20247</t>
+  </si>
+  <si>
+    <t>22.06.20248</t>
+  </si>
+  <si>
+    <t>22.06.20249</t>
+  </si>
+  <si>
+    <t>22.06.202410</t>
+  </si>
+  <si>
+    <t>22.06.202411</t>
+  </si>
+  <si>
+    <t>22.06.202412</t>
+  </si>
+  <si>
+    <t>22.06.202413</t>
+  </si>
+  <si>
+    <t>22.06.202414</t>
+  </si>
+  <si>
+    <t>22.06.202415</t>
+  </si>
+  <si>
+    <t>22.06.202416</t>
+  </si>
+  <si>
+    <t>22.06.202417</t>
+  </si>
+  <si>
+    <t>22.06.202418</t>
+  </si>
+  <si>
+    <t>22.06.202419</t>
+  </si>
+  <si>
+    <t>22.06.202420</t>
+  </si>
+  <si>
+    <t>22.06.202421</t>
+  </si>
+  <si>
+    <t>22.06.202422</t>
+  </si>
+  <si>
+    <t>22.06.202423</t>
+  </si>
+  <si>
+    <t>23.06.20240</t>
+  </si>
+  <si>
+    <t>23.06.20241</t>
+  </si>
+  <si>
+    <t>23.06.20242</t>
+  </si>
+  <si>
+    <t>23.06.20243</t>
+  </si>
+  <si>
+    <t>23.06.20244</t>
+  </si>
+  <si>
+    <t>23.06.20245</t>
+  </si>
+  <si>
+    <t>23.06.20246</t>
+  </si>
+  <si>
+    <t>23.06.20247</t>
+  </si>
+  <si>
+    <t>23.06.20248</t>
+  </si>
+  <si>
+    <t>23.06.20249</t>
+  </si>
+  <si>
+    <t>23.06.202410</t>
+  </si>
+  <si>
+    <t>23.06.202411</t>
+  </si>
+  <si>
+    <t>23.06.202412</t>
+  </si>
+  <si>
+    <t>23.06.202413</t>
+  </si>
+  <si>
+    <t>23.06.202414</t>
+  </si>
+  <si>
+    <t>23.06.202415</t>
+  </si>
+  <si>
+    <t>23.06.202416</t>
+  </si>
+  <si>
+    <t>23.06.202417</t>
+  </si>
+  <si>
+    <t>23.06.202418</t>
+  </si>
+  <si>
+    <t>23.06.202419</t>
+  </si>
+  <si>
+    <t>23.06.202420</t>
+  </si>
+  <si>
+    <t>23.06.202421</t>
+  </si>
+  <si>
+    <t>23.06.202422</t>
+  </si>
+  <si>
+    <t>23.06.202423</t>
+  </si>
+  <si>
+    <t>24.06.20240</t>
+  </si>
+  <si>
+    <t>24.06.20241</t>
+  </si>
+  <si>
+    <t>24.06.20242</t>
+  </si>
+  <si>
+    <t>24.06.20243</t>
+  </si>
+  <si>
+    <t>24.06.20244</t>
+  </si>
+  <si>
+    <t>24.06.20245</t>
+  </si>
+  <si>
+    <t>24.06.20246</t>
+  </si>
+  <si>
+    <t>24.06.20247</t>
+  </si>
+  <si>
+    <t>24.06.20248</t>
+  </si>
+  <si>
+    <t>24.06.20249</t>
+  </si>
+  <si>
+    <t>24.06.202410</t>
+  </si>
+  <si>
+    <t>24.06.202411</t>
+  </si>
+  <si>
+    <t>24.06.202412</t>
+  </si>
+  <si>
+    <t>24.06.202413</t>
+  </si>
+  <si>
+    <t>24.06.202414</t>
+  </si>
+  <si>
+    <t>24.06.202415</t>
+  </si>
+  <si>
+    <t>24.06.202416</t>
+  </si>
+  <si>
+    <t>24.06.202417</t>
+  </si>
+  <si>
+    <t>24.06.202418</t>
+  </si>
+  <si>
+    <t>24.06.202419</t>
+  </si>
+  <si>
+    <t>24.06.202420</t>
+  </si>
+  <si>
+    <t>24.06.202421</t>
+  </si>
+  <si>
+    <t>24.06.202422</t>
+  </si>
+  <si>
+    <t>24.06.202423</t>
+  </si>
+  <si>
+    <t>25.06.20240</t>
+  </si>
+  <si>
+    <t>25.06.20241</t>
+  </si>
+  <si>
+    <t>25.06.20242</t>
+  </si>
+  <si>
+    <t>25.06.20243</t>
+  </si>
+  <si>
+    <t>25.06.20244</t>
+  </si>
+  <si>
+    <t>25.06.20245</t>
+  </si>
+  <si>
+    <t>25.06.20246</t>
+  </si>
+  <si>
+    <t>25.06.20247</t>
+  </si>
+  <si>
+    <t>25.06.20248</t>
+  </si>
+  <si>
+    <t>25.06.20249</t>
+  </si>
+  <si>
+    <t>25.06.202410</t>
+  </si>
+  <si>
+    <t>25.06.202411</t>
+  </si>
+  <si>
+    <t>25.06.202412</t>
+  </si>
+  <si>
+    <t>25.06.202413</t>
+  </si>
+  <si>
+    <t>25.06.202414</t>
+  </si>
+  <si>
+    <t>25.06.202415</t>
+  </si>
+  <si>
+    <t>25.06.202416</t>
+  </si>
+  <si>
+    <t>25.06.202417</t>
+  </si>
+  <si>
+    <t>25.06.202418</t>
+  </si>
+  <si>
+    <t>25.06.202419</t>
+  </si>
+  <si>
+    <t>25.06.202420</t>
+  </si>
+  <si>
+    <t>25.06.202421</t>
+  </si>
+  <si>
+    <t>25.06.202422</t>
+  </si>
+  <si>
+    <t>25.06.202423</t>
+  </si>
+  <si>
+    <t>26.06.20240</t>
+  </si>
+  <si>
+    <t>26.06.20241</t>
+  </si>
+  <si>
+    <t>26.06.20242</t>
+  </si>
+  <si>
+    <t>26.06.20243</t>
+  </si>
+  <si>
+    <t>26.06.20244</t>
+  </si>
+  <si>
+    <t>26.06.20245</t>
+  </si>
+  <si>
+    <t>26.06.20246</t>
+  </si>
+  <si>
+    <t>26.06.20247</t>
+  </si>
+  <si>
+    <t>26.06.20248</t>
+  </si>
+  <si>
+    <t>26.06.20249</t>
+  </si>
+  <si>
+    <t>26.06.202410</t>
+  </si>
+  <si>
+    <t>26.06.202411</t>
+  </si>
+  <si>
+    <t>26.06.202412</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>2.392</v>
+        <v>3.091</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>2.949</v>
+        <v>2.865</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>3.003</v>
+        <v>2.423</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>2.717</v>
+        <v>1.8</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>2.44</v>
+        <v>1.148</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>1.772</v>
+        <v>0.502</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>1.208</v>
+        <v>0.097</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B11">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>0.776</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B12">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>0.386</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="B13">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>0.168</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45455</v>
+        <v>45463</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>0.046</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45455</v>
+        <v>45463</v>
       </c>
       <c r="B15">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45455</v>
+        <v>45463</v>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45455</v>
+        <v>45463</v>
       </c>
       <c r="B17">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.094</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>0.419</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1.122</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1.806</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>0.081</v>
+        <v>2.418</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>0.335</v>
+        <v>2.825</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>0.57</v>
+        <v>2.953</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>0.912</v>
+        <v>3.15</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>1.257</v>
+        <v>3.041</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>1.771</v>
+        <v>2.862</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>1.816</v>
+        <v>2.456</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B31">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>1.835</v>
+        <v>1.751</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B32">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <v>1.984</v>
+        <v>1.198</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B33">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C33">
-        <v>1.892</v>
+        <v>0.548</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B34">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C34">
-        <v>1.863</v>
+        <v>0.12</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B35">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>1.312</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C36">
-        <v>0.759</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="B37">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C37">
-        <v>0.426</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45456</v>
+        <v>45464</v>
       </c>
       <c r="B38">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>0.077</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45456</v>
+        <v>45464</v>
       </c>
       <c r="B39">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45456</v>
+        <v>45464</v>
       </c>
       <c r="B40">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45456</v>
+        <v>45464</v>
       </c>
       <c r="B41">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.139</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.489</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1.191</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1.94</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C48">
-        <v>0.097</v>
+        <v>2.425</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B49">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C49">
-        <v>0.454</v>
+        <v>2.871</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B50">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>0.729</v>
+        <v>3.055</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B51">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>1.291</v>
+        <v>3.139</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B52">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C52">
-        <v>1.786</v>
+        <v>3.024</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B53">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>2.329</v>
+        <v>2.816</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B54">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>2.683</v>
+        <v>2.426</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B55">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>2.793</v>
+        <v>1.799</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B56">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C56">
-        <v>2.825</v>
+        <v>1.124</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B57">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C57">
-        <v>2.65</v>
+        <v>0.479</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B58">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C58">
-        <v>2.288</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B59">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C59">
-        <v>1.683</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B60">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C60">
-        <v>1.143</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="B61">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C61">
-        <v>0.507</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45457</v>
+        <v>45465</v>
       </c>
       <c r="B62">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C62">
-        <v>0.097</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45457</v>
+        <v>45465</v>
       </c>
       <c r="B63">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45457</v>
+        <v>45465</v>
       </c>
       <c r="B64">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45457</v>
+        <v>45465</v>
       </c>
       <c r="B65">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.094</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>0.419</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B70">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1.085</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B71">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1.793</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B72">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>0.145</v>
+        <v>2.411</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B73">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C73">
-        <v>0.488</v>
+        <v>2.768</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B74">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C74">
-        <v>1.058</v>
+        <v>2.914</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B75">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C75">
-        <v>2.075</v>
+        <v>3.031</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B76">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>2.706</v>
+        <v>3.003</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B77">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>2.957</v>
+        <v>2.813</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B78">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>3.257</v>
+        <v>2.204</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B79">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C79">
-        <v>3.314</v>
+        <v>1.605</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B80">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C80">
-        <v>3.295</v>
+        <v>0.984</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B81">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C81">
-        <v>2.996</v>
+        <v>0.408</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B82">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>2.467</v>
+        <v>0.079</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B83">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C83">
-        <v>1.797</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B84">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C84">
-        <v>1.154</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="B85">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C85">
-        <v>0.535</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45458</v>
+        <v>45466</v>
       </c>
       <c r="B86">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>0.107</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45458</v>
+        <v>45466</v>
       </c>
       <c r="B87">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45458</v>
+        <v>45466</v>
       </c>
       <c r="B88">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45458</v>
+        <v>45466</v>
       </c>
       <c r="B89">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1.083</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B95">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>1.793</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B96">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C96">
-        <v>0.125</v>
+        <v>2.411</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B97">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C97">
-        <v>0.37</v>
+        <v>2.722</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B98">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C98">
-        <v>0.968</v>
+        <v>2.924</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B99">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C99">
-        <v>1.783</v>
+        <v>2.803</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B100">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C100">
-        <v>2.407</v>
+        <v>2.506</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B101">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C101">
-        <v>2.932</v>
+        <v>2.315</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B102">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C102">
-        <v>3.071</v>
+        <v>2.016</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B103">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C103">
-        <v>3.008</v>
+        <v>1.572</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B104">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C104">
-        <v>2.819</v>
+        <v>1.029</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B105">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C105">
-        <v>2.681</v>
+        <v>0.496</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B106">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C106">
-        <v>2.033</v>
+        <v>0.09</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B107">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C107">
-        <v>1.65</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B108">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C108">
-        <v>1.123</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="B109">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C109">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45459</v>
+        <v>45467</v>
       </c>
       <c r="B110">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C110">
-        <v>0.077</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45459</v>
+        <v>45467</v>
       </c>
       <c r="B111">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45459</v>
+        <v>45467</v>
       </c>
       <c r="B112">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45459</v>
+        <v>45467</v>
       </c>
       <c r="B113">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B116">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>0.099</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B117">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>0.366</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B118">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>0.972</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B119">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>1.651</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B120">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C120">
-        <v>0.111</v>
+        <v>2.383</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B121">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C121">
-        <v>0.446</v>
+        <v>2.8</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B122">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C122">
-        <v>1.169</v>
+        <v>2.9</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B123">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C123">
-        <v>1.839</v>
+        <v>2.779</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B124">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C124">
-        <v>2.425</v>
+        <v>2.479</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B125">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C125">
-        <v>2.871</v>
+        <v>2.325</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B126">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C126">
-        <v>3.071</v>
+        <v>2.036</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B127">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C127">
-        <v>3.259</v>
+        <v>1.595</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B128">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C128">
-        <v>3.151</v>
+        <v>0.999</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B129">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C129">
-        <v>2.868</v>
+        <v>0.52</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B130">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C130">
-        <v>2.462</v>
+        <v>0.077</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B131">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C131">
-        <v>1.813</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B132">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C132">
-        <v>1.154</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="B133">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C133">
-        <v>0.512</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45460</v>
+        <v>45468</v>
       </c>
       <c r="B134">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C134">
-        <v>0.107</v>
+        <v>0</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45460</v>
+        <v>45468</v>
       </c>
       <c r="B135">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45460</v>
+        <v>45468</v>
       </c>
       <c r="B136">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45460</v>
+        <v>45468</v>
       </c>
       <c r="B137">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B138">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B140">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>0.103</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B141">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B142">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>0.944</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B143">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>1.578</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B144">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C144">
-        <v>0.14</v>
+        <v>1.953</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B145">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C145">
-        <v>0.487</v>
+        <v>2.36</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B146">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C146">
-        <v>1.225</v>
+        <v>2.56</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B147">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C147">
-        <v>1.954</v>
+        <v>2.626</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B148">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C148">
-        <v>2.496</v>
+        <v>2.479</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B149">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C149">
-        <v>2.914</v>
+        <v>2.296</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B150">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C150">
-        <v>3.111</v>
+        <v>2.016</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B151">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C151">
-        <v>3.15</v>
+        <v>1.625</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B152">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C152">
-        <v>3.064</v>
+        <v>0.998</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B153">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C153">
-        <v>2.868</v>
+        <v>0.526</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B154">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C154">
-        <v>2.459</v>
+        <v>0.079</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B155">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C155">
-        <v>1.815</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B156">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C156">
-        <v>1.154</v>
+        <v>0</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="B157">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C157">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45461</v>
+        <v>45469</v>
       </c>
       <c r="B158">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C158">
-        <v>0.08699999999999999</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45461</v>
+        <v>45469</v>
       </c>
       <c r="B159">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45461</v>
+        <v>45469</v>
       </c>
       <c r="B160">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45461</v>
+        <v>45469</v>
       </c>
       <c r="B161">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B162">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B163">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B164">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>0.092</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B165">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>0.421</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B166">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>0.792</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B167">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>1.512</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B168">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C168">
-        <v>0.151</v>
+        <v>1.783</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B169">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C169">
-        <v>0.489</v>
+        <v>2.185</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="B170">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C170">
-        <v>1.229</v>
+        <v>2.205</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Updating the base model for Astro
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>19.06.202412</t>
-  </si>
-  <si>
-    <t>19.06.202413</t>
-  </si>
-  <si>
-    <t>19.06.202414</t>
-  </si>
-  <si>
-    <t>19.06.202415</t>
-  </si>
-  <si>
-    <t>19.06.202416</t>
-  </si>
-  <si>
-    <t>19.06.202417</t>
-  </si>
-  <si>
-    <t>19.06.202418</t>
-  </si>
-  <si>
-    <t>19.06.202419</t>
-  </si>
-  <si>
-    <t>19.06.202420</t>
-  </si>
-  <si>
-    <t>19.06.202421</t>
-  </si>
-  <si>
-    <t>19.06.202422</t>
-  </si>
-  <si>
-    <t>19.06.202423</t>
-  </si>
-  <si>
-    <t>20.06.20240</t>
-  </si>
-  <si>
-    <t>20.06.20241</t>
-  </si>
-  <si>
-    <t>20.06.20242</t>
-  </si>
-  <si>
-    <t>20.06.20243</t>
-  </si>
-  <si>
-    <t>20.06.20244</t>
-  </si>
-  <si>
-    <t>20.06.20245</t>
-  </si>
-  <si>
-    <t>20.06.20246</t>
-  </si>
-  <si>
-    <t>20.06.20247</t>
-  </si>
-  <si>
-    <t>20.06.20248</t>
-  </si>
-  <si>
-    <t>20.06.20249</t>
-  </si>
-  <si>
-    <t>20.06.202410</t>
-  </si>
-  <si>
-    <t>20.06.202411</t>
-  </si>
-  <si>
-    <t>20.06.202412</t>
-  </si>
-  <si>
-    <t>20.06.202413</t>
-  </si>
-  <si>
-    <t>20.06.202414</t>
-  </si>
-  <si>
-    <t>20.06.202415</t>
-  </si>
-  <si>
-    <t>20.06.202416</t>
-  </si>
-  <si>
-    <t>20.06.202417</t>
-  </si>
-  <si>
-    <t>20.06.202418</t>
-  </si>
-  <si>
-    <t>20.06.202419</t>
-  </si>
-  <si>
-    <t>20.06.202420</t>
-  </si>
-  <si>
-    <t>20.06.202421</t>
-  </si>
-  <si>
-    <t>20.06.202422</t>
-  </si>
-  <si>
-    <t>20.06.202423</t>
-  </si>
-  <si>
-    <t>21.06.20240</t>
-  </si>
-  <si>
-    <t>21.06.20241</t>
-  </si>
-  <si>
-    <t>21.06.20242</t>
-  </si>
-  <si>
-    <t>21.06.20243</t>
-  </si>
-  <si>
-    <t>21.06.20244</t>
-  </si>
-  <si>
-    <t>21.06.20245</t>
-  </si>
-  <si>
-    <t>21.06.20246</t>
-  </si>
-  <si>
-    <t>21.06.20247</t>
-  </si>
-  <si>
-    <t>21.06.20248</t>
-  </si>
-  <si>
-    <t>21.06.20249</t>
-  </si>
-  <si>
-    <t>21.06.202410</t>
-  </si>
-  <si>
-    <t>21.06.202411</t>
-  </si>
-  <si>
-    <t>21.06.202412</t>
-  </si>
-  <si>
-    <t>21.06.202413</t>
-  </si>
-  <si>
-    <t>21.06.202414</t>
-  </si>
-  <si>
-    <t>21.06.202415</t>
-  </si>
-  <si>
-    <t>21.06.202416</t>
-  </si>
-  <si>
-    <t>21.06.202417</t>
-  </si>
-  <si>
-    <t>21.06.202418</t>
-  </si>
-  <si>
-    <t>21.06.202419</t>
-  </si>
-  <si>
-    <t>21.06.202420</t>
-  </si>
-  <si>
-    <t>21.06.202421</t>
-  </si>
-  <si>
-    <t>21.06.202422</t>
-  </si>
-  <si>
-    <t>21.06.202423</t>
-  </si>
-  <si>
-    <t>22.06.20240</t>
-  </si>
-  <si>
-    <t>22.06.20241</t>
-  </si>
-  <si>
-    <t>22.06.20242</t>
-  </si>
-  <si>
-    <t>22.06.20243</t>
-  </si>
-  <si>
-    <t>22.06.20244</t>
-  </si>
-  <si>
-    <t>22.06.20245</t>
-  </si>
-  <si>
-    <t>22.06.20246</t>
-  </si>
-  <si>
-    <t>22.06.20247</t>
-  </si>
-  <si>
-    <t>22.06.20248</t>
-  </si>
-  <si>
-    <t>22.06.20249</t>
-  </si>
-  <si>
-    <t>22.06.202410</t>
-  </si>
-  <si>
-    <t>22.06.202411</t>
-  </si>
-  <si>
-    <t>22.06.202412</t>
-  </si>
-  <si>
-    <t>22.06.202413</t>
-  </si>
-  <si>
-    <t>22.06.202414</t>
-  </si>
-  <si>
-    <t>22.06.202415</t>
-  </si>
-  <si>
-    <t>22.06.202416</t>
-  </si>
-  <si>
-    <t>22.06.202417</t>
-  </si>
-  <si>
-    <t>22.06.202418</t>
-  </si>
-  <si>
-    <t>22.06.202419</t>
-  </si>
-  <si>
-    <t>22.06.202420</t>
-  </si>
-  <si>
-    <t>22.06.202421</t>
-  </si>
-  <si>
-    <t>22.06.202422</t>
-  </si>
-  <si>
-    <t>22.06.202423</t>
-  </si>
-  <si>
-    <t>23.06.20240</t>
-  </si>
-  <si>
-    <t>23.06.20241</t>
-  </si>
-  <si>
-    <t>23.06.20242</t>
-  </si>
-  <si>
-    <t>23.06.20243</t>
-  </si>
-  <si>
-    <t>23.06.20244</t>
-  </si>
-  <si>
-    <t>23.06.20245</t>
-  </si>
-  <si>
-    <t>23.06.20246</t>
-  </si>
-  <si>
-    <t>23.06.20247</t>
-  </si>
-  <si>
-    <t>23.06.20248</t>
-  </si>
-  <si>
-    <t>23.06.20249</t>
-  </si>
-  <si>
-    <t>23.06.202410</t>
-  </si>
-  <si>
-    <t>23.06.202411</t>
-  </si>
-  <si>
-    <t>23.06.202412</t>
-  </si>
-  <si>
-    <t>23.06.202413</t>
-  </si>
-  <si>
-    <t>23.06.202414</t>
-  </si>
-  <si>
-    <t>23.06.202415</t>
-  </si>
-  <si>
-    <t>23.06.202416</t>
-  </si>
-  <si>
-    <t>23.06.202417</t>
-  </si>
-  <si>
-    <t>23.06.202418</t>
-  </si>
-  <si>
-    <t>23.06.202419</t>
-  </si>
-  <si>
-    <t>23.06.202420</t>
-  </si>
-  <si>
-    <t>23.06.202421</t>
-  </si>
-  <si>
-    <t>23.06.202422</t>
-  </si>
-  <si>
-    <t>23.06.202423</t>
-  </si>
-  <si>
-    <t>24.06.20240</t>
-  </si>
-  <si>
-    <t>24.06.20241</t>
-  </si>
-  <si>
-    <t>24.06.20242</t>
-  </si>
-  <si>
-    <t>24.06.20243</t>
-  </si>
-  <si>
-    <t>24.06.20244</t>
-  </si>
-  <si>
-    <t>24.06.20245</t>
-  </si>
-  <si>
-    <t>24.06.20246</t>
-  </si>
-  <si>
-    <t>24.06.20247</t>
-  </si>
-  <si>
-    <t>24.06.20248</t>
-  </si>
-  <si>
-    <t>24.06.20249</t>
-  </si>
-  <si>
-    <t>24.06.202410</t>
-  </si>
-  <si>
-    <t>24.06.202411</t>
-  </si>
-  <si>
-    <t>24.06.202412</t>
-  </si>
-  <si>
-    <t>24.06.202413</t>
-  </si>
-  <si>
-    <t>24.06.202414</t>
-  </si>
-  <si>
-    <t>24.06.202415</t>
-  </si>
-  <si>
-    <t>24.06.202416</t>
-  </si>
-  <si>
-    <t>24.06.202417</t>
-  </si>
-  <si>
-    <t>24.06.202418</t>
-  </si>
-  <si>
-    <t>24.06.202419</t>
-  </si>
-  <si>
-    <t>24.06.202420</t>
-  </si>
-  <si>
-    <t>24.06.202421</t>
-  </si>
-  <si>
-    <t>24.06.202422</t>
-  </si>
-  <si>
-    <t>24.06.202423</t>
-  </si>
-  <si>
-    <t>25.06.20240</t>
-  </si>
-  <si>
-    <t>25.06.20241</t>
-  </si>
-  <si>
-    <t>25.06.20242</t>
-  </si>
-  <si>
-    <t>25.06.20243</t>
-  </si>
-  <si>
-    <t>25.06.20244</t>
-  </si>
-  <si>
-    <t>25.06.20245</t>
-  </si>
-  <si>
-    <t>25.06.20246</t>
-  </si>
-  <si>
-    <t>25.06.20247</t>
-  </si>
-  <si>
-    <t>25.06.20248</t>
-  </si>
-  <si>
-    <t>25.06.20249</t>
-  </si>
-  <si>
-    <t>25.06.202410</t>
-  </si>
-  <si>
-    <t>25.06.202411</t>
-  </si>
-  <si>
-    <t>25.06.202412</t>
-  </si>
-  <si>
-    <t>25.06.202413</t>
-  </si>
-  <si>
-    <t>25.06.202414</t>
-  </si>
-  <si>
-    <t>25.06.202415</t>
-  </si>
-  <si>
-    <t>25.06.202416</t>
-  </si>
-  <si>
-    <t>25.06.202417</t>
-  </si>
-  <si>
-    <t>25.06.202418</t>
-  </si>
-  <si>
-    <t>25.06.202419</t>
-  </si>
-  <si>
-    <t>25.06.202420</t>
-  </si>
-  <si>
-    <t>25.06.202421</t>
-  </si>
-  <si>
-    <t>25.06.202422</t>
-  </si>
-  <si>
-    <t>25.06.202423</t>
-  </si>
-  <si>
-    <t>26.06.20240</t>
-  </si>
-  <si>
-    <t>26.06.20241</t>
-  </si>
-  <si>
-    <t>26.06.20242</t>
-  </si>
-  <si>
-    <t>26.06.20243</t>
-  </si>
-  <si>
-    <t>26.06.20244</t>
-  </si>
-  <si>
-    <t>26.06.20245</t>
-  </si>
-  <si>
-    <t>26.06.20246</t>
-  </si>
-  <si>
-    <t>26.06.20247</t>
-  </si>
-  <si>
-    <t>26.06.20248</t>
-  </si>
-  <si>
-    <t>26.06.20249</t>
-  </si>
-  <si>
-    <t>26.06.202410</t>
-  </si>
-  <si>
-    <t>26.06.202411</t>
-  </si>
-  <si>
-    <t>26.06.202412</t>
+    <t>01.07.20249</t>
+  </si>
+  <si>
+    <t>01.07.202410</t>
+  </si>
+  <si>
+    <t>01.07.202411</t>
+  </si>
+  <si>
+    <t>01.07.202412</t>
+  </si>
+  <si>
+    <t>01.07.202413</t>
+  </si>
+  <si>
+    <t>01.07.202414</t>
+  </si>
+  <si>
+    <t>01.07.202415</t>
+  </si>
+  <si>
+    <t>01.07.202416</t>
+  </si>
+  <si>
+    <t>01.07.202417</t>
+  </si>
+  <si>
+    <t>01.07.202418</t>
+  </si>
+  <si>
+    <t>01.07.202419</t>
+  </si>
+  <si>
+    <t>01.07.202420</t>
+  </si>
+  <si>
+    <t>01.07.202421</t>
+  </si>
+  <si>
+    <t>01.07.202422</t>
+  </si>
+  <si>
+    <t>01.07.202423</t>
+  </si>
+  <si>
+    <t>02.07.20240</t>
+  </si>
+  <si>
+    <t>02.07.20241</t>
+  </si>
+  <si>
+    <t>02.07.20242</t>
+  </si>
+  <si>
+    <t>02.07.20243</t>
+  </si>
+  <si>
+    <t>02.07.20244</t>
+  </si>
+  <si>
+    <t>02.07.20245</t>
+  </si>
+  <si>
+    <t>02.07.20246</t>
+  </si>
+  <si>
+    <t>02.07.20247</t>
+  </si>
+  <si>
+    <t>02.07.20248</t>
+  </si>
+  <si>
+    <t>02.07.20249</t>
+  </si>
+  <si>
+    <t>02.07.202410</t>
+  </si>
+  <si>
+    <t>02.07.202411</t>
+  </si>
+  <si>
+    <t>02.07.202412</t>
+  </si>
+  <si>
+    <t>02.07.202413</t>
+  </si>
+  <si>
+    <t>02.07.202414</t>
+  </si>
+  <si>
+    <t>02.07.202415</t>
+  </si>
+  <si>
+    <t>02.07.202416</t>
+  </si>
+  <si>
+    <t>02.07.202417</t>
+  </si>
+  <si>
+    <t>02.07.202418</t>
+  </si>
+  <si>
+    <t>02.07.202419</t>
+  </si>
+  <si>
+    <t>02.07.202420</t>
+  </si>
+  <si>
+    <t>02.07.202421</t>
+  </si>
+  <si>
+    <t>02.07.202422</t>
+  </si>
+  <si>
+    <t>02.07.202423</t>
+  </si>
+  <si>
+    <t>03.07.20240</t>
+  </si>
+  <si>
+    <t>03.07.20241</t>
+  </si>
+  <si>
+    <t>03.07.20242</t>
+  </si>
+  <si>
+    <t>03.07.20243</t>
+  </si>
+  <si>
+    <t>03.07.20244</t>
+  </si>
+  <si>
+    <t>03.07.20245</t>
+  </si>
+  <si>
+    <t>03.07.20246</t>
+  </si>
+  <si>
+    <t>03.07.20247</t>
+  </si>
+  <si>
+    <t>03.07.20248</t>
+  </si>
+  <si>
+    <t>03.07.20249</t>
+  </si>
+  <si>
+    <t>03.07.202410</t>
+  </si>
+  <si>
+    <t>03.07.202411</t>
+  </si>
+  <si>
+    <t>03.07.202412</t>
+  </si>
+  <si>
+    <t>03.07.202413</t>
+  </si>
+  <si>
+    <t>03.07.202414</t>
+  </si>
+  <si>
+    <t>03.07.202415</t>
+  </si>
+  <si>
+    <t>03.07.202416</t>
+  </si>
+  <si>
+    <t>03.07.202417</t>
+  </si>
+  <si>
+    <t>03.07.202418</t>
+  </si>
+  <si>
+    <t>03.07.202419</t>
+  </si>
+  <si>
+    <t>03.07.202420</t>
+  </si>
+  <si>
+    <t>03.07.202421</t>
+  </si>
+  <si>
+    <t>03.07.202422</t>
+  </si>
+  <si>
+    <t>03.07.202423</t>
+  </si>
+  <si>
+    <t>04.07.20240</t>
+  </si>
+  <si>
+    <t>04.07.20241</t>
+  </si>
+  <si>
+    <t>04.07.20242</t>
+  </si>
+  <si>
+    <t>04.07.20243</t>
+  </si>
+  <si>
+    <t>04.07.20244</t>
+  </si>
+  <si>
+    <t>04.07.20245</t>
+  </si>
+  <si>
+    <t>04.07.20246</t>
+  </si>
+  <si>
+    <t>04.07.20247</t>
+  </si>
+  <si>
+    <t>04.07.20248</t>
+  </si>
+  <si>
+    <t>04.07.20249</t>
+  </si>
+  <si>
+    <t>04.07.202410</t>
+  </si>
+  <si>
+    <t>04.07.202411</t>
+  </si>
+  <si>
+    <t>04.07.202412</t>
+  </si>
+  <si>
+    <t>04.07.202413</t>
+  </si>
+  <si>
+    <t>04.07.202414</t>
+  </si>
+  <si>
+    <t>04.07.202415</t>
+  </si>
+  <si>
+    <t>04.07.202416</t>
+  </si>
+  <si>
+    <t>04.07.202417</t>
+  </si>
+  <si>
+    <t>04.07.202418</t>
+  </si>
+  <si>
+    <t>04.07.202419</t>
+  </si>
+  <si>
+    <t>04.07.202420</t>
+  </si>
+  <si>
+    <t>04.07.202421</t>
+  </si>
+  <si>
+    <t>04.07.202422</t>
+  </si>
+  <si>
+    <t>04.07.202423</t>
+  </si>
+  <si>
+    <t>05.07.20240</t>
+  </si>
+  <si>
+    <t>05.07.20241</t>
+  </si>
+  <si>
+    <t>05.07.20242</t>
+  </si>
+  <si>
+    <t>05.07.20243</t>
+  </si>
+  <si>
+    <t>05.07.20244</t>
+  </si>
+  <si>
+    <t>05.07.20245</t>
+  </si>
+  <si>
+    <t>05.07.20246</t>
+  </si>
+  <si>
+    <t>05.07.20247</t>
+  </si>
+  <si>
+    <t>05.07.20248</t>
+  </si>
+  <si>
+    <t>05.07.20249</t>
+  </si>
+  <si>
+    <t>05.07.202410</t>
+  </si>
+  <si>
+    <t>05.07.202411</t>
+  </si>
+  <si>
+    <t>05.07.202412</t>
+  </si>
+  <si>
+    <t>05.07.202413</t>
+  </si>
+  <si>
+    <t>05.07.202414</t>
+  </si>
+  <si>
+    <t>05.07.202415</t>
+  </si>
+  <si>
+    <t>05.07.202416</t>
+  </si>
+  <si>
+    <t>05.07.202417</t>
+  </si>
+  <si>
+    <t>05.07.202418</t>
+  </si>
+  <si>
+    <t>05.07.202419</t>
+  </si>
+  <si>
+    <t>05.07.202420</t>
+  </si>
+  <si>
+    <t>05.07.202421</t>
+  </si>
+  <si>
+    <t>05.07.202422</t>
+  </si>
+  <si>
+    <t>05.07.202423</t>
+  </si>
+  <si>
+    <t>06.07.20240</t>
+  </si>
+  <si>
+    <t>06.07.20241</t>
+  </si>
+  <si>
+    <t>06.07.20242</t>
+  </si>
+  <si>
+    <t>06.07.20243</t>
+  </si>
+  <si>
+    <t>06.07.20244</t>
+  </si>
+  <si>
+    <t>06.07.20245</t>
+  </si>
+  <si>
+    <t>06.07.20246</t>
+  </si>
+  <si>
+    <t>06.07.20247</t>
+  </si>
+  <si>
+    <t>06.07.20248</t>
+  </si>
+  <si>
+    <t>06.07.20249</t>
+  </si>
+  <si>
+    <t>06.07.202410</t>
+  </si>
+  <si>
+    <t>06.07.202411</t>
+  </si>
+  <si>
+    <t>06.07.202412</t>
+  </si>
+  <si>
+    <t>06.07.202413</t>
+  </si>
+  <si>
+    <t>06.07.202414</t>
+  </si>
+  <si>
+    <t>06.07.202415</t>
+  </si>
+  <si>
+    <t>06.07.202416</t>
+  </si>
+  <si>
+    <t>06.07.202417</t>
+  </si>
+  <si>
+    <t>06.07.202418</t>
+  </si>
+  <si>
+    <t>06.07.202419</t>
+  </si>
+  <si>
+    <t>06.07.202420</t>
+  </si>
+  <si>
+    <t>06.07.202421</t>
+  </si>
+  <si>
+    <t>06.07.202422</t>
+  </si>
+  <si>
+    <t>06.07.202423</t>
+  </si>
+  <si>
+    <t>07.07.20240</t>
+  </si>
+  <si>
+    <t>07.07.20241</t>
+  </si>
+  <si>
+    <t>07.07.20242</t>
+  </si>
+  <si>
+    <t>07.07.20243</t>
+  </si>
+  <si>
+    <t>07.07.20244</t>
+  </si>
+  <si>
+    <t>07.07.20245</t>
+  </si>
+  <si>
+    <t>07.07.20246</t>
+  </si>
+  <si>
+    <t>07.07.20247</t>
+  </si>
+  <si>
+    <t>07.07.20248</t>
+  </si>
+  <si>
+    <t>07.07.20249</t>
+  </si>
+  <si>
+    <t>07.07.202410</t>
+  </si>
+  <si>
+    <t>07.07.202411</t>
+  </si>
+  <si>
+    <t>07.07.202412</t>
+  </si>
+  <si>
+    <t>07.07.202413</t>
+  </si>
+  <si>
+    <t>07.07.202414</t>
+  </si>
+  <si>
+    <t>07.07.202415</t>
+  </si>
+  <si>
+    <t>07.07.202416</t>
+  </si>
+  <si>
+    <t>07.07.202417</t>
+  </si>
+  <si>
+    <t>07.07.202418</t>
+  </si>
+  <si>
+    <t>07.07.202419</t>
+  </si>
+  <si>
+    <t>07.07.202420</t>
+  </si>
+  <si>
+    <t>07.07.202421</t>
+  </si>
+  <si>
+    <t>07.07.202422</t>
+  </si>
+  <si>
+    <t>07.07.202423</t>
+  </si>
+  <si>
+    <t>08.07.20240</t>
+  </si>
+  <si>
+    <t>08.07.20241</t>
+  </si>
+  <si>
+    <t>08.07.20242</t>
+  </si>
+  <si>
+    <t>08.07.20243</t>
+  </si>
+  <si>
+    <t>08.07.20244</t>
+  </si>
+  <si>
+    <t>08.07.20245</t>
+  </si>
+  <si>
+    <t>08.07.20246</t>
+  </si>
+  <si>
+    <t>08.07.20247</t>
+  </si>
+  <si>
+    <t>08.07.20248</t>
+  </si>
+  <si>
+    <t>08.07.20249</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>3.091</v>
+        <v>2.768</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>2.865</v>
+        <v>2.914</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>2.423</v>
+        <v>2.939</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>1.8</v>
+        <v>2.137</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>1.148</v>
+        <v>1.923</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>0.502</v>
+        <v>1.777</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>0.097</v>
+        <v>1.597</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.028</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.492</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45462</v>
+        <v>45474</v>
       </c>
       <c r="B13">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45463</v>
+        <v>45474</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45463</v>
+        <v>45474</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45463</v>
+        <v>45474</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>0.094</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>0.419</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>1.122</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>1.806</v>
+        <v>0.061</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>2.418</v>
+        <v>0.183</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B25">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>2.825</v>
+        <v>0.362</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>2.953</v>
+        <v>0.758</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>3.15</v>
+        <v>0.962</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B28">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C28">
-        <v>3.041</v>
+        <v>1.292</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B29">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C29">
-        <v>2.862</v>
+        <v>1.724</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>2.456</v>
+        <v>1.687</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C31">
-        <v>1.751</v>
+        <v>1.536</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B32">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C32">
-        <v>1.198</v>
+        <v>1.227</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B33">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C33">
-        <v>0.548</v>
+        <v>0.899</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C34">
-        <v>0.12</v>
+        <v>0.636</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B35">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.307</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B36">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.157</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="B37">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.051</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45464</v>
+        <v>45475</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45464</v>
+        <v>45475</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45464</v>
+        <v>45475</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>0.139</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C45">
-        <v>0.489</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C46">
-        <v>1.191</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C47">
-        <v>1.94</v>
+        <v>0.061</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C48">
-        <v>2.425</v>
+        <v>0.174</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B49">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C49">
-        <v>2.871</v>
+        <v>0.286</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C50">
-        <v>3.055</v>
+        <v>0.439</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C51">
-        <v>3.139</v>
+        <v>0.514</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C52">
-        <v>3.024</v>
+        <v>0.771</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C53">
-        <v>2.816</v>
+        <v>0.784</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B54">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C54">
-        <v>2.426</v>
+        <v>1.067</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C55">
-        <v>1.799</v>
+        <v>0.975</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B56">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C56">
-        <v>1.124</v>
+        <v>0.861</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B57">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C57">
-        <v>0.479</v>
+        <v>0.783</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C58">
-        <v>0.08699999999999999</v>
+        <v>0.626</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.459</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.241</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45464</v>
+        <v>45476</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.175</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45465</v>
+        <v>45476</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45465</v>
+        <v>45476</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45465</v>
+        <v>45476</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>0.094</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C69">
-        <v>0.419</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C70">
-        <v>1.085</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B71">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C71">
-        <v>1.793</v>
+        <v>0.08</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C72">
-        <v>2.411</v>
+        <v>0.329</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C73">
-        <v>2.768</v>
+        <v>0.585</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C74">
-        <v>2.914</v>
+        <v>0.995</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C75">
-        <v>3.031</v>
+        <v>1.34</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C76">
-        <v>3.003</v>
+        <v>1.717</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C77">
-        <v>2.813</v>
+        <v>1.973</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B78">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C78">
-        <v>2.204</v>
+        <v>1.937</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C79">
-        <v>1.605</v>
+        <v>1.927</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C80">
-        <v>0.984</v>
+        <v>1.969</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B81">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C81">
-        <v>0.408</v>
+        <v>1.748</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C82">
-        <v>0.079</v>
+        <v>1.62</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B83">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1.034</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B84">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.469</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45465</v>
+        <v>45477</v>
       </c>
       <c r="B85">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.097</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45466</v>
+        <v>45477</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45466</v>
+        <v>45477</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45466</v>
+        <v>45477</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C92">
-        <v>0.08799999999999999</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B93">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C93">
-        <v>0.369</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B94">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C94">
-        <v>1.083</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B95">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C95">
-        <v>1.793</v>
+        <v>0.114</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C96">
-        <v>2.411</v>
+        <v>0.444</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B97">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C97">
-        <v>2.722</v>
+        <v>1.163</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B98">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C98">
-        <v>2.924</v>
+        <v>1.839</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B99">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C99">
-        <v>2.803</v>
+        <v>2.425</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B100">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C100">
-        <v>2.506</v>
+        <v>2.914</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B101">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C101">
-        <v>2.315</v>
+        <v>3.122</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B102">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C102">
-        <v>2.016</v>
+        <v>3.314</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B103">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C103">
-        <v>1.572</v>
+        <v>3.155</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B104">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C104">
-        <v>1.029</v>
+        <v>2.926</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B105">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C105">
-        <v>0.496</v>
+        <v>2.467</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B106">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C106">
-        <v>0.09</v>
+        <v>1.797</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B107">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>1.192</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B108">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.542</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45466</v>
+        <v>45478</v>
       </c>
       <c r="B109">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.114</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B114">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B115">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B116">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B117">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C117">
-        <v>0.366</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B118">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C118">
-        <v>0.972</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B119">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C119">
-        <v>1.651</v>
+        <v>0.106</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B120">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C120">
-        <v>2.383</v>
+        <v>0.446</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B121">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C121">
-        <v>2.8</v>
+        <v>1.127</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B122">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C122">
-        <v>2.9</v>
+        <v>1.812</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B123">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C123">
-        <v>2.779</v>
+        <v>2.425</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B124">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C124">
-        <v>2.479</v>
+        <v>2.871</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B125">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C125">
-        <v>2.325</v>
+        <v>3.111</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B126">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C126">
-        <v>2.036</v>
+        <v>3.169</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B127">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C127">
-        <v>1.595</v>
+        <v>3.042</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B128">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C128">
-        <v>0.999</v>
+        <v>2.862</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B129">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C129">
-        <v>0.52</v>
+        <v>2.455</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B130">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C130">
-        <v>0.077</v>
+        <v>1.815</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B131">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1.151</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B132">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.533</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45467</v>
+        <v>45479</v>
       </c>
       <c r="B133">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>0.107</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45468</v>
+        <v>45479</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45468</v>
+        <v>45479</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45468</v>
+        <v>45479</v>
       </c>
       <c r="B136">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B137">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B138">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B139">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B140">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C140">
-        <v>0.103</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B141">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C141">
-        <v>0.369</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B142">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C142">
-        <v>0.944</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B143">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C143">
-        <v>1.578</v>
+        <v>0.099</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B144">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C144">
-        <v>1.953</v>
+        <v>0.435</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B145">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C145">
-        <v>2.36</v>
+        <v>1.089</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B146">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C146">
-        <v>2.56</v>
+        <v>1.793</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B147">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C147">
-        <v>2.626</v>
+        <v>2.422</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B148">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C148">
-        <v>2.479</v>
+        <v>2.8</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B149">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C149">
-        <v>2.296</v>
+        <v>2.969</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B150">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C150">
-        <v>2.016</v>
+        <v>3.087</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B151">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C151">
-        <v>1.625</v>
+        <v>2.984</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B152">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C152">
-        <v>0.998</v>
+        <v>2.813</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B153">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C153">
-        <v>0.526</v>
+        <v>2.409</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B154">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C154">
-        <v>0.079</v>
+        <v>1.778</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B155">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>1.13</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B156">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>0.485</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45468</v>
+        <v>45480</v>
       </c>
       <c r="B157">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45469</v>
+        <v>45480</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45469</v>
+        <v>45480</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45469</v>
+        <v>45480</v>
       </c>
       <c r="B160">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B161">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B162">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B163">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B164">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C164">
-        <v>0.092</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B165">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C165">
-        <v>0.421</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B166">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C166">
-        <v>0.792</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B167">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C167">
-        <v>1.512</v>
+        <v>0.094</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B168">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C168">
-        <v>1.783</v>
+        <v>0.443</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B169">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C169">
-        <v>2.185</v>
+        <v>1.109</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45469</v>
+        <v>45481</v>
       </c>
       <c r="B170">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C170">
-        <v>2.205</v>
+        <v>1.801</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Updating the default model for Imperial up to June 2024
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>01.07.20249</t>
-  </si>
-  <si>
-    <t>01.07.202410</t>
-  </si>
-  <si>
-    <t>01.07.202411</t>
-  </si>
-  <si>
-    <t>01.07.202412</t>
-  </si>
-  <si>
-    <t>01.07.202413</t>
-  </si>
-  <si>
-    <t>01.07.202414</t>
-  </si>
-  <si>
-    <t>01.07.202415</t>
-  </si>
-  <si>
-    <t>01.07.202416</t>
-  </si>
-  <si>
-    <t>01.07.202417</t>
-  </si>
-  <si>
-    <t>01.07.202418</t>
-  </si>
-  <si>
-    <t>01.07.202419</t>
-  </si>
-  <si>
-    <t>01.07.202420</t>
-  </si>
-  <si>
-    <t>01.07.202421</t>
-  </si>
-  <si>
-    <t>01.07.202422</t>
-  </si>
-  <si>
-    <t>01.07.202423</t>
-  </si>
-  <si>
-    <t>02.07.20240</t>
-  </si>
-  <si>
-    <t>02.07.20241</t>
-  </si>
-  <si>
-    <t>02.07.20242</t>
-  </si>
-  <si>
-    <t>02.07.20243</t>
-  </si>
-  <si>
-    <t>02.07.20244</t>
-  </si>
-  <si>
-    <t>02.07.20245</t>
-  </si>
-  <si>
-    <t>02.07.20246</t>
-  </si>
-  <si>
-    <t>02.07.20247</t>
-  </si>
-  <si>
-    <t>02.07.20248</t>
-  </si>
-  <si>
-    <t>02.07.20249</t>
-  </si>
-  <si>
-    <t>02.07.202410</t>
-  </si>
-  <si>
-    <t>02.07.202411</t>
-  </si>
-  <si>
-    <t>02.07.202412</t>
-  </si>
-  <si>
-    <t>02.07.202413</t>
-  </si>
-  <si>
-    <t>02.07.202414</t>
-  </si>
-  <si>
-    <t>02.07.202415</t>
-  </si>
-  <si>
-    <t>02.07.202416</t>
-  </si>
-  <si>
-    <t>02.07.202417</t>
-  </si>
-  <si>
-    <t>02.07.202418</t>
-  </si>
-  <si>
-    <t>02.07.202419</t>
-  </si>
-  <si>
-    <t>02.07.202420</t>
-  </si>
-  <si>
-    <t>02.07.202421</t>
-  </si>
-  <si>
-    <t>02.07.202422</t>
-  </si>
-  <si>
-    <t>02.07.202423</t>
-  </si>
-  <si>
-    <t>03.07.20240</t>
-  </si>
-  <si>
-    <t>03.07.20241</t>
-  </si>
-  <si>
-    <t>03.07.20242</t>
-  </si>
-  <si>
-    <t>03.07.20243</t>
-  </si>
-  <si>
-    <t>03.07.20244</t>
-  </si>
-  <si>
-    <t>03.07.20245</t>
-  </si>
-  <si>
-    <t>03.07.20246</t>
-  </si>
-  <si>
-    <t>03.07.20247</t>
-  </si>
-  <si>
-    <t>03.07.20248</t>
-  </si>
-  <si>
-    <t>03.07.20249</t>
-  </si>
-  <si>
-    <t>03.07.202410</t>
-  </si>
-  <si>
-    <t>03.07.202411</t>
-  </si>
-  <si>
-    <t>03.07.202412</t>
-  </si>
-  <si>
-    <t>03.07.202413</t>
-  </si>
-  <si>
-    <t>03.07.202414</t>
-  </si>
-  <si>
-    <t>03.07.202415</t>
-  </si>
-  <si>
-    <t>03.07.202416</t>
-  </si>
-  <si>
-    <t>03.07.202417</t>
-  </si>
-  <si>
-    <t>03.07.202418</t>
-  </si>
-  <si>
-    <t>03.07.202419</t>
-  </si>
-  <si>
-    <t>03.07.202420</t>
-  </si>
-  <si>
-    <t>03.07.202421</t>
-  </si>
-  <si>
-    <t>03.07.202422</t>
-  </si>
-  <si>
-    <t>03.07.202423</t>
-  </si>
-  <si>
-    <t>04.07.20240</t>
-  </si>
-  <si>
-    <t>04.07.20241</t>
-  </si>
-  <si>
-    <t>04.07.20242</t>
-  </si>
-  <si>
-    <t>04.07.20243</t>
-  </si>
-  <si>
-    <t>04.07.20244</t>
-  </si>
-  <si>
-    <t>04.07.20245</t>
-  </si>
-  <si>
-    <t>04.07.20246</t>
-  </si>
-  <si>
-    <t>04.07.20247</t>
-  </si>
-  <si>
-    <t>04.07.20248</t>
-  </si>
-  <si>
-    <t>04.07.20249</t>
-  </si>
-  <si>
-    <t>04.07.202410</t>
-  </si>
-  <si>
-    <t>04.07.202411</t>
-  </si>
-  <si>
-    <t>04.07.202412</t>
-  </si>
-  <si>
-    <t>04.07.202413</t>
-  </si>
-  <si>
-    <t>04.07.202414</t>
-  </si>
-  <si>
-    <t>04.07.202415</t>
-  </si>
-  <si>
-    <t>04.07.202416</t>
-  </si>
-  <si>
-    <t>04.07.202417</t>
-  </si>
-  <si>
-    <t>04.07.202418</t>
-  </si>
-  <si>
-    <t>04.07.202419</t>
-  </si>
-  <si>
-    <t>04.07.202420</t>
-  </si>
-  <si>
-    <t>04.07.202421</t>
-  </si>
-  <si>
-    <t>04.07.202422</t>
-  </si>
-  <si>
-    <t>04.07.202423</t>
-  </si>
-  <si>
-    <t>05.07.20240</t>
-  </si>
-  <si>
-    <t>05.07.20241</t>
-  </si>
-  <si>
-    <t>05.07.20242</t>
-  </si>
-  <si>
-    <t>05.07.20243</t>
-  </si>
-  <si>
-    <t>05.07.20244</t>
-  </si>
-  <si>
-    <t>05.07.20245</t>
-  </si>
-  <si>
-    <t>05.07.20246</t>
-  </si>
-  <si>
-    <t>05.07.20247</t>
-  </si>
-  <si>
-    <t>05.07.20248</t>
-  </si>
-  <si>
-    <t>05.07.20249</t>
-  </si>
-  <si>
-    <t>05.07.202410</t>
-  </si>
-  <si>
-    <t>05.07.202411</t>
-  </si>
-  <si>
-    <t>05.07.202412</t>
-  </si>
-  <si>
-    <t>05.07.202413</t>
-  </si>
-  <si>
-    <t>05.07.202414</t>
-  </si>
-  <si>
-    <t>05.07.202415</t>
-  </si>
-  <si>
-    <t>05.07.202416</t>
-  </si>
-  <si>
-    <t>05.07.202417</t>
-  </si>
-  <si>
-    <t>05.07.202418</t>
-  </si>
-  <si>
-    <t>05.07.202419</t>
-  </si>
-  <si>
-    <t>05.07.202420</t>
-  </si>
-  <si>
-    <t>05.07.202421</t>
-  </si>
-  <si>
-    <t>05.07.202422</t>
-  </si>
-  <si>
-    <t>05.07.202423</t>
-  </si>
-  <si>
-    <t>06.07.20240</t>
-  </si>
-  <si>
-    <t>06.07.20241</t>
-  </si>
-  <si>
-    <t>06.07.20242</t>
-  </si>
-  <si>
-    <t>06.07.20243</t>
-  </si>
-  <si>
-    <t>06.07.20244</t>
-  </si>
-  <si>
-    <t>06.07.20245</t>
-  </si>
-  <si>
-    <t>06.07.20246</t>
-  </si>
-  <si>
-    <t>06.07.20247</t>
-  </si>
-  <si>
-    <t>06.07.20248</t>
-  </si>
-  <si>
-    <t>06.07.20249</t>
-  </si>
-  <si>
-    <t>06.07.202410</t>
-  </si>
-  <si>
-    <t>06.07.202411</t>
-  </si>
-  <si>
-    <t>06.07.202412</t>
-  </si>
-  <si>
-    <t>06.07.202413</t>
-  </si>
-  <si>
-    <t>06.07.202414</t>
-  </si>
-  <si>
-    <t>06.07.202415</t>
-  </si>
-  <si>
-    <t>06.07.202416</t>
-  </si>
-  <si>
-    <t>06.07.202417</t>
-  </si>
-  <si>
-    <t>06.07.202418</t>
-  </si>
-  <si>
-    <t>06.07.202419</t>
-  </si>
-  <si>
-    <t>06.07.202420</t>
-  </si>
-  <si>
-    <t>06.07.202421</t>
-  </si>
-  <si>
-    <t>06.07.202422</t>
-  </si>
-  <si>
-    <t>06.07.202423</t>
-  </si>
-  <si>
-    <t>07.07.20240</t>
-  </si>
-  <si>
-    <t>07.07.20241</t>
-  </si>
-  <si>
-    <t>07.07.20242</t>
-  </si>
-  <si>
-    <t>07.07.20243</t>
-  </si>
-  <si>
-    <t>07.07.20244</t>
-  </si>
-  <si>
-    <t>07.07.20245</t>
-  </si>
-  <si>
-    <t>07.07.20246</t>
-  </si>
-  <si>
-    <t>07.07.20247</t>
-  </si>
-  <si>
-    <t>07.07.20248</t>
-  </si>
-  <si>
-    <t>07.07.20249</t>
-  </si>
-  <si>
-    <t>07.07.202410</t>
-  </si>
-  <si>
-    <t>07.07.202411</t>
-  </si>
-  <si>
-    <t>07.07.202412</t>
-  </si>
-  <si>
-    <t>07.07.202413</t>
-  </si>
-  <si>
-    <t>07.07.202414</t>
-  </si>
-  <si>
-    <t>07.07.202415</t>
-  </si>
-  <si>
-    <t>07.07.202416</t>
-  </si>
-  <si>
-    <t>07.07.202417</t>
-  </si>
-  <si>
-    <t>07.07.202418</t>
-  </si>
-  <si>
-    <t>07.07.202419</t>
-  </si>
-  <si>
-    <t>07.07.202420</t>
-  </si>
-  <si>
-    <t>07.07.202421</t>
-  </si>
-  <si>
-    <t>07.07.202422</t>
-  </si>
-  <si>
-    <t>07.07.202423</t>
-  </si>
-  <si>
-    <t>08.07.20240</t>
-  </si>
-  <si>
-    <t>08.07.20241</t>
-  </si>
-  <si>
-    <t>08.07.20242</t>
-  </si>
-  <si>
-    <t>08.07.20243</t>
-  </si>
-  <si>
-    <t>08.07.20244</t>
-  </si>
-  <si>
-    <t>08.07.20245</t>
-  </si>
-  <si>
-    <t>08.07.20246</t>
-  </si>
-  <si>
-    <t>08.07.20247</t>
-  </si>
-  <si>
-    <t>08.07.20248</t>
-  </si>
-  <si>
-    <t>08.07.20249</t>
+    <t>25.07.202412</t>
+  </si>
+  <si>
+    <t>25.07.202413</t>
+  </si>
+  <si>
+    <t>25.07.202414</t>
+  </si>
+  <si>
+    <t>25.07.202415</t>
+  </si>
+  <si>
+    <t>25.07.202416</t>
+  </si>
+  <si>
+    <t>25.07.202417</t>
+  </si>
+  <si>
+    <t>25.07.202418</t>
+  </si>
+  <si>
+    <t>25.07.202419</t>
+  </si>
+  <si>
+    <t>25.07.202420</t>
+  </si>
+  <si>
+    <t>25.07.202421</t>
+  </si>
+  <si>
+    <t>25.07.202422</t>
+  </si>
+  <si>
+    <t>25.07.202423</t>
+  </si>
+  <si>
+    <t>26.07.20240</t>
+  </si>
+  <si>
+    <t>26.07.20241</t>
+  </si>
+  <si>
+    <t>26.07.20242</t>
+  </si>
+  <si>
+    <t>26.07.20243</t>
+  </si>
+  <si>
+    <t>26.07.20244</t>
+  </si>
+  <si>
+    <t>26.07.20245</t>
+  </si>
+  <si>
+    <t>26.07.20246</t>
+  </si>
+  <si>
+    <t>26.07.20247</t>
+  </si>
+  <si>
+    <t>26.07.20248</t>
+  </si>
+  <si>
+    <t>26.07.20249</t>
+  </si>
+  <si>
+    <t>26.07.202410</t>
+  </si>
+  <si>
+    <t>26.07.202411</t>
+  </si>
+  <si>
+    <t>26.07.202412</t>
+  </si>
+  <si>
+    <t>26.07.202413</t>
+  </si>
+  <si>
+    <t>26.07.202414</t>
+  </si>
+  <si>
+    <t>26.07.202415</t>
+  </si>
+  <si>
+    <t>26.07.202416</t>
+  </si>
+  <si>
+    <t>26.07.202417</t>
+  </si>
+  <si>
+    <t>26.07.202418</t>
+  </si>
+  <si>
+    <t>26.07.202419</t>
+  </si>
+  <si>
+    <t>26.07.202420</t>
+  </si>
+  <si>
+    <t>26.07.202421</t>
+  </si>
+  <si>
+    <t>26.07.202422</t>
+  </si>
+  <si>
+    <t>26.07.202423</t>
+  </si>
+  <si>
+    <t>27.07.20240</t>
+  </si>
+  <si>
+    <t>27.07.20241</t>
+  </si>
+  <si>
+    <t>27.07.20242</t>
+  </si>
+  <si>
+    <t>27.07.20243</t>
+  </si>
+  <si>
+    <t>27.07.20244</t>
+  </si>
+  <si>
+    <t>27.07.20245</t>
+  </si>
+  <si>
+    <t>27.07.20246</t>
+  </si>
+  <si>
+    <t>27.07.20247</t>
+  </si>
+  <si>
+    <t>27.07.20248</t>
+  </si>
+  <si>
+    <t>27.07.20249</t>
+  </si>
+  <si>
+    <t>27.07.202410</t>
+  </si>
+  <si>
+    <t>27.07.202411</t>
+  </si>
+  <si>
+    <t>27.07.202412</t>
+  </si>
+  <si>
+    <t>27.07.202413</t>
+  </si>
+  <si>
+    <t>27.07.202414</t>
+  </si>
+  <si>
+    <t>27.07.202415</t>
+  </si>
+  <si>
+    <t>27.07.202416</t>
+  </si>
+  <si>
+    <t>27.07.202417</t>
+  </si>
+  <si>
+    <t>27.07.202418</t>
+  </si>
+  <si>
+    <t>27.07.202419</t>
+  </si>
+  <si>
+    <t>27.07.202420</t>
+  </si>
+  <si>
+    <t>27.07.202421</t>
+  </si>
+  <si>
+    <t>27.07.202422</t>
+  </si>
+  <si>
+    <t>27.07.202423</t>
+  </si>
+  <si>
+    <t>28.07.20240</t>
+  </si>
+  <si>
+    <t>28.07.20241</t>
+  </si>
+  <si>
+    <t>28.07.20242</t>
+  </si>
+  <si>
+    <t>28.07.20243</t>
+  </si>
+  <si>
+    <t>28.07.20244</t>
+  </si>
+  <si>
+    <t>28.07.20245</t>
+  </si>
+  <si>
+    <t>28.07.20246</t>
+  </si>
+  <si>
+    <t>28.07.20247</t>
+  </si>
+  <si>
+    <t>28.07.20248</t>
+  </si>
+  <si>
+    <t>28.07.20249</t>
+  </si>
+  <si>
+    <t>28.07.202410</t>
+  </si>
+  <si>
+    <t>28.07.202411</t>
+  </si>
+  <si>
+    <t>28.07.202412</t>
+  </si>
+  <si>
+    <t>28.07.202413</t>
+  </si>
+  <si>
+    <t>28.07.202414</t>
+  </si>
+  <si>
+    <t>28.07.202415</t>
+  </si>
+  <si>
+    <t>28.07.202416</t>
+  </si>
+  <si>
+    <t>28.07.202417</t>
+  </si>
+  <si>
+    <t>28.07.202418</t>
+  </si>
+  <si>
+    <t>28.07.202419</t>
+  </si>
+  <si>
+    <t>28.07.202420</t>
+  </si>
+  <si>
+    <t>28.07.202421</t>
+  </si>
+  <si>
+    <t>28.07.202422</t>
+  </si>
+  <si>
+    <t>28.07.202423</t>
+  </si>
+  <si>
+    <t>29.07.20240</t>
+  </si>
+  <si>
+    <t>29.07.20241</t>
+  </si>
+  <si>
+    <t>29.07.20242</t>
+  </si>
+  <si>
+    <t>29.07.20243</t>
+  </si>
+  <si>
+    <t>29.07.20244</t>
+  </si>
+  <si>
+    <t>29.07.20245</t>
+  </si>
+  <si>
+    <t>29.07.20246</t>
+  </si>
+  <si>
+    <t>29.07.20247</t>
+  </si>
+  <si>
+    <t>29.07.20248</t>
+  </si>
+  <si>
+    <t>29.07.20249</t>
+  </si>
+  <si>
+    <t>29.07.202410</t>
+  </si>
+  <si>
+    <t>29.07.202411</t>
+  </si>
+  <si>
+    <t>29.07.202412</t>
+  </si>
+  <si>
+    <t>29.07.202413</t>
+  </si>
+  <si>
+    <t>29.07.202414</t>
+  </si>
+  <si>
+    <t>29.07.202415</t>
+  </si>
+  <si>
+    <t>29.07.202416</t>
+  </si>
+  <si>
+    <t>29.07.202417</t>
+  </si>
+  <si>
+    <t>29.07.202418</t>
+  </si>
+  <si>
+    <t>29.07.202419</t>
+  </si>
+  <si>
+    <t>29.07.202420</t>
+  </si>
+  <si>
+    <t>29.07.202421</t>
+  </si>
+  <si>
+    <t>29.07.202422</t>
+  </si>
+  <si>
+    <t>29.07.202423</t>
+  </si>
+  <si>
+    <t>30.07.20240</t>
+  </si>
+  <si>
+    <t>30.07.20241</t>
+  </si>
+  <si>
+    <t>30.07.20242</t>
+  </si>
+  <si>
+    <t>30.07.20243</t>
+  </si>
+  <si>
+    <t>30.07.20244</t>
+  </si>
+  <si>
+    <t>30.07.20245</t>
+  </si>
+  <si>
+    <t>30.07.20246</t>
+  </si>
+  <si>
+    <t>30.07.20247</t>
+  </si>
+  <si>
+    <t>30.07.20248</t>
+  </si>
+  <si>
+    <t>30.07.20249</t>
+  </si>
+  <si>
+    <t>30.07.202410</t>
+  </si>
+  <si>
+    <t>30.07.202411</t>
+  </si>
+  <si>
+    <t>30.07.202412</t>
+  </si>
+  <si>
+    <t>30.07.202413</t>
+  </si>
+  <si>
+    <t>30.07.202414</t>
+  </si>
+  <si>
+    <t>30.07.202415</t>
+  </si>
+  <si>
+    <t>30.07.202416</t>
+  </si>
+  <si>
+    <t>30.07.202417</t>
+  </si>
+  <si>
+    <t>30.07.202418</t>
+  </si>
+  <si>
+    <t>30.07.202419</t>
+  </si>
+  <si>
+    <t>30.07.202420</t>
+  </si>
+  <si>
+    <t>30.07.202421</t>
+  </si>
+  <si>
+    <t>30.07.202422</t>
+  </si>
+  <si>
+    <t>30.07.202423</t>
+  </si>
+  <si>
+    <t>31.07.20240</t>
+  </si>
+  <si>
+    <t>31.07.20241</t>
+  </si>
+  <si>
+    <t>31.07.20242</t>
+  </si>
+  <si>
+    <t>31.07.20243</t>
+  </si>
+  <si>
+    <t>31.07.20244</t>
+  </si>
+  <si>
+    <t>31.07.20245</t>
+  </si>
+  <si>
+    <t>31.07.20246</t>
+  </si>
+  <si>
+    <t>31.07.20247</t>
+  </si>
+  <si>
+    <t>31.07.20248</t>
+  </si>
+  <si>
+    <t>31.07.20249</t>
+  </si>
+  <si>
+    <t>31.07.202410</t>
+  </si>
+  <si>
+    <t>31.07.202411</t>
+  </si>
+  <si>
+    <t>31.07.202412</t>
+  </si>
+  <si>
+    <t>31.07.202413</t>
+  </si>
+  <si>
+    <t>31.07.202414</t>
+  </si>
+  <si>
+    <t>31.07.202415</t>
+  </si>
+  <si>
+    <t>31.07.202416</t>
+  </si>
+  <si>
+    <t>31.07.202417</t>
+  </si>
+  <si>
+    <t>31.07.202418</t>
+  </si>
+  <si>
+    <t>31.07.202419</t>
+  </si>
+  <si>
+    <t>31.07.202420</t>
+  </si>
+  <si>
+    <t>31.07.202421</t>
+  </si>
+  <si>
+    <t>31.07.202422</t>
+  </si>
+  <si>
+    <t>31.07.202423</t>
+  </si>
+  <si>
+    <t>01.08.20240</t>
+  </si>
+  <si>
+    <t>01.08.20241</t>
+  </si>
+  <si>
+    <t>01.08.20242</t>
+  </si>
+  <si>
+    <t>01.08.20243</t>
+  </si>
+  <si>
+    <t>01.08.20244</t>
+  </si>
+  <si>
+    <t>01.08.20245</t>
+  </si>
+  <si>
+    <t>01.08.20246</t>
+  </si>
+  <si>
+    <t>01.08.20247</t>
+  </si>
+  <si>
+    <t>01.08.20248</t>
+  </si>
+  <si>
+    <t>01.08.20249</t>
+  </si>
+  <si>
+    <t>01.08.202410</t>
+  </si>
+  <si>
+    <t>01.08.202411</t>
+  </si>
+  <si>
+    <t>01.08.202412</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>2.768</v>
+        <v>2.686</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>2.914</v>
+        <v>2.08</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>2.939</v>
+        <v>1.739</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>2.137</v>
+        <v>1.453</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>1.923</v>
+        <v>0.917</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>1.777</v>
+        <v>0.44</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>1.597</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>1.028</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>0.492</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45474</v>
+        <v>45498</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>0.08699999999999999</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45474</v>
+        <v>45499</v>
       </c>
       <c r="B14">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45474</v>
+        <v>45499</v>
       </c>
       <c r="B15">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45474</v>
+        <v>45499</v>
       </c>
       <c r="B16">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>0.352</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>0.061</v>
+        <v>1.762</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>0.183</v>
+        <v>2.437</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>0.362</v>
+        <v>2.705</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>0.758</v>
+        <v>2.914</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>0.962</v>
+        <v>3.261</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>1.292</v>
+        <v>3.151</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B29">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>1.724</v>
+        <v>2.868</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B30">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>1.687</v>
+        <v>2.458</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B31">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>1.536</v>
+        <v>1.741</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B32">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <v>1.227</v>
+        <v>1.127</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B33">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C33">
-        <v>0.899</v>
+        <v>0.457</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B34">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C34">
-        <v>0.636</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>0.307</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B36">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C36">
-        <v>0.157</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45475</v>
+        <v>45499</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C37">
-        <v>0.051</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45475</v>
+        <v>45500</v>
       </c>
       <c r="B38">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45475</v>
+        <v>45500</v>
       </c>
       <c r="B39">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45475</v>
+        <v>45500</v>
       </c>
       <c r="B40">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B45">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1.007</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C47">
-        <v>0.061</v>
+        <v>1.753</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C48">
-        <v>0.174</v>
+        <v>2.34</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C49">
-        <v>0.286</v>
+        <v>2.797</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B50">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>0.439</v>
+        <v>2.824</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B51">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>0.514</v>
+        <v>3.094</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C52">
-        <v>0.771</v>
+        <v>3.024</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B53">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>0.784</v>
+        <v>2.816</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B54">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>1.067</v>
+        <v>2.426</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B55">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>0.975</v>
+        <v>1.799</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B56">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C56">
-        <v>0.861</v>
+        <v>1.124</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B57">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C57">
-        <v>0.783</v>
+        <v>0.466</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B58">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C58">
-        <v>0.626</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B59">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C59">
-        <v>0.459</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B60">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C60">
-        <v>0.241</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45476</v>
+        <v>45500</v>
       </c>
       <c r="B61">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C61">
-        <v>0.175</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45476</v>
+        <v>45501</v>
       </c>
       <c r="B62">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45476</v>
+        <v>45501</v>
       </c>
       <c r="B63">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45476</v>
+        <v>45501</v>
       </c>
       <c r="B64">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B70">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1.014</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B71">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>0.08</v>
+        <v>1.756</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B72">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>0.329</v>
+        <v>2.322</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C73">
-        <v>0.585</v>
+        <v>2.722</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B74">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C74">
-        <v>0.995</v>
+        <v>2.924</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B75">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C75">
-        <v>1.34</v>
+        <v>3.031</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B76">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>1.717</v>
+        <v>2.978</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B77">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>1.973</v>
+        <v>2.806</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B78">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>1.937</v>
+        <v>2.218</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B79">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C79">
-        <v>1.927</v>
+        <v>1.771</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B80">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C80">
-        <v>1.969</v>
+        <v>1.062</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B81">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C81">
-        <v>1.748</v>
+        <v>0.454</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B82">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>1.62</v>
+        <v>0.268</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B83">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C83">
-        <v>1.034</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B84">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C84">
-        <v>0.469</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45477</v>
+        <v>45501</v>
       </c>
       <c r="B85">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C85">
-        <v>0.097</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45477</v>
+        <v>45502</v>
       </c>
       <c r="B86">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45477</v>
+        <v>45502</v>
       </c>
       <c r="B87">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45477</v>
+        <v>45502</v>
       </c>
       <c r="B88">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B92">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B94">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>0.867</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B95">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C95">
-        <v>0.114</v>
+        <v>1.586</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B96">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C96">
-        <v>0.444</v>
+        <v>2.28</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B97">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C97">
-        <v>1.163</v>
+        <v>2.793</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B98">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C98">
-        <v>1.839</v>
+        <v>3.028</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B99">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C99">
-        <v>2.425</v>
+        <v>3.038</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B100">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C100">
-        <v>2.914</v>
+        <v>2.984</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B101">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C101">
-        <v>3.122</v>
+        <v>2.831</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B102">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C102">
-        <v>3.314</v>
+        <v>2.426</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B103">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C103">
-        <v>3.155</v>
+        <v>1.8</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B104">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C104">
-        <v>2.926</v>
+        <v>1.128</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B105">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C105">
-        <v>2.467</v>
+        <v>0.447</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B106">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C106">
-        <v>1.797</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B107">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C107">
-        <v>1.192</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B108">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C108">
-        <v>0.542</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45478</v>
+        <v>45502</v>
       </c>
       <c r="B109">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C109">
-        <v>0.114</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45478</v>
+        <v>45503</v>
       </c>
       <c r="B110">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45478</v>
+        <v>45503</v>
       </c>
       <c r="B111">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45478</v>
+        <v>45503</v>
       </c>
       <c r="B112">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B115">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B117">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B118">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>1.017</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B119">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C119">
-        <v>0.106</v>
+        <v>1.787</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B120">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C120">
-        <v>0.446</v>
+        <v>2.419</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B121">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C121">
-        <v>1.127</v>
+        <v>2.816</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B122">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C122">
-        <v>1.812</v>
+        <v>3.059</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B123">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C123">
-        <v>2.425</v>
+        <v>3.15</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B124">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C124">
-        <v>2.871</v>
+        <v>3.042</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B125">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C125">
-        <v>3.111</v>
+        <v>2.831</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B126">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C126">
-        <v>3.169</v>
+        <v>2.454</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B127">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C127">
-        <v>3.042</v>
+        <v>1.812</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B128">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C128">
-        <v>2.862</v>
+        <v>1.131</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B129">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C129">
-        <v>2.455</v>
+        <v>0.411</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B130">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C130">
-        <v>1.815</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B131">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C131">
-        <v>1.151</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B132">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C132">
-        <v>0.533</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45479</v>
+        <v>45503</v>
       </c>
       <c r="B133">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C133">
-        <v>0.107</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45479</v>
+        <v>45504</v>
       </c>
       <c r="B134">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45479</v>
+        <v>45504</v>
       </c>
       <c r="B135">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45479</v>
+        <v>45504</v>
       </c>
       <c r="B136">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B139">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B140">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>0.052</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B141">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B142">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>1.005</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B143">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C143">
-        <v>0.099</v>
+        <v>1.765</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B144">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C144">
-        <v>0.435</v>
+        <v>2.419</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B145">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C145">
-        <v>1.089</v>
+        <v>2.816</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B146">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C146">
-        <v>1.793</v>
+        <v>2.849</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B147">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C147">
-        <v>2.422</v>
+        <v>3.139</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B148">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C148">
-        <v>2.8</v>
+        <v>3.034</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B149">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C149">
-        <v>2.969</v>
+        <v>2.831</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B150">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C150">
-        <v>3.087</v>
+        <v>2.426</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B151">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C151">
-        <v>2.984</v>
+        <v>1.799</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B152">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C152">
-        <v>2.813</v>
+        <v>1.127</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B153">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C153">
-        <v>2.409</v>
+        <v>0.418</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B154">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C154">
-        <v>1.778</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B155">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C155">
-        <v>1.13</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B156">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C156">
-        <v>0.485</v>
+        <v>0</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45480</v>
+        <v>45504</v>
       </c>
       <c r="B157">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C157">
-        <v>0.08699999999999999</v>
+        <v>0</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45480</v>
+        <v>45505</v>
       </c>
       <c r="B158">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45480</v>
+        <v>45505</v>
       </c>
       <c r="B159">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45480</v>
+        <v>45505</v>
       </c>
       <c r="B160">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B161">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B163">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B164">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>0.052</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B165">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>0.359</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B166">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>1.045</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B167">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C167">
-        <v>0.094</v>
+        <v>1.825</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B168">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C168">
-        <v>0.443</v>
+        <v>2.349</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B169">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C169">
-        <v>1.109</v>
+        <v>2.717</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45481</v>
+        <v>45505</v>
       </c>
       <c r="B170">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C170">
-        <v>1.801</v>
+        <v>2.876</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Splitting the Weather data to each location for both models - base and intraday
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,357 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>25.07.202412</t>
-  </si>
-  <si>
-    <t>25.07.202413</t>
-  </si>
-  <si>
-    <t>25.07.202414</t>
-  </si>
-  <si>
-    <t>25.07.202415</t>
-  </si>
-  <si>
-    <t>25.07.202416</t>
-  </si>
-  <si>
-    <t>25.07.202417</t>
-  </si>
-  <si>
-    <t>25.07.202418</t>
-  </si>
-  <si>
-    <t>25.07.202419</t>
-  </si>
-  <si>
-    <t>25.07.202420</t>
-  </si>
-  <si>
-    <t>25.07.202421</t>
-  </si>
-  <si>
-    <t>25.07.202422</t>
-  </si>
-  <si>
-    <t>25.07.202423</t>
-  </si>
-  <si>
-    <t>26.07.20240</t>
-  </si>
-  <si>
-    <t>26.07.20241</t>
-  </si>
-  <si>
-    <t>26.07.20242</t>
-  </si>
-  <si>
-    <t>26.07.20243</t>
-  </si>
-  <si>
-    <t>26.07.20244</t>
-  </si>
-  <si>
-    <t>26.07.20245</t>
-  </si>
-  <si>
-    <t>26.07.20246</t>
-  </si>
-  <si>
-    <t>26.07.20247</t>
-  </si>
-  <si>
-    <t>26.07.20248</t>
-  </si>
-  <si>
-    <t>26.07.20249</t>
-  </si>
-  <si>
-    <t>26.07.202410</t>
-  </si>
-  <si>
-    <t>26.07.202411</t>
-  </si>
-  <si>
-    <t>26.07.202412</t>
-  </si>
-  <si>
-    <t>26.07.202413</t>
-  </si>
-  <si>
-    <t>26.07.202414</t>
-  </si>
-  <si>
-    <t>26.07.202415</t>
-  </si>
-  <si>
-    <t>26.07.202416</t>
-  </si>
-  <si>
-    <t>26.07.202417</t>
-  </si>
-  <si>
-    <t>26.07.202418</t>
-  </si>
-  <si>
-    <t>26.07.202419</t>
-  </si>
-  <si>
-    <t>26.07.202420</t>
-  </si>
-  <si>
-    <t>26.07.202421</t>
-  </si>
-  <si>
-    <t>26.07.202422</t>
-  </si>
-  <si>
-    <t>26.07.202423</t>
-  </si>
-  <si>
-    <t>27.07.20240</t>
-  </si>
-  <si>
-    <t>27.07.20241</t>
-  </si>
-  <si>
-    <t>27.07.20242</t>
-  </si>
-  <si>
-    <t>27.07.20243</t>
-  </si>
-  <si>
-    <t>27.07.20244</t>
-  </si>
-  <si>
-    <t>27.07.20245</t>
-  </si>
-  <si>
-    <t>27.07.20246</t>
-  </si>
-  <si>
-    <t>27.07.20247</t>
-  </si>
-  <si>
-    <t>27.07.20248</t>
-  </si>
-  <si>
-    <t>27.07.20249</t>
-  </si>
-  <si>
-    <t>27.07.202410</t>
-  </si>
-  <si>
-    <t>27.07.202411</t>
-  </si>
-  <si>
-    <t>27.07.202412</t>
-  </si>
-  <si>
-    <t>27.07.202413</t>
-  </si>
-  <si>
-    <t>27.07.202414</t>
-  </si>
-  <si>
-    <t>27.07.202415</t>
-  </si>
-  <si>
-    <t>27.07.202416</t>
-  </si>
-  <si>
-    <t>27.07.202417</t>
-  </si>
-  <si>
-    <t>27.07.202418</t>
-  </si>
-  <si>
-    <t>27.07.202419</t>
-  </si>
-  <si>
-    <t>27.07.202420</t>
-  </si>
-  <si>
-    <t>27.07.202421</t>
-  </si>
-  <si>
-    <t>27.07.202422</t>
-  </si>
-  <si>
-    <t>27.07.202423</t>
-  </si>
-  <si>
-    <t>28.07.20240</t>
-  </si>
-  <si>
-    <t>28.07.20241</t>
-  </si>
-  <si>
-    <t>28.07.20242</t>
-  </si>
-  <si>
-    <t>28.07.20243</t>
-  </si>
-  <si>
-    <t>28.07.20244</t>
-  </si>
-  <si>
-    <t>28.07.20245</t>
-  </si>
-  <si>
-    <t>28.07.20246</t>
-  </si>
-  <si>
-    <t>28.07.20247</t>
-  </si>
-  <si>
-    <t>28.07.20248</t>
-  </si>
-  <si>
-    <t>28.07.20249</t>
-  </si>
-  <si>
-    <t>28.07.202410</t>
-  </si>
-  <si>
-    <t>28.07.202411</t>
-  </si>
-  <si>
-    <t>28.07.202412</t>
-  </si>
-  <si>
-    <t>28.07.202413</t>
-  </si>
-  <si>
-    <t>28.07.202414</t>
-  </si>
-  <si>
-    <t>28.07.202415</t>
-  </si>
-  <si>
-    <t>28.07.202416</t>
-  </si>
-  <si>
-    <t>28.07.202417</t>
-  </si>
-  <si>
-    <t>28.07.202418</t>
-  </si>
-  <si>
-    <t>28.07.202419</t>
-  </si>
-  <si>
-    <t>28.07.202420</t>
-  </si>
-  <si>
-    <t>28.07.202421</t>
-  </si>
-  <si>
-    <t>28.07.202422</t>
-  </si>
-  <si>
-    <t>28.07.202423</t>
-  </si>
-  <si>
-    <t>29.07.20240</t>
-  </si>
-  <si>
-    <t>29.07.20241</t>
-  </si>
-  <si>
-    <t>29.07.20242</t>
-  </si>
-  <si>
-    <t>29.07.20243</t>
-  </si>
-  <si>
-    <t>29.07.20244</t>
-  </si>
-  <si>
-    <t>29.07.20245</t>
-  </si>
-  <si>
-    <t>29.07.20246</t>
-  </si>
-  <si>
-    <t>29.07.20247</t>
-  </si>
-  <si>
-    <t>29.07.20248</t>
-  </si>
-  <si>
-    <t>29.07.20249</t>
-  </si>
-  <si>
-    <t>29.07.202410</t>
-  </si>
-  <si>
-    <t>29.07.202411</t>
-  </si>
-  <si>
-    <t>29.07.202412</t>
-  </si>
-  <si>
-    <t>29.07.202413</t>
-  </si>
-  <si>
-    <t>29.07.202414</t>
-  </si>
-  <si>
-    <t>29.07.202415</t>
-  </si>
-  <si>
-    <t>29.07.202416</t>
-  </si>
-  <si>
-    <t>29.07.202417</t>
-  </si>
-  <si>
-    <t>29.07.202418</t>
-  </si>
-  <si>
-    <t>29.07.202419</t>
-  </si>
-  <si>
-    <t>29.07.202420</t>
-  </si>
-  <si>
-    <t>29.07.202421</t>
-  </si>
-  <si>
-    <t>29.07.202422</t>
-  </si>
-  <si>
-    <t>29.07.202423</t>
-  </si>
-  <si>
-    <t>30.07.20240</t>
-  </si>
-  <si>
-    <t>30.07.20241</t>
-  </si>
-  <si>
-    <t>30.07.20242</t>
-  </si>
-  <si>
-    <t>30.07.20243</t>
-  </si>
-  <si>
-    <t>30.07.20244</t>
-  </si>
-  <si>
-    <t>30.07.20245</t>
-  </si>
-  <si>
-    <t>30.07.20246</t>
-  </si>
-  <si>
-    <t>30.07.20247</t>
-  </si>
-  <si>
-    <t>30.07.20248</t>
-  </si>
-  <si>
     <t>30.07.20249</t>
   </si>
   <si>
@@ -533,6 +182,357 @@
   </si>
   <si>
     <t>01.08.202412</t>
+  </si>
+  <si>
+    <t>01.08.202413</t>
+  </si>
+  <si>
+    <t>01.08.202414</t>
+  </si>
+  <si>
+    <t>01.08.202415</t>
+  </si>
+  <si>
+    <t>01.08.202416</t>
+  </si>
+  <si>
+    <t>01.08.202417</t>
+  </si>
+  <si>
+    <t>01.08.202418</t>
+  </si>
+  <si>
+    <t>01.08.202419</t>
+  </si>
+  <si>
+    <t>01.08.202420</t>
+  </si>
+  <si>
+    <t>01.08.202421</t>
+  </si>
+  <si>
+    <t>01.08.202422</t>
+  </si>
+  <si>
+    <t>01.08.202423</t>
+  </si>
+  <si>
+    <t>02.08.20240</t>
+  </si>
+  <si>
+    <t>02.08.20241</t>
+  </si>
+  <si>
+    <t>02.08.20242</t>
+  </si>
+  <si>
+    <t>02.08.20243</t>
+  </si>
+  <si>
+    <t>02.08.20244</t>
+  </si>
+  <si>
+    <t>02.08.20245</t>
+  </si>
+  <si>
+    <t>02.08.20246</t>
+  </si>
+  <si>
+    <t>02.08.20247</t>
+  </si>
+  <si>
+    <t>02.08.20248</t>
+  </si>
+  <si>
+    <t>02.08.20249</t>
+  </si>
+  <si>
+    <t>02.08.202410</t>
+  </si>
+  <si>
+    <t>02.08.202411</t>
+  </si>
+  <si>
+    <t>02.08.202412</t>
+  </si>
+  <si>
+    <t>02.08.202413</t>
+  </si>
+  <si>
+    <t>02.08.202414</t>
+  </si>
+  <si>
+    <t>02.08.202415</t>
+  </si>
+  <si>
+    <t>02.08.202416</t>
+  </si>
+  <si>
+    <t>02.08.202417</t>
+  </si>
+  <si>
+    <t>02.08.202418</t>
+  </si>
+  <si>
+    <t>02.08.202419</t>
+  </si>
+  <si>
+    <t>02.08.202420</t>
+  </si>
+  <si>
+    <t>02.08.202421</t>
+  </si>
+  <si>
+    <t>02.08.202422</t>
+  </si>
+  <si>
+    <t>02.08.202423</t>
+  </si>
+  <si>
+    <t>03.08.20240</t>
+  </si>
+  <si>
+    <t>03.08.20241</t>
+  </si>
+  <si>
+    <t>03.08.20242</t>
+  </si>
+  <si>
+    <t>03.08.20243</t>
+  </si>
+  <si>
+    <t>03.08.20244</t>
+  </si>
+  <si>
+    <t>03.08.20245</t>
+  </si>
+  <si>
+    <t>03.08.20246</t>
+  </si>
+  <si>
+    <t>03.08.20247</t>
+  </si>
+  <si>
+    <t>03.08.20248</t>
+  </si>
+  <si>
+    <t>03.08.20249</t>
+  </si>
+  <si>
+    <t>03.08.202410</t>
+  </si>
+  <si>
+    <t>03.08.202411</t>
+  </si>
+  <si>
+    <t>03.08.202412</t>
+  </si>
+  <si>
+    <t>03.08.202413</t>
+  </si>
+  <si>
+    <t>03.08.202414</t>
+  </si>
+  <si>
+    <t>03.08.202415</t>
+  </si>
+  <si>
+    <t>03.08.202416</t>
+  </si>
+  <si>
+    <t>03.08.202417</t>
+  </si>
+  <si>
+    <t>03.08.202418</t>
+  </si>
+  <si>
+    <t>03.08.202419</t>
+  </si>
+  <si>
+    <t>03.08.202420</t>
+  </si>
+  <si>
+    <t>03.08.202421</t>
+  </si>
+  <si>
+    <t>03.08.202422</t>
+  </si>
+  <si>
+    <t>03.08.202423</t>
+  </si>
+  <si>
+    <t>04.08.20240</t>
+  </si>
+  <si>
+    <t>04.08.20241</t>
+  </si>
+  <si>
+    <t>04.08.20242</t>
+  </si>
+  <si>
+    <t>04.08.20243</t>
+  </si>
+  <si>
+    <t>04.08.20244</t>
+  </si>
+  <si>
+    <t>04.08.20245</t>
+  </si>
+  <si>
+    <t>04.08.20246</t>
+  </si>
+  <si>
+    <t>04.08.20247</t>
+  </si>
+  <si>
+    <t>04.08.20248</t>
+  </si>
+  <si>
+    <t>04.08.20249</t>
+  </si>
+  <si>
+    <t>04.08.202410</t>
+  </si>
+  <si>
+    <t>04.08.202411</t>
+  </si>
+  <si>
+    <t>04.08.202412</t>
+  </si>
+  <si>
+    <t>04.08.202413</t>
+  </si>
+  <si>
+    <t>04.08.202414</t>
+  </si>
+  <si>
+    <t>04.08.202415</t>
+  </si>
+  <si>
+    <t>04.08.202416</t>
+  </si>
+  <si>
+    <t>04.08.202417</t>
+  </si>
+  <si>
+    <t>04.08.202418</t>
+  </si>
+  <si>
+    <t>04.08.202419</t>
+  </si>
+  <si>
+    <t>04.08.202420</t>
+  </si>
+  <si>
+    <t>04.08.202421</t>
+  </si>
+  <si>
+    <t>04.08.202422</t>
+  </si>
+  <si>
+    <t>04.08.202423</t>
+  </si>
+  <si>
+    <t>05.08.20240</t>
+  </si>
+  <si>
+    <t>05.08.20241</t>
+  </si>
+  <si>
+    <t>05.08.20242</t>
+  </si>
+  <si>
+    <t>05.08.20243</t>
+  </si>
+  <si>
+    <t>05.08.20244</t>
+  </si>
+  <si>
+    <t>05.08.20245</t>
+  </si>
+  <si>
+    <t>05.08.20246</t>
+  </si>
+  <si>
+    <t>05.08.20247</t>
+  </si>
+  <si>
+    <t>05.08.20248</t>
+  </si>
+  <si>
+    <t>05.08.20249</t>
+  </si>
+  <si>
+    <t>05.08.202410</t>
+  </si>
+  <si>
+    <t>05.08.202411</t>
+  </si>
+  <si>
+    <t>05.08.202412</t>
+  </si>
+  <si>
+    <t>05.08.202413</t>
+  </si>
+  <si>
+    <t>05.08.202414</t>
+  </si>
+  <si>
+    <t>05.08.202415</t>
+  </si>
+  <si>
+    <t>05.08.202416</t>
+  </si>
+  <si>
+    <t>05.08.202417</t>
+  </si>
+  <si>
+    <t>05.08.202418</t>
+  </si>
+  <si>
+    <t>05.08.202419</t>
+  </si>
+  <si>
+    <t>05.08.202420</t>
+  </si>
+  <si>
+    <t>05.08.202421</t>
+  </si>
+  <si>
+    <t>05.08.202422</t>
+  </si>
+  <si>
+    <t>05.08.202423</t>
+  </si>
+  <si>
+    <t>06.08.20240</t>
+  </si>
+  <si>
+    <t>06.08.20241</t>
+  </si>
+  <si>
+    <t>06.08.20242</t>
+  </si>
+  <si>
+    <t>06.08.20243</t>
+  </si>
+  <si>
+    <t>06.08.20244</t>
+  </si>
+  <si>
+    <t>06.08.20245</t>
+  </si>
+  <si>
+    <t>06.08.20246</t>
+  </si>
+  <si>
+    <t>06.08.20247</t>
+  </si>
+  <si>
+    <t>06.08.20248</t>
+  </si>
+  <si>
+    <t>06.08.20249</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>2.686</v>
+        <v>2.798</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>2.08</v>
+        <v>3.088</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>1.739</v>
+        <v>3.267</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>1.453</v>
+        <v>3.161</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>0.917</v>
+        <v>2.94</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>0.44</v>
+        <v>2.444</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>0.07199999999999999</v>
+        <v>1.868</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.203</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.466</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45498</v>
+        <v>45503</v>
       </c>
       <c r="B13">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45499</v>
+        <v>45503</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45499</v>
+        <v>45503</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45499</v>
+        <v>45503</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>0.07099999999999999</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>0.352</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>1.03</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>1.762</v>
+        <v>0.066</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>2.437</v>
+        <v>0.368</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B25">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>2.705</v>
+        <v>1.017</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>2.914</v>
+        <v>1.756</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>3.261</v>
+        <v>2.404</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B28">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C28">
-        <v>3.151</v>
+        <v>2.747</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B29">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C29">
-        <v>2.868</v>
+        <v>2.936</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>2.458</v>
+        <v>3.139</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C31">
-        <v>1.741</v>
+        <v>3.035</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B32">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C32">
-        <v>1.127</v>
+        <v>2.893</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B33">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C33">
-        <v>0.457</v>
+        <v>2.345</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C34">
-        <v>0.07099999999999999</v>
+        <v>1.805</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B35">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1.166</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B36">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.452</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="B37">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45500</v>
+        <v>45504</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45500</v>
+        <v>45504</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45500</v>
+        <v>45504</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>0.07099999999999999</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C45">
-        <v>0.369</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C46">
-        <v>1.007</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C47">
-        <v>1.753</v>
+        <v>0.046</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C48">
-        <v>2.34</v>
+        <v>0.368</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B49">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C49">
-        <v>2.797</v>
+        <v>0.955</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C50">
-        <v>2.824</v>
+        <v>1.59</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C51">
-        <v>3.094</v>
+        <v>2.335</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C52">
-        <v>3.024</v>
+        <v>2.437</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C53">
-        <v>2.816</v>
+        <v>2.915</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B54">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C54">
-        <v>2.426</v>
+        <v>3.084</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C55">
-        <v>1.799</v>
+        <v>3.085</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B56">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C56">
-        <v>1.124</v>
+        <v>2.911</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B57">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C57">
-        <v>0.466</v>
+        <v>2.33</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C58">
-        <v>0.07099999999999999</v>
+        <v>1.723</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.425</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45501</v>
+        <v>45505</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45501</v>
+        <v>45505</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45501</v>
+        <v>45505</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>0.07099999999999999</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C69">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C70">
-        <v>1.014</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B71">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C71">
-        <v>1.756</v>
+        <v>0.04</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C72">
-        <v>2.322</v>
+        <v>0.247</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C73">
-        <v>2.722</v>
+        <v>0.53</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C74">
-        <v>2.924</v>
+        <v>0.978</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C75">
-        <v>3.031</v>
+        <v>1.48</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C76">
-        <v>2.978</v>
+        <v>1.753</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C77">
-        <v>2.806</v>
+        <v>2.061</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B78">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C78">
-        <v>2.218</v>
+        <v>2.176</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C79">
-        <v>1.771</v>
+        <v>2.126</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C80">
-        <v>1.062</v>
+        <v>2.027</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B81">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C81">
-        <v>0.454</v>
+        <v>1.836</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C82">
-        <v>0.268</v>
+        <v>1.422</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B83">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.823</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B84">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.292</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45501</v>
+        <v>45506</v>
       </c>
       <c r="B85">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.036</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45502</v>
+        <v>45506</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45502</v>
+        <v>45506</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45502</v>
+        <v>45506</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C92">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B93">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C93">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B94">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C94">
-        <v>0.867</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B95">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C95">
-        <v>1.586</v>
+        <v>0.046</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C96">
-        <v>2.28</v>
+        <v>0.364</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B97">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C97">
-        <v>2.793</v>
+        <v>0.895</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B98">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C98">
-        <v>3.028</v>
+        <v>1.486</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B99">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C99">
-        <v>3.038</v>
+        <v>1.625</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B100">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C100">
-        <v>2.984</v>
+        <v>1.884</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B101">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C101">
-        <v>2.831</v>
+        <v>1.878</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B102">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C102">
-        <v>2.426</v>
+        <v>1.824</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B103">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C103">
-        <v>1.8</v>
+        <v>1.767</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B104">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C104">
-        <v>1.128</v>
+        <v>1.637</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B105">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C105">
-        <v>0.447</v>
+        <v>1.52</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B106">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C106">
-        <v>0.07099999999999999</v>
+        <v>1.126</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B107">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.789</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B108">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.292</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45502</v>
+        <v>45507</v>
       </c>
       <c r="B109">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45503</v>
+        <v>45507</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45503</v>
+        <v>45507</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45503</v>
+        <v>45507</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B114">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B115">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B116">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>0.07099999999999999</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B117">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C117">
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B118">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C118">
-        <v>1.017</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B119">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C119">
-        <v>1.787</v>
+        <v>0.039</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B120">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C120">
-        <v>2.419</v>
+        <v>0.319</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B121">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C121">
-        <v>2.816</v>
+        <v>0.656</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B122">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C122">
-        <v>3.059</v>
+        <v>1.525</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B123">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C123">
-        <v>3.15</v>
+        <v>2.129</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B124">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C124">
-        <v>3.042</v>
+        <v>2.61</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B125">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C125">
-        <v>2.831</v>
+        <v>2.788</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B126">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C126">
-        <v>2.454</v>
+        <v>2.933</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B127">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C127">
-        <v>1.812</v>
+        <v>2.84</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B128">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C128">
-        <v>1.131</v>
+        <v>2.715</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B129">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C129">
-        <v>0.411</v>
+        <v>2.139</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B130">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C130">
-        <v>0.07099999999999999</v>
+        <v>1.602</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B131">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1.004</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B132">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.367</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45503</v>
+        <v>45508</v>
       </c>
       <c r="B133">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>0.041</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45504</v>
+        <v>45508</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45504</v>
+        <v>45508</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45504</v>
+        <v>45508</v>
       </c>
       <c r="B136">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B137">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B138">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B139">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B140">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C140">
-        <v>0.052</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B141">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C141">
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B142">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C142">
-        <v>1.005</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B143">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C143">
-        <v>1.765</v>
+        <v>0.039</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B144">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C144">
-        <v>2.419</v>
+        <v>0.306</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B145">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C145">
-        <v>2.816</v>
+        <v>0.788</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B146">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C146">
-        <v>2.849</v>
+        <v>1.532</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B147">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C147">
-        <v>3.139</v>
+        <v>2.208</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B148">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C148">
-        <v>3.034</v>
+        <v>2.594</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B149">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C149">
-        <v>2.831</v>
+        <v>2.873</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B150">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C150">
-        <v>2.426</v>
+        <v>3.086</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B151">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C151">
-        <v>1.799</v>
+        <v>2.841</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B152">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C152">
-        <v>1.127</v>
+        <v>2.579</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B153">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C153">
-        <v>0.418</v>
+        <v>2.057</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B154">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C154">
-        <v>0.07099999999999999</v>
+        <v>1.533</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B155">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>0.896</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B156">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>0.364</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45504</v>
+        <v>45509</v>
       </c>
       <c r="B157">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.041</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45505</v>
+        <v>45509</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45505</v>
+        <v>45509</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45505</v>
+        <v>45509</v>
       </c>
       <c r="B160">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B161">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B162">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B163">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B164">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C164">
-        <v>0.052</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B165">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C165">
-        <v>0.359</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B166">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C166">
-        <v>1.045</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B167">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C167">
-        <v>1.825</v>
+        <v>0.042</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B168">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C168">
-        <v>2.349</v>
+        <v>0.333</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B169">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C169">
-        <v>2.717</v>
+        <v>0.957</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="B170">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C170">
-        <v>2.876</v>
+        <v>1.628</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Updating the Imperial hourly production forecast model
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,18 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>30.07.20249</t>
-  </si>
-  <si>
-    <t>30.07.202410</t>
-  </si>
-  <si>
-    <t>30.07.202411</t>
-  </si>
-  <si>
-    <t>30.07.202412</t>
-  </si>
-  <si>
     <t>30.07.202413</t>
   </si>
   <si>
@@ -533,6 +521,18 @@
   </si>
   <si>
     <t>06.08.20249</t>
+  </si>
+  <si>
+    <t>06.08.202410</t>
+  </si>
+  <si>
+    <t>06.08.202411</t>
+  </si>
+  <si>
+    <t>06.08.202412</t>
+  </si>
+  <si>
+    <t>06.08.202413</t>
   </si>
 </sst>
 </file>
@@ -919,7 +919,7 @@
         <v>45503</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -933,7 +933,7 @@
         <v>45503</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -947,10 +947,10 @@
         <v>45503</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>2.798</v>
+        <v>2.944</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -961,10 +961,10 @@
         <v>45503</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>3.088</v>
+        <v>2.446</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -975,10 +975,10 @@
         <v>45503</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>3.267</v>
+        <v>1.868</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -989,10 +989,10 @@
         <v>45503</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>3.161</v>
+        <v>1.203</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1003,10 +1003,10 @@
         <v>45503</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>2.94</v>
+        <v>0.465</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1017,10 +1017,10 @@
         <v>45503</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>2.444</v>
+        <v>0.065</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1031,10 +1031,10 @@
         <v>45503</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>1.868</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1045,10 +1045,10 @@
         <v>45503</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>1.203</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1059,10 +1059,10 @@
         <v>45503</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>0.466</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45503</v>
+        <v>45504</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0.065</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45503</v>
+        <v>45504</v>
       </c>
       <c r="B14">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45503</v>
+        <v>45504</v>
       </c>
       <c r="B15">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45503</v>
+        <v>45504</v>
       </c>
       <c r="B16">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1129,7 +1129,7 @@
         <v>45504</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1143,7 +1143,7 @@
         <v>45504</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1157,10 +1157,10 @@
         <v>45504</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.066</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1171,10 +1171,10 @@
         <v>45504</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.365</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1185,10 +1185,10 @@
         <v>45504</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1.002</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1199,10 +1199,10 @@
         <v>45504</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1.756</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1213,10 +1213,10 @@
         <v>45504</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>0.066</v>
+        <v>2.404</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1227,10 +1227,10 @@
         <v>45504</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>0.368</v>
+        <v>2.71</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1241,10 +1241,10 @@
         <v>45504</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>1.017</v>
+        <v>2.936</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1255,10 +1255,10 @@
         <v>45504</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>1.756</v>
+        <v>3.139</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1269,10 +1269,10 @@
         <v>45504</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>2.404</v>
+        <v>3.035</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1283,10 +1283,10 @@
         <v>45504</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>2.747</v>
+        <v>2.893</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1297,10 +1297,10 @@
         <v>45504</v>
       </c>
       <c r="B29">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>2.936</v>
+        <v>2.345</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1311,10 +1311,10 @@
         <v>45504</v>
       </c>
       <c r="B30">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>3.139</v>
+        <v>1.83</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1325,10 +1325,10 @@
         <v>45504</v>
       </c>
       <c r="B31">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>3.035</v>
+        <v>1.168</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1339,10 +1339,10 @@
         <v>45504</v>
       </c>
       <c r="B32">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>2.893</v>
+        <v>0.456</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1353,10 +1353,10 @@
         <v>45504</v>
       </c>
       <c r="B33">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C33">
-        <v>2.345</v>
+        <v>0.063</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1367,10 +1367,10 @@
         <v>45504</v>
       </c>
       <c r="B34">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>1.805</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1381,10 +1381,10 @@
         <v>45504</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C35">
-        <v>1.166</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1395,10 +1395,10 @@
         <v>45504</v>
       </c>
       <c r="B36">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C36">
-        <v>0.452</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45504</v>
+        <v>45505</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>0.063</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45504</v>
+        <v>45505</v>
       </c>
       <c r="B38">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45504</v>
+        <v>45505</v>
       </c>
       <c r="B39">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45504</v>
+        <v>45505</v>
       </c>
       <c r="B40">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1465,7 +1465,7 @@
         <v>45505</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>45505</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1493,10 +1493,10 @@
         <v>45505</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1507,10 +1507,10 @@
         <v>45505</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1521,10 +1521,10 @@
         <v>45505</v>
       </c>
       <c r="B45">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.957</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1535,10 +1535,10 @@
         <v>45505</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1.599</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1549,10 +1549,10 @@
         <v>45505</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>0.046</v>
+        <v>2.335</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1563,10 +1563,10 @@
         <v>45505</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>0.368</v>
+        <v>2.437</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1577,10 +1577,10 @@
         <v>45505</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>0.955</v>
+        <v>2.915</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1591,10 +1591,10 @@
         <v>45505</v>
       </c>
       <c r="B50">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>1.59</v>
+        <v>3.086</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1605,10 +1605,10 @@
         <v>45505</v>
       </c>
       <c r="B51">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C51">
-        <v>2.335</v>
+        <v>3.085</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1619,10 +1619,10 @@
         <v>45505</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C52">
-        <v>2.437</v>
+        <v>2.919</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1633,10 +1633,10 @@
         <v>45505</v>
       </c>
       <c r="B53">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>2.915</v>
+        <v>2.246</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1647,10 +1647,10 @@
         <v>45505</v>
       </c>
       <c r="B54">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>3.084</v>
+        <v>1.711</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1661,10 +1661,10 @@
         <v>45505</v>
       </c>
       <c r="B55">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C55">
-        <v>3.085</v>
+        <v>0.992</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1675,10 +1675,10 @@
         <v>45505</v>
       </c>
       <c r="B56">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>2.911</v>
+        <v>0.368</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1689,10 +1689,10 @@
         <v>45505</v>
       </c>
       <c r="B57">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>2.33</v>
+        <v>0.041</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1703,10 +1703,10 @@
         <v>45505</v>
       </c>
       <c r="B58">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>1.723</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1717,10 +1717,10 @@
         <v>45505</v>
       </c>
       <c r="B59">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C59">
-        <v>1.02</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1731,10 +1731,10 @@
         <v>45505</v>
       </c>
       <c r="B60">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C60">
-        <v>0.425</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45505</v>
+        <v>45506</v>
       </c>
       <c r="B61">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45505</v>
+        <v>45506</v>
       </c>
       <c r="B62">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45505</v>
+        <v>45506</v>
       </c>
       <c r="B63">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45505</v>
+        <v>45506</v>
       </c>
       <c r="B64">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1801,7 +1801,7 @@
         <v>45506</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>45506</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>45506</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1843,10 +1843,10 @@
         <v>45506</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.298</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1857,10 +1857,10 @@
         <v>45506</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>0.657</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1871,10 +1871,10 @@
         <v>45506</v>
       </c>
       <c r="B70">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1.159</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1885,10 +1885,10 @@
         <v>45506</v>
       </c>
       <c r="B71">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>0.04</v>
+        <v>1.728</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1899,10 +1899,10 @@
         <v>45506</v>
       </c>
       <c r="B72">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>0.247</v>
+        <v>1.674</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1913,10 +1913,10 @@
         <v>45506</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>0.53</v>
+        <v>1.745</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1927,10 +1927,10 @@
         <v>45506</v>
       </c>
       <c r="B74">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C74">
-        <v>0.978</v>
+        <v>1.846</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1941,10 +1941,10 @@
         <v>45506</v>
       </c>
       <c r="B75">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C75">
-        <v>1.48</v>
+        <v>1.342</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1955,10 +1955,10 @@
         <v>45506</v>
       </c>
       <c r="B76">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C76">
-        <v>1.753</v>
+        <v>1.413</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1969,10 +1969,10 @@
         <v>45506</v>
       </c>
       <c r="B77">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C77">
-        <v>2.061</v>
+        <v>1.37</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1983,10 +1983,10 @@
         <v>45506</v>
       </c>
       <c r="B78">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C78">
-        <v>2.176</v>
+        <v>1.093</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1997,10 +1997,10 @@
         <v>45506</v>
       </c>
       <c r="B79">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C79">
-        <v>2.126</v>
+        <v>0.72</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2011,10 +2011,10 @@
         <v>45506</v>
       </c>
       <c r="B80">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C80">
-        <v>2.027</v>
+        <v>0.29</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2025,10 +2025,10 @@
         <v>45506</v>
       </c>
       <c r="B81">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C81">
-        <v>1.836</v>
+        <v>0.036</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2039,10 +2039,10 @@
         <v>45506</v>
       </c>
       <c r="B82">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C82">
-        <v>1.422</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2053,10 +2053,10 @@
         <v>45506</v>
       </c>
       <c r="B83">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C83">
-        <v>0.823</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2067,10 +2067,10 @@
         <v>45506</v>
       </c>
       <c r="B84">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C84">
-        <v>0.292</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="B85">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="B86">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="B87">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="B88">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2137,7 +2137,7 @@
         <v>45507</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2151,7 +2151,7 @@
         <v>45507</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2165,10 +2165,10 @@
         <v>45507</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2179,10 +2179,10 @@
         <v>45507</v>
       </c>
       <c r="B92">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.304</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2193,10 +2193,10 @@
         <v>45507</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>0.621</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2207,10 +2207,10 @@
         <v>45507</v>
       </c>
       <c r="B94">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1.091</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2221,10 +2221,10 @@
         <v>45507</v>
       </c>
       <c r="B95">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C95">
-        <v>0.046</v>
+        <v>1.599</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2235,10 +2235,10 @@
         <v>45507</v>
       </c>
       <c r="B96">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C96">
-        <v>0.364</v>
+        <v>1.713</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2249,10 +2249,10 @@
         <v>45507</v>
       </c>
       <c r="B97">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C97">
-        <v>0.895</v>
+        <v>1.671</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2263,10 +2263,10 @@
         <v>45507</v>
       </c>
       <c r="B98">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C98">
-        <v>1.486</v>
+        <v>1.414</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2277,10 +2277,10 @@
         <v>45507</v>
       </c>
       <c r="B99">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C99">
-        <v>1.625</v>
+        <v>1.137</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2291,10 +2291,10 @@
         <v>45507</v>
       </c>
       <c r="B100">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C100">
-        <v>1.884</v>
+        <v>1.133</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2305,10 +2305,10 @@
         <v>45507</v>
       </c>
       <c r="B101">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C101">
-        <v>1.878</v>
+        <v>1.085</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2319,10 +2319,10 @@
         <v>45507</v>
       </c>
       <c r="B102">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C102">
-        <v>1.824</v>
+        <v>0.86</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2333,10 +2333,10 @@
         <v>45507</v>
       </c>
       <c r="B103">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C103">
-        <v>1.767</v>
+        <v>0.556</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2347,10 +2347,10 @@
         <v>45507</v>
       </c>
       <c r="B104">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C104">
-        <v>1.637</v>
+        <v>0.258</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2361,10 +2361,10 @@
         <v>45507</v>
       </c>
       <c r="B105">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C105">
-        <v>1.52</v>
+        <v>0.038</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2375,10 +2375,10 @@
         <v>45507</v>
       </c>
       <c r="B106">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>1.126</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2389,10 +2389,10 @@
         <v>45507</v>
       </c>
       <c r="B107">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>0.789</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2403,10 +2403,10 @@
         <v>45507</v>
       </c>
       <c r="B108">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C108">
-        <v>0.292</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45507</v>
+        <v>45508</v>
       </c>
       <c r="B109">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C109">
-        <v>0.038</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45507</v>
+        <v>45508</v>
       </c>
       <c r="B110">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45507</v>
+        <v>45508</v>
       </c>
       <c r="B111">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45507</v>
+        <v>45508</v>
       </c>
       <c r="B112">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>45508</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2487,7 +2487,7 @@
         <v>45508</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2501,10 +2501,10 @@
         <v>45508</v>
       </c>
       <c r="B115">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2515,10 +2515,10 @@
         <v>45508</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2529,10 +2529,10 @@
         <v>45508</v>
       </c>
       <c r="B117">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>0.972</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2543,10 +2543,10 @@
         <v>45508</v>
       </c>
       <c r="B118">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>1.662</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2557,10 +2557,10 @@
         <v>45508</v>
       </c>
       <c r="B119">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C119">
-        <v>0.039</v>
+        <v>2.128</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2571,10 +2571,10 @@
         <v>45508</v>
       </c>
       <c r="B120">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C120">
-        <v>0.319</v>
+        <v>2.5</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2585,10 +2585,10 @@
         <v>45508</v>
       </c>
       <c r="B121">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C121">
-        <v>0.656</v>
+        <v>2.592</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2599,10 +2599,10 @@
         <v>45508</v>
       </c>
       <c r="B122">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C122">
-        <v>1.525</v>
+        <v>2.647</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2613,10 +2613,10 @@
         <v>45508</v>
       </c>
       <c r="B123">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C123">
-        <v>2.129</v>
+        <v>2.723</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2627,10 +2627,10 @@
         <v>45508</v>
       </c>
       <c r="B124">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C124">
-        <v>2.61</v>
+        <v>2.583</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2641,10 +2641,10 @@
         <v>45508</v>
       </c>
       <c r="B125">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C125">
-        <v>2.788</v>
+        <v>2.418</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2655,10 +2655,10 @@
         <v>45508</v>
       </c>
       <c r="B126">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C126">
-        <v>2.933</v>
+        <v>1.758</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2669,10 +2669,10 @@
         <v>45508</v>
       </c>
       <c r="B127">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C127">
-        <v>2.84</v>
+        <v>1.144</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2683,10 +2683,10 @@
         <v>45508</v>
       </c>
       <c r="B128">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C128">
-        <v>2.715</v>
+        <v>0.374</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2697,10 +2697,10 @@
         <v>45508</v>
       </c>
       <c r="B129">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C129">
-        <v>2.139</v>
+        <v>0.044</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2711,10 +2711,10 @@
         <v>45508</v>
       </c>
       <c r="B130">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C130">
-        <v>1.602</v>
+        <v>0</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2725,10 +2725,10 @@
         <v>45508</v>
       </c>
       <c r="B131">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C131">
-        <v>1.004</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2739,10 +2739,10 @@
         <v>45508</v>
       </c>
       <c r="B132">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C132">
-        <v>0.367</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45508</v>
+        <v>45509</v>
       </c>
       <c r="B133">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C133">
-        <v>0.041</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45508</v>
+        <v>45509</v>
       </c>
       <c r="B134">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45508</v>
+        <v>45509</v>
       </c>
       <c r="B135">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45508</v>
+        <v>45509</v>
       </c>
       <c r="B136">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2809,7 +2809,7 @@
         <v>45509</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2823,7 +2823,7 @@
         <v>45509</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2837,10 +2837,10 @@
         <v>45509</v>
       </c>
       <c r="B139">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>0.035</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2851,10 +2851,10 @@
         <v>45509</v>
       </c>
       <c r="B140">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>0.245</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2865,10 +2865,10 @@
         <v>45509</v>
       </c>
       <c r="B141">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>0.498</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2879,10 +2879,10 @@
         <v>45509</v>
       </c>
       <c r="B142">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>1.049</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2893,10 +2893,10 @@
         <v>45509</v>
       </c>
       <c r="B143">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C143">
-        <v>0.039</v>
+        <v>1.592</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2907,10 +2907,10 @@
         <v>45509</v>
       </c>
       <c r="B144">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C144">
-        <v>0.306</v>
+        <v>2.08</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2921,10 +2921,10 @@
         <v>45509</v>
       </c>
       <c r="B145">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C145">
-        <v>0.788</v>
+        <v>2.467</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2935,10 +2935,10 @@
         <v>45509</v>
       </c>
       <c r="B146">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C146">
-        <v>1.532</v>
+        <v>2.575</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2949,10 +2949,10 @@
         <v>45509</v>
       </c>
       <c r="B147">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C147">
-        <v>2.208</v>
+        <v>2.538</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2963,10 +2963,10 @@
         <v>45509</v>
       </c>
       <c r="B148">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C148">
-        <v>2.594</v>
+        <v>2.322</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2977,10 +2977,10 @@
         <v>45509</v>
       </c>
       <c r="B149">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C149">
-        <v>2.873</v>
+        <v>1.912</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2991,10 +2991,10 @@
         <v>45509</v>
       </c>
       <c r="B150">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C150">
-        <v>3.086</v>
+        <v>1.528</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3005,10 +3005,10 @@
         <v>45509</v>
       </c>
       <c r="B151">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C151">
-        <v>2.841</v>
+        <v>0.868</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3019,10 +3019,10 @@
         <v>45509</v>
       </c>
       <c r="B152">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C152">
-        <v>2.579</v>
+        <v>0.361</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3033,10 +3033,10 @@
         <v>45509</v>
       </c>
       <c r="B153">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C153">
-        <v>2.057</v>
+        <v>0.041</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3047,10 +3047,10 @@
         <v>45509</v>
       </c>
       <c r="B154">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C154">
-        <v>1.533</v>
+        <v>0</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3061,10 +3061,10 @@
         <v>45509</v>
       </c>
       <c r="B155">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C155">
-        <v>0.896</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3075,10 +3075,10 @@
         <v>45509</v>
       </c>
       <c r="B156">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C156">
-        <v>0.364</v>
+        <v>0</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45509</v>
+        <v>45510</v>
       </c>
       <c r="B157">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C157">
-        <v>0.041</v>
+        <v>0</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45509</v>
+        <v>45510</v>
       </c>
       <c r="B158">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45509</v>
+        <v>45510</v>
       </c>
       <c r="B159">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45509</v>
+        <v>45510</v>
       </c>
       <c r="B160">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3145,7 +3145,7 @@
         <v>45510</v>
       </c>
       <c r="B161">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3159,7 +3159,7 @@
         <v>45510</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3173,10 +3173,10 @@
         <v>45510</v>
       </c>
       <c r="B163">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3187,10 +3187,10 @@
         <v>45510</v>
       </c>
       <c r="B164">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>0.367</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3201,10 +3201,10 @@
         <v>45510</v>
       </c>
       <c r="B165">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>0.926</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3215,10 +3215,10 @@
         <v>45510</v>
       </c>
       <c r="B166">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>1.629</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3229,10 +3229,10 @@
         <v>45510</v>
       </c>
       <c r="B167">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C167">
-        <v>0.042</v>
+        <v>2.33</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3243,10 +3243,10 @@
         <v>45510</v>
       </c>
       <c r="B168">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C168">
-        <v>0.333</v>
+        <v>2.616</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3257,10 +3257,10 @@
         <v>45510</v>
       </c>
       <c r="B169">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C169">
-        <v>0.957</v>
+        <v>2.884</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3271,10 +3271,10 @@
         <v>45510</v>
       </c>
       <c r="B170">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C170">
-        <v>1.628</v>
+        <v>3.085</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
FIxing the converting from UTC to EET of the Transavia Consumption input dataset
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,444 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>30.07.202413</t>
-  </si>
-  <si>
-    <t>30.07.202414</t>
-  </si>
-  <si>
-    <t>30.07.202415</t>
-  </si>
-  <si>
-    <t>30.07.202416</t>
-  </si>
-  <si>
-    <t>30.07.202417</t>
-  </si>
-  <si>
-    <t>30.07.202418</t>
-  </si>
-  <si>
-    <t>30.07.202419</t>
-  </si>
-  <si>
-    <t>30.07.202420</t>
-  </si>
-  <si>
-    <t>30.07.202421</t>
-  </si>
-  <si>
-    <t>30.07.202422</t>
-  </si>
-  <si>
-    <t>30.07.202423</t>
-  </si>
-  <si>
-    <t>31.07.20240</t>
-  </si>
-  <si>
-    <t>31.07.20241</t>
-  </si>
-  <si>
-    <t>31.07.20242</t>
-  </si>
-  <si>
-    <t>31.07.20243</t>
-  </si>
-  <si>
-    <t>31.07.20244</t>
-  </si>
-  <si>
-    <t>31.07.20245</t>
-  </si>
-  <si>
-    <t>31.07.20246</t>
-  </si>
-  <si>
-    <t>31.07.20247</t>
-  </si>
-  <si>
-    <t>31.07.20248</t>
-  </si>
-  <si>
-    <t>31.07.20249</t>
-  </si>
-  <si>
-    <t>31.07.202410</t>
-  </si>
-  <si>
-    <t>31.07.202411</t>
-  </si>
-  <si>
-    <t>31.07.202412</t>
-  </si>
-  <si>
-    <t>31.07.202413</t>
-  </si>
-  <si>
-    <t>31.07.202414</t>
-  </si>
-  <si>
-    <t>31.07.202415</t>
-  </si>
-  <si>
-    <t>31.07.202416</t>
-  </si>
-  <si>
-    <t>31.07.202417</t>
-  </si>
-  <si>
-    <t>31.07.202418</t>
-  </si>
-  <si>
-    <t>31.07.202419</t>
-  </si>
-  <si>
-    <t>31.07.202420</t>
-  </si>
-  <si>
-    <t>31.07.202421</t>
-  </si>
-  <si>
-    <t>31.07.202422</t>
-  </si>
-  <si>
-    <t>31.07.202423</t>
-  </si>
-  <si>
-    <t>01.08.20240</t>
-  </si>
-  <si>
-    <t>01.08.20241</t>
-  </si>
-  <si>
-    <t>01.08.20242</t>
-  </si>
-  <si>
-    <t>01.08.20243</t>
-  </si>
-  <si>
-    <t>01.08.20244</t>
-  </si>
-  <si>
-    <t>01.08.20245</t>
-  </si>
-  <si>
-    <t>01.08.20246</t>
-  </si>
-  <si>
-    <t>01.08.20247</t>
-  </si>
-  <si>
-    <t>01.08.20248</t>
-  </si>
-  <si>
-    <t>01.08.20249</t>
-  </si>
-  <si>
-    <t>01.08.202410</t>
-  </si>
-  <si>
-    <t>01.08.202411</t>
-  </si>
-  <si>
-    <t>01.08.202412</t>
-  </si>
-  <si>
-    <t>01.08.202413</t>
-  </si>
-  <si>
-    <t>01.08.202414</t>
-  </si>
-  <si>
-    <t>01.08.202415</t>
-  </si>
-  <si>
-    <t>01.08.202416</t>
-  </si>
-  <si>
-    <t>01.08.202417</t>
-  </si>
-  <si>
-    <t>01.08.202418</t>
-  </si>
-  <si>
-    <t>01.08.202419</t>
-  </si>
-  <si>
-    <t>01.08.202420</t>
-  </si>
-  <si>
-    <t>01.08.202421</t>
-  </si>
-  <si>
-    <t>01.08.202422</t>
-  </si>
-  <si>
-    <t>01.08.202423</t>
-  </si>
-  <si>
-    <t>02.08.20240</t>
-  </si>
-  <si>
-    <t>02.08.20241</t>
-  </si>
-  <si>
-    <t>02.08.20242</t>
-  </si>
-  <si>
-    <t>02.08.20243</t>
-  </si>
-  <si>
-    <t>02.08.20244</t>
-  </si>
-  <si>
-    <t>02.08.20245</t>
-  </si>
-  <si>
-    <t>02.08.20246</t>
-  </si>
-  <si>
-    <t>02.08.20247</t>
-  </si>
-  <si>
-    <t>02.08.20248</t>
-  </si>
-  <si>
-    <t>02.08.20249</t>
-  </si>
-  <si>
-    <t>02.08.202410</t>
-  </si>
-  <si>
-    <t>02.08.202411</t>
-  </si>
-  <si>
-    <t>02.08.202412</t>
-  </si>
-  <si>
-    <t>02.08.202413</t>
-  </si>
-  <si>
-    <t>02.08.202414</t>
-  </si>
-  <si>
-    <t>02.08.202415</t>
-  </si>
-  <si>
-    <t>02.08.202416</t>
-  </si>
-  <si>
-    <t>02.08.202417</t>
-  </si>
-  <si>
-    <t>02.08.202418</t>
-  </si>
-  <si>
-    <t>02.08.202419</t>
-  </si>
-  <si>
-    <t>02.08.202420</t>
-  </si>
-  <si>
-    <t>02.08.202421</t>
-  </si>
-  <si>
-    <t>02.08.202422</t>
-  </si>
-  <si>
-    <t>02.08.202423</t>
-  </si>
-  <si>
-    <t>03.08.20240</t>
-  </si>
-  <si>
-    <t>03.08.20241</t>
-  </si>
-  <si>
-    <t>03.08.20242</t>
-  </si>
-  <si>
-    <t>03.08.20243</t>
-  </si>
-  <si>
-    <t>03.08.20244</t>
-  </si>
-  <si>
-    <t>03.08.20245</t>
-  </si>
-  <si>
-    <t>03.08.20246</t>
-  </si>
-  <si>
-    <t>03.08.20247</t>
-  </si>
-  <si>
-    <t>03.08.20248</t>
-  </si>
-  <si>
-    <t>03.08.20249</t>
-  </si>
-  <si>
-    <t>03.08.202410</t>
-  </si>
-  <si>
-    <t>03.08.202411</t>
-  </si>
-  <si>
-    <t>03.08.202412</t>
-  </si>
-  <si>
-    <t>03.08.202413</t>
-  </si>
-  <si>
-    <t>03.08.202414</t>
-  </si>
-  <si>
-    <t>03.08.202415</t>
-  </si>
-  <si>
-    <t>03.08.202416</t>
-  </si>
-  <si>
-    <t>03.08.202417</t>
-  </si>
-  <si>
-    <t>03.08.202418</t>
-  </si>
-  <si>
-    <t>03.08.202419</t>
-  </si>
-  <si>
-    <t>03.08.202420</t>
-  </si>
-  <si>
-    <t>03.08.202421</t>
-  </si>
-  <si>
-    <t>03.08.202422</t>
-  </si>
-  <si>
-    <t>03.08.202423</t>
-  </si>
-  <si>
-    <t>04.08.20240</t>
-  </si>
-  <si>
-    <t>04.08.20241</t>
-  </si>
-  <si>
-    <t>04.08.20242</t>
-  </si>
-  <si>
-    <t>04.08.20243</t>
-  </si>
-  <si>
-    <t>04.08.20244</t>
-  </si>
-  <si>
-    <t>04.08.20245</t>
-  </si>
-  <si>
-    <t>04.08.20246</t>
-  </si>
-  <si>
-    <t>04.08.20247</t>
-  </si>
-  <si>
-    <t>04.08.20248</t>
-  </si>
-  <si>
-    <t>04.08.20249</t>
-  </si>
-  <si>
-    <t>04.08.202410</t>
-  </si>
-  <si>
-    <t>04.08.202411</t>
-  </si>
-  <si>
-    <t>04.08.202412</t>
-  </si>
-  <si>
-    <t>04.08.202413</t>
-  </si>
-  <si>
-    <t>04.08.202414</t>
-  </si>
-  <si>
-    <t>04.08.202415</t>
-  </si>
-  <si>
-    <t>04.08.202416</t>
-  </si>
-  <si>
-    <t>04.08.202417</t>
-  </si>
-  <si>
-    <t>04.08.202418</t>
-  </si>
-  <si>
-    <t>04.08.202419</t>
-  </si>
-  <si>
-    <t>04.08.202420</t>
-  </si>
-  <si>
-    <t>04.08.202421</t>
-  </si>
-  <si>
-    <t>04.08.202422</t>
-  </si>
-  <si>
-    <t>04.08.202423</t>
-  </si>
-  <si>
-    <t>05.08.20240</t>
-  </si>
-  <si>
-    <t>05.08.20241</t>
-  </si>
-  <si>
-    <t>05.08.20242</t>
-  </si>
-  <si>
-    <t>05.08.20243</t>
-  </si>
-  <si>
-    <t>05.08.20244</t>
-  </si>
-  <si>
-    <t>05.08.20245</t>
-  </si>
-  <si>
-    <t>05.08.20246</t>
-  </si>
-  <si>
-    <t>05.08.20247</t>
-  </si>
-  <si>
-    <t>05.08.20248</t>
-  </si>
-  <si>
-    <t>05.08.20249</t>
-  </si>
-  <si>
-    <t>05.08.202410</t>
-  </si>
-  <si>
-    <t>05.08.202411</t>
-  </si>
-  <si>
-    <t>05.08.202412</t>
-  </si>
-  <si>
-    <t>05.08.202413</t>
-  </si>
-  <si>
-    <t>05.08.202414</t>
-  </si>
-  <si>
     <t>05.08.202415</t>
   </si>
   <si>
@@ -533,6 +95,444 @@
   </si>
   <si>
     <t>06.08.202413</t>
+  </si>
+  <si>
+    <t>06.08.202414</t>
+  </si>
+  <si>
+    <t>06.08.202415</t>
+  </si>
+  <si>
+    <t>06.08.202416</t>
+  </si>
+  <si>
+    <t>06.08.202417</t>
+  </si>
+  <si>
+    <t>06.08.202418</t>
+  </si>
+  <si>
+    <t>06.08.202419</t>
+  </si>
+  <si>
+    <t>06.08.202420</t>
+  </si>
+  <si>
+    <t>06.08.202421</t>
+  </si>
+  <si>
+    <t>06.08.202422</t>
+  </si>
+  <si>
+    <t>06.08.202423</t>
+  </si>
+  <si>
+    <t>07.08.20240</t>
+  </si>
+  <si>
+    <t>07.08.20241</t>
+  </si>
+  <si>
+    <t>07.08.20242</t>
+  </si>
+  <si>
+    <t>07.08.20243</t>
+  </si>
+  <si>
+    <t>07.08.20244</t>
+  </si>
+  <si>
+    <t>07.08.20245</t>
+  </si>
+  <si>
+    <t>07.08.20246</t>
+  </si>
+  <si>
+    <t>07.08.20247</t>
+  </si>
+  <si>
+    <t>07.08.20248</t>
+  </si>
+  <si>
+    <t>07.08.20249</t>
+  </si>
+  <si>
+    <t>07.08.202410</t>
+  </si>
+  <si>
+    <t>07.08.202411</t>
+  </si>
+  <si>
+    <t>07.08.202412</t>
+  </si>
+  <si>
+    <t>07.08.202413</t>
+  </si>
+  <si>
+    <t>07.08.202414</t>
+  </si>
+  <si>
+    <t>07.08.202415</t>
+  </si>
+  <si>
+    <t>07.08.202416</t>
+  </si>
+  <si>
+    <t>07.08.202417</t>
+  </si>
+  <si>
+    <t>07.08.202418</t>
+  </si>
+  <si>
+    <t>07.08.202419</t>
+  </si>
+  <si>
+    <t>07.08.202420</t>
+  </si>
+  <si>
+    <t>07.08.202421</t>
+  </si>
+  <si>
+    <t>07.08.202422</t>
+  </si>
+  <si>
+    <t>07.08.202423</t>
+  </si>
+  <si>
+    <t>08.08.20240</t>
+  </si>
+  <si>
+    <t>08.08.20241</t>
+  </si>
+  <si>
+    <t>08.08.20242</t>
+  </si>
+  <si>
+    <t>08.08.20243</t>
+  </si>
+  <si>
+    <t>08.08.20244</t>
+  </si>
+  <si>
+    <t>08.08.20245</t>
+  </si>
+  <si>
+    <t>08.08.20246</t>
+  </si>
+  <si>
+    <t>08.08.20247</t>
+  </si>
+  <si>
+    <t>08.08.20248</t>
+  </si>
+  <si>
+    <t>08.08.20249</t>
+  </si>
+  <si>
+    <t>08.08.202410</t>
+  </si>
+  <si>
+    <t>08.08.202411</t>
+  </si>
+  <si>
+    <t>08.08.202412</t>
+  </si>
+  <si>
+    <t>08.08.202413</t>
+  </si>
+  <si>
+    <t>08.08.202414</t>
+  </si>
+  <si>
+    <t>08.08.202415</t>
+  </si>
+  <si>
+    <t>08.08.202416</t>
+  </si>
+  <si>
+    <t>08.08.202417</t>
+  </si>
+  <si>
+    <t>08.08.202418</t>
+  </si>
+  <si>
+    <t>08.08.202419</t>
+  </si>
+  <si>
+    <t>08.08.202420</t>
+  </si>
+  <si>
+    <t>08.08.202421</t>
+  </si>
+  <si>
+    <t>08.08.202422</t>
+  </si>
+  <si>
+    <t>08.08.202423</t>
+  </si>
+  <si>
+    <t>09.08.20240</t>
+  </si>
+  <si>
+    <t>09.08.20241</t>
+  </si>
+  <si>
+    <t>09.08.20242</t>
+  </si>
+  <si>
+    <t>09.08.20243</t>
+  </si>
+  <si>
+    <t>09.08.20244</t>
+  </si>
+  <si>
+    <t>09.08.20245</t>
+  </si>
+  <si>
+    <t>09.08.20246</t>
+  </si>
+  <si>
+    <t>09.08.20247</t>
+  </si>
+  <si>
+    <t>09.08.20248</t>
+  </si>
+  <si>
+    <t>09.08.20249</t>
+  </si>
+  <si>
+    <t>09.08.202410</t>
+  </si>
+  <si>
+    <t>09.08.202411</t>
+  </si>
+  <si>
+    <t>09.08.202412</t>
+  </si>
+  <si>
+    <t>09.08.202413</t>
+  </si>
+  <si>
+    <t>09.08.202414</t>
+  </si>
+  <si>
+    <t>09.08.202415</t>
+  </si>
+  <si>
+    <t>09.08.202416</t>
+  </si>
+  <si>
+    <t>09.08.202417</t>
+  </si>
+  <si>
+    <t>09.08.202418</t>
+  </si>
+  <si>
+    <t>09.08.202419</t>
+  </si>
+  <si>
+    <t>09.08.202420</t>
+  </si>
+  <si>
+    <t>09.08.202421</t>
+  </si>
+  <si>
+    <t>09.08.202422</t>
+  </si>
+  <si>
+    <t>09.08.202423</t>
+  </si>
+  <si>
+    <t>10.08.20240</t>
+  </si>
+  <si>
+    <t>10.08.20241</t>
+  </si>
+  <si>
+    <t>10.08.20242</t>
+  </si>
+  <si>
+    <t>10.08.20243</t>
+  </si>
+  <si>
+    <t>10.08.20244</t>
+  </si>
+  <si>
+    <t>10.08.20245</t>
+  </si>
+  <si>
+    <t>10.08.20246</t>
+  </si>
+  <si>
+    <t>10.08.20247</t>
+  </si>
+  <si>
+    <t>10.08.20248</t>
+  </si>
+  <si>
+    <t>10.08.20249</t>
+  </si>
+  <si>
+    <t>10.08.202410</t>
+  </si>
+  <si>
+    <t>10.08.202411</t>
+  </si>
+  <si>
+    <t>10.08.202412</t>
+  </si>
+  <si>
+    <t>10.08.202413</t>
+  </si>
+  <si>
+    <t>10.08.202414</t>
+  </si>
+  <si>
+    <t>10.08.202415</t>
+  </si>
+  <si>
+    <t>10.08.202416</t>
+  </si>
+  <si>
+    <t>10.08.202417</t>
+  </si>
+  <si>
+    <t>10.08.202418</t>
+  </si>
+  <si>
+    <t>10.08.202419</t>
+  </si>
+  <si>
+    <t>10.08.202420</t>
+  </si>
+  <si>
+    <t>10.08.202421</t>
+  </si>
+  <si>
+    <t>10.08.202422</t>
+  </si>
+  <si>
+    <t>10.08.202423</t>
+  </si>
+  <si>
+    <t>11.08.20240</t>
+  </si>
+  <si>
+    <t>11.08.20241</t>
+  </si>
+  <si>
+    <t>11.08.20242</t>
+  </si>
+  <si>
+    <t>11.08.20243</t>
+  </si>
+  <si>
+    <t>11.08.20244</t>
+  </si>
+  <si>
+    <t>11.08.20245</t>
+  </si>
+  <si>
+    <t>11.08.20246</t>
+  </si>
+  <si>
+    <t>11.08.20247</t>
+  </si>
+  <si>
+    <t>11.08.20248</t>
+  </si>
+  <si>
+    <t>11.08.20249</t>
+  </si>
+  <si>
+    <t>11.08.202410</t>
+  </si>
+  <si>
+    <t>11.08.202411</t>
+  </si>
+  <si>
+    <t>11.08.202412</t>
+  </si>
+  <si>
+    <t>11.08.202413</t>
+  </si>
+  <si>
+    <t>11.08.202414</t>
+  </si>
+  <si>
+    <t>11.08.202415</t>
+  </si>
+  <si>
+    <t>11.08.202416</t>
+  </si>
+  <si>
+    <t>11.08.202417</t>
+  </si>
+  <si>
+    <t>11.08.202418</t>
+  </si>
+  <si>
+    <t>11.08.202419</t>
+  </si>
+  <si>
+    <t>11.08.202420</t>
+  </si>
+  <si>
+    <t>11.08.202421</t>
+  </si>
+  <si>
+    <t>11.08.202422</t>
+  </si>
+  <si>
+    <t>11.08.202423</t>
+  </si>
+  <si>
+    <t>12.08.20240</t>
+  </si>
+  <si>
+    <t>12.08.20241</t>
+  </si>
+  <si>
+    <t>12.08.20242</t>
+  </si>
+  <si>
+    <t>12.08.20243</t>
+  </si>
+  <si>
+    <t>12.08.20244</t>
+  </si>
+  <si>
+    <t>12.08.20245</t>
+  </si>
+  <si>
+    <t>12.08.20246</t>
+  </si>
+  <si>
+    <t>12.08.20247</t>
+  </si>
+  <si>
+    <t>12.08.20248</t>
+  </si>
+  <si>
+    <t>12.08.20249</t>
+  </si>
+  <si>
+    <t>12.08.202410</t>
+  </si>
+  <si>
+    <t>12.08.202411</t>
+  </si>
+  <si>
+    <t>12.08.202412</t>
+  </si>
+  <si>
+    <t>12.08.202413</t>
+  </si>
+  <si>
+    <t>12.08.202414</t>
+  </si>
+  <si>
+    <t>12.08.202415</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>2.944</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>2.446</v>
+        <v>0.835</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>1.868</v>
+        <v>0.432</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>1.203</v>
+        <v>0.115</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8">
-        <v>0.465</v>
+        <v>0.022</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>0.065</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,10 +1028,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45503</v>
+        <v>45509</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45503</v>
+        <v>45510</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1056,10 +1056,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45503</v>
+        <v>45510</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.035</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>0.066</v>
+        <v>0.266</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>0.365</v>
+        <v>0.837</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>1.002</v>
+        <v>1.249</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>1.756</v>
+        <v>1.487</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>2.404</v>
+        <v>1.898</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>2.71</v>
+        <v>2.319</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C25">
-        <v>2.936</v>
+        <v>2.187</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>3.139</v>
+        <v>2.025</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>3.035</v>
+        <v>1.792</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>2.893</v>
+        <v>1.676</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C29">
-        <v>2.345</v>
+        <v>1.321</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B30">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C30">
-        <v>1.83</v>
+        <v>0.671</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31">
-        <v>1.168</v>
+        <v>0.259</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B32">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C32">
-        <v>0.456</v>
+        <v>0.041</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C33">
-        <v>0.063</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45504</v>
+        <v>45510</v>
       </c>
       <c r="B34">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45504</v>
+        <v>45511</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45504</v>
+        <v>45511</v>
       </c>
       <c r="B36">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>0.046</v>
+        <v>0.35</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>0.36</v>
+        <v>1.009</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>0.957</v>
+        <v>1.745</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>1.599</v>
+        <v>2.452</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>2.335</v>
+        <v>2.928</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>2.437</v>
+        <v>3.153</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>2.915</v>
+        <v>3.124</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B50">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>3.086</v>
+        <v>3.048</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B51">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>3.085</v>
+        <v>2.721</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B52">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>2.919</v>
+        <v>2.3</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B53">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C53">
-        <v>2.246</v>
+        <v>1.497</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B54">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C54">
-        <v>1.711</v>
+        <v>0.727</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B55">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>0.992</v>
+        <v>0.245</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C56">
-        <v>0.368</v>
+        <v>0.041</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C57">
-        <v>0.041</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,10 +1700,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="B58">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45505</v>
+        <v>45512</v>
       </c>
       <c r="B59">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45505</v>
+        <v>45512</v>
       </c>
       <c r="B60">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C67">
-        <v>0.042</v>
+        <v>0.34</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C68">
-        <v>0.298</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>0.657</v>
+        <v>1.658</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C70">
-        <v>1.159</v>
+        <v>2.391</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B71">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C71">
-        <v>1.728</v>
+        <v>2.839</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B72">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C72">
-        <v>1.674</v>
+        <v>3.054</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C73">
-        <v>1.745</v>
+        <v>3.088</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B74">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C74">
-        <v>1.846</v>
+        <v>2.993</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B75">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C75">
-        <v>1.342</v>
+        <v>2.677</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B76">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C76">
-        <v>1.413</v>
+        <v>2.11</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B77">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C77">
-        <v>1.37</v>
+        <v>1.355</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B78">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C78">
-        <v>1.093</v>
+        <v>0.66</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B79">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C79">
-        <v>0.72</v>
+        <v>0.274</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B80">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C80">
-        <v>0.29</v>
+        <v>0.036</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B81">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C81">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,10 +2036,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="B82">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45506</v>
+        <v>45513</v>
       </c>
       <c r="B83">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2064,10 +2064,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45506</v>
+        <v>45513</v>
       </c>
       <c r="B84">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.041</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B91">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C91">
-        <v>0.046</v>
+        <v>0.324</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B92">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C92">
-        <v>0.304</v>
+        <v>0.96</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B93">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C93">
-        <v>0.621</v>
+        <v>1.666</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B94">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C94">
-        <v>1.091</v>
+        <v>2.261</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B95">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C95">
-        <v>1.599</v>
+        <v>2.797</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B96">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C96">
-        <v>1.713</v>
+        <v>3.031</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B97">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C97">
-        <v>1.671</v>
+        <v>2.723</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B98">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C98">
-        <v>1.414</v>
+        <v>2.266</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B99">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C99">
-        <v>1.137</v>
+        <v>2.143</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B100">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C100">
-        <v>1.133</v>
+        <v>1.863</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B101">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C101">
-        <v>1.085</v>
+        <v>1.216</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B102">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C102">
-        <v>0.86</v>
+        <v>0.654</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B103">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C103">
-        <v>0.556</v>
+        <v>0.272</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B104">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C104">
-        <v>0.258</v>
+        <v>0.034</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C105">
-        <v>0.038</v>
+        <v>0</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,10 +2372,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45507</v>
+        <v>45513</v>
       </c>
       <c r="B106">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45507</v>
+        <v>45514</v>
       </c>
       <c r="B107">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45507</v>
+        <v>45514</v>
       </c>
       <c r="B108">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B113">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B114">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>0.034</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B115">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C115">
-        <v>0.046</v>
+        <v>0.303</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B116">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C116">
-        <v>0.35</v>
+        <v>0.948</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B117">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C117">
-        <v>0.972</v>
+        <v>1.666</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B118">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C118">
-        <v>1.662</v>
+        <v>2.261</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B119">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C119">
-        <v>2.128</v>
+        <v>2.778</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B120">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C120">
-        <v>2.5</v>
+        <v>2.79</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B121">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C121">
-        <v>2.592</v>
+        <v>2.954</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B122">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C122">
-        <v>2.647</v>
+        <v>2.786</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B123">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C123">
-        <v>2.723</v>
+        <v>2.468</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B124">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C124">
-        <v>2.583</v>
+        <v>2.086</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B125">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C125">
-        <v>2.418</v>
+        <v>1.42</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B126">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C126">
-        <v>1.758</v>
+        <v>0.71</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B127">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C127">
-        <v>1.144</v>
+        <v>0.239</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B128">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C128">
-        <v>0.374</v>
+        <v>0.034</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B129">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C129">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45508</v>
+        <v>45514</v>
       </c>
       <c r="B130">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45508</v>
+        <v>45515</v>
       </c>
       <c r="B131">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45508</v>
+        <v>45515</v>
       </c>
       <c r="B132">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B136">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B137">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B138">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B139">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C139">
-        <v>0.035</v>
+        <v>0.282</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B140">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C140">
-        <v>0.245</v>
+        <v>0.947</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B141">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C141">
-        <v>0.498</v>
+        <v>1.67</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B142">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C142">
-        <v>1.049</v>
+        <v>2.265</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B143">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C143">
-        <v>1.592</v>
+        <v>2.818</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B144">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C144">
-        <v>2.08</v>
+        <v>3.027</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B145">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C145">
-        <v>2.467</v>
+        <v>3.059</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B146">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C146">
-        <v>2.575</v>
+        <v>2.974</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B147">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C147">
-        <v>2.538</v>
+        <v>2.671</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B148">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C148">
-        <v>2.322</v>
+        <v>2.154</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B149">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C149">
-        <v>1.912</v>
+        <v>1.518</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B150">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C150">
-        <v>1.528</v>
+        <v>0.738</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B151">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C151">
-        <v>0.868</v>
+        <v>0.218</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B152">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C152">
-        <v>0.361</v>
+        <v>0.034</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B153">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C153">
-        <v>0.041</v>
+        <v>0</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,10 +3044,10 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45509</v>
+        <v>45515</v>
       </c>
       <c r="B154">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -3058,10 +3058,10 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45509</v>
+        <v>45516</v>
       </c>
       <c r="B155">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45509</v>
+        <v>45516</v>
       </c>
       <c r="B156">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B157">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B158">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B159">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B160">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B161">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B162">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B163">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C163">
-        <v>0.042</v>
+        <v>0.337</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B164">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C164">
-        <v>0.367</v>
+        <v>0.96</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B165">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C165">
-        <v>0.926</v>
+        <v>1.667</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B166">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C166">
-        <v>1.629</v>
+        <v>2.252</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B167">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C167">
-        <v>2.33</v>
+        <v>2.796</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B168">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C168">
-        <v>2.616</v>
+        <v>3.045</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B169">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C169">
-        <v>2.884</v>
+        <v>3.085</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45510</v>
+        <v>45516</v>
       </c>
       <c r="B170">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C170">
-        <v>3.085</v>
+        <v>2.981</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Storing the indisponibilities for each asset
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>05.08.202415</t>
-  </si>
-  <si>
-    <t>05.08.202416</t>
-  </si>
-  <si>
-    <t>05.08.202417</t>
-  </si>
-  <si>
-    <t>05.08.202418</t>
-  </si>
-  <si>
-    <t>05.08.202419</t>
-  </si>
-  <si>
-    <t>05.08.202420</t>
-  </si>
-  <si>
-    <t>05.08.202421</t>
-  </si>
-  <si>
-    <t>05.08.202422</t>
-  </si>
-  <si>
-    <t>05.08.202423</t>
-  </si>
-  <si>
-    <t>06.08.20240</t>
-  </si>
-  <si>
-    <t>06.08.20241</t>
-  </si>
-  <si>
-    <t>06.08.20242</t>
-  </si>
-  <si>
-    <t>06.08.20243</t>
-  </si>
-  <si>
-    <t>06.08.20244</t>
-  </si>
-  <si>
-    <t>06.08.20245</t>
-  </si>
-  <si>
-    <t>06.08.20246</t>
-  </si>
-  <si>
-    <t>06.08.20247</t>
-  </si>
-  <si>
-    <t>06.08.20248</t>
-  </si>
-  <si>
-    <t>06.08.20249</t>
-  </si>
-  <si>
-    <t>06.08.202410</t>
-  </si>
-  <si>
-    <t>06.08.202411</t>
-  </si>
-  <si>
-    <t>06.08.202412</t>
-  </si>
-  <si>
-    <t>06.08.202413</t>
-  </si>
-  <si>
-    <t>06.08.202414</t>
-  </si>
-  <si>
-    <t>06.08.202415</t>
-  </si>
-  <si>
-    <t>06.08.202416</t>
-  </si>
-  <si>
-    <t>06.08.202417</t>
-  </si>
-  <si>
-    <t>06.08.202418</t>
-  </si>
-  <si>
-    <t>06.08.202419</t>
-  </si>
-  <si>
-    <t>06.08.202420</t>
-  </si>
-  <si>
-    <t>06.08.202421</t>
-  </si>
-  <si>
-    <t>06.08.202422</t>
-  </si>
-  <si>
-    <t>06.08.202423</t>
-  </si>
-  <si>
-    <t>07.08.20240</t>
-  </si>
-  <si>
-    <t>07.08.20241</t>
-  </si>
-  <si>
-    <t>07.08.20242</t>
-  </si>
-  <si>
-    <t>07.08.20243</t>
-  </si>
-  <si>
-    <t>07.08.20244</t>
-  </si>
-  <si>
-    <t>07.08.20245</t>
-  </si>
-  <si>
-    <t>07.08.20246</t>
-  </si>
-  <si>
-    <t>07.08.20247</t>
-  </si>
-  <si>
-    <t>07.08.20248</t>
-  </si>
-  <si>
-    <t>07.08.20249</t>
-  </si>
-  <si>
-    <t>07.08.202410</t>
-  </si>
-  <si>
-    <t>07.08.202411</t>
-  </si>
-  <si>
-    <t>07.08.202412</t>
-  </si>
-  <si>
-    <t>07.08.202413</t>
-  </si>
-  <si>
-    <t>07.08.202414</t>
-  </si>
-  <si>
-    <t>07.08.202415</t>
-  </si>
-  <si>
-    <t>07.08.202416</t>
-  </si>
-  <si>
-    <t>07.08.202417</t>
-  </si>
-  <si>
-    <t>07.08.202418</t>
-  </si>
-  <si>
-    <t>07.08.202419</t>
-  </si>
-  <si>
-    <t>07.08.202420</t>
-  </si>
-  <si>
-    <t>07.08.202421</t>
-  </si>
-  <si>
-    <t>07.08.202422</t>
-  </si>
-  <si>
-    <t>07.08.202423</t>
-  </si>
-  <si>
-    <t>08.08.20240</t>
-  </si>
-  <si>
-    <t>08.08.20241</t>
-  </si>
-  <si>
-    <t>08.08.20242</t>
-  </si>
-  <si>
-    <t>08.08.20243</t>
-  </si>
-  <si>
-    <t>08.08.20244</t>
-  </si>
-  <si>
-    <t>08.08.20245</t>
-  </si>
-  <si>
-    <t>08.08.20246</t>
-  </si>
-  <si>
-    <t>08.08.20247</t>
-  </si>
-  <si>
-    <t>08.08.20248</t>
-  </si>
-  <si>
-    <t>08.08.20249</t>
-  </si>
-  <si>
-    <t>08.08.202410</t>
-  </si>
-  <si>
-    <t>08.08.202411</t>
-  </si>
-  <si>
-    <t>08.08.202412</t>
-  </si>
-  <si>
-    <t>08.08.202413</t>
-  </si>
-  <si>
-    <t>08.08.202414</t>
-  </si>
-  <si>
-    <t>08.08.202415</t>
-  </si>
-  <si>
-    <t>08.08.202416</t>
-  </si>
-  <si>
-    <t>08.08.202417</t>
-  </si>
-  <si>
-    <t>08.08.202418</t>
-  </si>
-  <si>
-    <t>08.08.202419</t>
-  </si>
-  <si>
-    <t>08.08.202420</t>
-  </si>
-  <si>
-    <t>08.08.202421</t>
-  </si>
-  <si>
-    <t>08.08.202422</t>
-  </si>
-  <si>
-    <t>08.08.202423</t>
-  </si>
-  <si>
-    <t>09.08.20240</t>
-  </si>
-  <si>
-    <t>09.08.20241</t>
-  </si>
-  <si>
-    <t>09.08.20242</t>
-  </si>
-  <si>
-    <t>09.08.20243</t>
-  </si>
-  <si>
-    <t>09.08.20244</t>
-  </si>
-  <si>
-    <t>09.08.20245</t>
-  </si>
-  <si>
-    <t>09.08.20246</t>
-  </si>
-  <si>
-    <t>09.08.20247</t>
-  </si>
-  <si>
-    <t>09.08.20248</t>
-  </si>
-  <si>
-    <t>09.08.20249</t>
-  </si>
-  <si>
-    <t>09.08.202410</t>
-  </si>
-  <si>
-    <t>09.08.202411</t>
-  </si>
-  <si>
-    <t>09.08.202412</t>
-  </si>
-  <si>
-    <t>09.08.202413</t>
-  </si>
-  <si>
-    <t>09.08.202414</t>
-  </si>
-  <si>
-    <t>09.08.202415</t>
-  </si>
-  <si>
-    <t>09.08.202416</t>
-  </si>
-  <si>
-    <t>09.08.202417</t>
-  </si>
-  <si>
-    <t>09.08.202418</t>
-  </si>
-  <si>
-    <t>09.08.202419</t>
-  </si>
-  <si>
-    <t>09.08.202420</t>
-  </si>
-  <si>
-    <t>09.08.202421</t>
-  </si>
-  <si>
-    <t>09.08.202422</t>
-  </si>
-  <si>
-    <t>09.08.202423</t>
-  </si>
-  <si>
-    <t>10.08.20240</t>
-  </si>
-  <si>
-    <t>10.08.20241</t>
-  </si>
-  <si>
-    <t>10.08.20242</t>
-  </si>
-  <si>
-    <t>10.08.20243</t>
-  </si>
-  <si>
-    <t>10.08.20244</t>
-  </si>
-  <si>
-    <t>10.08.20245</t>
-  </si>
-  <si>
-    <t>10.08.20246</t>
-  </si>
-  <si>
-    <t>10.08.20247</t>
-  </si>
-  <si>
-    <t>10.08.20248</t>
-  </si>
-  <si>
-    <t>10.08.20249</t>
-  </si>
-  <si>
-    <t>10.08.202410</t>
-  </si>
-  <si>
-    <t>10.08.202411</t>
-  </si>
-  <si>
-    <t>10.08.202412</t>
-  </si>
-  <si>
-    <t>10.08.202413</t>
-  </si>
-  <si>
-    <t>10.08.202414</t>
-  </si>
-  <si>
-    <t>10.08.202415</t>
-  </si>
-  <si>
-    <t>10.08.202416</t>
-  </si>
-  <si>
-    <t>10.08.202417</t>
-  </si>
-  <si>
-    <t>10.08.202418</t>
-  </si>
-  <si>
-    <t>10.08.202419</t>
-  </si>
-  <si>
-    <t>10.08.202420</t>
-  </si>
-  <si>
-    <t>10.08.202421</t>
-  </si>
-  <si>
-    <t>10.08.202422</t>
-  </si>
-  <si>
-    <t>10.08.202423</t>
-  </si>
-  <si>
-    <t>11.08.20240</t>
-  </si>
-  <si>
-    <t>11.08.20241</t>
-  </si>
-  <si>
-    <t>11.08.20242</t>
-  </si>
-  <si>
-    <t>11.08.20243</t>
-  </si>
-  <si>
-    <t>11.08.20244</t>
-  </si>
-  <si>
-    <t>11.08.20245</t>
-  </si>
-  <si>
-    <t>11.08.20246</t>
-  </si>
-  <si>
-    <t>11.08.20247</t>
-  </si>
-  <si>
-    <t>11.08.20248</t>
-  </si>
-  <si>
-    <t>11.08.20249</t>
-  </si>
-  <si>
-    <t>11.08.202410</t>
-  </si>
-  <si>
-    <t>11.08.202411</t>
-  </si>
-  <si>
-    <t>11.08.202412</t>
-  </si>
-  <si>
-    <t>11.08.202413</t>
-  </si>
-  <si>
-    <t>11.08.202414</t>
-  </si>
-  <si>
-    <t>11.08.202415</t>
-  </si>
-  <si>
-    <t>11.08.202416</t>
-  </si>
-  <si>
-    <t>11.08.202417</t>
-  </si>
-  <si>
-    <t>11.08.202418</t>
-  </si>
-  <si>
-    <t>11.08.202419</t>
-  </si>
-  <si>
-    <t>11.08.202420</t>
-  </si>
-  <si>
-    <t>11.08.202421</t>
-  </si>
-  <si>
-    <t>11.08.202422</t>
-  </si>
-  <si>
-    <t>11.08.202423</t>
-  </si>
-  <si>
-    <t>12.08.20240</t>
-  </si>
-  <si>
-    <t>12.08.20241</t>
-  </si>
-  <si>
-    <t>12.08.20242</t>
-  </si>
-  <si>
-    <t>12.08.20243</t>
-  </si>
-  <si>
-    <t>12.08.20244</t>
-  </si>
-  <si>
-    <t>12.08.20245</t>
-  </si>
-  <si>
-    <t>12.08.20246</t>
-  </si>
-  <si>
-    <t>12.08.20247</t>
-  </si>
-  <si>
-    <t>12.08.20248</t>
-  </si>
-  <si>
-    <t>12.08.20249</t>
-  </si>
-  <si>
-    <t>12.08.202410</t>
-  </si>
-  <si>
-    <t>12.08.202411</t>
-  </si>
-  <si>
-    <t>12.08.202412</t>
-  </si>
-  <si>
-    <t>12.08.202413</t>
-  </si>
-  <si>
-    <t>12.08.202414</t>
-  </si>
-  <si>
-    <t>12.08.202415</t>
+    <t>21.08.202411</t>
+  </si>
+  <si>
+    <t>21.08.202412</t>
+  </si>
+  <si>
+    <t>21.08.202413</t>
+  </si>
+  <si>
+    <t>21.08.202414</t>
+  </si>
+  <si>
+    <t>21.08.202415</t>
+  </si>
+  <si>
+    <t>21.08.202416</t>
+  </si>
+  <si>
+    <t>21.08.202417</t>
+  </si>
+  <si>
+    <t>21.08.202418</t>
+  </si>
+  <si>
+    <t>21.08.202419</t>
+  </si>
+  <si>
+    <t>21.08.202420</t>
+  </si>
+  <si>
+    <t>21.08.202421</t>
+  </si>
+  <si>
+    <t>21.08.202422</t>
+  </si>
+  <si>
+    <t>21.08.202423</t>
+  </si>
+  <si>
+    <t>21.08.202424</t>
+  </si>
+  <si>
+    <t>22.08.20241</t>
+  </si>
+  <si>
+    <t>22.08.20242</t>
+  </si>
+  <si>
+    <t>22.08.20243</t>
+  </si>
+  <si>
+    <t>22.08.20244</t>
+  </si>
+  <si>
+    <t>22.08.20245</t>
+  </si>
+  <si>
+    <t>22.08.20246</t>
+  </si>
+  <si>
+    <t>22.08.20247</t>
+  </si>
+  <si>
+    <t>22.08.20248</t>
+  </si>
+  <si>
+    <t>22.08.20249</t>
+  </si>
+  <si>
+    <t>22.08.202410</t>
+  </si>
+  <si>
+    <t>22.08.202411</t>
+  </si>
+  <si>
+    <t>22.08.202412</t>
+  </si>
+  <si>
+    <t>22.08.202413</t>
+  </si>
+  <si>
+    <t>22.08.202414</t>
+  </si>
+  <si>
+    <t>22.08.202415</t>
+  </si>
+  <si>
+    <t>22.08.202416</t>
+  </si>
+  <si>
+    <t>22.08.202417</t>
+  </si>
+  <si>
+    <t>22.08.202418</t>
+  </si>
+  <si>
+    <t>22.08.202419</t>
+  </si>
+  <si>
+    <t>22.08.202420</t>
+  </si>
+  <si>
+    <t>22.08.202421</t>
+  </si>
+  <si>
+    <t>22.08.202422</t>
+  </si>
+  <si>
+    <t>22.08.202423</t>
+  </si>
+  <si>
+    <t>22.08.202424</t>
+  </si>
+  <si>
+    <t>23.08.20241</t>
+  </si>
+  <si>
+    <t>23.08.20242</t>
+  </si>
+  <si>
+    <t>23.08.20243</t>
+  </si>
+  <si>
+    <t>23.08.20244</t>
+  </si>
+  <si>
+    <t>23.08.20245</t>
+  </si>
+  <si>
+    <t>23.08.20246</t>
+  </si>
+  <si>
+    <t>23.08.20247</t>
+  </si>
+  <si>
+    <t>23.08.20248</t>
+  </si>
+  <si>
+    <t>23.08.20249</t>
+  </si>
+  <si>
+    <t>23.08.202410</t>
+  </si>
+  <si>
+    <t>23.08.202411</t>
+  </si>
+  <si>
+    <t>23.08.202412</t>
+  </si>
+  <si>
+    <t>23.08.202413</t>
+  </si>
+  <si>
+    <t>23.08.202414</t>
+  </si>
+  <si>
+    <t>23.08.202415</t>
+  </si>
+  <si>
+    <t>23.08.202416</t>
+  </si>
+  <si>
+    <t>23.08.202417</t>
+  </si>
+  <si>
+    <t>23.08.202418</t>
+  </si>
+  <si>
+    <t>23.08.202419</t>
+  </si>
+  <si>
+    <t>23.08.202420</t>
+  </si>
+  <si>
+    <t>23.08.202421</t>
+  </si>
+  <si>
+    <t>23.08.202422</t>
+  </si>
+  <si>
+    <t>23.08.202423</t>
+  </si>
+  <si>
+    <t>23.08.202424</t>
+  </si>
+  <si>
+    <t>24.08.20241</t>
+  </si>
+  <si>
+    <t>24.08.20242</t>
+  </si>
+  <si>
+    <t>24.08.20243</t>
+  </si>
+  <si>
+    <t>24.08.20244</t>
+  </si>
+  <si>
+    <t>24.08.20245</t>
+  </si>
+  <si>
+    <t>24.08.20246</t>
+  </si>
+  <si>
+    <t>24.08.20247</t>
+  </si>
+  <si>
+    <t>24.08.20248</t>
+  </si>
+  <si>
+    <t>24.08.20249</t>
+  </si>
+  <si>
+    <t>24.08.202410</t>
+  </si>
+  <si>
+    <t>24.08.202411</t>
+  </si>
+  <si>
+    <t>24.08.202412</t>
+  </si>
+  <si>
+    <t>24.08.202413</t>
+  </si>
+  <si>
+    <t>24.08.202414</t>
+  </si>
+  <si>
+    <t>24.08.202415</t>
+  </si>
+  <si>
+    <t>24.08.202416</t>
+  </si>
+  <si>
+    <t>24.08.202417</t>
+  </si>
+  <si>
+    <t>24.08.202418</t>
+  </si>
+  <si>
+    <t>24.08.202419</t>
+  </si>
+  <si>
+    <t>24.08.202420</t>
+  </si>
+  <si>
+    <t>24.08.202421</t>
+  </si>
+  <si>
+    <t>24.08.202422</t>
+  </si>
+  <si>
+    <t>24.08.202423</t>
+  </si>
+  <si>
+    <t>24.08.202424</t>
+  </si>
+  <si>
+    <t>25.08.20241</t>
+  </si>
+  <si>
+    <t>25.08.20242</t>
+  </si>
+  <si>
+    <t>25.08.20243</t>
+  </si>
+  <si>
+    <t>25.08.20244</t>
+  </si>
+  <si>
+    <t>25.08.20245</t>
+  </si>
+  <si>
+    <t>25.08.20246</t>
+  </si>
+  <si>
+    <t>25.08.20247</t>
+  </si>
+  <si>
+    <t>25.08.20248</t>
+  </si>
+  <si>
+    <t>25.08.20249</t>
+  </si>
+  <si>
+    <t>25.08.202410</t>
+  </si>
+  <si>
+    <t>25.08.202411</t>
+  </si>
+  <si>
+    <t>25.08.202412</t>
+  </si>
+  <si>
+    <t>25.08.202413</t>
+  </si>
+  <si>
+    <t>25.08.202414</t>
+  </si>
+  <si>
+    <t>25.08.202415</t>
+  </si>
+  <si>
+    <t>25.08.202416</t>
+  </si>
+  <si>
+    <t>25.08.202417</t>
+  </si>
+  <si>
+    <t>25.08.202418</t>
+  </si>
+  <si>
+    <t>25.08.202419</t>
+  </si>
+  <si>
+    <t>25.08.202420</t>
+  </si>
+  <si>
+    <t>25.08.202421</t>
+  </si>
+  <si>
+    <t>25.08.202422</t>
+  </si>
+  <si>
+    <t>25.08.202423</t>
+  </si>
+  <si>
+    <t>25.08.202424</t>
+  </si>
+  <si>
+    <t>26.08.20241</t>
+  </si>
+  <si>
+    <t>26.08.20242</t>
+  </si>
+  <si>
+    <t>26.08.20243</t>
+  </si>
+  <si>
+    <t>26.08.20244</t>
+  </si>
+  <si>
+    <t>26.08.20245</t>
+  </si>
+  <si>
+    <t>26.08.20246</t>
+  </si>
+  <si>
+    <t>26.08.20247</t>
+  </si>
+  <si>
+    <t>26.08.20248</t>
+  </si>
+  <si>
+    <t>26.08.20249</t>
+  </si>
+  <si>
+    <t>26.08.202410</t>
+  </si>
+  <si>
+    <t>26.08.202411</t>
+  </si>
+  <si>
+    <t>26.08.202412</t>
+  </si>
+  <si>
+    <t>26.08.202413</t>
+  </si>
+  <si>
+    <t>26.08.202414</t>
+  </si>
+  <si>
+    <t>26.08.202415</t>
+  </si>
+  <si>
+    <t>26.08.202416</t>
+  </si>
+  <si>
+    <t>26.08.202417</t>
+  </si>
+  <si>
+    <t>26.08.202418</t>
+  </si>
+  <si>
+    <t>26.08.202419</t>
+  </si>
+  <si>
+    <t>26.08.202420</t>
+  </si>
+  <si>
+    <t>26.08.202421</t>
+  </si>
+  <si>
+    <t>26.08.202422</t>
+  </si>
+  <si>
+    <t>26.08.202423</t>
+  </si>
+  <si>
+    <t>26.08.202424</t>
+  </si>
+  <si>
+    <t>27.08.20241</t>
+  </si>
+  <si>
+    <t>27.08.20242</t>
+  </si>
+  <si>
+    <t>27.08.20243</t>
+  </si>
+  <si>
+    <t>27.08.20244</t>
+  </si>
+  <si>
+    <t>27.08.20245</t>
+  </si>
+  <si>
+    <t>27.08.20246</t>
+  </si>
+  <si>
+    <t>27.08.20247</t>
+  </si>
+  <si>
+    <t>27.08.20248</t>
+  </si>
+  <si>
+    <t>27.08.20249</t>
+  </si>
+  <si>
+    <t>27.08.202410</t>
+  </si>
+  <si>
+    <t>27.08.202411</t>
+  </si>
+  <si>
+    <t>27.08.202412</t>
+  </si>
+  <si>
+    <t>27.08.202413</t>
+  </si>
+  <si>
+    <t>27.08.202414</t>
+  </si>
+  <si>
+    <t>27.08.202415</t>
+  </si>
+  <si>
+    <t>27.08.202416</t>
+  </si>
+  <si>
+    <t>27.08.202417</t>
+  </si>
+  <si>
+    <t>27.08.202418</t>
+  </si>
+  <si>
+    <t>27.08.202419</t>
+  </si>
+  <si>
+    <t>27.08.202420</t>
+  </si>
+  <si>
+    <t>27.08.202421</t>
+  </si>
+  <si>
+    <t>27.08.202422</t>
+  </si>
+  <si>
+    <t>27.08.202423</t>
+  </si>
+  <si>
+    <t>27.08.202424</t>
+  </si>
+  <si>
+    <t>28.08.20241</t>
+  </si>
+  <si>
+    <t>28.08.20242</t>
+  </si>
+  <si>
+    <t>28.08.20243</t>
+  </si>
+  <si>
+    <t>28.08.20244</t>
+  </si>
+  <si>
+    <t>28.08.20245</t>
+  </si>
+  <si>
+    <t>28.08.20246</t>
+  </si>
+  <si>
+    <t>28.08.20247</t>
+  </si>
+  <si>
+    <t>28.08.20248</t>
+  </si>
+  <si>
+    <t>28.08.20249</t>
+  </si>
+  <si>
+    <t>28.08.202410</t>
+  </si>
+  <si>
+    <t>28.08.202411</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3.019</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>0.835</v>
+        <v>3.048</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>0.432</v>
+        <v>2.963</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>0.115</v>
+        <v>2.554</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>0.022</v>
+        <v>2.151</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1.45</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45509</v>
+        <v>45525</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.652</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45510</v>
+        <v>45525</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,10 +1056,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45510</v>
+        <v>45525</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45510</v>
+        <v>45525</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45510</v>
+        <v>45525</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45510</v>
+        <v>45525</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>0.035</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>0.266</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>0.837</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>1.249</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>1.487</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>1.898</v>
+        <v>0.061</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>2.319</v>
+        <v>0.292</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>2.187</v>
+        <v>0.625</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B26">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>2.025</v>
+        <v>0.913</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C27">
-        <v>1.792</v>
+        <v>1.434</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B28">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>1.676</v>
+        <v>1.832</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B29">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C29">
-        <v>1.321</v>
+        <v>1.906</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B30">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>0.671</v>
+        <v>1.884</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C31">
-        <v>0.259</v>
+        <v>1.841</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B32">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C32">
-        <v>0.041</v>
+        <v>1.656</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B33">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45510</v>
+        <v>45526</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.531</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45511</v>
+        <v>45526</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.134</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45511</v>
+        <v>45526</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45511</v>
+        <v>45526</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45511</v>
+        <v>45526</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45511</v>
+        <v>45526</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C44">
-        <v>1.009</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C45">
-        <v>1.745</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C46">
-        <v>2.452</v>
+        <v>0.022</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B47">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C47">
-        <v>2.928</v>
+        <v>0.206</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C48">
-        <v>3.153</v>
+        <v>0.924</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B49">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C49">
-        <v>3.124</v>
+        <v>1.581</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B50">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C50">
-        <v>3.048</v>
+        <v>2.278</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B51">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C51">
-        <v>2.721</v>
+        <v>2.763</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B52">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C52">
-        <v>2.3</v>
+        <v>3.022</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B53">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>1.497</v>
+        <v>3.049</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B54">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C54">
-        <v>0.727</v>
+        <v>2.95</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C55">
-        <v>0.245</v>
+        <v>2.55</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C56">
-        <v>0.041</v>
+        <v>2.131</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B57">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1.36</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45511</v>
+        <v>45527</v>
       </c>
       <c r="B58">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45512</v>
+        <v>45527</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.147</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45512</v>
+        <v>45527</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45512</v>
+        <v>45527</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45512</v>
+        <v>45527</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45512</v>
+        <v>45527</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B65">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>0.042</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B67">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C67">
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B68">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C68">
-        <v>0.9409999999999999</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B69">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C69">
-        <v>1.658</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B70">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C70">
-        <v>2.391</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C71">
-        <v>2.839</v>
+        <v>0.201</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B72">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C72">
-        <v>3.054</v>
+        <v>0.828</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B73">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C73">
-        <v>3.088</v>
+        <v>1.577</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B74">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C74">
-        <v>2.993</v>
+        <v>2.264</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B75">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <v>2.677</v>
+        <v>2.685</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B76">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C76">
-        <v>2.11</v>
+        <v>2.989</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B77">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C77">
-        <v>1.355</v>
+        <v>3.03</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B78">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C78">
-        <v>0.66</v>
+        <v>2.903</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B79">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C79">
-        <v>0.274</v>
+        <v>2.456</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B80">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C80">
-        <v>0.036</v>
+        <v>2.118</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B81">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1.424</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45512</v>
+        <v>45528</v>
       </c>
       <c r="B82">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>0.629</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45513</v>
+        <v>45528</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,10 +2064,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45513</v>
+        <v>45528</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45513</v>
+        <v>45528</v>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45513</v>
+        <v>45528</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45513</v>
+        <v>45528</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B89">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B90">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C90">
-        <v>0.041</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B91">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C91">
-        <v>0.324</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B92">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C92">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B93">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C93">
-        <v>1.666</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B94">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C94">
-        <v>2.261</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B95">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C95">
-        <v>2.797</v>
+        <v>0.161</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B96">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C96">
-        <v>3.031</v>
+        <v>0.847</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B97">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C97">
-        <v>2.723</v>
+        <v>1.634</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B98">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C98">
-        <v>2.266</v>
+        <v>2.21</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B99">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C99">
-        <v>2.143</v>
+        <v>2.576</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B100">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C100">
-        <v>1.863</v>
+        <v>2.972</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B101">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C101">
-        <v>1.216</v>
+        <v>2.982</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B102">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C102">
-        <v>0.654</v>
+        <v>2.914</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B103">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C103">
-        <v>0.272</v>
+        <v>2.36</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B104">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C104">
-        <v>0.034</v>
+        <v>1.93</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B105">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>1.26</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45513</v>
+        <v>45529</v>
       </c>
       <c r="B106">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>0.539</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45514</v>
+        <v>45529</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.121</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45514</v>
+        <v>45529</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45514</v>
+        <v>45529</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45514</v>
+        <v>45529</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45514</v>
+        <v>45529</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B112">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B113">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B114">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C114">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B115">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C115">
-        <v>0.303</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B116">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C116">
-        <v>0.948</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B117">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C117">
-        <v>1.666</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B118">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C118">
-        <v>2.261</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B119">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C119">
-        <v>2.778</v>
+        <v>0.167</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B120">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C120">
-        <v>2.79</v>
+        <v>0.846</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B121">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C121">
-        <v>2.954</v>
+        <v>1.635</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B122">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C122">
-        <v>2.786</v>
+        <v>2.23</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B123">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C123">
-        <v>2.468</v>
+        <v>2.654</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B124">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C124">
-        <v>2.086</v>
+        <v>2.962</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B125">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C125">
-        <v>1.42</v>
+        <v>3.027</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B126">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C126">
-        <v>0.71</v>
+        <v>2.911</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B127">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C127">
-        <v>0.239</v>
+        <v>2.456</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B128">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C128">
-        <v>0.034</v>
+        <v>2.07</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B129">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45514</v>
+        <v>45530</v>
       </c>
       <c r="B130">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>0.537</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45515</v>
+        <v>45530</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45515</v>
+        <v>45530</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45515</v>
+        <v>45530</v>
       </c>
       <c r="B133">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45515</v>
+        <v>45530</v>
       </c>
       <c r="B134">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45515</v>
+        <v>45530</v>
       </c>
       <c r="B135">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B136">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B137">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B138">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C138">
-        <v>0.037</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B139">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C139">
-        <v>0.282</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B140">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C140">
-        <v>0.947</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B141">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C141">
-        <v>1.67</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B142">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C142">
-        <v>2.265</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B143">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C143">
-        <v>2.818</v>
+        <v>0.169</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B144">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C144">
-        <v>3.027</v>
+        <v>0.837</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B145">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C145">
-        <v>3.059</v>
+        <v>1.634</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B146">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C146">
-        <v>2.974</v>
+        <v>2.23</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B147">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C147">
-        <v>2.671</v>
+        <v>2.654</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B148">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C148">
-        <v>2.154</v>
+        <v>2.962</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B149">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C149">
-        <v>1.518</v>
+        <v>3.008</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B150">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C150">
-        <v>0.738</v>
+        <v>2.911</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B151">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C151">
-        <v>0.218</v>
+        <v>2.455</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B152">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C152">
-        <v>0.034</v>
+        <v>2.07</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B153">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45515</v>
+        <v>45531</v>
       </c>
       <c r="B154">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45516</v>
+        <v>45531</v>
       </c>
       <c r="B155">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>0.107</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45516</v>
+        <v>45531</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45516</v>
+        <v>45531</v>
       </c>
       <c r="B157">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45516</v>
+        <v>45531</v>
       </c>
       <c r="B158">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45516</v>
+        <v>45531</v>
       </c>
       <c r="B159">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B160">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B161">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B162">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C162">
-        <v>0.037</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B163">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C163">
-        <v>0.337</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B164">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C164">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B165">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C165">
-        <v>1.667</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B166">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C166">
-        <v>2.252</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B167">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C167">
-        <v>2.796</v>
+        <v>0.142</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B168">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C168">
-        <v>3.045</v>
+        <v>0.77</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B169">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C169">
-        <v>3.085</v>
+        <v>1.608</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45516</v>
+        <v>45532</v>
       </c>
       <c r="B170">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C170">
-        <v>2.981</v>
+        <v>1.97</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the postgresql database
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>21.08.202411</t>
-  </si>
-  <si>
-    <t>21.08.202412</t>
-  </si>
-  <si>
-    <t>21.08.202413</t>
-  </si>
-  <si>
-    <t>21.08.202414</t>
-  </si>
-  <si>
-    <t>21.08.202415</t>
-  </si>
-  <si>
-    <t>21.08.202416</t>
-  </si>
-  <si>
-    <t>21.08.202417</t>
-  </si>
-  <si>
-    <t>21.08.202418</t>
-  </si>
-  <si>
-    <t>21.08.202419</t>
-  </si>
-  <si>
-    <t>21.08.202420</t>
-  </si>
-  <si>
-    <t>21.08.202421</t>
-  </si>
-  <si>
-    <t>21.08.202422</t>
-  </si>
-  <si>
-    <t>21.08.202423</t>
-  </si>
-  <si>
-    <t>21.08.202424</t>
-  </si>
-  <si>
-    <t>22.08.20241</t>
-  </si>
-  <si>
-    <t>22.08.20242</t>
-  </si>
-  <si>
-    <t>22.08.20243</t>
-  </si>
-  <si>
-    <t>22.08.20244</t>
-  </si>
-  <si>
-    <t>22.08.20245</t>
-  </si>
-  <si>
-    <t>22.08.20246</t>
-  </si>
-  <si>
-    <t>22.08.20247</t>
-  </si>
-  <si>
-    <t>22.08.20248</t>
-  </si>
-  <si>
-    <t>22.08.20249</t>
-  </si>
-  <si>
-    <t>22.08.202410</t>
-  </si>
-  <si>
-    <t>22.08.202411</t>
-  </si>
-  <si>
-    <t>22.08.202412</t>
-  </si>
-  <si>
-    <t>22.08.202413</t>
-  </si>
-  <si>
-    <t>22.08.202414</t>
-  </si>
-  <si>
-    <t>22.08.202415</t>
-  </si>
-  <si>
-    <t>22.08.202416</t>
-  </si>
-  <si>
-    <t>22.08.202417</t>
-  </si>
-  <si>
-    <t>22.08.202418</t>
-  </si>
-  <si>
-    <t>22.08.202419</t>
-  </si>
-  <si>
-    <t>22.08.202420</t>
-  </si>
-  <si>
-    <t>22.08.202421</t>
-  </si>
-  <si>
-    <t>22.08.202422</t>
-  </si>
-  <si>
-    <t>22.08.202423</t>
-  </si>
-  <si>
-    <t>22.08.202424</t>
-  </si>
-  <si>
-    <t>23.08.20241</t>
-  </si>
-  <si>
-    <t>23.08.20242</t>
-  </si>
-  <si>
-    <t>23.08.20243</t>
-  </si>
-  <si>
-    <t>23.08.20244</t>
-  </si>
-  <si>
-    <t>23.08.20245</t>
-  </si>
-  <si>
-    <t>23.08.20246</t>
-  </si>
-  <si>
-    <t>23.08.20247</t>
-  </si>
-  <si>
-    <t>23.08.20248</t>
-  </si>
-  <si>
-    <t>23.08.20249</t>
-  </si>
-  <si>
-    <t>23.08.202410</t>
-  </si>
-  <si>
-    <t>23.08.202411</t>
-  </si>
-  <si>
-    <t>23.08.202412</t>
-  </si>
-  <si>
-    <t>23.08.202413</t>
-  </si>
-  <si>
-    <t>23.08.202414</t>
-  </si>
-  <si>
-    <t>23.08.202415</t>
-  </si>
-  <si>
-    <t>23.08.202416</t>
-  </si>
-  <si>
-    <t>23.08.202417</t>
-  </si>
-  <si>
-    <t>23.08.202418</t>
-  </si>
-  <si>
-    <t>23.08.202419</t>
-  </si>
-  <si>
-    <t>23.08.202420</t>
-  </si>
-  <si>
-    <t>23.08.202421</t>
-  </si>
-  <si>
-    <t>23.08.202422</t>
-  </si>
-  <si>
-    <t>23.08.202423</t>
-  </si>
-  <si>
-    <t>23.08.202424</t>
-  </si>
-  <si>
-    <t>24.08.20241</t>
-  </si>
-  <si>
-    <t>24.08.20242</t>
-  </si>
-  <si>
-    <t>24.08.20243</t>
-  </si>
-  <si>
-    <t>24.08.20244</t>
-  </si>
-  <si>
-    <t>24.08.20245</t>
-  </si>
-  <si>
-    <t>24.08.20246</t>
-  </si>
-  <si>
-    <t>24.08.20247</t>
-  </si>
-  <si>
-    <t>24.08.20248</t>
-  </si>
-  <si>
-    <t>24.08.20249</t>
-  </si>
-  <si>
-    <t>24.08.202410</t>
-  </si>
-  <si>
-    <t>24.08.202411</t>
-  </si>
-  <si>
-    <t>24.08.202412</t>
-  </si>
-  <si>
-    <t>24.08.202413</t>
-  </si>
-  <si>
-    <t>24.08.202414</t>
-  </si>
-  <si>
-    <t>24.08.202415</t>
-  </si>
-  <si>
-    <t>24.08.202416</t>
-  </si>
-  <si>
-    <t>24.08.202417</t>
-  </si>
-  <si>
-    <t>24.08.202418</t>
-  </si>
-  <si>
-    <t>24.08.202419</t>
-  </si>
-  <si>
-    <t>24.08.202420</t>
-  </si>
-  <si>
-    <t>24.08.202421</t>
-  </si>
-  <si>
-    <t>24.08.202422</t>
-  </si>
-  <si>
-    <t>24.08.202423</t>
-  </si>
-  <si>
-    <t>24.08.202424</t>
-  </si>
-  <si>
-    <t>25.08.20241</t>
-  </si>
-  <si>
-    <t>25.08.20242</t>
-  </si>
-  <si>
-    <t>25.08.20243</t>
-  </si>
-  <si>
-    <t>25.08.20244</t>
-  </si>
-  <si>
-    <t>25.08.20245</t>
-  </si>
-  <si>
-    <t>25.08.20246</t>
-  </si>
-  <si>
-    <t>25.08.20247</t>
-  </si>
-  <si>
-    <t>25.08.20248</t>
-  </si>
-  <si>
-    <t>25.08.20249</t>
-  </si>
-  <si>
-    <t>25.08.202410</t>
-  </si>
-  <si>
-    <t>25.08.202411</t>
-  </si>
-  <si>
-    <t>25.08.202412</t>
-  </si>
-  <si>
-    <t>25.08.202413</t>
-  </si>
-  <si>
-    <t>25.08.202414</t>
-  </si>
-  <si>
-    <t>25.08.202415</t>
-  </si>
-  <si>
-    <t>25.08.202416</t>
-  </si>
-  <si>
-    <t>25.08.202417</t>
-  </si>
-  <si>
-    <t>25.08.202418</t>
-  </si>
-  <si>
-    <t>25.08.202419</t>
-  </si>
-  <si>
-    <t>25.08.202420</t>
-  </si>
-  <si>
-    <t>25.08.202421</t>
-  </si>
-  <si>
-    <t>25.08.202422</t>
-  </si>
-  <si>
-    <t>25.08.202423</t>
-  </si>
-  <si>
-    <t>25.08.202424</t>
-  </si>
-  <si>
-    <t>26.08.20241</t>
-  </si>
-  <si>
-    <t>26.08.20242</t>
-  </si>
-  <si>
-    <t>26.08.20243</t>
-  </si>
-  <si>
-    <t>26.08.20244</t>
-  </si>
-  <si>
-    <t>26.08.20245</t>
-  </si>
-  <si>
-    <t>26.08.20246</t>
-  </si>
-  <si>
-    <t>26.08.20247</t>
-  </si>
-  <si>
-    <t>26.08.20248</t>
-  </si>
-  <si>
-    <t>26.08.20249</t>
-  </si>
-  <si>
-    <t>26.08.202410</t>
-  </si>
-  <si>
-    <t>26.08.202411</t>
-  </si>
-  <si>
-    <t>26.08.202412</t>
-  </si>
-  <si>
-    <t>26.08.202413</t>
-  </si>
-  <si>
-    <t>26.08.202414</t>
-  </si>
-  <si>
-    <t>26.08.202415</t>
-  </si>
-  <si>
-    <t>26.08.202416</t>
-  </si>
-  <si>
-    <t>26.08.202417</t>
-  </si>
-  <si>
-    <t>26.08.202418</t>
-  </si>
-  <si>
-    <t>26.08.202419</t>
-  </si>
-  <si>
-    <t>26.08.202420</t>
-  </si>
-  <si>
-    <t>26.08.202421</t>
-  </si>
-  <si>
-    <t>26.08.202422</t>
-  </si>
-  <si>
-    <t>26.08.202423</t>
-  </si>
-  <si>
-    <t>26.08.202424</t>
-  </si>
-  <si>
-    <t>27.08.20241</t>
-  </si>
-  <si>
-    <t>27.08.20242</t>
-  </si>
-  <si>
-    <t>27.08.20243</t>
-  </si>
-  <si>
-    <t>27.08.20244</t>
-  </si>
-  <si>
-    <t>27.08.20245</t>
-  </si>
-  <si>
-    <t>27.08.20246</t>
-  </si>
-  <si>
-    <t>27.08.20247</t>
-  </si>
-  <si>
-    <t>27.08.20248</t>
-  </si>
-  <si>
-    <t>27.08.20249</t>
-  </si>
-  <si>
-    <t>27.08.202410</t>
-  </si>
-  <si>
-    <t>27.08.202411</t>
-  </si>
-  <si>
-    <t>27.08.202412</t>
-  </si>
-  <si>
-    <t>27.08.202413</t>
-  </si>
-  <si>
-    <t>27.08.202414</t>
-  </si>
-  <si>
-    <t>27.08.202415</t>
-  </si>
-  <si>
-    <t>27.08.202416</t>
-  </si>
-  <si>
-    <t>27.08.202417</t>
-  </si>
-  <si>
-    <t>27.08.202418</t>
-  </si>
-  <si>
-    <t>27.08.202419</t>
-  </si>
-  <si>
-    <t>27.08.202420</t>
-  </si>
-  <si>
-    <t>27.08.202421</t>
-  </si>
-  <si>
-    <t>27.08.202422</t>
-  </si>
-  <si>
-    <t>27.08.202423</t>
-  </si>
-  <si>
-    <t>27.08.202424</t>
-  </si>
-  <si>
-    <t>28.08.20241</t>
-  </si>
-  <si>
-    <t>28.08.20242</t>
-  </si>
-  <si>
-    <t>28.08.20243</t>
-  </si>
-  <si>
-    <t>28.08.20244</t>
-  </si>
-  <si>
-    <t>28.08.20245</t>
-  </si>
-  <si>
-    <t>28.08.20246</t>
-  </si>
-  <si>
-    <t>28.08.20247</t>
-  </si>
-  <si>
-    <t>28.08.20248</t>
-  </si>
-  <si>
-    <t>28.08.20249</t>
-  </si>
-  <si>
-    <t>28.08.202410</t>
-  </si>
-  <si>
-    <t>28.08.202411</t>
+    <t>29.08.202411</t>
+  </si>
+  <si>
+    <t>29.08.202412</t>
+  </si>
+  <si>
+    <t>29.08.202413</t>
+  </si>
+  <si>
+    <t>29.08.202414</t>
+  </si>
+  <si>
+    <t>29.08.202415</t>
+  </si>
+  <si>
+    <t>29.08.202416</t>
+  </si>
+  <si>
+    <t>29.08.202417</t>
+  </si>
+  <si>
+    <t>29.08.202418</t>
+  </si>
+  <si>
+    <t>29.08.202419</t>
+  </si>
+  <si>
+    <t>29.08.202420</t>
+  </si>
+  <si>
+    <t>29.08.202421</t>
+  </si>
+  <si>
+    <t>29.08.202422</t>
+  </si>
+  <si>
+    <t>29.08.202423</t>
+  </si>
+  <si>
+    <t>29.08.202424</t>
+  </si>
+  <si>
+    <t>30.08.20241</t>
+  </si>
+  <si>
+    <t>30.08.20242</t>
+  </si>
+  <si>
+    <t>30.08.20243</t>
+  </si>
+  <si>
+    <t>30.08.20244</t>
+  </si>
+  <si>
+    <t>30.08.20245</t>
+  </si>
+  <si>
+    <t>30.08.20246</t>
+  </si>
+  <si>
+    <t>30.08.20247</t>
+  </si>
+  <si>
+    <t>30.08.20248</t>
+  </si>
+  <si>
+    <t>30.08.20249</t>
+  </si>
+  <si>
+    <t>30.08.202410</t>
+  </si>
+  <si>
+    <t>30.08.202411</t>
+  </si>
+  <si>
+    <t>30.08.202412</t>
+  </si>
+  <si>
+    <t>30.08.202413</t>
+  </si>
+  <si>
+    <t>30.08.202414</t>
+  </si>
+  <si>
+    <t>30.08.202415</t>
+  </si>
+  <si>
+    <t>30.08.202416</t>
+  </si>
+  <si>
+    <t>30.08.202417</t>
+  </si>
+  <si>
+    <t>30.08.202418</t>
+  </si>
+  <si>
+    <t>30.08.202419</t>
+  </si>
+  <si>
+    <t>30.08.202420</t>
+  </si>
+  <si>
+    <t>30.08.202421</t>
+  </si>
+  <si>
+    <t>30.08.202422</t>
+  </si>
+  <si>
+    <t>30.08.202423</t>
+  </si>
+  <si>
+    <t>30.08.202424</t>
+  </si>
+  <si>
+    <t>31.08.20241</t>
+  </si>
+  <si>
+    <t>31.08.20242</t>
+  </si>
+  <si>
+    <t>31.08.20243</t>
+  </si>
+  <si>
+    <t>31.08.20244</t>
+  </si>
+  <si>
+    <t>31.08.20245</t>
+  </si>
+  <si>
+    <t>31.08.20246</t>
+  </si>
+  <si>
+    <t>31.08.20247</t>
+  </si>
+  <si>
+    <t>31.08.20248</t>
+  </si>
+  <si>
+    <t>31.08.20249</t>
+  </si>
+  <si>
+    <t>31.08.202410</t>
+  </si>
+  <si>
+    <t>31.08.202411</t>
+  </si>
+  <si>
+    <t>31.08.202412</t>
+  </si>
+  <si>
+    <t>31.08.202413</t>
+  </si>
+  <si>
+    <t>31.08.202414</t>
+  </si>
+  <si>
+    <t>31.08.202415</t>
+  </si>
+  <si>
+    <t>31.08.202416</t>
+  </si>
+  <si>
+    <t>31.08.202417</t>
+  </si>
+  <si>
+    <t>31.08.202418</t>
+  </si>
+  <si>
+    <t>31.08.202419</t>
+  </si>
+  <si>
+    <t>31.08.202420</t>
+  </si>
+  <si>
+    <t>31.08.202421</t>
+  </si>
+  <si>
+    <t>31.08.202422</t>
+  </si>
+  <si>
+    <t>31.08.202423</t>
+  </si>
+  <si>
+    <t>31.08.202424</t>
+  </si>
+  <si>
+    <t>01.09.20241</t>
+  </si>
+  <si>
+    <t>01.09.20242</t>
+  </si>
+  <si>
+    <t>01.09.20243</t>
+  </si>
+  <si>
+    <t>01.09.20244</t>
+  </si>
+  <si>
+    <t>01.09.20245</t>
+  </si>
+  <si>
+    <t>01.09.20246</t>
+  </si>
+  <si>
+    <t>01.09.20247</t>
+  </si>
+  <si>
+    <t>01.09.20248</t>
+  </si>
+  <si>
+    <t>01.09.20249</t>
+  </si>
+  <si>
+    <t>01.09.202410</t>
+  </si>
+  <si>
+    <t>01.09.202411</t>
+  </si>
+  <si>
+    <t>01.09.202412</t>
+  </si>
+  <si>
+    <t>01.09.202413</t>
+  </si>
+  <si>
+    <t>01.09.202414</t>
+  </si>
+  <si>
+    <t>01.09.202415</t>
+  </si>
+  <si>
+    <t>01.09.202416</t>
+  </si>
+  <si>
+    <t>01.09.202417</t>
+  </si>
+  <si>
+    <t>01.09.202418</t>
+  </si>
+  <si>
+    <t>01.09.202419</t>
+  </si>
+  <si>
+    <t>01.09.202420</t>
+  </si>
+  <si>
+    <t>01.09.202421</t>
+  </si>
+  <si>
+    <t>01.09.202422</t>
+  </si>
+  <si>
+    <t>01.09.202423</t>
+  </si>
+  <si>
+    <t>01.09.202424</t>
+  </si>
+  <si>
+    <t>02.09.20241</t>
+  </si>
+  <si>
+    <t>02.09.20242</t>
+  </si>
+  <si>
+    <t>02.09.20243</t>
+  </si>
+  <si>
+    <t>02.09.20244</t>
+  </si>
+  <si>
+    <t>02.09.20245</t>
+  </si>
+  <si>
+    <t>02.09.20246</t>
+  </si>
+  <si>
+    <t>02.09.20247</t>
+  </si>
+  <si>
+    <t>02.09.20248</t>
+  </si>
+  <si>
+    <t>02.09.20249</t>
+  </si>
+  <si>
+    <t>02.09.202410</t>
+  </si>
+  <si>
+    <t>02.09.202411</t>
+  </si>
+  <si>
+    <t>02.09.202412</t>
+  </si>
+  <si>
+    <t>02.09.202413</t>
+  </si>
+  <si>
+    <t>02.09.202414</t>
+  </si>
+  <si>
+    <t>02.09.202415</t>
+  </si>
+  <si>
+    <t>02.09.202416</t>
+  </si>
+  <si>
+    <t>02.09.202417</t>
+  </si>
+  <si>
+    <t>02.09.202418</t>
+  </si>
+  <si>
+    <t>02.09.202419</t>
+  </si>
+  <si>
+    <t>02.09.202420</t>
+  </si>
+  <si>
+    <t>02.09.202421</t>
+  </si>
+  <si>
+    <t>02.09.202422</t>
+  </si>
+  <si>
+    <t>02.09.202423</t>
+  </si>
+  <si>
+    <t>02.09.202424</t>
+  </si>
+  <si>
+    <t>03.09.20241</t>
+  </si>
+  <si>
+    <t>03.09.20242</t>
+  </si>
+  <si>
+    <t>03.09.20243</t>
+  </si>
+  <si>
+    <t>03.09.20244</t>
+  </si>
+  <si>
+    <t>03.09.20245</t>
+  </si>
+  <si>
+    <t>03.09.20246</t>
+  </si>
+  <si>
+    <t>03.09.20247</t>
+  </si>
+  <si>
+    <t>03.09.20248</t>
+  </si>
+  <si>
+    <t>03.09.20249</t>
+  </si>
+  <si>
+    <t>03.09.202410</t>
+  </si>
+  <si>
+    <t>03.09.202411</t>
+  </si>
+  <si>
+    <t>03.09.202412</t>
+  </si>
+  <si>
+    <t>03.09.202413</t>
+  </si>
+  <si>
+    <t>03.09.202414</t>
+  </si>
+  <si>
+    <t>03.09.202415</t>
+  </si>
+  <si>
+    <t>03.09.202416</t>
+  </si>
+  <si>
+    <t>03.09.202417</t>
+  </si>
+  <si>
+    <t>03.09.202418</t>
+  </si>
+  <si>
+    <t>03.09.202419</t>
+  </si>
+  <si>
+    <t>03.09.202420</t>
+  </si>
+  <si>
+    <t>03.09.202421</t>
+  </si>
+  <si>
+    <t>03.09.202422</t>
+  </si>
+  <si>
+    <t>03.09.202423</t>
+  </si>
+  <si>
+    <t>03.09.202424</t>
+  </si>
+  <si>
+    <t>04.09.20241</t>
+  </si>
+  <si>
+    <t>04.09.20242</t>
+  </si>
+  <si>
+    <t>04.09.20243</t>
+  </si>
+  <si>
+    <t>04.09.20244</t>
+  </si>
+  <si>
+    <t>04.09.20245</t>
+  </si>
+  <si>
+    <t>04.09.20246</t>
+  </si>
+  <si>
+    <t>04.09.20247</t>
+  </si>
+  <si>
+    <t>04.09.20248</t>
+  </si>
+  <si>
+    <t>04.09.20249</t>
+  </si>
+  <si>
+    <t>04.09.202410</t>
+  </si>
+  <si>
+    <t>04.09.202411</t>
+  </si>
+  <si>
+    <t>04.09.202412</t>
+  </si>
+  <si>
+    <t>04.09.202413</t>
+  </si>
+  <si>
+    <t>04.09.202414</t>
+  </si>
+  <si>
+    <t>04.09.202415</t>
+  </si>
+  <si>
+    <t>04.09.202416</t>
+  </si>
+  <si>
+    <t>04.09.202417</t>
+  </si>
+  <si>
+    <t>04.09.202418</t>
+  </si>
+  <si>
+    <t>04.09.202419</t>
+  </si>
+  <si>
+    <t>04.09.202420</t>
+  </si>
+  <si>
+    <t>04.09.202421</t>
+  </si>
+  <si>
+    <t>04.09.202422</t>
+  </si>
+  <si>
+    <t>04.09.202423</t>
+  </si>
+  <si>
+    <t>04.09.202424</t>
+  </si>
+  <si>
+    <t>05.09.20241</t>
+  </si>
+  <si>
+    <t>05.09.20242</t>
+  </si>
+  <si>
+    <t>05.09.20243</t>
+  </si>
+  <si>
+    <t>05.09.20244</t>
+  </si>
+  <si>
+    <t>05.09.20245</t>
+  </si>
+  <si>
+    <t>05.09.20246</t>
+  </si>
+  <si>
+    <t>05.09.20247</t>
+  </si>
+  <si>
+    <t>05.09.20248</t>
+  </si>
+  <si>
+    <t>05.09.20249</t>
+  </si>
+  <si>
+    <t>05.09.202410</t>
+  </si>
+  <si>
+    <t>05.09.202411</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B4">
         <v>13</v>
       </c>
       <c r="C4">
-        <v>3.019</v>
+        <v>2.834</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B5">
         <v>14</v>
       </c>
       <c r="C5">
-        <v>3.048</v>
+        <v>2.195</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6">
-        <v>2.963</v>
+        <v>1.713</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
       <c r="C7">
-        <v>2.554</v>
+        <v>1.721</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B8">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>2.151</v>
+        <v>1.446</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>1.45</v>
+        <v>0.848</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B10">
         <v>19</v>
       </c>
       <c r="C10">
-        <v>0.652</v>
+        <v>0.351</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B11">
         <v>20</v>
       </c>
       <c r="C11">
-        <v>0.15</v>
+        <v>0.045</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B12">
         <v>21</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B13">
         <v>22</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B14">
         <v>23</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B15">
         <v>24</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B23">
         <v>8</v>
       </c>
       <c r="C23">
-        <v>0.061</v>
+        <v>0.079</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B24">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0.292</v>
+        <v>0.481</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25">
-        <v>0.625</v>
+        <v>0.889</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B26">
         <v>11</v>
       </c>
       <c r="C26">
-        <v>0.913</v>
+        <v>1.405</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B27">
         <v>12</v>
       </c>
       <c r="C27">
-        <v>1.434</v>
+        <v>1.637</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B28">
         <v>13</v>
       </c>
       <c r="C28">
-        <v>1.832</v>
+        <v>1.827</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B29">
         <v>14</v>
       </c>
       <c r="C29">
-        <v>1.906</v>
+        <v>1.79</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B30">
         <v>15</v>
       </c>
       <c r="C30">
-        <v>1.884</v>
+        <v>1.793</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B31">
         <v>16</v>
       </c>
       <c r="C31">
-        <v>1.841</v>
+        <v>1.699</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B32">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>1.656</v>
+        <v>1.573</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B33">
         <v>18</v>
       </c>
       <c r="C33">
-        <v>1.1</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B34">
         <v>19</v>
       </c>
       <c r="C34">
-        <v>0.531</v>
+        <v>0.437</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B35">
         <v>20</v>
       </c>
       <c r="C35">
-        <v>0.134</v>
+        <v>0.054</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B36">
         <v>21</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B37">
         <v>22</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B38">
         <v>23</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B39">
         <v>24</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B46">
         <v>7</v>
       </c>
       <c r="C46">
-        <v>0.022</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
       <c r="C47">
-        <v>0.206</v>
+        <v>0.105</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B48">
         <v>9</v>
       </c>
       <c r="C48">
-        <v>0.924</v>
+        <v>0.711</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B49">
         <v>10</v>
       </c>
       <c r="C49">
-        <v>1.581</v>
+        <v>1.543</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B50">
         <v>11</v>
       </c>
       <c r="C50">
-        <v>2.278</v>
+        <v>1.977</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B51">
         <v>12</v>
       </c>
       <c r="C51">
-        <v>2.763</v>
+        <v>2.602</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B52">
         <v>13</v>
       </c>
       <c r="C52">
-        <v>3.022</v>
+        <v>2.975</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B53">
         <v>14</v>
       </c>
       <c r="C53">
-        <v>3.049</v>
+        <v>2.779</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B54">
         <v>15</v>
       </c>
       <c r="C54">
-        <v>2.95</v>
+        <v>2.486</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B55">
         <v>16</v>
       </c>
       <c r="C55">
-        <v>2.55</v>
+        <v>2.08</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B56">
         <v>17</v>
       </c>
       <c r="C56">
-        <v>2.131</v>
+        <v>1.704</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
       <c r="C57">
-        <v>1.36</v>
+        <v>1.132</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B58">
         <v>19</v>
       </c>
       <c r="C58">
-        <v>0.59</v>
+        <v>0.503</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B59">
         <v>20</v>
       </c>
       <c r="C59">
-        <v>0.147</v>
+        <v>0.067</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B60">
         <v>21</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B61">
         <v>22</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B62">
         <v>23</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45527</v>
+        <v>45535</v>
       </c>
       <c r="B63">
         <v>24</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B67">
         <v>4</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B69">
         <v>6</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B70">
         <v>7</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B71">
         <v>8</v>
       </c>
       <c r="C71">
-        <v>0.201</v>
+        <v>0.061</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B72">
         <v>9</v>
       </c>
       <c r="C72">
-        <v>0.828</v>
+        <v>0.413</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B73">
         <v>10</v>
       </c>
       <c r="C73">
-        <v>1.577</v>
+        <v>0.853</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B74">
         <v>11</v>
       </c>
       <c r="C74">
-        <v>2.264</v>
+        <v>1.312</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B75">
         <v>12</v>
       </c>
       <c r="C75">
-        <v>2.685</v>
+        <v>1.915</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B76">
         <v>13</v>
       </c>
       <c r="C76">
-        <v>2.989</v>
+        <v>2.105</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B77">
         <v>14</v>
       </c>
       <c r="C77">
-        <v>3.03</v>
+        <v>2.225</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B78">
         <v>15</v>
       </c>
       <c r="C78">
-        <v>2.903</v>
+        <v>2.277</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B79">
         <v>16</v>
       </c>
       <c r="C79">
-        <v>2.456</v>
+        <v>2.103</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B80">
         <v>17</v>
       </c>
       <c r="C80">
-        <v>2.118</v>
+        <v>1.803</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B81">
         <v>18</v>
       </c>
       <c r="C81">
-        <v>1.424</v>
+        <v>1.09</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B82">
         <v>19</v>
       </c>
       <c r="C82">
-        <v>0.629</v>
+        <v>0.39</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B83">
         <v>20</v>
       </c>
       <c r="C83">
-        <v>0.125</v>
+        <v>0.046</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B84">
         <v>21</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B85">
         <v>22</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B86">
         <v>23</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45528</v>
+        <v>45536</v>
       </c>
       <c r="B87">
         <v>24</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B91">
         <v>4</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B92">
         <v>5</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B93">
         <v>6</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B94">
         <v>7</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B95">
         <v>8</v>
       </c>
       <c r="C95">
-        <v>0.161</v>
+        <v>0.097</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B96">
         <v>9</v>
       </c>
       <c r="C96">
-        <v>0.847</v>
+        <v>0.789</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B97">
         <v>10</v>
       </c>
       <c r="C97">
-        <v>1.634</v>
+        <v>1.724</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B98">
         <v>11</v>
       </c>
       <c r="C98">
-        <v>2.21</v>
+        <v>2.294</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B99">
         <v>12</v>
       </c>
       <c r="C99">
-        <v>2.576</v>
+        <v>2.86</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B100">
         <v>13</v>
       </c>
       <c r="C100">
-        <v>2.972</v>
+        <v>3.07</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B101">
         <v>14</v>
       </c>
       <c r="C101">
-        <v>2.982</v>
+        <v>3.066</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B102">
         <v>15</v>
       </c>
       <c r="C102">
-        <v>2.914</v>
+        <v>3.008</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B103">
         <v>16</v>
       </c>
       <c r="C103">
-        <v>2.36</v>
+        <v>2.67</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B104">
         <v>17</v>
       </c>
       <c r="C104">
-        <v>1.93</v>
+        <v>1.982</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B105">
         <v>18</v>
       </c>
       <c r="C105">
-        <v>1.26</v>
+        <v>1.121</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B106">
         <v>19</v>
       </c>
       <c r="C106">
-        <v>0.539</v>
+        <v>0.46</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B107">
         <v>20</v>
       </c>
       <c r="C107">
-        <v>0.121</v>
+        <v>0.054</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B108">
         <v>21</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B109">
         <v>22</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B110">
         <v>23</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45529</v>
+        <v>45537</v>
       </c>
       <c r="B111">
         <v>24</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B116">
         <v>5</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B117">
         <v>6</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B118">
         <v>7</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B119">
         <v>8</v>
       </c>
       <c r="C119">
-        <v>0.167</v>
+        <v>0.1</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B120">
         <v>9</v>
       </c>
       <c r="C120">
-        <v>0.846</v>
+        <v>0.65</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B121">
         <v>10</v>
       </c>
       <c r="C121">
-        <v>1.635</v>
+        <v>1.621</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B122">
         <v>11</v>
       </c>
       <c r="C122">
-        <v>2.23</v>
+        <v>2.291</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B123">
         <v>12</v>
       </c>
       <c r="C123">
-        <v>2.654</v>
+        <v>2.77</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B124">
         <v>13</v>
       </c>
       <c r="C124">
-        <v>2.962</v>
+        <v>3.003</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B125">
         <v>14</v>
       </c>
       <c r="C125">
-        <v>3.027</v>
+        <v>3.067</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B126">
         <v>15</v>
       </c>
       <c r="C126">
-        <v>2.911</v>
+        <v>2.965</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B127">
         <v>16</v>
       </c>
       <c r="C127">
-        <v>2.456</v>
+        <v>2.646</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B128">
         <v>17</v>
       </c>
       <c r="C128">
-        <v>2.07</v>
+        <v>2.011</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B129">
         <v>18</v>
       </c>
       <c r="C129">
-        <v>1.25</v>
+        <v>1.153</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B130">
         <v>19</v>
       </c>
       <c r="C130">
-        <v>0.537</v>
+        <v>0.459</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B131">
         <v>20</v>
       </c>
       <c r="C131">
-        <v>0.08699999999999999</v>
+        <v>0.065</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B132">
         <v>21</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B133">
         <v>22</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B134">
         <v>23</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B135">
         <v>24</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B137">
         <v>2</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B138">
         <v>3</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B139">
         <v>4</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B140">
         <v>5</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B141">
         <v>6</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B142">
         <v>7</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B143">
         <v>8</v>
       </c>
       <c r="C143">
-        <v>0.169</v>
+        <v>0.098</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B144">
         <v>9</v>
       </c>
       <c r="C144">
-        <v>0.837</v>
+        <v>0.649</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B145">
         <v>10</v>
       </c>
       <c r="C145">
-        <v>1.634</v>
+        <v>1.662</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B146">
         <v>11</v>
       </c>
       <c r="C146">
-        <v>2.23</v>
+        <v>2.289</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B147">
         <v>12</v>
       </c>
       <c r="C147">
-        <v>2.654</v>
+        <v>2.778</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B148">
         <v>13</v>
       </c>
       <c r="C148">
-        <v>2.962</v>
+        <v>3.069</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B149">
         <v>14</v>
       </c>
       <c r="C149">
-        <v>3.008</v>
+        <v>3.066</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B150">
         <v>15</v>
       </c>
       <c r="C150">
-        <v>2.911</v>
+        <v>3.008</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B151">
         <v>16</v>
       </c>
       <c r="C151">
-        <v>2.455</v>
+        <v>2.67</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B152">
         <v>17</v>
       </c>
       <c r="C152">
-        <v>2.07</v>
+        <v>2.1</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B153">
         <v>18</v>
       </c>
       <c r="C153">
-        <v>1.3</v>
+        <v>1.162</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B154">
         <v>19</v>
       </c>
       <c r="C154">
-        <v>0.5600000000000001</v>
+        <v>0.507</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B155">
         <v>20</v>
       </c>
       <c r="C155">
-        <v>0.107</v>
+        <v>0.065</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B156">
         <v>21</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B157">
         <v>22</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B158">
         <v>23</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B159">
         <v>24</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B161">
         <v>2</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B162">
         <v>3</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B163">
         <v>4</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B164">
         <v>5</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B165">
         <v>6</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B166">
         <v>7</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B167">
         <v>8</v>
       </c>
       <c r="C167">
-        <v>0.142</v>
+        <v>0.1</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B168">
         <v>9</v>
       </c>
       <c r="C168">
-        <v>0.77</v>
+        <v>0.743</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B169">
         <v>10</v>
       </c>
       <c r="C169">
-        <v>1.608</v>
+        <v>1.66</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B170">
         <v>11</v>
       </c>
       <c r="C170">
-        <v>1.97</v>
+        <v>2.295</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the Wind Production Forecasst and changing the meta styles
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>29.08.202411</t>
-  </si>
-  <si>
-    <t>29.08.202412</t>
-  </si>
-  <si>
-    <t>29.08.202413</t>
-  </si>
-  <si>
-    <t>29.08.202414</t>
-  </si>
-  <si>
-    <t>29.08.202415</t>
-  </si>
-  <si>
-    <t>29.08.202416</t>
-  </si>
-  <si>
-    <t>29.08.202417</t>
-  </si>
-  <si>
-    <t>29.08.202418</t>
-  </si>
-  <si>
-    <t>29.08.202419</t>
-  </si>
-  <si>
-    <t>29.08.202420</t>
-  </si>
-  <si>
-    <t>29.08.202421</t>
-  </si>
-  <si>
-    <t>29.08.202422</t>
-  </si>
-  <si>
-    <t>29.08.202423</t>
-  </si>
-  <si>
-    <t>29.08.202424</t>
-  </si>
-  <si>
-    <t>30.08.20241</t>
-  </si>
-  <si>
-    <t>30.08.20242</t>
-  </si>
-  <si>
-    <t>30.08.20243</t>
-  </si>
-  <si>
-    <t>30.08.20244</t>
-  </si>
-  <si>
-    <t>30.08.20245</t>
-  </si>
-  <si>
-    <t>30.08.20246</t>
-  </si>
-  <si>
-    <t>30.08.20247</t>
-  </si>
-  <si>
-    <t>30.08.20248</t>
-  </si>
-  <si>
-    <t>30.08.20249</t>
-  </si>
-  <si>
-    <t>30.08.202410</t>
-  </si>
-  <si>
-    <t>30.08.202411</t>
-  </si>
-  <si>
-    <t>30.08.202412</t>
-  </si>
-  <si>
-    <t>30.08.202413</t>
-  </si>
-  <si>
-    <t>30.08.202414</t>
-  </si>
-  <si>
-    <t>30.08.202415</t>
-  </si>
-  <si>
-    <t>30.08.202416</t>
-  </si>
-  <si>
-    <t>30.08.202417</t>
-  </si>
-  <si>
-    <t>30.08.202418</t>
-  </si>
-  <si>
-    <t>30.08.202419</t>
-  </si>
-  <si>
-    <t>30.08.202420</t>
-  </si>
-  <si>
-    <t>30.08.202421</t>
-  </si>
-  <si>
-    <t>30.08.202422</t>
-  </si>
-  <si>
-    <t>30.08.202423</t>
-  </si>
-  <si>
-    <t>30.08.202424</t>
-  </si>
-  <si>
-    <t>31.08.20241</t>
-  </si>
-  <si>
-    <t>31.08.20242</t>
-  </si>
-  <si>
-    <t>31.08.20243</t>
-  </si>
-  <si>
-    <t>31.08.20244</t>
-  </si>
-  <si>
-    <t>31.08.20245</t>
-  </si>
-  <si>
-    <t>31.08.20246</t>
-  </si>
-  <si>
-    <t>31.08.20247</t>
-  </si>
-  <si>
-    <t>31.08.20248</t>
-  </si>
-  <si>
-    <t>31.08.20249</t>
-  </si>
-  <si>
-    <t>31.08.202410</t>
-  </si>
-  <si>
-    <t>31.08.202411</t>
-  </si>
-  <si>
-    <t>31.08.202412</t>
-  </si>
-  <si>
-    <t>31.08.202413</t>
-  </si>
-  <si>
-    <t>31.08.202414</t>
-  </si>
-  <si>
-    <t>31.08.202415</t>
-  </si>
-  <si>
-    <t>31.08.202416</t>
-  </si>
-  <si>
-    <t>31.08.202417</t>
-  </si>
-  <si>
-    <t>31.08.202418</t>
-  </si>
-  <si>
-    <t>31.08.202419</t>
-  </si>
-  <si>
-    <t>31.08.202420</t>
-  </si>
-  <si>
-    <t>31.08.202421</t>
-  </si>
-  <si>
-    <t>31.08.202422</t>
-  </si>
-  <si>
-    <t>31.08.202423</t>
-  </si>
-  <si>
-    <t>31.08.202424</t>
-  </si>
-  <si>
-    <t>01.09.20241</t>
-  </si>
-  <si>
-    <t>01.09.20242</t>
-  </si>
-  <si>
-    <t>01.09.20243</t>
-  </si>
-  <si>
-    <t>01.09.20244</t>
-  </si>
-  <si>
-    <t>01.09.20245</t>
-  </si>
-  <si>
-    <t>01.09.20246</t>
-  </si>
-  <si>
-    <t>01.09.20247</t>
-  </si>
-  <si>
-    <t>01.09.20248</t>
-  </si>
-  <si>
-    <t>01.09.20249</t>
-  </si>
-  <si>
-    <t>01.09.202410</t>
-  </si>
-  <si>
-    <t>01.09.202411</t>
-  </si>
-  <si>
-    <t>01.09.202412</t>
-  </si>
-  <si>
-    <t>01.09.202413</t>
-  </si>
-  <si>
-    <t>01.09.202414</t>
-  </si>
-  <si>
-    <t>01.09.202415</t>
-  </si>
-  <si>
-    <t>01.09.202416</t>
-  </si>
-  <si>
-    <t>01.09.202417</t>
-  </si>
-  <si>
-    <t>01.09.202418</t>
-  </si>
-  <si>
-    <t>01.09.202419</t>
-  </si>
-  <si>
-    <t>01.09.202420</t>
-  </si>
-  <si>
-    <t>01.09.202421</t>
-  </si>
-  <si>
-    <t>01.09.202422</t>
-  </si>
-  <si>
-    <t>01.09.202423</t>
-  </si>
-  <si>
-    <t>01.09.202424</t>
-  </si>
-  <si>
-    <t>02.09.20241</t>
-  </si>
-  <si>
-    <t>02.09.20242</t>
-  </si>
-  <si>
-    <t>02.09.20243</t>
-  </si>
-  <si>
-    <t>02.09.20244</t>
-  </si>
-  <si>
-    <t>02.09.20245</t>
-  </si>
-  <si>
-    <t>02.09.20246</t>
-  </si>
-  <si>
-    <t>02.09.20247</t>
-  </si>
-  <si>
-    <t>02.09.20248</t>
-  </si>
-  <si>
-    <t>02.09.20249</t>
-  </si>
-  <si>
-    <t>02.09.202410</t>
-  </si>
-  <si>
-    <t>02.09.202411</t>
-  </si>
-  <si>
-    <t>02.09.202412</t>
-  </si>
-  <si>
-    <t>02.09.202413</t>
-  </si>
-  <si>
-    <t>02.09.202414</t>
-  </si>
-  <si>
-    <t>02.09.202415</t>
-  </si>
-  <si>
-    <t>02.09.202416</t>
-  </si>
-  <si>
-    <t>02.09.202417</t>
-  </si>
-  <si>
-    <t>02.09.202418</t>
-  </si>
-  <si>
-    <t>02.09.202419</t>
-  </si>
-  <si>
-    <t>02.09.202420</t>
-  </si>
-  <si>
-    <t>02.09.202421</t>
-  </si>
-  <si>
-    <t>02.09.202422</t>
-  </si>
-  <si>
-    <t>02.09.202423</t>
-  </si>
-  <si>
-    <t>02.09.202424</t>
-  </si>
-  <si>
-    <t>03.09.20241</t>
-  </si>
-  <si>
-    <t>03.09.20242</t>
-  </si>
-  <si>
-    <t>03.09.20243</t>
-  </si>
-  <si>
-    <t>03.09.20244</t>
-  </si>
-  <si>
-    <t>03.09.20245</t>
-  </si>
-  <si>
-    <t>03.09.20246</t>
-  </si>
-  <si>
-    <t>03.09.20247</t>
-  </si>
-  <si>
-    <t>03.09.20248</t>
-  </si>
-  <si>
-    <t>03.09.20249</t>
-  </si>
-  <si>
-    <t>03.09.202410</t>
-  </si>
-  <si>
-    <t>03.09.202411</t>
-  </si>
-  <si>
-    <t>03.09.202412</t>
-  </si>
-  <si>
-    <t>03.09.202413</t>
-  </si>
-  <si>
-    <t>03.09.202414</t>
-  </si>
-  <si>
-    <t>03.09.202415</t>
-  </si>
-  <si>
-    <t>03.09.202416</t>
-  </si>
-  <si>
-    <t>03.09.202417</t>
-  </si>
-  <si>
-    <t>03.09.202418</t>
-  </si>
-  <si>
-    <t>03.09.202419</t>
-  </si>
-  <si>
-    <t>03.09.202420</t>
-  </si>
-  <si>
-    <t>03.09.202421</t>
-  </si>
-  <si>
-    <t>03.09.202422</t>
-  </si>
-  <si>
-    <t>03.09.202423</t>
-  </si>
-  <si>
-    <t>03.09.202424</t>
-  </si>
-  <si>
-    <t>04.09.20241</t>
-  </si>
-  <si>
-    <t>04.09.20242</t>
-  </si>
-  <si>
-    <t>04.09.20243</t>
-  </si>
-  <si>
-    <t>04.09.20244</t>
-  </si>
-  <si>
-    <t>04.09.20245</t>
-  </si>
-  <si>
-    <t>04.09.20246</t>
-  </si>
-  <si>
-    <t>04.09.20247</t>
-  </si>
-  <si>
-    <t>04.09.20248</t>
-  </si>
-  <si>
-    <t>04.09.20249</t>
-  </si>
-  <si>
-    <t>04.09.202410</t>
-  </si>
-  <si>
-    <t>04.09.202411</t>
-  </si>
-  <si>
-    <t>04.09.202412</t>
-  </si>
-  <si>
-    <t>04.09.202413</t>
-  </si>
-  <si>
-    <t>04.09.202414</t>
-  </si>
-  <si>
-    <t>04.09.202415</t>
-  </si>
-  <si>
-    <t>04.09.202416</t>
-  </si>
-  <si>
-    <t>04.09.202417</t>
-  </si>
-  <si>
-    <t>04.09.202418</t>
-  </si>
-  <si>
-    <t>04.09.202419</t>
-  </si>
-  <si>
-    <t>04.09.202420</t>
-  </si>
-  <si>
-    <t>04.09.202421</t>
-  </si>
-  <si>
-    <t>04.09.202422</t>
-  </si>
-  <si>
-    <t>04.09.202423</t>
-  </si>
-  <si>
-    <t>04.09.202424</t>
-  </si>
-  <si>
-    <t>05.09.20241</t>
-  </si>
-  <si>
-    <t>05.09.20242</t>
-  </si>
-  <si>
-    <t>05.09.20243</t>
-  </si>
-  <si>
-    <t>05.09.20244</t>
-  </si>
-  <si>
-    <t>05.09.20245</t>
-  </si>
-  <si>
-    <t>05.09.20246</t>
-  </si>
-  <si>
-    <t>05.09.20247</t>
-  </si>
-  <si>
-    <t>05.09.20248</t>
-  </si>
-  <si>
-    <t>05.09.20249</t>
-  </si>
-  <si>
-    <t>05.09.202410</t>
-  </si>
-  <si>
-    <t>05.09.202411</t>
+    <t>15.09.202411</t>
+  </si>
+  <si>
+    <t>15.09.202412</t>
+  </si>
+  <si>
+    <t>15.09.202413</t>
+  </si>
+  <si>
+    <t>15.09.202414</t>
+  </si>
+  <si>
+    <t>15.09.202415</t>
+  </si>
+  <si>
+    <t>15.09.202416</t>
+  </si>
+  <si>
+    <t>15.09.202417</t>
+  </si>
+  <si>
+    <t>15.09.202418</t>
+  </si>
+  <si>
+    <t>15.09.202419</t>
+  </si>
+  <si>
+    <t>15.09.202420</t>
+  </si>
+  <si>
+    <t>15.09.202421</t>
+  </si>
+  <si>
+    <t>15.09.202422</t>
+  </si>
+  <si>
+    <t>15.09.202423</t>
+  </si>
+  <si>
+    <t>15.09.202424</t>
+  </si>
+  <si>
+    <t>16.09.20241</t>
+  </si>
+  <si>
+    <t>16.09.20242</t>
+  </si>
+  <si>
+    <t>16.09.20243</t>
+  </si>
+  <si>
+    <t>16.09.20244</t>
+  </si>
+  <si>
+    <t>16.09.20245</t>
+  </si>
+  <si>
+    <t>16.09.20246</t>
+  </si>
+  <si>
+    <t>16.09.20247</t>
+  </si>
+  <si>
+    <t>16.09.20248</t>
+  </si>
+  <si>
+    <t>16.09.20249</t>
+  </si>
+  <si>
+    <t>16.09.202410</t>
+  </si>
+  <si>
+    <t>16.09.202411</t>
+  </si>
+  <si>
+    <t>16.09.202412</t>
+  </si>
+  <si>
+    <t>16.09.202413</t>
+  </si>
+  <si>
+    <t>16.09.202414</t>
+  </si>
+  <si>
+    <t>16.09.202415</t>
+  </si>
+  <si>
+    <t>16.09.202416</t>
+  </si>
+  <si>
+    <t>16.09.202417</t>
+  </si>
+  <si>
+    <t>16.09.202418</t>
+  </si>
+  <si>
+    <t>16.09.202419</t>
+  </si>
+  <si>
+    <t>16.09.202420</t>
+  </si>
+  <si>
+    <t>16.09.202421</t>
+  </si>
+  <si>
+    <t>16.09.202422</t>
+  </si>
+  <si>
+    <t>16.09.202423</t>
+  </si>
+  <si>
+    <t>16.09.202424</t>
+  </si>
+  <si>
+    <t>17.09.20241</t>
+  </si>
+  <si>
+    <t>17.09.20242</t>
+  </si>
+  <si>
+    <t>17.09.20243</t>
+  </si>
+  <si>
+    <t>17.09.20244</t>
+  </si>
+  <si>
+    <t>17.09.20245</t>
+  </si>
+  <si>
+    <t>17.09.20246</t>
+  </si>
+  <si>
+    <t>17.09.20247</t>
+  </si>
+  <si>
+    <t>17.09.20248</t>
+  </si>
+  <si>
+    <t>17.09.20249</t>
+  </si>
+  <si>
+    <t>17.09.202410</t>
+  </si>
+  <si>
+    <t>17.09.202411</t>
+  </si>
+  <si>
+    <t>17.09.202412</t>
+  </si>
+  <si>
+    <t>17.09.202413</t>
+  </si>
+  <si>
+    <t>17.09.202414</t>
+  </si>
+  <si>
+    <t>17.09.202415</t>
+  </si>
+  <si>
+    <t>17.09.202416</t>
+  </si>
+  <si>
+    <t>17.09.202417</t>
+  </si>
+  <si>
+    <t>17.09.202418</t>
+  </si>
+  <si>
+    <t>17.09.202419</t>
+  </si>
+  <si>
+    <t>17.09.202420</t>
+  </si>
+  <si>
+    <t>17.09.202421</t>
+  </si>
+  <si>
+    <t>17.09.202422</t>
+  </si>
+  <si>
+    <t>17.09.202423</t>
+  </si>
+  <si>
+    <t>17.09.202424</t>
+  </si>
+  <si>
+    <t>18.09.20241</t>
+  </si>
+  <si>
+    <t>18.09.20242</t>
+  </si>
+  <si>
+    <t>18.09.20243</t>
+  </si>
+  <si>
+    <t>18.09.20244</t>
+  </si>
+  <si>
+    <t>18.09.20245</t>
+  </si>
+  <si>
+    <t>18.09.20246</t>
+  </si>
+  <si>
+    <t>18.09.20247</t>
+  </si>
+  <si>
+    <t>18.09.20248</t>
+  </si>
+  <si>
+    <t>18.09.20249</t>
+  </si>
+  <si>
+    <t>18.09.202410</t>
+  </si>
+  <si>
+    <t>18.09.202411</t>
+  </si>
+  <si>
+    <t>18.09.202412</t>
+  </si>
+  <si>
+    <t>18.09.202413</t>
+  </si>
+  <si>
+    <t>18.09.202414</t>
+  </si>
+  <si>
+    <t>18.09.202415</t>
+  </si>
+  <si>
+    <t>18.09.202416</t>
+  </si>
+  <si>
+    <t>18.09.202417</t>
+  </si>
+  <si>
+    <t>18.09.202418</t>
+  </si>
+  <si>
+    <t>18.09.202419</t>
+  </si>
+  <si>
+    <t>18.09.202420</t>
+  </si>
+  <si>
+    <t>18.09.202421</t>
+  </si>
+  <si>
+    <t>18.09.202422</t>
+  </si>
+  <si>
+    <t>18.09.202423</t>
+  </si>
+  <si>
+    <t>18.09.202424</t>
+  </si>
+  <si>
+    <t>19.09.20241</t>
+  </si>
+  <si>
+    <t>19.09.20242</t>
+  </si>
+  <si>
+    <t>19.09.20243</t>
+  </si>
+  <si>
+    <t>19.09.20244</t>
+  </si>
+  <si>
+    <t>19.09.20245</t>
+  </si>
+  <si>
+    <t>19.09.20246</t>
+  </si>
+  <si>
+    <t>19.09.20247</t>
+  </si>
+  <si>
+    <t>19.09.20248</t>
+  </si>
+  <si>
+    <t>19.09.20249</t>
+  </si>
+  <si>
+    <t>19.09.202410</t>
+  </si>
+  <si>
+    <t>19.09.202411</t>
+  </si>
+  <si>
+    <t>19.09.202412</t>
+  </si>
+  <si>
+    <t>19.09.202413</t>
+  </si>
+  <si>
+    <t>19.09.202414</t>
+  </si>
+  <si>
+    <t>19.09.202415</t>
+  </si>
+  <si>
+    <t>19.09.202416</t>
+  </si>
+  <si>
+    <t>19.09.202417</t>
+  </si>
+  <si>
+    <t>19.09.202418</t>
+  </si>
+  <si>
+    <t>19.09.202419</t>
+  </si>
+  <si>
+    <t>19.09.202420</t>
+  </si>
+  <si>
+    <t>19.09.202421</t>
+  </si>
+  <si>
+    <t>19.09.202422</t>
+  </si>
+  <si>
+    <t>19.09.202423</t>
+  </si>
+  <si>
+    <t>19.09.202424</t>
+  </si>
+  <si>
+    <t>20.09.20241</t>
+  </si>
+  <si>
+    <t>20.09.20242</t>
+  </si>
+  <si>
+    <t>20.09.20243</t>
+  </si>
+  <si>
+    <t>20.09.20244</t>
+  </si>
+  <si>
+    <t>20.09.20245</t>
+  </si>
+  <si>
+    <t>20.09.20246</t>
+  </si>
+  <si>
+    <t>20.09.20247</t>
+  </si>
+  <si>
+    <t>20.09.20248</t>
+  </si>
+  <si>
+    <t>20.09.20249</t>
+  </si>
+  <si>
+    <t>20.09.202410</t>
+  </si>
+  <si>
+    <t>20.09.202411</t>
+  </si>
+  <si>
+    <t>20.09.202412</t>
+  </si>
+  <si>
+    <t>20.09.202413</t>
+  </si>
+  <si>
+    <t>20.09.202414</t>
+  </si>
+  <si>
+    <t>20.09.202415</t>
+  </si>
+  <si>
+    <t>20.09.202416</t>
+  </si>
+  <si>
+    <t>20.09.202417</t>
+  </si>
+  <si>
+    <t>20.09.202418</t>
+  </si>
+  <si>
+    <t>20.09.202419</t>
+  </si>
+  <si>
+    <t>20.09.202420</t>
+  </si>
+  <si>
+    <t>20.09.202421</t>
+  </si>
+  <si>
+    <t>20.09.202422</t>
+  </si>
+  <si>
+    <t>20.09.202423</t>
+  </si>
+  <si>
+    <t>20.09.202424</t>
+  </si>
+  <si>
+    <t>21.09.20241</t>
+  </si>
+  <si>
+    <t>21.09.20242</t>
+  </si>
+  <si>
+    <t>21.09.20243</t>
+  </si>
+  <si>
+    <t>21.09.20244</t>
+  </si>
+  <si>
+    <t>21.09.20245</t>
+  </si>
+  <si>
+    <t>21.09.20246</t>
+  </si>
+  <si>
+    <t>21.09.20247</t>
+  </si>
+  <si>
+    <t>21.09.20248</t>
+  </si>
+  <si>
+    <t>21.09.20249</t>
+  </si>
+  <si>
+    <t>21.09.202410</t>
+  </si>
+  <si>
+    <t>21.09.202411</t>
+  </si>
+  <si>
+    <t>21.09.202412</t>
+  </si>
+  <si>
+    <t>21.09.202413</t>
+  </si>
+  <si>
+    <t>21.09.202414</t>
+  </si>
+  <si>
+    <t>21.09.202415</t>
+  </si>
+  <si>
+    <t>21.09.202416</t>
+  </si>
+  <si>
+    <t>21.09.202417</t>
+  </si>
+  <si>
+    <t>21.09.202418</t>
+  </si>
+  <si>
+    <t>21.09.202419</t>
+  </si>
+  <si>
+    <t>21.09.202420</t>
+  </si>
+  <si>
+    <t>21.09.202421</t>
+  </si>
+  <si>
+    <t>21.09.202422</t>
+  </si>
+  <si>
+    <t>21.09.202423</t>
+  </si>
+  <si>
+    <t>21.09.202424</t>
+  </si>
+  <si>
+    <t>22.09.20241</t>
+  </si>
+  <si>
+    <t>22.09.20242</t>
+  </si>
+  <si>
+    <t>22.09.20243</t>
+  </si>
+  <si>
+    <t>22.09.20244</t>
+  </si>
+  <si>
+    <t>22.09.20245</t>
+  </si>
+  <si>
+    <t>22.09.20246</t>
+  </si>
+  <si>
+    <t>22.09.20247</t>
+  </si>
+  <si>
+    <t>22.09.20248</t>
+  </si>
+  <si>
+    <t>22.09.20249</t>
+  </si>
+  <si>
+    <t>22.09.202410</t>
+  </si>
+  <si>
+    <t>22.09.202411</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B4">
         <v>13</v>
       </c>
       <c r="C4">
-        <v>2.834</v>
+        <v>3.1</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B5">
         <v>14</v>
       </c>
       <c r="C5">
-        <v>2.195</v>
+        <v>3.155</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6">
-        <v>1.713</v>
+        <v>2.66</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
       <c r="C7">
-        <v>1.721</v>
+        <v>2.344</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B8">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>1.446</v>
+        <v>1.969</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>0.848</v>
+        <v>1.073</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B10">
         <v>19</v>
       </c>
       <c r="C10">
-        <v>0.351</v>
+        <v>0.344</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B11">
         <v>20</v>
       </c>
       <c r="C11">
-        <v>0.045</v>
+        <v>0.033</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B12">
         <v>21</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B13">
         <v>22</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B14">
         <v>23</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45533</v>
+        <v>45550</v>
       </c>
       <c r="B15">
         <v>24</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B23">
         <v>8</v>
       </c>
       <c r="C23">
-        <v>0.079</v>
+        <v>0.039</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B24">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0.481</v>
+        <v>0.18</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25">
-        <v>0.889</v>
+        <v>0.422</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B26">
         <v>11</v>
       </c>
       <c r="C26">
-        <v>1.405</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B27">
         <v>12</v>
       </c>
       <c r="C27">
-        <v>1.637</v>
+        <v>0.84</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B28">
         <v>13</v>
       </c>
       <c r="C28">
-        <v>1.827</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B29">
         <v>14</v>
       </c>
       <c r="C29">
-        <v>1.79</v>
+        <v>0.951</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B30">
         <v>15</v>
       </c>
       <c r="C30">
-        <v>1.793</v>
+        <v>1.005</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B31">
         <v>16</v>
       </c>
       <c r="C31">
-        <v>1.699</v>
+        <v>1.231</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B32">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>1.573</v>
+        <v>1.141</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B33">
         <v>18</v>
       </c>
       <c r="C33">
-        <v>0.9350000000000001</v>
+        <v>0.71</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B34">
         <v>19</v>
       </c>
       <c r="C34">
-        <v>0.437</v>
+        <v>0.234</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B35">
         <v>20</v>
       </c>
       <c r="C35">
-        <v>0.054</v>
+        <v>0.022</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B36">
         <v>21</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B37">
         <v>22</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B38">
         <v>23</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45534</v>
+        <v>45551</v>
       </c>
       <c r="B39">
         <v>24</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B46">
         <v>7</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
       <c r="C47">
-        <v>0.105</v>
+        <v>0.04</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B48">
         <v>9</v>
       </c>
       <c r="C48">
-        <v>0.711</v>
+        <v>0.278</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B49">
         <v>10</v>
       </c>
       <c r="C49">
-        <v>1.543</v>
+        <v>0.732</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B50">
         <v>11</v>
       </c>
       <c r="C50">
-        <v>1.977</v>
+        <v>1.165</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B51">
         <v>12</v>
       </c>
       <c r="C51">
-        <v>2.602</v>
+        <v>1.562</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B52">
         <v>13</v>
       </c>
       <c r="C52">
-        <v>2.975</v>
+        <v>1.954</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B53">
         <v>14</v>
       </c>
       <c r="C53">
-        <v>2.779</v>
+        <v>2.005</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B54">
         <v>15</v>
       </c>
       <c r="C54">
-        <v>2.486</v>
+        <v>1.978</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B55">
         <v>16</v>
       </c>
       <c r="C55">
-        <v>2.08</v>
+        <v>1.653</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B56">
         <v>17</v>
       </c>
       <c r="C56">
-        <v>1.704</v>
+        <v>1.1</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
       <c r="C57">
-        <v>1.132</v>
+        <v>0.711</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B58">
         <v>19</v>
       </c>
       <c r="C58">
-        <v>0.503</v>
+        <v>0.177</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B59">
         <v>20</v>
       </c>
       <c r="C59">
-        <v>0.067</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B60">
         <v>21</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B61">
         <v>22</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B62">
         <v>23</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45535</v>
+        <v>45552</v>
       </c>
       <c r="B63">
         <v>24</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B67">
         <v>4</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B69">
         <v>6</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B70">
         <v>7</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B71">
         <v>8</v>
       </c>
       <c r="C71">
-        <v>0.061</v>
+        <v>0.038</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B72">
         <v>9</v>
       </c>
       <c r="C72">
-        <v>0.413</v>
+        <v>0.277</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B73">
         <v>10</v>
       </c>
       <c r="C73">
-        <v>0.853</v>
+        <v>0.728</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B74">
         <v>11</v>
       </c>
       <c r="C74">
-        <v>1.312</v>
+        <v>1.092</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B75">
         <v>12</v>
       </c>
       <c r="C75">
-        <v>1.915</v>
+        <v>1.338</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B76">
         <v>13</v>
       </c>
       <c r="C76">
-        <v>2.105</v>
+        <v>1.605</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B77">
         <v>14</v>
       </c>
       <c r="C77">
-        <v>2.225</v>
+        <v>1.79</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B78">
         <v>15</v>
       </c>
       <c r="C78">
-        <v>2.277</v>
+        <v>1.638</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B79">
         <v>16</v>
       </c>
       <c r="C79">
-        <v>2.103</v>
+        <v>1.429</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B80">
         <v>17</v>
       </c>
       <c r="C80">
-        <v>1.803</v>
+        <v>0.968</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B81">
         <v>18</v>
       </c>
       <c r="C81">
-        <v>1.09</v>
+        <v>0.543</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B82">
         <v>19</v>
       </c>
       <c r="C82">
-        <v>0.39</v>
+        <v>0.122</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B83">
         <v>20</v>
       </c>
       <c r="C83">
-        <v>0.046</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B84">
         <v>21</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B85">
         <v>22</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B86">
         <v>23</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45536</v>
+        <v>45553</v>
       </c>
       <c r="B87">
         <v>24</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B91">
         <v>4</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B92">
         <v>5</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B93">
         <v>6</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B94">
         <v>7</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B95">
         <v>8</v>
       </c>
       <c r="C95">
-        <v>0.097</v>
+        <v>0.043</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B96">
         <v>9</v>
       </c>
       <c r="C96">
-        <v>0.789</v>
+        <v>0.409</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B97">
         <v>10</v>
       </c>
       <c r="C97">
-        <v>1.724</v>
+        <v>1.029</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B98">
         <v>11</v>
       </c>
       <c r="C98">
-        <v>2.294</v>
+        <v>1.924</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B99">
         <v>12</v>
       </c>
       <c r="C99">
-        <v>2.86</v>
+        <v>2.333</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B100">
         <v>13</v>
       </c>
       <c r="C100">
-        <v>3.07</v>
+        <v>2.572</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B101">
         <v>14</v>
       </c>
       <c r="C101">
-        <v>3.066</v>
+        <v>2.647</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B102">
         <v>15</v>
       </c>
       <c r="C102">
-        <v>3.008</v>
+        <v>2.53</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B103">
         <v>16</v>
       </c>
       <c r="C103">
-        <v>2.67</v>
+        <v>2.204</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B104">
         <v>17</v>
       </c>
       <c r="C104">
-        <v>1.982</v>
+        <v>1.737</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B105">
         <v>18</v>
       </c>
       <c r="C105">
-        <v>1.121</v>
+        <v>0.831</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B106">
         <v>19</v>
       </c>
       <c r="C106">
-        <v>0.46</v>
+        <v>0.226</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B107">
         <v>20</v>
       </c>
       <c r="C107">
-        <v>0.054</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B108">
         <v>21</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B109">
         <v>22</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B110">
         <v>23</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45537</v>
+        <v>45554</v>
       </c>
       <c r="B111">
         <v>24</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B116">
         <v>5</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B117">
         <v>6</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B118">
         <v>7</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B119">
         <v>8</v>
       </c>
       <c r="C119">
-        <v>0.1</v>
+        <v>0.057</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B120">
         <v>9</v>
       </c>
       <c r="C120">
-        <v>0.65</v>
+        <v>0.656</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B121">
         <v>10</v>
       </c>
       <c r="C121">
-        <v>1.621</v>
+        <v>1.557</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B122">
         <v>11</v>
       </c>
       <c r="C122">
-        <v>2.291</v>
+        <v>2.391</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B123">
         <v>12</v>
       </c>
       <c r="C123">
-        <v>2.77</v>
+        <v>2.817</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B124">
         <v>13</v>
       </c>
       <c r="C124">
-        <v>3.003</v>
+        <v>3.068</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B125">
         <v>14</v>
       </c>
       <c r="C125">
-        <v>3.067</v>
+        <v>3.1</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B126">
         <v>15</v>
       </c>
       <c r="C126">
-        <v>2.965</v>
+        <v>2.901</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B127">
         <v>16</v>
       </c>
       <c r="C127">
-        <v>2.646</v>
+        <v>2.579</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B128">
         <v>17</v>
       </c>
       <c r="C128">
-        <v>2.011</v>
+        <v>1.942</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B129">
         <v>18</v>
       </c>
       <c r="C129">
-        <v>1.153</v>
+        <v>1.113</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B130">
         <v>19</v>
       </c>
       <c r="C130">
-        <v>0.459</v>
+        <v>0.3</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B131">
         <v>20</v>
       </c>
       <c r="C131">
-        <v>0.065</v>
+        <v>0.021</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B132">
         <v>21</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B133">
         <v>22</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B134">
         <v>23</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45538</v>
+        <v>45555</v>
       </c>
       <c r="B135">
         <v>24</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B137">
         <v>2</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B138">
         <v>3</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B139">
         <v>4</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B140">
         <v>5</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B141">
         <v>6</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B142">
         <v>7</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B143">
         <v>8</v>
       </c>
       <c r="C143">
-        <v>0.098</v>
+        <v>0.057</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B144">
         <v>9</v>
       </c>
       <c r="C144">
-        <v>0.649</v>
+        <v>0.553</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B145">
         <v>10</v>
       </c>
       <c r="C145">
-        <v>1.662</v>
+        <v>1.483</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B146">
         <v>11</v>
       </c>
       <c r="C146">
-        <v>2.289</v>
+        <v>2.282</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B147">
         <v>12</v>
       </c>
       <c r="C147">
-        <v>2.778</v>
+        <v>2.798</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B148">
         <v>13</v>
       </c>
       <c r="C148">
-        <v>3.069</v>
+        <v>2.974</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B149">
         <v>14</v>
       </c>
       <c r="C149">
-        <v>3.066</v>
+        <v>2.992</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B150">
         <v>15</v>
       </c>
       <c r="C150">
-        <v>3.008</v>
+        <v>2.833</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B151">
         <v>16</v>
       </c>
       <c r="C151">
-        <v>2.67</v>
+        <v>2.285</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B152">
         <v>17</v>
       </c>
       <c r="C152">
-        <v>2.1</v>
+        <v>1.92</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B153">
         <v>18</v>
       </c>
       <c r="C153">
-        <v>1.162</v>
+        <v>0.998</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B154">
         <v>19</v>
       </c>
       <c r="C154">
-        <v>0.507</v>
+        <v>0.179</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B155">
         <v>20</v>
       </c>
       <c r="C155">
-        <v>0.065</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B156">
         <v>21</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B157">
         <v>22</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B158">
         <v>23</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45539</v>
+        <v>45556</v>
       </c>
       <c r="B159">
         <v>24</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B161">
         <v>2</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B162">
         <v>3</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B163">
         <v>4</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B164">
         <v>5</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B165">
         <v>6</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B166">
         <v>7</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B167">
         <v>8</v>
       </c>
       <c r="C167">
-        <v>0.1</v>
+        <v>0.046</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B168">
         <v>9</v>
       </c>
       <c r="C168">
-        <v>0.743</v>
+        <v>0.552</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B169">
         <v>10</v>
       </c>
       <c r="C169">
-        <v>1.66</v>
+        <v>1.479</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45540</v>
+        <v>45557</v>
       </c>
       <c r="B170">
         <v>11</v>
       </c>
       <c r="C170">
-        <v>2.295</v>
+        <v>2.188</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the RES Hourly Production Forecast to the Portfolio
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,222 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>15.09.202411</t>
-  </si>
-  <si>
-    <t>15.09.202412</t>
-  </si>
-  <si>
-    <t>15.09.202413</t>
-  </si>
-  <si>
-    <t>15.09.202414</t>
-  </si>
-  <si>
-    <t>15.09.202415</t>
-  </si>
-  <si>
-    <t>15.09.202416</t>
-  </si>
-  <si>
-    <t>15.09.202417</t>
-  </si>
-  <si>
-    <t>15.09.202418</t>
-  </si>
-  <si>
-    <t>15.09.202419</t>
-  </si>
-  <si>
-    <t>15.09.202420</t>
-  </si>
-  <si>
-    <t>15.09.202421</t>
-  </si>
-  <si>
-    <t>15.09.202422</t>
-  </si>
-  <si>
-    <t>15.09.202423</t>
-  </si>
-  <si>
-    <t>15.09.202424</t>
-  </si>
-  <si>
-    <t>16.09.20241</t>
-  </si>
-  <si>
-    <t>16.09.20242</t>
-  </si>
-  <si>
-    <t>16.09.20243</t>
-  </si>
-  <si>
-    <t>16.09.20244</t>
-  </si>
-  <si>
-    <t>16.09.20245</t>
-  </si>
-  <si>
-    <t>16.09.20246</t>
-  </si>
-  <si>
-    <t>16.09.20247</t>
-  </si>
-  <si>
-    <t>16.09.20248</t>
-  </si>
-  <si>
-    <t>16.09.20249</t>
-  </si>
-  <si>
-    <t>16.09.202410</t>
-  </si>
-  <si>
-    <t>16.09.202411</t>
-  </si>
-  <si>
-    <t>16.09.202412</t>
-  </si>
-  <si>
-    <t>16.09.202413</t>
-  </si>
-  <si>
-    <t>16.09.202414</t>
-  </si>
-  <si>
-    <t>16.09.202415</t>
-  </si>
-  <si>
-    <t>16.09.202416</t>
-  </si>
-  <si>
-    <t>16.09.202417</t>
-  </si>
-  <si>
-    <t>16.09.202418</t>
-  </si>
-  <si>
-    <t>16.09.202419</t>
-  </si>
-  <si>
-    <t>16.09.202420</t>
-  </si>
-  <si>
-    <t>16.09.202421</t>
-  </si>
-  <si>
-    <t>16.09.202422</t>
-  </si>
-  <si>
-    <t>16.09.202423</t>
-  </si>
-  <si>
-    <t>16.09.202424</t>
-  </si>
-  <si>
-    <t>17.09.20241</t>
-  </si>
-  <si>
-    <t>17.09.20242</t>
-  </si>
-  <si>
-    <t>17.09.20243</t>
-  </si>
-  <si>
-    <t>17.09.20244</t>
-  </si>
-  <si>
-    <t>17.09.20245</t>
-  </si>
-  <si>
-    <t>17.09.20246</t>
-  </si>
-  <si>
-    <t>17.09.20247</t>
-  </si>
-  <si>
-    <t>17.09.20248</t>
-  </si>
-  <si>
-    <t>17.09.20249</t>
-  </si>
-  <si>
-    <t>17.09.202410</t>
-  </si>
-  <si>
-    <t>17.09.202411</t>
-  </si>
-  <si>
-    <t>17.09.202412</t>
-  </si>
-  <si>
-    <t>17.09.202413</t>
-  </si>
-  <si>
-    <t>17.09.202414</t>
-  </si>
-  <si>
-    <t>17.09.202415</t>
-  </si>
-  <si>
-    <t>17.09.202416</t>
-  </si>
-  <si>
-    <t>17.09.202417</t>
-  </si>
-  <si>
-    <t>17.09.202418</t>
-  </si>
-  <si>
-    <t>17.09.202419</t>
-  </si>
-  <si>
-    <t>17.09.202420</t>
-  </si>
-  <si>
-    <t>17.09.202421</t>
-  </si>
-  <si>
-    <t>17.09.202422</t>
-  </si>
-  <si>
-    <t>17.09.202423</t>
-  </si>
-  <si>
-    <t>17.09.202424</t>
-  </si>
-  <si>
-    <t>18.09.20241</t>
-  </si>
-  <si>
-    <t>18.09.20242</t>
-  </si>
-  <si>
-    <t>18.09.20243</t>
-  </si>
-  <si>
-    <t>18.09.20244</t>
-  </si>
-  <si>
-    <t>18.09.20245</t>
-  </si>
-  <si>
-    <t>18.09.20246</t>
-  </si>
-  <si>
-    <t>18.09.20247</t>
-  </si>
-  <si>
-    <t>18.09.20248</t>
-  </si>
-  <si>
-    <t>18.09.20249</t>
-  </si>
-  <si>
-    <t>18.09.202410</t>
-  </si>
-  <si>
     <t>18.09.202411</t>
   </si>
   <si>
@@ -533,6 +317,222 @@
   </si>
   <si>
     <t>22.09.202411</t>
+  </si>
+  <si>
+    <t>22.09.202412</t>
+  </si>
+  <si>
+    <t>22.09.202413</t>
+  </si>
+  <si>
+    <t>22.09.202414</t>
+  </si>
+  <si>
+    <t>22.09.202415</t>
+  </si>
+  <si>
+    <t>22.09.202416</t>
+  </si>
+  <si>
+    <t>22.09.202417</t>
+  </si>
+  <si>
+    <t>22.09.202418</t>
+  </si>
+  <si>
+    <t>22.09.202419</t>
+  </si>
+  <si>
+    <t>22.09.202420</t>
+  </si>
+  <si>
+    <t>22.09.202421</t>
+  </si>
+  <si>
+    <t>22.09.202422</t>
+  </si>
+  <si>
+    <t>22.09.202423</t>
+  </si>
+  <si>
+    <t>22.09.202424</t>
+  </si>
+  <si>
+    <t>23.09.20241</t>
+  </si>
+  <si>
+    <t>23.09.20242</t>
+  </si>
+  <si>
+    <t>23.09.20243</t>
+  </si>
+  <si>
+    <t>23.09.20244</t>
+  </si>
+  <si>
+    <t>23.09.20245</t>
+  </si>
+  <si>
+    <t>23.09.20246</t>
+  </si>
+  <si>
+    <t>23.09.20247</t>
+  </si>
+  <si>
+    <t>23.09.20248</t>
+  </si>
+  <si>
+    <t>23.09.20249</t>
+  </si>
+  <si>
+    <t>23.09.202410</t>
+  </si>
+  <si>
+    <t>23.09.202411</t>
+  </si>
+  <si>
+    <t>23.09.202412</t>
+  </si>
+  <si>
+    <t>23.09.202413</t>
+  </si>
+  <si>
+    <t>23.09.202414</t>
+  </si>
+  <si>
+    <t>23.09.202415</t>
+  </si>
+  <si>
+    <t>23.09.202416</t>
+  </si>
+  <si>
+    <t>23.09.202417</t>
+  </si>
+  <si>
+    <t>23.09.202418</t>
+  </si>
+  <si>
+    <t>23.09.202419</t>
+  </si>
+  <si>
+    <t>23.09.202420</t>
+  </si>
+  <si>
+    <t>23.09.202421</t>
+  </si>
+  <si>
+    <t>23.09.202422</t>
+  </si>
+  <si>
+    <t>23.09.202423</t>
+  </si>
+  <si>
+    <t>23.09.202424</t>
+  </si>
+  <si>
+    <t>24.09.20241</t>
+  </si>
+  <si>
+    <t>24.09.20242</t>
+  </si>
+  <si>
+    <t>24.09.20243</t>
+  </si>
+  <si>
+    <t>24.09.20244</t>
+  </si>
+  <si>
+    <t>24.09.20245</t>
+  </si>
+  <si>
+    <t>24.09.20246</t>
+  </si>
+  <si>
+    <t>24.09.20247</t>
+  </si>
+  <si>
+    <t>24.09.20248</t>
+  </si>
+  <si>
+    <t>24.09.20249</t>
+  </si>
+  <si>
+    <t>24.09.202410</t>
+  </si>
+  <si>
+    <t>24.09.202411</t>
+  </si>
+  <si>
+    <t>24.09.202412</t>
+  </si>
+  <si>
+    <t>24.09.202413</t>
+  </si>
+  <si>
+    <t>24.09.202414</t>
+  </si>
+  <si>
+    <t>24.09.202415</t>
+  </si>
+  <si>
+    <t>24.09.202416</t>
+  </si>
+  <si>
+    <t>24.09.202417</t>
+  </si>
+  <si>
+    <t>24.09.202418</t>
+  </si>
+  <si>
+    <t>24.09.202419</t>
+  </si>
+  <si>
+    <t>24.09.202420</t>
+  </si>
+  <si>
+    <t>24.09.202421</t>
+  </si>
+  <si>
+    <t>24.09.202422</t>
+  </si>
+  <si>
+    <t>24.09.202423</t>
+  </si>
+  <si>
+    <t>24.09.202424</t>
+  </si>
+  <si>
+    <t>25.09.20241</t>
+  </si>
+  <si>
+    <t>25.09.20242</t>
+  </si>
+  <si>
+    <t>25.09.20243</t>
+  </si>
+  <si>
+    <t>25.09.20244</t>
+  </si>
+  <si>
+    <t>25.09.20245</t>
+  </si>
+  <si>
+    <t>25.09.20246</t>
+  </si>
+  <si>
+    <t>25.09.20247</t>
+  </si>
+  <si>
+    <t>25.09.20248</t>
+  </si>
+  <si>
+    <t>25.09.20249</t>
+  </si>
+  <si>
+    <t>25.09.202410</t>
+  </si>
+  <si>
+    <t>25.09.202411</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B4">
         <v>13</v>
       </c>
       <c r="C4">
-        <v>3.1</v>
+        <v>2.968</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B5">
         <v>14</v>
       </c>
       <c r="C5">
-        <v>3.155</v>
+        <v>2.466</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6">
-        <v>2.66</v>
+        <v>2.119</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
       <c r="C7">
-        <v>2.344</v>
+        <v>1.865</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B8">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>1.969</v>
+        <v>1.325</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>1.073</v>
+        <v>0.766</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B10">
         <v>19</v>
       </c>
       <c r="C10">
-        <v>0.344</v>
+        <v>0.172</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B11">
         <v>20</v>
       </c>
       <c r="C11">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B12">
         <v>21</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B13">
         <v>22</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B14">
         <v>23</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45550</v>
+        <v>45553</v>
       </c>
       <c r="B15">
         <v>24</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B23">
         <v>8</v>
       </c>
       <c r="C23">
-        <v>0.039</v>
+        <v>0.057</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B24">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0.18</v>
+        <v>0.51</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25">
-        <v>0.422</v>
+        <v>1.323</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B26">
         <v>11</v>
       </c>
       <c r="C26">
-        <v>0.6850000000000001</v>
+        <v>1.792</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B27">
         <v>12</v>
       </c>
       <c r="C27">
-        <v>0.84</v>
+        <v>1.999</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B28">
         <v>13</v>
       </c>
       <c r="C28">
-        <v>0.9330000000000001</v>
+        <v>2.074</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B29">
         <v>14</v>
       </c>
       <c r="C29">
-        <v>0.951</v>
+        <v>1.994</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B30">
         <v>15</v>
       </c>
       <c r="C30">
-        <v>1.005</v>
+        <v>1.892</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B31">
         <v>16</v>
       </c>
       <c r="C31">
-        <v>1.231</v>
+        <v>1.533</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B32">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>1.141</v>
+        <v>0.98</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B33">
         <v>18</v>
       </c>
       <c r="C33">
-        <v>0.71</v>
+        <v>0.482</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B34">
         <v>19</v>
       </c>
       <c r="C34">
-        <v>0.234</v>
+        <v>0.118</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B35">
         <v>20</v>
       </c>
       <c r="C35">
-        <v>0.022</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B36">
         <v>21</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B37">
         <v>22</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B38">
         <v>23</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="B39">
         <v>24</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B46">
         <v>7</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
       <c r="C47">
-        <v>0.04</v>
+        <v>0.047</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B48">
         <v>9</v>
       </c>
       <c r="C48">
-        <v>0.278</v>
+        <v>0.504</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B49">
         <v>10</v>
       </c>
       <c r="C49">
-        <v>0.732</v>
+        <v>1.232</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B50">
         <v>11</v>
       </c>
       <c r="C50">
-        <v>1.165</v>
+        <v>2.048</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B51">
         <v>12</v>
       </c>
       <c r="C51">
-        <v>1.562</v>
+        <v>2.794</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B52">
         <v>13</v>
       </c>
       <c r="C52">
-        <v>1.954</v>
+        <v>2.991</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B53">
         <v>14</v>
       </c>
       <c r="C53">
-        <v>2.005</v>
+        <v>3.078</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B54">
         <v>15</v>
       </c>
       <c r="C54">
-        <v>1.978</v>
+        <v>2.911</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B55">
         <v>16</v>
       </c>
       <c r="C55">
-        <v>1.653</v>
+        <v>2.677</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B56">
         <v>17</v>
       </c>
       <c r="C56">
-        <v>1.1</v>
+        <v>1.912</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
       <c r="C57">
-        <v>0.711</v>
+        <v>0.953</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B58">
         <v>19</v>
       </c>
       <c r="C58">
-        <v>0.177</v>
+        <v>0.249</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B59">
         <v>20</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B60">
         <v>21</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B61">
         <v>22</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B62">
         <v>23</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="B63">
         <v>24</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B67">
         <v>4</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B69">
         <v>6</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B70">
         <v>7</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B71">
         <v>8</v>
       </c>
       <c r="C71">
-        <v>0.038</v>
+        <v>0.057</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B72">
         <v>9</v>
       </c>
       <c r="C72">
-        <v>0.277</v>
+        <v>0.658</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B73">
         <v>10</v>
       </c>
       <c r="C73">
-        <v>0.728</v>
+        <v>1.613</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B74">
         <v>11</v>
       </c>
       <c r="C74">
-        <v>1.092</v>
+        <v>2.391</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B75">
         <v>12</v>
       </c>
       <c r="C75">
-        <v>1.338</v>
+        <v>2.836</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B76">
         <v>13</v>
       </c>
       <c r="C76">
-        <v>1.605</v>
+        <v>2.992</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B77">
         <v>14</v>
       </c>
       <c r="C77">
-        <v>1.79</v>
+        <v>3.078</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B78">
         <v>15</v>
       </c>
       <c r="C78">
-        <v>1.638</v>
+        <v>2.897</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B79">
         <v>16</v>
       </c>
       <c r="C79">
-        <v>1.429</v>
+        <v>2.579</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B80">
         <v>17</v>
       </c>
       <c r="C80">
-        <v>0.968</v>
+        <v>1.942</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B81">
         <v>18</v>
       </c>
       <c r="C81">
-        <v>0.543</v>
+        <v>1.094</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B82">
         <v>19</v>
       </c>
       <c r="C82">
-        <v>0.122</v>
+        <v>0.226</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B83">
         <v>20</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B84">
         <v>21</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B85">
         <v>22</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B86">
         <v>23</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45553</v>
+        <v>45556</v>
       </c>
       <c r="B87">
         <v>24</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B91">
         <v>4</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B92">
         <v>5</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B93">
         <v>6</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B94">
         <v>7</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B95">
         <v>8</v>
       </c>
       <c r="C95">
-        <v>0.043</v>
+        <v>0.057</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B96">
         <v>9</v>
       </c>
       <c r="C96">
-        <v>0.409</v>
+        <v>0.552</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B97">
         <v>10</v>
       </c>
       <c r="C97">
-        <v>1.029</v>
+        <v>1.483</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B98">
         <v>11</v>
       </c>
       <c r="C98">
-        <v>1.924</v>
+        <v>2.282</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B99">
         <v>12</v>
       </c>
       <c r="C99">
-        <v>2.333</v>
+        <v>2.798</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B100">
         <v>13</v>
       </c>
       <c r="C100">
-        <v>2.572</v>
+        <v>2.968</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B101">
         <v>14</v>
       </c>
       <c r="C101">
-        <v>2.647</v>
+        <v>2.988</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B102">
         <v>15</v>
       </c>
       <c r="C102">
-        <v>2.53</v>
+        <v>2.815</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B103">
         <v>16</v>
       </c>
       <c r="C103">
-        <v>2.204</v>
+        <v>2.285</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B104">
         <v>17</v>
       </c>
       <c r="C104">
-        <v>1.737</v>
+        <v>1.847</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B105">
         <v>18</v>
       </c>
       <c r="C105">
-        <v>0.831</v>
+        <v>0.897</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B106">
         <v>19</v>
       </c>
       <c r="C106">
-        <v>0.226</v>
+        <v>0.182</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B107">
         <v>20</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B108">
         <v>21</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B109">
         <v>22</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B110">
         <v>23</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45554</v>
+        <v>45557</v>
       </c>
       <c r="B111">
         <v>24</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B116">
         <v>5</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B117">
         <v>6</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B118">
         <v>7</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B119">
         <v>8</v>
       </c>
       <c r="C119">
-        <v>0.057</v>
+        <v>0.046</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B120">
         <v>9</v>
       </c>
       <c r="C120">
-        <v>0.656</v>
+        <v>0.483</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B121">
         <v>10</v>
       </c>
       <c r="C121">
-        <v>1.557</v>
+        <v>1.477</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B122">
         <v>11</v>
       </c>
       <c r="C122">
-        <v>2.391</v>
+        <v>2.143</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B123">
         <v>12</v>
       </c>
       <c r="C123">
-        <v>2.817</v>
+        <v>2.685</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B124">
         <v>13</v>
       </c>
       <c r="C124">
-        <v>3.068</v>
+        <v>2.913</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B125">
         <v>14</v>
       </c>
       <c r="C125">
-        <v>3.1</v>
+        <v>2.954</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B126">
         <v>15</v>
       </c>
       <c r="C126">
-        <v>2.901</v>
+        <v>2.774</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B127">
         <v>16</v>
       </c>
       <c r="C127">
-        <v>2.579</v>
+        <v>2.28</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B128">
         <v>17</v>
       </c>
       <c r="C128">
-        <v>1.942</v>
+        <v>1.777</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B129">
         <v>18</v>
       </c>
       <c r="C129">
-        <v>1.113</v>
+        <v>0.905</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B130">
         <v>19</v>
       </c>
       <c r="C130">
-        <v>0.3</v>
+        <v>0.152</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B131">
         <v>20</v>
       </c>
       <c r="C131">
-        <v>0.021</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B132">
         <v>21</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B133">
         <v>22</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B134">
         <v>23</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="B135">
         <v>24</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B137">
         <v>2</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B138">
         <v>3</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B139">
         <v>4</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B140">
         <v>5</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B141">
         <v>6</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B142">
         <v>7</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B143">
         <v>8</v>
       </c>
       <c r="C143">
-        <v>0.057</v>
+        <v>0.041</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B144">
         <v>9</v>
       </c>
       <c r="C144">
-        <v>0.553</v>
+        <v>0.428</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B145">
         <v>10</v>
       </c>
       <c r="C145">
-        <v>1.483</v>
+        <v>1.191</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B146">
         <v>11</v>
       </c>
       <c r="C146">
-        <v>2.282</v>
+        <v>2.113</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B147">
         <v>12</v>
       </c>
       <c r="C147">
-        <v>2.798</v>
+        <v>2.549</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B148">
         <v>13</v>
       </c>
       <c r="C148">
-        <v>2.974</v>
+        <v>2.853</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B149">
         <v>14</v>
       </c>
       <c r="C149">
-        <v>2.992</v>
+        <v>2.898</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B150">
         <v>15</v>
       </c>
       <c r="C150">
-        <v>2.833</v>
+        <v>2.772</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B151">
         <v>16</v>
       </c>
       <c r="C151">
-        <v>2.285</v>
+        <v>2.27</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B152">
         <v>17</v>
       </c>
       <c r="C152">
-        <v>1.92</v>
+        <v>1.774</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B153">
         <v>18</v>
       </c>
       <c r="C153">
-        <v>0.998</v>
+        <v>0.904</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B154">
         <v>19</v>
       </c>
       <c r="C154">
-        <v>0.179</v>
+        <v>0.14</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B155">
         <v>20</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B156">
         <v>21</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B157">
         <v>22</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B158">
         <v>23</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="B159">
         <v>24</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B161">
         <v>2</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B162">
         <v>3</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B163">
         <v>4</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B164">
         <v>5</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B165">
         <v>6</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B166">
         <v>7</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B167">
         <v>8</v>
       </c>
       <c r="C167">
-        <v>0.046</v>
+        <v>0.042</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B168">
         <v>9</v>
       </c>
       <c r="C168">
-        <v>0.552</v>
+        <v>0.395</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B169">
         <v>10</v>
       </c>
       <c r="C169">
-        <v>1.479</v>
+        <v>1.114</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="B170">
         <v>11</v>
       </c>
       <c r="C170">
-        <v>2.188</v>
+        <v>2.073</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Revert "Adding the RES Hourly Production Forecast to the Portfolio"
This reverts commit 98951293087cc5082762df163c4479aa0528f2a3.
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb.xlsx
+++ b/Astro/Results_Production_Astro_xgb.xlsx
@@ -28,6 +28,222 @@
     <t>Lookup</t>
   </si>
   <si>
+    <t>15.09.202411</t>
+  </si>
+  <si>
+    <t>15.09.202412</t>
+  </si>
+  <si>
+    <t>15.09.202413</t>
+  </si>
+  <si>
+    <t>15.09.202414</t>
+  </si>
+  <si>
+    <t>15.09.202415</t>
+  </si>
+  <si>
+    <t>15.09.202416</t>
+  </si>
+  <si>
+    <t>15.09.202417</t>
+  </si>
+  <si>
+    <t>15.09.202418</t>
+  </si>
+  <si>
+    <t>15.09.202419</t>
+  </si>
+  <si>
+    <t>15.09.202420</t>
+  </si>
+  <si>
+    <t>15.09.202421</t>
+  </si>
+  <si>
+    <t>15.09.202422</t>
+  </si>
+  <si>
+    <t>15.09.202423</t>
+  </si>
+  <si>
+    <t>15.09.202424</t>
+  </si>
+  <si>
+    <t>16.09.20241</t>
+  </si>
+  <si>
+    <t>16.09.20242</t>
+  </si>
+  <si>
+    <t>16.09.20243</t>
+  </si>
+  <si>
+    <t>16.09.20244</t>
+  </si>
+  <si>
+    <t>16.09.20245</t>
+  </si>
+  <si>
+    <t>16.09.20246</t>
+  </si>
+  <si>
+    <t>16.09.20247</t>
+  </si>
+  <si>
+    <t>16.09.20248</t>
+  </si>
+  <si>
+    <t>16.09.20249</t>
+  </si>
+  <si>
+    <t>16.09.202410</t>
+  </si>
+  <si>
+    <t>16.09.202411</t>
+  </si>
+  <si>
+    <t>16.09.202412</t>
+  </si>
+  <si>
+    <t>16.09.202413</t>
+  </si>
+  <si>
+    <t>16.09.202414</t>
+  </si>
+  <si>
+    <t>16.09.202415</t>
+  </si>
+  <si>
+    <t>16.09.202416</t>
+  </si>
+  <si>
+    <t>16.09.202417</t>
+  </si>
+  <si>
+    <t>16.09.202418</t>
+  </si>
+  <si>
+    <t>16.09.202419</t>
+  </si>
+  <si>
+    <t>16.09.202420</t>
+  </si>
+  <si>
+    <t>16.09.202421</t>
+  </si>
+  <si>
+    <t>16.09.202422</t>
+  </si>
+  <si>
+    <t>16.09.202423</t>
+  </si>
+  <si>
+    <t>16.09.202424</t>
+  </si>
+  <si>
+    <t>17.09.20241</t>
+  </si>
+  <si>
+    <t>17.09.20242</t>
+  </si>
+  <si>
+    <t>17.09.20243</t>
+  </si>
+  <si>
+    <t>17.09.20244</t>
+  </si>
+  <si>
+    <t>17.09.20245</t>
+  </si>
+  <si>
+    <t>17.09.20246</t>
+  </si>
+  <si>
+    <t>17.09.20247</t>
+  </si>
+  <si>
+    <t>17.09.20248</t>
+  </si>
+  <si>
+    <t>17.09.20249</t>
+  </si>
+  <si>
+    <t>17.09.202410</t>
+  </si>
+  <si>
+    <t>17.09.202411</t>
+  </si>
+  <si>
+    <t>17.09.202412</t>
+  </si>
+  <si>
+    <t>17.09.202413</t>
+  </si>
+  <si>
+    <t>17.09.202414</t>
+  </si>
+  <si>
+    <t>17.09.202415</t>
+  </si>
+  <si>
+    <t>17.09.202416</t>
+  </si>
+  <si>
+    <t>17.09.202417</t>
+  </si>
+  <si>
+    <t>17.09.202418</t>
+  </si>
+  <si>
+    <t>17.09.202419</t>
+  </si>
+  <si>
+    <t>17.09.202420</t>
+  </si>
+  <si>
+    <t>17.09.202421</t>
+  </si>
+  <si>
+    <t>17.09.202422</t>
+  </si>
+  <si>
+    <t>17.09.202423</t>
+  </si>
+  <si>
+    <t>17.09.202424</t>
+  </si>
+  <si>
+    <t>18.09.20241</t>
+  </si>
+  <si>
+    <t>18.09.20242</t>
+  </si>
+  <si>
+    <t>18.09.20243</t>
+  </si>
+  <si>
+    <t>18.09.20244</t>
+  </si>
+  <si>
+    <t>18.09.20245</t>
+  </si>
+  <si>
+    <t>18.09.20246</t>
+  </si>
+  <si>
+    <t>18.09.20247</t>
+  </si>
+  <si>
+    <t>18.09.20248</t>
+  </si>
+  <si>
+    <t>18.09.20249</t>
+  </si>
+  <si>
+    <t>18.09.202410</t>
+  </si>
+  <si>
     <t>18.09.202411</t>
   </si>
   <si>
@@ -317,222 +533,6 @@
   </si>
   <si>
     <t>22.09.202411</t>
-  </si>
-  <si>
-    <t>22.09.202412</t>
-  </si>
-  <si>
-    <t>22.09.202413</t>
-  </si>
-  <si>
-    <t>22.09.202414</t>
-  </si>
-  <si>
-    <t>22.09.202415</t>
-  </si>
-  <si>
-    <t>22.09.202416</t>
-  </si>
-  <si>
-    <t>22.09.202417</t>
-  </si>
-  <si>
-    <t>22.09.202418</t>
-  </si>
-  <si>
-    <t>22.09.202419</t>
-  </si>
-  <si>
-    <t>22.09.202420</t>
-  </si>
-  <si>
-    <t>22.09.202421</t>
-  </si>
-  <si>
-    <t>22.09.202422</t>
-  </si>
-  <si>
-    <t>22.09.202423</t>
-  </si>
-  <si>
-    <t>22.09.202424</t>
-  </si>
-  <si>
-    <t>23.09.20241</t>
-  </si>
-  <si>
-    <t>23.09.20242</t>
-  </si>
-  <si>
-    <t>23.09.20243</t>
-  </si>
-  <si>
-    <t>23.09.20244</t>
-  </si>
-  <si>
-    <t>23.09.20245</t>
-  </si>
-  <si>
-    <t>23.09.20246</t>
-  </si>
-  <si>
-    <t>23.09.20247</t>
-  </si>
-  <si>
-    <t>23.09.20248</t>
-  </si>
-  <si>
-    <t>23.09.20249</t>
-  </si>
-  <si>
-    <t>23.09.202410</t>
-  </si>
-  <si>
-    <t>23.09.202411</t>
-  </si>
-  <si>
-    <t>23.09.202412</t>
-  </si>
-  <si>
-    <t>23.09.202413</t>
-  </si>
-  <si>
-    <t>23.09.202414</t>
-  </si>
-  <si>
-    <t>23.09.202415</t>
-  </si>
-  <si>
-    <t>23.09.202416</t>
-  </si>
-  <si>
-    <t>23.09.202417</t>
-  </si>
-  <si>
-    <t>23.09.202418</t>
-  </si>
-  <si>
-    <t>23.09.202419</t>
-  </si>
-  <si>
-    <t>23.09.202420</t>
-  </si>
-  <si>
-    <t>23.09.202421</t>
-  </si>
-  <si>
-    <t>23.09.202422</t>
-  </si>
-  <si>
-    <t>23.09.202423</t>
-  </si>
-  <si>
-    <t>23.09.202424</t>
-  </si>
-  <si>
-    <t>24.09.20241</t>
-  </si>
-  <si>
-    <t>24.09.20242</t>
-  </si>
-  <si>
-    <t>24.09.20243</t>
-  </si>
-  <si>
-    <t>24.09.20244</t>
-  </si>
-  <si>
-    <t>24.09.20245</t>
-  </si>
-  <si>
-    <t>24.09.20246</t>
-  </si>
-  <si>
-    <t>24.09.20247</t>
-  </si>
-  <si>
-    <t>24.09.20248</t>
-  </si>
-  <si>
-    <t>24.09.20249</t>
-  </si>
-  <si>
-    <t>24.09.202410</t>
-  </si>
-  <si>
-    <t>24.09.202411</t>
-  </si>
-  <si>
-    <t>24.09.202412</t>
-  </si>
-  <si>
-    <t>24.09.202413</t>
-  </si>
-  <si>
-    <t>24.09.202414</t>
-  </si>
-  <si>
-    <t>24.09.202415</t>
-  </si>
-  <si>
-    <t>24.09.202416</t>
-  </si>
-  <si>
-    <t>24.09.202417</t>
-  </si>
-  <si>
-    <t>24.09.202418</t>
-  </si>
-  <si>
-    <t>24.09.202419</t>
-  </si>
-  <si>
-    <t>24.09.202420</t>
-  </si>
-  <si>
-    <t>24.09.202421</t>
-  </si>
-  <si>
-    <t>24.09.202422</t>
-  </si>
-  <si>
-    <t>24.09.202423</t>
-  </si>
-  <si>
-    <t>24.09.202424</t>
-  </si>
-  <si>
-    <t>25.09.20241</t>
-  </si>
-  <si>
-    <t>25.09.20242</t>
-  </si>
-  <si>
-    <t>25.09.20243</t>
-  </si>
-  <si>
-    <t>25.09.20244</t>
-  </si>
-  <si>
-    <t>25.09.20245</t>
-  </si>
-  <si>
-    <t>25.09.20246</t>
-  </si>
-  <si>
-    <t>25.09.20247</t>
-  </si>
-  <si>
-    <t>25.09.20248</t>
-  </si>
-  <si>
-    <t>25.09.20249</t>
-  </si>
-  <si>
-    <t>25.09.202410</t>
-  </si>
-  <si>
-    <t>25.09.202411</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B4">
         <v>13</v>
       </c>
       <c r="C4">
-        <v>2.968</v>
+        <v>3.1</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B5">
         <v>14</v>
       </c>
       <c r="C5">
-        <v>2.466</v>
+        <v>3.155</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6">
-        <v>2.119</v>
+        <v>2.66</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
       <c r="C7">
-        <v>1.865</v>
+        <v>2.344</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B8">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>1.325</v>
+        <v>1.969</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>0.766</v>
+        <v>1.073</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B10">
         <v>19</v>
       </c>
       <c r="C10">
-        <v>0.172</v>
+        <v>0.344</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B11">
         <v>20</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.033</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B12">
         <v>21</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B13">
         <v>22</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B14">
         <v>23</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45553</v>
+        <v>45550</v>
       </c>
       <c r="B15">
         <v>24</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B23">
         <v>8</v>
       </c>
       <c r="C23">
-        <v>0.057</v>
+        <v>0.039</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B24">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0.51</v>
+        <v>0.18</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25">
-        <v>1.323</v>
+        <v>0.422</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B26">
         <v>11</v>
       </c>
       <c r="C26">
-        <v>1.792</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B27">
         <v>12</v>
       </c>
       <c r="C27">
-        <v>1.999</v>
+        <v>0.84</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B28">
         <v>13</v>
       </c>
       <c r="C28">
-        <v>2.074</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B29">
         <v>14</v>
       </c>
       <c r="C29">
-        <v>1.994</v>
+        <v>0.951</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B30">
         <v>15</v>
       </c>
       <c r="C30">
-        <v>1.892</v>
+        <v>1.005</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B31">
         <v>16</v>
       </c>
       <c r="C31">
-        <v>1.533</v>
+        <v>1.231</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B32">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>0.98</v>
+        <v>1.141</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B33">
         <v>18</v>
       </c>
       <c r="C33">
-        <v>0.482</v>
+        <v>0.71</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B34">
         <v>19</v>
       </c>
       <c r="C34">
-        <v>0.118</v>
+        <v>0.234</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B35">
         <v>20</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.022</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B36">
         <v>21</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B37">
         <v>22</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B38">
         <v>23</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45554</v>
+        <v>45551</v>
       </c>
       <c r="B39">
         <v>24</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B46">
         <v>7</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
       <c r="C47">
-        <v>0.047</v>
+        <v>0.04</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B48">
         <v>9</v>
       </c>
       <c r="C48">
-        <v>0.504</v>
+        <v>0.278</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B49">
         <v>10</v>
       </c>
       <c r="C49">
-        <v>1.232</v>
+        <v>0.732</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B50">
         <v>11</v>
       </c>
       <c r="C50">
-        <v>2.048</v>
+        <v>1.165</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B51">
         <v>12</v>
       </c>
       <c r="C51">
-        <v>2.794</v>
+        <v>1.562</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B52">
         <v>13</v>
       </c>
       <c r="C52">
-        <v>2.991</v>
+        <v>1.954</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B53">
         <v>14</v>
       </c>
       <c r="C53">
-        <v>3.078</v>
+        <v>2.005</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B54">
         <v>15</v>
       </c>
       <c r="C54">
-        <v>2.911</v>
+        <v>1.978</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B55">
         <v>16</v>
       </c>
       <c r="C55">
-        <v>2.677</v>
+        <v>1.653</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B56">
         <v>17</v>
       </c>
       <c r="C56">
-        <v>1.912</v>
+        <v>1.1</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
       <c r="C57">
-        <v>0.953</v>
+        <v>0.711</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B58">
         <v>19</v>
       </c>
       <c r="C58">
-        <v>0.249</v>
+        <v>0.177</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B59">
         <v>20</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B60">
         <v>21</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B61">
         <v>22</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B62">
         <v>23</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45555</v>
+        <v>45552</v>
       </c>
       <c r="B63">
         <v>24</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B67">
         <v>4</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B69">
         <v>6</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B70">
         <v>7</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B71">
         <v>8</v>
       </c>
       <c r="C71">
-        <v>0.057</v>
+        <v>0.038</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B72">
         <v>9</v>
       </c>
       <c r="C72">
-        <v>0.658</v>
+        <v>0.277</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B73">
         <v>10</v>
       </c>
       <c r="C73">
-        <v>1.613</v>
+        <v>0.728</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B74">
         <v>11</v>
       </c>
       <c r="C74">
-        <v>2.391</v>
+        <v>1.092</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B75">
         <v>12</v>
       </c>
       <c r="C75">
-        <v>2.836</v>
+        <v>1.338</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B76">
         <v>13</v>
       </c>
       <c r="C76">
-        <v>2.992</v>
+        <v>1.605</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B77">
         <v>14</v>
       </c>
       <c r="C77">
-        <v>3.078</v>
+        <v>1.79</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B78">
         <v>15</v>
       </c>
       <c r="C78">
-        <v>2.897</v>
+        <v>1.638</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B79">
         <v>16</v>
       </c>
       <c r="C79">
-        <v>2.579</v>
+        <v>1.429</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B80">
         <v>17</v>
       </c>
       <c r="C80">
-        <v>1.942</v>
+        <v>0.968</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B81">
         <v>18</v>
       </c>
       <c r="C81">
-        <v>1.094</v>
+        <v>0.543</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B82">
         <v>19</v>
       </c>
       <c r="C82">
-        <v>0.226</v>
+        <v>0.122</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B83">
         <v>20</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B84">
         <v>21</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B85">
         <v>22</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B86">
         <v>23</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45556</v>
+        <v>45553</v>
       </c>
       <c r="B87">
         <v>24</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B91">
         <v>4</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B92">
         <v>5</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B93">
         <v>6</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B94">
         <v>7</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B95">
         <v>8</v>
       </c>
       <c r="C95">
-        <v>0.057</v>
+        <v>0.043</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B96">
         <v>9</v>
       </c>
       <c r="C96">
-        <v>0.552</v>
+        <v>0.409</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B97">
         <v>10</v>
       </c>
       <c r="C97">
-        <v>1.483</v>
+        <v>1.029</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B98">
         <v>11</v>
       </c>
       <c r="C98">
-        <v>2.282</v>
+        <v>1.924</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B99">
         <v>12</v>
       </c>
       <c r="C99">
-        <v>2.798</v>
+        <v>2.333</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B100">
         <v>13</v>
       </c>
       <c r="C100">
-        <v>2.968</v>
+        <v>2.572</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B101">
         <v>14</v>
       </c>
       <c r="C101">
-        <v>2.988</v>
+        <v>2.647</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B102">
         <v>15</v>
       </c>
       <c r="C102">
-        <v>2.815</v>
+        <v>2.53</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B103">
         <v>16</v>
       </c>
       <c r="C103">
-        <v>2.285</v>
+        <v>2.204</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B104">
         <v>17</v>
       </c>
       <c r="C104">
-        <v>1.847</v>
+        <v>1.737</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B105">
         <v>18</v>
       </c>
       <c r="C105">
-        <v>0.897</v>
+        <v>0.831</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B106">
         <v>19</v>
       </c>
       <c r="C106">
-        <v>0.182</v>
+        <v>0.226</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B107">
         <v>20</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B108">
         <v>21</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B109">
         <v>22</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B110">
         <v>23</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45557</v>
+        <v>45554</v>
       </c>
       <c r="B111">
         <v>24</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B116">
         <v>5</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B117">
         <v>6</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B118">
         <v>7</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B119">
         <v>8</v>
       </c>
       <c r="C119">
-        <v>0.046</v>
+        <v>0.057</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B120">
         <v>9</v>
       </c>
       <c r="C120">
-        <v>0.483</v>
+        <v>0.656</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B121">
         <v>10</v>
       </c>
       <c r="C121">
-        <v>1.477</v>
+        <v>1.557</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B122">
         <v>11</v>
       </c>
       <c r="C122">
-        <v>2.143</v>
+        <v>2.391</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B123">
         <v>12</v>
       </c>
       <c r="C123">
-        <v>2.685</v>
+        <v>2.817</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B124">
         <v>13</v>
       </c>
       <c r="C124">
-        <v>2.913</v>
+        <v>3.068</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B125">
         <v>14</v>
       </c>
       <c r="C125">
-        <v>2.954</v>
+        <v>3.1</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B126">
         <v>15</v>
       </c>
       <c r="C126">
-        <v>2.774</v>
+        <v>2.901</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B127">
         <v>16</v>
       </c>
       <c r="C127">
-        <v>2.28</v>
+        <v>2.579</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B128">
         <v>17</v>
       </c>
       <c r="C128">
-        <v>1.777</v>
+        <v>1.942</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B129">
         <v>18</v>
       </c>
       <c r="C129">
-        <v>0.905</v>
+        <v>1.113</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B130">
         <v>19</v>
       </c>
       <c r="C130">
-        <v>0.152</v>
+        <v>0.3</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B131">
         <v>20</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.021</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B132">
         <v>21</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B133">
         <v>22</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B134">
         <v>23</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45558</v>
+        <v>45555</v>
       </c>
       <c r="B135">
         <v>24</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B137">
         <v>2</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B138">
         <v>3</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B139">
         <v>4</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B140">
         <v>5</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B141">
         <v>6</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B142">
         <v>7</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B143">
         <v>8</v>
       </c>
       <c r="C143">
-        <v>0.041</v>
+        <v>0.057</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B144">
         <v>9</v>
       </c>
       <c r="C144">
-        <v>0.428</v>
+        <v>0.553</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B145">
         <v>10</v>
       </c>
       <c r="C145">
-        <v>1.191</v>
+        <v>1.483</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B146">
         <v>11</v>
       </c>
       <c r="C146">
-        <v>2.113</v>
+        <v>2.282</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B147">
         <v>12</v>
       </c>
       <c r="C147">
-        <v>2.549</v>
+        <v>2.798</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B148">
         <v>13</v>
       </c>
       <c r="C148">
-        <v>2.853</v>
+        <v>2.974</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B149">
         <v>14</v>
       </c>
       <c r="C149">
-        <v>2.898</v>
+        <v>2.992</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B150">
         <v>15</v>
       </c>
       <c r="C150">
-        <v>2.772</v>
+        <v>2.833</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B151">
         <v>16</v>
       </c>
       <c r="C151">
-        <v>2.27</v>
+        <v>2.285</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B152">
         <v>17</v>
       </c>
       <c r="C152">
-        <v>1.774</v>
+        <v>1.92</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B153">
         <v>18</v>
       </c>
       <c r="C153">
-        <v>0.904</v>
+        <v>0.998</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B154">
         <v>19</v>
       </c>
       <c r="C154">
-        <v>0.14</v>
+        <v>0.179</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B155">
         <v>20</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B156">
         <v>21</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B157">
         <v>22</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B158">
         <v>23</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45559</v>
+        <v>45556</v>
       </c>
       <c r="B159">
         <v>24</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B161">
         <v>2</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B162">
         <v>3</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B163">
         <v>4</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B164">
         <v>5</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B165">
         <v>6</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B166">
         <v>7</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B167">
         <v>8</v>
       </c>
       <c r="C167">
-        <v>0.042</v>
+        <v>0.046</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B168">
         <v>9</v>
       </c>
       <c r="C168">
-        <v>0.395</v>
+        <v>0.552</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B169">
         <v>10</v>
       </c>
       <c r="C169">
-        <v>1.114</v>
+        <v>1.479</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45560</v>
+        <v>45557</v>
       </c>
       <c r="B170">
         <v>11</v>
       </c>
       <c r="C170">
-        <v>2.073</v>
+        <v>2.188</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>